<commit_message>
value prop banner advance padding admin system testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5215371-77F8-460C-9235-8C7C13AB35DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76C04C2-B457-4828-8B03-FC9321DCABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>DataSet</t>
   </si>
@@ -148,10 +148,25 @@
     <t>QATESTINGLOTUSWAVEpromocontent1</t>
   </si>
   <si>
-    <t>vraikanti@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Baprvtyfaqtt2!</t>
+    <t>avayugundla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ayuyjipqhf1!</t>
+  </si>
+  <si>
+    <t>Valuepropbanner</t>
+  </si>
+  <si>
+    <t>valuepropcard2</t>
+  </si>
+  <si>
+    <t>valuepropcard3</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
   </si>
 </sst>
 </file>
@@ -540,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +781,102 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4">
+        <v>25</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4">
+        <v>30</v>
+      </c>
+      <c r="V4">
+        <v>35</v>
+      </c>
+      <c r="W4">
+        <v>32</v>
+      </c>
+      <c r="X4">
+        <v>23</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <v>32</v>
+      </c>
+      <c r="S5">
+        <v>22</v>
+      </c>
+      <c r="T5">
+        <v>12</v>
+      </c>
+      <c r="U5">
+        <v>23</v>
+      </c>
+      <c r="V5">
+        <v>20</v>
+      </c>
+      <c r="W5">
+        <v>32</v>
+      </c>
+      <c r="X5">
+        <v>21</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6">
+        <v>32</v>
+      </c>
+      <c r="R6">
+        <v>34</v>
+      </c>
+      <c r="S6">
+        <v>54</v>
+      </c>
+      <c r="T6">
+        <v>21</v>
+      </c>
+      <c r="U6">
+        <v>13</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>12</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
close all uncomments admin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76C04C2-B457-4828-8B03-FC9321DCABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1BF78A-39D0-4CD9-A5D4-C5D084C94DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1710" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -148,12 +148,6 @@
     <t>QATESTINGLOTUSWAVEpromocontent1</t>
   </si>
   <si>
-    <t>avayugundla@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Ayuyjipqhf1!</t>
-  </si>
-  <si>
     <t>Valuepropbanner</t>
   </si>
   <si>
@@ -167,6 +161,12 @@
   </si>
   <si>
     <t>testing2</t>
+  </si>
+  <si>
+    <t>vraikanti@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Baprvtyfaqtt2!</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,10 +698,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -783,7 +783,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q4">
         <v>25</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q5">
         <v>12</v>
@@ -842,12 +842,12 @@
         <v>21</v>
       </c>
       <c r="Y5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q6">
         <v>32</v>
@@ -874,7 +874,7 @@
         <v>12</v>
       </c>
       <c r="Y6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -882,7 +882,7 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{33154F04-32FD-49D7-83B8-F24B45A21135}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{48A24322-C31B-44BB-AF56-D96437544032}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
PLP CMS Block test case commit helper, tetsdata,tetscase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1BF78A-39D0-4CD9-A5D4-C5D084C94DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0F1BF78A-39D0-4CD9-A5D4-C5D084C94DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D56382-1E63-4220-9FBF-073C28192DC5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1710" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
+    <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
   <si>
     <t>DataSet</t>
   </si>
@@ -167,13 +168,406 @@
   </si>
   <si>
     <t>Baprvtyfaqtt2!</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>customergroupname</t>
+  </si>
+  <si>
+    <t>Updatecustomergroupname</t>
+  </si>
+  <si>
+    <t>errormessage</t>
+  </si>
+  <si>
+    <t>Tiletext</t>
+  </si>
+  <si>
+    <t>textbutton</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>CategorySelect</t>
+  </si>
+  <si>
+    <t>productnames</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>CardTitle</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>image2</t>
+  </si>
+  <si>
+    <t>Buttontext</t>
+  </si>
+  <si>
+    <t>Buttontype</t>
+  </si>
+  <si>
+    <t>ButtonLinknavigation</t>
+  </si>
+  <si>
+    <t>ButtonlinkURL</t>
+  </si>
+  <si>
+    <t>Buttonlinkcategory</t>
+  </si>
+  <si>
+    <t>Buttonlinkproduct</t>
+  </si>
+  <si>
+    <t>Buttonlinkpage</t>
+  </si>
+  <si>
+    <t>Categorydisplay</t>
+  </si>
+  <si>
+    <t>No.ofproductsdisplay</t>
+  </si>
+  <si>
+    <t>productcategory</t>
+  </si>
+  <si>
+    <t>Editpagetitle</t>
+  </si>
+  <si>
+    <t>datacontenttype</t>
+  </si>
+  <si>
+    <t>Deletcomponent</t>
+  </si>
+  <si>
+    <t>headingtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description Type</t>
+  </si>
+  <si>
+    <t>alterantivetext</t>
+  </si>
+  <si>
+    <t>titleaatribute</t>
+  </si>
+  <si>
+    <t>Customergrouppagetitle</t>
+  </si>
+  <si>
+    <t>MYAccountlinks</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Productname</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>CTA Type</t>
+  </si>
+  <si>
+    <t>CTA Link</t>
+  </si>
+  <si>
+    <t>CTAText</t>
+  </si>
+  <si>
+    <t>CTAurl</t>
+  </si>
+  <si>
+    <t>categoryname</t>
+  </si>
+  <si>
+    <t>SubTitle</t>
+  </si>
+  <si>
+    <t>ChooseCondition</t>
+  </si>
+  <si>
+    <t>nmanuka@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Acxbynsvtbqe1!</t>
+  </si>
+  <si>
+    <t>pagetitle</t>
+  </si>
+  <si>
+    <t>mkoppanadam@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Acyqadtkonic1!</t>
+  </si>
+  <si>
+    <t>Customer Login,Create New Customer Account,Orders and Returns</t>
+  </si>
+  <si>
+    <t>Sign In,Create an Account,Track my order</t>
+  </si>
+  <si>
+    <t>CTAElements</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVE</t>
+  </si>
+  <si>
+    <t>QAHYDRO</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com/QATestingHydro</t>
+  </si>
+  <si>
+    <t>ProductcardTile</t>
+  </si>
+  <si>
+    <t>The page is for Testing only.</t>
+  </si>
+  <si>
+    <t>LOTUSQATITLE</t>
+  </si>
+  <si>
+    <t>LOTUSQABUTTON</t>
+  </si>
+  <si>
+    <t>m-media-card</t>
+  </si>
+  <si>
+    <t>tiles__wrapper</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>32-oz-wide-mouth-copper-brown,32-oz-wide-mouth-everest-blue,32-oz-wide-mouth-acai-purple</t>
+  </si>
+  <si>
+    <t>Price: high to low</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>QATesting</t>
+  </si>
+  <si>
+    <t>cms-corporate-</t>
+  </si>
+  <si>
+    <t>QATEST</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com/shop/bottles-drinkware/bottles.html</t>
+  </si>
+  <si>
+    <t>Outdoor Kitchen</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Acai Purple</t>
+  </si>
+  <si>
+    <t>Test Page PT</t>
+  </si>
+  <si>
+    <t>Cups &amp; Tumblers,Food Jars</t>
+  </si>
+  <si>
+    <t>Bottles</t>
+  </si>
+  <si>
+    <t>Edit Card Tiles</t>
+  </si>
+  <si>
+    <t>hot_card_tiles</t>
+  </si>
+  <si>
+    <t>hot-card-tiles</t>
+  </si>
+  <si>
+    <t>qatestalt</t>
+  </si>
+  <si>
+    <t>qatesttitle</t>
+  </si>
+  <si>
+    <t>W32075,W32410,W32520,1115580,1165700,1071499B</t>
+  </si>
+  <si>
+    <t>#a8d098</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEPRODUCTCARDTILE</t>
+  </si>
+  <si>
+    <t>OXOproducttile</t>
+  </si>
+  <si>
+    <t>oxo-10-piece-pop-container-set,3-piece-mixing-bowl-set-colored-handles,cherry-olive-pitter</t>
+  </si>
+  <si>
+    <t>cms-corporate-pur</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/shop/kitchenware/pop-containers.html</t>
+  </si>
+  <si>
+    <t>POP Containers</t>
+  </si>
+  <si>
+    <t>POP Container Set</t>
+  </si>
+  <si>
+    <t>Test Page</t>
+  </si>
+  <si>
+    <t>POP Containers,Cookware &amp; Bakeware Sets</t>
+  </si>
+  <si>
+    <t>#a8d099</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-preprod.oxo.com/</t>
+  </si>
+  <si>
+    <t>PLPBLOCK</t>
+  </si>
+  <si>
+    <t>Thi PLP Block is to configure and validate on the front end</t>
+  </si>
+  <si>
+    <t>plp-block</t>
+  </si>
+  <si>
+    <t>c-plp-cms-block</t>
+  </si>
+  <si>
+    <t>qatest123</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>Screenshot_1.png</t>
+  </si>
+  <si>
+    <t>Screenshot_1_1.png</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Edit PLP Block</t>
+  </si>
+  <si>
+    <t>hot_plp_block</t>
+  </si>
+  <si>
+    <t>type-wrapper</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>QATESTtitle</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEPLPBLOCK</t>
+  </si>
+  <si>
+    <t>Qatest2</t>
+  </si>
+  <si>
+    <t>message_3.png</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>OXOPLPBLOCK</t>
+  </si>
+  <si>
+    <t>qatest124</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>CLPHerobanner</t>
+  </si>
+  <si>
+    <t>Lotus Testing the CLP Hero banner</t>
+  </si>
+  <si>
+    <t>c-clp-hero</t>
+  </si>
+  <si>
+    <t>Lotusqa.png</t>
+  </si>
+  <si>
+    <t>Edit CLP Hero Banner</t>
+  </si>
+  <si>
+    <t>hot_clp_banner</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>QALOTUSTEST</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVECLPHEROBANNER</t>
+  </si>
+  <si>
+    <t>OXOCLPHerobanner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +598,27 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -274,6 +689,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,66 +981,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +1117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -710,7 +1134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -781,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -813,7 +1237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -845,7 +1269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -887,4 +1311,1122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB5A4B-EC66-4209-8F6B-550483823EC8}">
+  <dimension ref="A1:BX10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:76" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="BT1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="BU1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="BV1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="BW1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BX1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+    </row>
+    <row r="3" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="BA4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC4" s="7"/>
+      <c r="BI4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BJ4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="BL4">
+        <v>25</v>
+      </c>
+      <c r="BM4">
+        <v>27</v>
+      </c>
+      <c r="BN4">
+        <v>15</v>
+      </c>
+      <c r="BO4">
+        <v>10</v>
+      </c>
+      <c r="BP4">
+        <v>30</v>
+      </c>
+      <c r="BQ4">
+        <v>35</v>
+      </c>
+      <c r="BR4">
+        <v>32</v>
+      </c>
+      <c r="BS4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:76" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>118</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR5" s="2"/>
+      <c r="AS5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BL5">
+        <v>25</v>
+      </c>
+      <c r="BM5">
+        <v>27</v>
+      </c>
+      <c r="BN5">
+        <v>15</v>
+      </c>
+      <c r="BO5">
+        <v>10</v>
+      </c>
+      <c r="BP5">
+        <v>30</v>
+      </c>
+      <c r="BQ5">
+        <v>35</v>
+      </c>
+      <c r="BR5">
+        <v>32</v>
+      </c>
+      <c r="BS5">
+        <v>23</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:76" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="J6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P6" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>118</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR6" s="2"/>
+      <c r="AX6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BL6">
+        <v>25</v>
+      </c>
+      <c r="BM6">
+        <v>27</v>
+      </c>
+      <c r="BN6">
+        <v>15</v>
+      </c>
+      <c r="BO6">
+        <v>10</v>
+      </c>
+      <c r="BP6">
+        <v>30</v>
+      </c>
+      <c r="BQ6">
+        <v>35</v>
+      </c>
+      <c r="BR6">
+        <v>32</v>
+      </c>
+      <c r="BS6">
+        <v>23</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" t="s">
+        <v>155</v>
+      </c>
+      <c r="X7" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="BA7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BL7">
+        <v>25</v>
+      </c>
+      <c r="BM7">
+        <v>27</v>
+      </c>
+      <c r="BN7">
+        <v>15</v>
+      </c>
+      <c r="BO7">
+        <v>10</v>
+      </c>
+      <c r="BP7">
+        <v>30</v>
+      </c>
+      <c r="BQ7">
+        <v>35</v>
+      </c>
+      <c r="BR7">
+        <v>32</v>
+      </c>
+      <c r="BS7">
+        <v>23</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="BA8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC8" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AM9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AQ9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AZ9" s="12"/>
+      <c r="BA9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BB9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC9" s="2"/>
+      <c r="BL9">
+        <v>25</v>
+      </c>
+      <c r="BM9">
+        <v>27</v>
+      </c>
+      <c r="BN9">
+        <v>15</v>
+      </c>
+      <c r="BO9">
+        <v>10</v>
+      </c>
+      <c r="BP9">
+        <v>30</v>
+      </c>
+      <c r="BQ9">
+        <v>35</v>
+      </c>
+      <c r="BR9">
+        <v>32</v>
+      </c>
+      <c r="BS9">
+        <v>23</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC10" s="13"/>
+      <c r="AR10" s="2"/>
+      <c r="BA10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BC10" s="2"/>
+      <c r="BL10">
+        <v>25</v>
+      </c>
+      <c r="BM10">
+        <v>27</v>
+      </c>
+      <c r="BN10">
+        <v>15</v>
+      </c>
+      <c r="BO10">
+        <v>10</v>
+      </c>
+      <c r="BP10">
+        <v>30</v>
+      </c>
+      <c r="BQ10">
+        <v>35</v>
+      </c>
+      <c r="BR10">
+        <v>32</v>
+      </c>
+      <c r="BS10">
+        <v>23</v>
+      </c>
+      <c r="BT10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D80F0928-8295-4AEE-BB44-407350F797C6}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{DA1131E6-3937-4FBF-8346-6A69C93730B1}"/>
+    <hyperlink ref="BJ4" r:id="rId3" xr:uid="{281E9B47-22C0-48F3-AC83-70FAB4BCE947}"/>
+    <hyperlink ref="BB4" r:id="rId4" xr:uid="{F2CB3DD1-8289-4BBB-B2B7-8060F0AA781E}"/>
+    <hyperlink ref="AB5" r:id="rId5" xr:uid="{2C7FBA0B-B216-4CF9-8BAC-41AD7F102B25}"/>
+    <hyperlink ref="BB5" r:id="rId6" xr:uid="{D3439697-9288-4322-A017-1FE7908E0A5D}"/>
+    <hyperlink ref="R5" r:id="rId7" xr:uid="{EE609DB9-C125-4457-9565-F46E3725F39C}"/>
+    <hyperlink ref="BC5" r:id="rId8" xr:uid="{473B1FFE-1414-4AD1-89D8-C2DAD5613F02}"/>
+    <hyperlink ref="AB6" r:id="rId9" xr:uid="{B180B19F-6548-4964-B383-80264FCEDDBA}"/>
+    <hyperlink ref="BB6" r:id="rId10" xr:uid="{26A11598-6614-4E41-8637-FC98158A27B6}"/>
+    <hyperlink ref="R6" r:id="rId11" xr:uid="{F4E34AA6-8DB2-4BDC-89B0-03CBF14C13EF}"/>
+    <hyperlink ref="BC6" r:id="rId12" xr:uid="{F75F9212-AD3E-4382-8794-8F5AE650A30B}"/>
+    <hyperlink ref="R7" r:id="rId13" xr:uid="{8C8BA6DD-9026-4E25-ABE4-7DA69D5973BA}"/>
+    <hyperlink ref="BC7" r:id="rId14" xr:uid="{C58BF9BB-7FEF-488A-BBF6-25ADF711D56D}"/>
+    <hyperlink ref="BB7" r:id="rId15" xr:uid="{49419B2B-1A8A-4D39-A05F-72D614FF021D}"/>
+    <hyperlink ref="AB7" r:id="rId16" xr:uid="{DB9290EF-C8F5-48B6-836C-DE58F6DE870D}"/>
+    <hyperlink ref="BB9" r:id="rId17" xr:uid="{1813D67C-9103-4D48-B5E7-568F95782DE7}"/>
+    <hyperlink ref="BB10" r:id="rId18" xr:uid="{EEFCA7A0-4794-4921-A2AD-8B837E7B4E00}"/>
+    <hyperlink ref="BB8" r:id="rId19" xr:uid="{BA55DAE3-26DE-4483-9D99-476BAA07D329}"/>
+    <hyperlink ref="BC8" r:id="rId20" xr:uid="{63F28980-77E8-441A-8D70-BC7A973201D4}"/>
+    <hyperlink ref="AB8" r:id="rId21" xr:uid="{0956164A-8716-4318-84DD-834A226F0770}"/>
+    <hyperlink ref="R8" r:id="rId22" xr:uid="{A0FCE175-3799-458D-9EEA-CC4B72494EB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Admin herobanner test case, helper, testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0F1BF78A-39D0-4CD9-A5D4-C5D084C94DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D56382-1E63-4220-9FBF-073C28192DC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56755E47-5DB8-4BDD-A8F1-C91C5E93642F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
     <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
+    <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="218">
   <si>
     <t>DataSet</t>
   </si>
@@ -561,12 +562,129 @@
   </si>
   <si>
     <t>OXOCLPHerobanner</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>SegmentName</t>
+  </si>
+  <si>
+    <t>taxclass</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>ApplyTo</t>
+  </si>
+  <si>
+    <t>AssignedStatus</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Welcome Email</t>
+  </si>
+  <si>
+    <t>ProDeal</t>
+  </si>
+  <si>
+    <t>Acceptdate</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Phonenumber</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>ordernumber</t>
+  </si>
+  <si>
+    <t>Herobanner</t>
+  </si>
+  <si>
+    <t>QA Testing Hero Banner</t>
+  </si>
+  <si>
+    <t>32 OZ WIDE MOUTH STAINLESS</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>QA test Hero Banner</t>
+  </si>
+  <si>
+    <t>Test Banner</t>
+  </si>
+  <si>
+    <t>HydroFlask</t>
+  </si>
+  <si>
+    <t>Right Alignment</t>
+  </si>
+  <si>
+    <t>qaFlask</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>HYDROFLASK</t>
+  </si>
+  <si>
+    <t>QaTester</t>
+  </si>
+  <si>
+    <t>TestingHydro</t>
+  </si>
+  <si>
+    <t>Amtlmcflmipq1!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -677,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -698,6 +816,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,7 +1438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB5A4B-EC66-4209-8F6B-550483823EC8}">
   <dimension ref="A1:BX10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -2429,4 +2550,474 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B278CB69-F3ED-4115-B521-97E3E0FC6D90}">
+  <dimension ref="A1:CU3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CI1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CJ1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="CK1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="CM1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="CN1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="CO1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CQ1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="CR1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="CS1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="CT1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV2" s="2"/>
+      <c r="AW2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AY2" s="2"/>
+      <c r="BR2" s="14"/>
+      <c r="BS2" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="BT2" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="CA2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="CB2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="CC2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CG2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CI2">
+        <v>12</v>
+      </c>
+      <c r="CJ2">
+        <v>13</v>
+      </c>
+      <c r="CK2">
+        <v>14</v>
+      </c>
+      <c r="CL2">
+        <v>15</v>
+      </c>
+      <c r="CM2">
+        <v>16</v>
+      </c>
+      <c r="CN2">
+        <v>11</v>
+      </c>
+      <c r="CO2">
+        <v>17</v>
+      </c>
+      <c r="CP2">
+        <v>10</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>13</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>215</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>215</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{4ECB1189-452C-417A-A16B-ABA88FA414D9}"/>
+    <hyperlink ref="BY2" r:id="rId2" xr:uid="{3D679BEE-97C8-4868-B708-1A4E8F6C42B4}"/>
+    <hyperlink ref="BZ2" r:id="rId3" xr:uid="{6ADB74A0-C7FE-4B08-9EF3-111224C3CF8B}"/>
+    <hyperlink ref="CG2" r:id="rId4" xr:uid="{06A155BF-8092-479E-9FF6-C50BDB8682C9}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{A76F3705-53DF-4E1C-9A2A-9DCEC1A82E34}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Admin Category Product Slider Helper,Test case and Test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56755E47-5DB8-4BDD-A8F1-C91C5E93642F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EB11F-66D0-4783-9724-BA31471269AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
     <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
+    <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="229">
   <si>
     <t>DataSet</t>
   </si>
@@ -676,6 +677,39 @@
   </si>
   <si>
     <t>Amtlmcflmipq1!</t>
+  </si>
+  <si>
+    <t>Sortby</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown</t>
+  </si>
+  <si>
+    <t>Categorydetails</t>
+  </si>
+  <si>
+    <t>QATESTING</t>
+  </si>
+  <si>
+    <t>CategoryProducts</t>
+  </si>
+  <si>
+    <t>Bottles &amp; Drinkware</t>
+  </si>
+  <si>
+    <t>HYDROFLASK QA TESTING</t>
+  </si>
+  <si>
+    <t>Qa Testing</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEProductSlider</t>
+  </si>
+  <si>
+    <t>less than</t>
   </si>
 </sst>
 </file>
@@ -685,7 +719,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +775,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -795,7 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -819,6 +859,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1106,62 +1147,62 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" customWidth="1"/>
-    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.77734375" customWidth="1"/>
+    <col min="12" max="12" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.77734375" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1279,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1255,7 +1296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1358,7 +1399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1390,7 +1431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1442,14 +1483,14 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:76" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1720,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1733,7 +1774,7 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1789,7 +1830,7 @@
       </c>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1868,7 +1909,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:76" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2008,7 +2049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:76" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:76" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2137,7 +2178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -2274,7 +2315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -2369,7 +2410,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -2470,7 +2511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -2556,13 +2597,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B278CB69-F3ED-4115-B521-97E3E0FC6D90}">
   <dimension ref="A1:CU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2861,7 +2902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -2999,7 +3040,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3020,4 +3061,778 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424A69D1-55C8-43D3-BFB0-720A34E1B905}">
+  <dimension ref="A1:CW6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CI1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="CJ1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="CK1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="CM1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="CN1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="CO1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="CQ1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="CR1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="CS1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="CT1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="CW1" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+    </row>
+    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R3" t="s">
+        <v>112</v>
+      </c>
+      <c r="S3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="W3" t="s">
+        <v>117</v>
+      </c>
+      <c r="X3" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AY3" s="2"/>
+      <c r="BB3" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BU3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="BW3" s="10"/>
+      <c r="BX3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BY3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BZ3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="CI3">
+        <v>25</v>
+      </c>
+      <c r="CJ3">
+        <v>27</v>
+      </c>
+      <c r="CK3">
+        <v>15</v>
+      </c>
+      <c r="CL3">
+        <v>10</v>
+      </c>
+      <c r="CM3">
+        <v>30</v>
+      </c>
+      <c r="CN3">
+        <v>35</v>
+      </c>
+      <c r="CO3">
+        <v>32</v>
+      </c>
+      <c r="CP3">
+        <v>23</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>13</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="U4" t="s">
+        <v>118</v>
+      </c>
+      <c r="V4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>216</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>123</v>
+      </c>
+      <c r="CG4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>214</v>
+      </c>
+      <c r="CI4">
+        <v>25</v>
+      </c>
+      <c r="CJ4">
+        <v>27</v>
+      </c>
+      <c r="CK4">
+        <v>15</v>
+      </c>
+      <c r="CL4">
+        <v>10</v>
+      </c>
+      <c r="CM4">
+        <v>30</v>
+      </c>
+      <c r="CN4">
+        <v>35</v>
+      </c>
+      <c r="CO4">
+        <v>32</v>
+      </c>
+      <c r="CP4">
+        <v>23</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="U5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>226</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>227</v>
+      </c>
+      <c r="BZ5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="CI5">
+        <v>55</v>
+      </c>
+      <c r="CJ5">
+        <v>27</v>
+      </c>
+      <c r="CK5">
+        <v>15</v>
+      </c>
+      <c r="CL5">
+        <v>10</v>
+      </c>
+      <c r="CM5">
+        <v>30</v>
+      </c>
+      <c r="CN5">
+        <v>35</v>
+      </c>
+      <c r="CO5">
+        <v>32</v>
+      </c>
+      <c r="CP5">
+        <v>23</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT5" t="s">
+        <v>226</v>
+      </c>
+      <c r="CU5" t="s">
+        <v>219</v>
+      </c>
+      <c r="CW5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="Y6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV6" s="2"/>
+      <c r="AW6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AY6" s="2"/>
+      <c r="BR6" s="14"/>
+      <c r="BS6" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="BT6" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>17</v>
+      </c>
+      <c r="BX6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BY6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BZ6" s="2"/>
+      <c r="CA6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="CB6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="CC6" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CI6">
+        <v>25</v>
+      </c>
+      <c r="CJ6">
+        <v>27</v>
+      </c>
+      <c r="CK6">
+        <v>15</v>
+      </c>
+      <c r="CL6">
+        <v>10</v>
+      </c>
+      <c r="CM6">
+        <v>30</v>
+      </c>
+      <c r="CN6">
+        <v>35</v>
+      </c>
+      <c r="CO6">
+        <v>32</v>
+      </c>
+      <c r="CP6">
+        <v>23</v>
+      </c>
+      <c r="CQ6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DF83D5E4-D7A4-40AE-BADA-7B6F01513272}"/>
+    <hyperlink ref="AH3" r:id="rId2" xr:uid="{BAEF4C00-5796-47C6-AAC0-103BF25B5854}"/>
+    <hyperlink ref="BY3" r:id="rId3" xr:uid="{CA68FB99-4694-4F39-9CC8-C7DC06D07519}"/>
+    <hyperlink ref="Y3" r:id="rId4" xr:uid="{4B76FD30-B042-41B3-B10A-EE82AEE749A0}"/>
+    <hyperlink ref="BZ3" r:id="rId5" xr:uid="{4F54752F-4912-4C7B-81BD-70AB736EC114}"/>
+    <hyperlink ref="CG4" r:id="rId6" xr:uid="{F2C46F32-F6AF-4880-838A-9D5F8D6C20BF}"/>
+    <hyperlink ref="BZ5" r:id="rId7" xr:uid="{034D436D-5CFE-4100-A9A4-36E66EF0A42C}"/>
+    <hyperlink ref="Y6" r:id="rId8" xr:uid="{6B061070-193D-4958-8A43-25D72940BAEF}"/>
+    <hyperlink ref="BY6" r:id="rId9" xr:uid="{45984C68-C2C1-4033-B146-62097928B16E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Admin Catalog Product Update-Testcase,Helper,Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EB11F-66D0-4783-9724-BA31471269AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BEFCA3-CB30-4227-88DE-07E066E72794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
     <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="246">
   <si>
     <t>DataSet</t>
   </si>
@@ -710,6 +711,57 @@
   </si>
   <si>
     <t>less than</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Updateproductname</t>
+  </si>
+  <si>
+    <t>Stock Status</t>
+  </si>
+  <si>
+    <t>Updateprice</t>
+  </si>
+  <si>
+    <t>updateStock Status</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>QATEST product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 QATEST product </t>
+  </si>
+  <si>
+    <t>Out of Stock</t>
+  </si>
+  <si>
+    <t>In Stock</t>
+  </si>
+  <si>
+    <t>Lowest Price</t>
+  </si>
+  <si>
+    <t>Productupdate</t>
+  </si>
+  <si>
+    <t>Bottles,POP Containers</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com//</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Home Page (Hydroflask)</t>
   </si>
 </sst>
 </file>
@@ -1147,62 +1199,62 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.77734375" customWidth="1"/>
-    <col min="12" max="12" width="54.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1331,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1296,7 +1348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1367,7 +1419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1399,7 +1451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1431,7 +1483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1483,14 +1535,14 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:76" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1720,7 +1772,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +1826,7 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1830,7 +1882,7 @@
       </c>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1909,7 +1961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:76" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2049,7 +2101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:76" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2178,7 +2230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -2315,7 +2367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -2410,7 +2462,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -2511,7 +2563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -2601,9 +2653,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +2954,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -3040,7 +3092,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3067,13 +3119,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424A69D1-55C8-43D3-BFB0-720A34E1B905}">
   <dimension ref="A1:CW6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3378,7 +3430,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3444,7 +3496,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3586,7 +3638,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -3651,7 +3703,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>223</v>
       </c>
@@ -3707,7 +3759,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -3835,4 +3887,438 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1682-39F3-49F0-A5E3-7423827666C1}">
+  <dimension ref="A1:DB4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>237</v>
+      </c>
+      <c r="CX2">
+        <v>5</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>238</v>
+      </c>
+      <c r="CZ2">
+        <v>30</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>241</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>242</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>235</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>243</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>40</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>237</v>
+      </c>
+      <c r="CX3">
+        <v>5</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>238</v>
+      </c>
+      <c r="CZ3">
+        <v>30</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>244</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>236</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>245</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>243</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Category cared tiles code commit - helper,testdata,testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BEFCA3-CB30-4227-88DE-07E066E72794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{08BEFCA3-CB30-4227-88DE-07E066E72794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AE125B0-C824-457C-8E05-9816ACDB4720}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="customer" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="290">
   <si>
     <t>DataSet</t>
   </si>
@@ -461,9 +462,6 @@
     <t>Test Page</t>
   </si>
   <si>
-    <t>POP Containers,Cookware &amp; Bakeware Sets</t>
-  </si>
-  <si>
     <t>#a8d099</t>
   </si>
   <si>
@@ -762,6 +760,141 @@
   </si>
   <si>
     <t>Home Page (Hydroflask)</t>
+  </si>
+  <si>
+    <t>POP Containers,Cooking &amp; Baking</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>honeywelltest159@gmail.com</t>
+  </si>
+  <si>
+    <t>Hydroflask Website</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>12/5/1995</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Hydroflask Store/Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>7/8/2022</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>844 N colony rd</t>
+  </si>
+  <si>
+    <t>wallingford</t>
+  </si>
+  <si>
+    <t>06492</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>1256233</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>1526</t>
+  </si>
+  <si>
+    <t>Whishlist</t>
+  </si>
+  <si>
+    <t>32 oz</t>
+  </si>
+  <si>
+    <t>Customer Segment</t>
+  </si>
+  <si>
+    <t>QA Test Test</t>
+  </si>
+  <si>
+    <t>Visitors and Registered Customers</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Test Test</t>
+  </si>
+  <si>
+    <t>CustomerGroup</t>
+  </si>
+  <si>
+    <t>QA Testing Lotuswave</t>
+  </si>
+  <si>
+    <t>QA_Testing_Lotuswave</t>
+  </si>
+  <si>
+    <t>Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>Createcustomergroup</t>
+  </si>
+  <si>
+    <t>Retail Customer</t>
+  </si>
+  <si>
+    <t>You saved the customer group.</t>
+  </si>
+  <si>
+    <t>New Customer Group / Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>UpdatecustomerGroup</t>
+  </si>
+  <si>
+    <t>QA Testing Lotuswave / Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>DeleteCustomergroup</t>
+  </si>
+  <si>
+    <t>You deleted the customer group.</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Hydroflask Website,OXO Website</t>
   </si>
 </sst>
 </file>
@@ -771,7 +904,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,6 +966,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -887,7 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -906,12 +1045,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1199,62 +1344,62 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1476,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1348,7 +1493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1451,7 +1596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1483,7 +1628,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1529,20 +1674,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB5A4B-EC66-4209-8F6B-550483823EC8}">
-  <dimension ref="A1:BX10"/>
+  <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.453125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.90625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1601,178 +1758,139 @@
         <v>61</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="BT1" s="6" t="s">
+      <c r="BK1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="BU1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="BV1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="BW1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="BX1" s="6" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1816,17 +1934,13 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
+      <c r="AM2" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1870,19 +1984,15 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
+      <c r="AM3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1919,49 +2029,45 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-      <c r="BA4" s="2" t="s">
+      <c r="AR4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="BB4" s="7" t="s">
+      <c r="AS4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="BC4" s="7"/>
-      <c r="BI4" t="s">
+      <c r="AT4" s="7"/>
+      <c r="AZ4" t="s">
         <v>107</v>
       </c>
-      <c r="BJ4" s="7" t="s">
+      <c r="BA4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="BL4">
+      <c r="BC4">
         <v>25</v>
       </c>
-      <c r="BM4">
+      <c r="BD4">
         <v>27</v>
       </c>
-      <c r="BN4">
+      <c r="BE4">
         <v>15</v>
       </c>
-      <c r="BO4">
+      <c r="BF4">
         <v>10</v>
       </c>
-      <c r="BP4">
+      <c r="BG4">
         <v>30</v>
       </c>
-      <c r="BQ4">
+      <c r="BH4">
         <v>35</v>
       </c>
-      <c r="BR4">
+      <c r="BI4">
         <v>32</v>
       </c>
-      <c r="BS4">
+      <c r="BJ4">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:76" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2001,107 +2107,103 @@
       <c r="S5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="8" t="s">
+      <c r="T5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8" t="s">
+      <c r="U5" s="8"/>
+      <c r="V5" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="Y5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="AB5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD5" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>3</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>3</v>
+        <v>130</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AN5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="AO5" s="2" t="s">
+      <c r="AL5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AR5" s="2"/>
-      <c r="AS5" t="s">
+      <c r="AN5" s="2"/>
+      <c r="AO5" t="s">
         <v>25</v>
       </c>
+      <c r="AP5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="AT5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AX5" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ5" s="10"/>
-      <c r="BA5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="BC5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="BL5">
+      <c r="BC5">
         <v>25</v>
       </c>
-      <c r="BM5">
+      <c r="BD5">
         <v>27</v>
       </c>
-      <c r="BN5">
+      <c r="BE5">
         <v>15</v>
       </c>
-      <c r="BO5">
+      <c r="BF5">
         <v>10</v>
       </c>
-      <c r="BP5">
+      <c r="BG5">
         <v>30</v>
       </c>
-      <c r="BQ5">
+      <c r="BH5">
         <v>35</v>
       </c>
-      <c r="BR5">
+      <c r="BI5">
         <v>32</v>
       </c>
-      <c r="BS5">
+      <c r="BJ5">
         <v>23</v>
       </c>
-      <c r="BT5" t="s">
+      <c r="BK5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:76" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2136,106 +2238,102 @@
       <c r="S6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="8" t="s">
+      <c r="T6" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8" t="s">
+      <c r="U6" s="8"/>
+      <c r="V6" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="X6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="AA6" s="2" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC6" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>3</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="AF6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN6" s="2"/>
+      <c r="AQ6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AG6" s="2">
-        <v>3</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AN6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AR6" s="2"/>
-      <c r="AX6" s="2" t="s">
+      <c r="AR6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AZ6" s="10"/>
-      <c r="BA6" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BB6" s="2" t="s">
+      <c r="AT6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="BC6" s="2" t="s">
+      <c r="BC6">
+        <v>25</v>
+      </c>
+      <c r="BD6">
+        <v>27</v>
+      </c>
+      <c r="BE6">
+        <v>15</v>
+      </c>
+      <c r="BF6">
+        <v>10</v>
+      </c>
+      <c r="BG6">
+        <v>30</v>
+      </c>
+      <c r="BH6">
+        <v>35</v>
+      </c>
+      <c r="BI6">
+        <v>32</v>
+      </c>
+      <c r="BJ6">
+        <v>23</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>148</v>
       </c>
-      <c r="BL6">
-        <v>25</v>
-      </c>
-      <c r="BM6">
-        <v>27</v>
-      </c>
-      <c r="BN6">
-        <v>15</v>
-      </c>
-      <c r="BO6">
-        <v>10</v>
-      </c>
-      <c r="BP6">
-        <v>30</v>
-      </c>
-      <c r="BQ6">
-        <v>35</v>
-      </c>
-      <c r="BR6">
-        <v>32</v>
-      </c>
-      <c r="BS6">
-        <v>23</v>
-      </c>
-      <c r="BT6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="H7" t="s">
         <v>25</v>
@@ -2248,18 +2346,18 @@
         <v>112</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>24</v>
@@ -2267,112 +2365,108 @@
       <c r="S7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="T7" t="s">
+        <v>154</v>
+      </c>
+      <c r="U7" t="s">
+        <v>155</v>
+      </c>
       <c r="V7" s="2"/>
-      <c r="W7" t="s">
-        <v>155</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="W7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="X7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2" t="s">
-        <v>122</v>
+      <c r="Y7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="AA7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AB7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
+      <c r="AG7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="AI7" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ7" s="2" t="s">
-        <v>159</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="AJ7" s="2"/>
       <c r="AK7" s="2" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="AL7" s="2" t="s">
         <v>161</v>
       </c>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO7" s="2" t="s">
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AR7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AP7" s="2"/>
-      <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
-      <c r="BA7" s="2" t="s">
+      <c r="AS7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU7" t="s">
         <v>163</v>
       </c>
-      <c r="BB7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="BC7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD7" t="s">
+      <c r="AV7" t="s">
         <v>164</v>
       </c>
-      <c r="BE7" t="s">
+      <c r="AZ7" t="s">
         <v>165</v>
       </c>
-      <c r="BI7" t="s">
+      <c r="BC7">
+        <v>25</v>
+      </c>
+      <c r="BD7">
+        <v>27</v>
+      </c>
+      <c r="BE7">
+        <v>15</v>
+      </c>
+      <c r="BF7">
+        <v>10</v>
+      </c>
+      <c r="BG7">
+        <v>30</v>
+      </c>
+      <c r="BH7">
+        <v>35</v>
+      </c>
+      <c r="BI7">
+        <v>32</v>
+      </c>
+      <c r="BJ7">
+        <v>23</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>166</v>
       </c>
-      <c r="BL7">
-        <v>25</v>
-      </c>
-      <c r="BM7">
-        <v>27</v>
-      </c>
-      <c r="BN7">
-        <v>15</v>
-      </c>
-      <c r="BO7">
-        <v>10</v>
-      </c>
-      <c r="BP7">
-        <v>30</v>
-      </c>
-      <c r="BQ7">
-        <v>35</v>
-      </c>
-      <c r="BR7">
-        <v>32</v>
-      </c>
-      <c r="BS7">
-        <v>23</v>
-      </c>
-      <c r="BT7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>167</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -2385,18 +2479,18 @@
         <v>112</v>
       </c>
       <c r="L8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>24</v>
@@ -2404,70 +2498,66 @@
       <c r="S8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="X8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="AA8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AB8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC8" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
+      <c r="AG8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="AI8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ8" s="2" t="s">
-        <v>159</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="AJ8" s="2"/>
       <c r="AK8" s="2" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="AL8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AR8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT8" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>169</v>
       </c>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO8" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="BA8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="BB8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="BC8" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E9" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" t="s">
@@ -2475,10 +2565,10 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2488,158 +2578,154 @@
       <c r="S9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
+      <c r="Z9" s="11"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="11"/>
+      <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
+      <c r="AF9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="AI9" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AJ9" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="AK9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AL9" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
       <c r="AM9" s="2" t="s">
         <v>176</v>
       </c>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
-      <c r="AQ9" s="2" t="s">
+      <c r="AR9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AZ9" s="12"/>
-      <c r="BA9" s="2" t="s">
+      <c r="AS9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT9" s="2"/>
+      <c r="BC9">
+        <v>25</v>
+      </c>
+      <c r="BD9">
+        <v>27</v>
+      </c>
+      <c r="BE9">
+        <v>15</v>
+      </c>
+      <c r="BF9">
+        <v>10</v>
+      </c>
+      <c r="BG9">
+        <v>30</v>
+      </c>
+      <c r="BH9">
+        <v>35</v>
+      </c>
+      <c r="BI9">
+        <v>32</v>
+      </c>
+      <c r="BJ9">
+        <v>23</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>178</v>
       </c>
-      <c r="BB9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="BC9" s="2"/>
-      <c r="BL9">
-        <v>25</v>
-      </c>
-      <c r="BM9">
-        <v>27</v>
-      </c>
-      <c r="BN9">
-        <v>15</v>
-      </c>
-      <c r="BO9">
-        <v>10</v>
-      </c>
-      <c r="BP9">
-        <v>30</v>
-      </c>
-      <c r="BQ9">
-        <v>35</v>
-      </c>
-      <c r="BR9">
-        <v>32</v>
-      </c>
-      <c r="BS9">
-        <v>23</v>
-      </c>
-      <c r="BT9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>179</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J10" t="s">
         <v>111</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AC10" s="13"/>
-      <c r="AR10" s="2"/>
-      <c r="BA10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BB10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z10" s="12"/>
+      <c r="AN10" s="2"/>
+      <c r="AR10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BC10" s="2"/>
-      <c r="BL10">
+      <c r="AT10" s="2"/>
+      <c r="BC10">
         <v>25</v>
       </c>
-      <c r="BM10">
+      <c r="BD10">
         <v>27</v>
       </c>
-      <c r="BN10">
+      <c r="BE10">
         <v>15</v>
       </c>
-      <c r="BO10">
+      <c r="BF10">
         <v>10</v>
       </c>
-      <c r="BP10">
+      <c r="BG10">
         <v>30</v>
       </c>
-      <c r="BQ10">
+      <c r="BH10">
         <v>35</v>
       </c>
-      <c r="BR10">
+      <c r="BI10">
         <v>32</v>
       </c>
-      <c r="BS10">
+      <c r="BJ10">
         <v>23</v>
       </c>
-      <c r="BT10" t="s">
+      <c r="BK10" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D80F0928-8295-4AEE-BB44-407350F797C6}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{DA1131E6-3937-4FBF-8346-6A69C93730B1}"/>
-    <hyperlink ref="BJ4" r:id="rId3" xr:uid="{281E9B47-22C0-48F3-AC83-70FAB4BCE947}"/>
-    <hyperlink ref="BB4" r:id="rId4" xr:uid="{F2CB3DD1-8289-4BBB-B2B7-8060F0AA781E}"/>
-    <hyperlink ref="AB5" r:id="rId5" xr:uid="{2C7FBA0B-B216-4CF9-8BAC-41AD7F102B25}"/>
-    <hyperlink ref="BB5" r:id="rId6" xr:uid="{D3439697-9288-4322-A017-1FE7908E0A5D}"/>
-    <hyperlink ref="R5" r:id="rId7" xr:uid="{EE609DB9-C125-4457-9565-F46E3725F39C}"/>
-    <hyperlink ref="BC5" r:id="rId8" xr:uid="{473B1FFE-1414-4AD1-89D8-C2DAD5613F02}"/>
-    <hyperlink ref="AB6" r:id="rId9" xr:uid="{B180B19F-6548-4964-B383-80264FCEDDBA}"/>
-    <hyperlink ref="BB6" r:id="rId10" xr:uid="{26A11598-6614-4E41-8637-FC98158A27B6}"/>
-    <hyperlink ref="R6" r:id="rId11" xr:uid="{F4E34AA6-8DB2-4BDC-89B0-03CBF14C13EF}"/>
-    <hyperlink ref="BC6" r:id="rId12" xr:uid="{F75F9212-AD3E-4382-8794-8F5AE650A30B}"/>
-    <hyperlink ref="R7" r:id="rId13" xr:uid="{8C8BA6DD-9026-4E25-ABE4-7DA69D5973BA}"/>
-    <hyperlink ref="BC7" r:id="rId14" xr:uid="{C58BF9BB-7FEF-488A-BBF6-25ADF711D56D}"/>
-    <hyperlink ref="BB7" r:id="rId15" xr:uid="{49419B2B-1A8A-4D39-A05F-72D614FF021D}"/>
-    <hyperlink ref="AB7" r:id="rId16" xr:uid="{DB9290EF-C8F5-48B6-836C-DE58F6DE870D}"/>
-    <hyperlink ref="BB9" r:id="rId17" xr:uid="{1813D67C-9103-4D48-B5E7-568F95782DE7}"/>
-    <hyperlink ref="BB10" r:id="rId18" xr:uid="{EEFCA7A0-4794-4921-A2AD-8B837E7B4E00}"/>
-    <hyperlink ref="BB8" r:id="rId19" xr:uid="{BA55DAE3-26DE-4483-9D99-476BAA07D329}"/>
-    <hyperlink ref="BC8" r:id="rId20" xr:uid="{63F28980-77E8-441A-8D70-BC7A973201D4}"/>
-    <hyperlink ref="AB8" r:id="rId21" xr:uid="{0956164A-8716-4318-84DD-834A226F0770}"/>
-    <hyperlink ref="R8" r:id="rId22" xr:uid="{A0FCE175-3799-458D-9EEA-CC4B72494EB4}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{545C81EF-212C-4914-B1CC-38F035FF5397}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{D2391A34-C224-4D1B-AA97-6E45CEB8888F}"/>
+    <hyperlink ref="BA4" r:id="rId3" xr:uid="{90DF9A91-2B57-4701-8133-0E287637405F}"/>
+    <hyperlink ref="AS4" r:id="rId4" xr:uid="{110F003F-F0E4-48E3-9CE4-29321C22F745}"/>
+    <hyperlink ref="Y5" r:id="rId5" xr:uid="{5B81D980-D1F9-47AD-8BF6-1B550950F2C9}"/>
+    <hyperlink ref="AS5" r:id="rId6" xr:uid="{22FF8997-7CDA-4D43-86BB-A68F74B93FB7}"/>
+    <hyperlink ref="R5" r:id="rId7" xr:uid="{34149B8C-AE91-4B93-A719-2B620428B77E}"/>
+    <hyperlink ref="AT5" r:id="rId8" xr:uid="{D40BC6A3-3254-477C-BA79-AB0AE3225BF0}"/>
+    <hyperlink ref="Y6" r:id="rId9" xr:uid="{8D0A20FF-A2B1-4279-8CE5-AC8AC352464A}"/>
+    <hyperlink ref="AS6" r:id="rId10" xr:uid="{F8C69F88-F404-4F8C-AA9A-B134A23981A6}"/>
+    <hyperlink ref="R6" r:id="rId11" xr:uid="{FFA99EE9-509D-4484-945B-7E7EF8C59D67}"/>
+    <hyperlink ref="AT6" r:id="rId12" xr:uid="{B7C67D78-9B1A-47EA-8556-D6F58269B36E}"/>
+    <hyperlink ref="R7" r:id="rId13" xr:uid="{5613E5CF-47A7-44AD-9DBE-FB80C653FCAC}"/>
+    <hyperlink ref="AT7" r:id="rId14" xr:uid="{DF6DEB9F-5DDC-47C5-A87C-F96C16C6D76B}"/>
+    <hyperlink ref="AS7" r:id="rId15" xr:uid="{54C1BDAF-13A1-4751-88C7-DAD09DF38375}"/>
+    <hyperlink ref="Y7" r:id="rId16" xr:uid="{54B6AADA-6FC0-49ED-A1A1-04E4D88FD3CE}"/>
+    <hyperlink ref="AS9" r:id="rId17" xr:uid="{7A7B1448-4BAA-44FA-9FB8-4C9CB7CA30BB}"/>
+    <hyperlink ref="AS10" r:id="rId18" xr:uid="{B2A10DA5-CEB4-4A4E-B85D-0EC7B9DD90CE}"/>
+    <hyperlink ref="AS8" r:id="rId19" xr:uid="{37E9B5E7-E113-4834-B9B6-52B8CD7EDDAB}"/>
+    <hyperlink ref="AT8" r:id="rId20" xr:uid="{0B9952CD-CD69-40E8-8B11-D116CFA2DC80}"/>
+    <hyperlink ref="Y8" r:id="rId21" xr:uid="{26816123-993E-49C8-AC97-793421E97E23}"/>
+    <hyperlink ref="R8" r:id="rId22" xr:uid="{680A5F23-D0BB-40D7-954F-ACF0059C3C3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2653,9 +2739,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2669,25 +2755,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -2804,61 +2890,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -2954,9 +3040,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2965,7 +3051,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2978,7 +3064,7 @@
         <v>118</v>
       </c>
       <c r="V2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>24</v>
@@ -2992,7 +3078,7 @@
         <v>107</v>
       </c>
       <c r="AG2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -3005,22 +3091,22 @@
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AV2" s="2"/>
       <c r="AW2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX2" t="s">
         <v>208</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" s="2"/>
+      <c r="BR2" s="13"/>
+      <c r="BS2" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="AY2" s="2"/>
-      <c r="BR2" s="14"/>
-      <c r="BS2" s="14" t="s">
+      <c r="BT2" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="BT2" s="14" t="s">
-        <v>211</v>
       </c>
       <c r="BU2" t="s">
         <v>15</v>
@@ -3032,7 +3118,7 @@
         <v>17</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BY2" s="2" t="s">
         <v>18</v>
@@ -3047,13 +3133,13 @@
         <v>123</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CG2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="CH2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="CI2">
         <v>12</v>
@@ -3083,16 +3169,16 @@
         <v>13</v>
       </c>
       <c r="CR2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>214</v>
+      </c>
+      <c r="CT2" t="s">
         <v>215</v>
       </c>
-      <c r="CS2" t="s">
-        <v>215</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>216</v>
-      </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3100,7 +3186,7 @@
         <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3123,9 +3209,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3139,25 +3225,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -3274,61 +3360,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -3424,13 +3510,13 @@
         <v>97</v>
       </c>
       <c r="CV1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="CW1" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="CW1" s="6" t="s">
-        <v>219</v>
-      </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3438,7 +3524,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3496,7 +3582,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3549,16 +3635,16 @@
         <v>122</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AI3" s="15" t="s">
+      <c r="AI3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="AJ3" s="15" t="s">
-        <v>220</v>
+      <c r="AJ3" s="14" t="s">
+        <v>219</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>144</v>
@@ -3638,30 +3724,30 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U4" t="s">
         <v>118</v>
       </c>
       <c r="V4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AE4" t="s">
         <v>107</v>
       </c>
       <c r="AG4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AR4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AW4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AX4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="CB4" t="s">
         <v>123</v>
@@ -3670,7 +3756,7 @@
         <v>40</v>
       </c>
       <c r="CH4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="CI4">
         <v>25</v>
@@ -3700,24 +3786,24 @@
         <v>13</v>
       </c>
       <c r="CT4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="U5" t="s">
         <v>223</v>
       </c>
-      <c r="U5" t="s">
+      <c r="AW5" t="s">
         <v>224</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>225</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BX5" t="s">
         <v>226</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>227</v>
       </c>
       <c r="BZ5" s="7" t="s">
         <v>40</v>
@@ -3750,18 +3836,18 @@
         <v>13</v>
       </c>
       <c r="CT5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CU5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CW5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3770,7 +3856,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -3803,22 +3889,22 @@
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AV6" s="2"/>
       <c r="AW6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX6" t="s">
         <v>208</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" s="2"/>
+      <c r="BR6" s="13"/>
+      <c r="BS6" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="AY6" s="2"/>
-      <c r="BR6" s="14"/>
-      <c r="BS6" s="14" t="s">
+      <c r="BT6" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="BT6" s="14" t="s">
-        <v>211</v>
       </c>
       <c r="BU6" t="s">
         <v>15</v>
@@ -3830,7 +3916,7 @@
         <v>17</v>
       </c>
       <c r="BX6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BY6" s="2" t="s">
         <v>18</v>
@@ -3843,7 +3929,7 @@
         <v>27</v>
       </c>
       <c r="CC6" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CI6">
         <v>25</v>
@@ -3893,13 +3979,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1682-39F3-49F0-A5E3-7423827666C1}">
   <dimension ref="A1:DB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3913,25 +3999,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -4048,61 +4134,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -4198,28 +4284,28 @@
         <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CW1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="CY1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="CX1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="DB1" s="1" t="s">
-        <v>234</v>
-      </c>
     </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4227,7 +4313,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
         <v>101</v>
@@ -4236,83 +4322,83 @@
         <v>12</v>
       </c>
       <c r="BR2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BX2" t="s">
         <v>235</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BY2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>147</v>
+      </c>
+      <c r="CW2" t="s">
         <v>236</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>147</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>148</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>237</v>
       </c>
       <c r="CX2">
         <v>5</v>
       </c>
       <c r="CY2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="CZ2">
         <v>30</v>
       </c>
       <c r="DA2" t="s">
+        <v>238</v>
+      </c>
+      <c r="DB2" t="s">
         <v>239</v>
       </c>
-      <c r="DB2" t="s">
+    </row>
+    <row r="3" spans="1:106" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AL3" t="s">
         <v>241</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="BR3" t="s">
+        <v>234</v>
+      </c>
+      <c r="BY3" t="s">
         <v>242</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>235</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>243</v>
       </c>
       <c r="BZ3" t="s">
         <v>40</v>
       </c>
       <c r="CW3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="CX3">
         <v>5</v>
       </c>
       <c r="CY3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="CZ3">
         <v>30</v>
       </c>
       <c r="DA3" t="s">
+        <v>238</v>
+      </c>
+      <c r="DB3" t="s">
         <v>239</v>
       </c>
-      <c r="DB3" t="s">
-        <v>240</v>
-      </c>
     </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>235</v>
+      </c>
+      <c r="BX4" t="s">
         <v>244</v>
       </c>
-      <c r="AW4" t="s">
-        <v>236</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>245</v>
-      </c>
       <c r="BY4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="BZ4" t="s">
         <v>40</v>
@@ -4321,4 +4407,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1B6EC-8A60-42BD-BAEF-62942967E41D}">
+  <dimension ref="A1:AN13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="T3" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z3" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" t="s">
+        <v>249</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF4" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="AH4" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI4" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ5" s="17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK6" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>270</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="G8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I8" t="s">
+        <v>249</v>
+      </c>
+      <c r="J8" t="s">
+        <v>273</v>
+      </c>
+      <c r="K8" t="s">
+        <v>274</v>
+      </c>
+      <c r="L8" t="s">
+        <v>275</v>
+      </c>
+      <c r="AL8" s="13"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H10" t="s">
+        <v>281</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="S10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19"/>
+      <c r="AM11" s="19"/>
+      <c r="AN11" s="19"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>288</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" t="s">
+        <v>289</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8607AD4F-E933-4946-AE61-ACEE031DBC7D}"/>
+    <hyperlink ref="AN4" r:id="rId2" xr:uid="{7FB9CA71-95B2-4DE1-B0EC-70F14D79F945}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{7F6153F1-CDB4-48E8-83D0-3D4343E5711E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Admin catlog product update Testdata update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{08BEFCA3-CB30-4227-88DE-07E066E72794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AE125B0-C824-457C-8E05-9816ACDB4720}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD4E422-694E-40A5-8570-1F1D22341D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
     <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Catalog" sheetId="5" r:id="rId5"/>
     <sheet name="customer" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -1676,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB5A4B-EC66-4209-8F6B-550483823EC8}">
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
@@ -3979,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1682-39F3-49F0-A5E3-7423827666C1}">
   <dimension ref="A1:DB4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
+      <selection activeCell="DI2" sqref="DI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Admin Testimonialproduct card-Test case, helper, Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD4E422-694E-40A5-8570-1F1D22341D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{2DB1CE75-D0E9-488E-88D1-11668EF19B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350F0BAA-A603-4FEE-9E8D-7A02399B8F86}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
     <sheet name="Catalog" sheetId="5" r:id="rId5"/>
-    <sheet name="customer" sheetId="6" r:id="rId6"/>
+    <sheet name="TestmonialProductcard" sheetId="7" r:id="rId6"/>
+    <sheet name="customer" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="310">
   <si>
     <t>DataSet</t>
   </si>
@@ -895,6 +896,66 @@
   </si>
   <si>
     <t>Hydroflask Website,OXO Website</t>
+  </si>
+  <si>
+    <t>TestmonialProductcard</t>
+  </si>
+  <si>
+    <t>W32075</t>
+  </si>
+  <si>
+    <t>#21ffff</t>
+  </si>
+  <si>
+    <t>Qatester</t>
+  </si>
+  <si>
+    <t>Author one</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>4 Stars</t>
+  </si>
+  <si>
+    <t>The product quality is too good</t>
+  </si>
+  <si>
+    <t>W32410</t>
+  </si>
+  <si>
+    <t>Author Two</t>
+  </si>
+  <si>
+    <t>Lotusqa</t>
+  </si>
+  <si>
+    <t>5 Stars</t>
+  </si>
+  <si>
+    <t>Very reasonable Product</t>
+  </si>
+  <si>
+    <t>W32520</t>
+  </si>
+  <si>
+    <t>Author Three</t>
+  </si>
+  <si>
+    <t>Lotuswave</t>
+  </si>
+  <si>
+    <t>1 Star</t>
+  </si>
+  <si>
+    <t>Product price is too High</t>
+  </si>
+  <si>
+    <t>#23ff09</t>
+  </si>
+  <si>
+    <t>testing3</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1057,6 +1118,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2735,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B278CB69-F3ED-4115-B521-97E3E0FC6D90}">
   <dimension ref="A1:CU3"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3979,7 +4057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1682-39F3-49F0-A5E3-7423827666C1}">
   <dimension ref="A1:DB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
+    <sheetView topLeftCell="CQ1" workbookViewId="0">
       <selection activeCell="DI2" sqref="DI2"/>
     </sheetView>
   </sheetViews>
@@ -4410,6 +4488,960 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C75DCD-0AB4-4356-90E0-6B798572C63C}">
+  <dimension ref="A1:CU6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BA1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BB1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD1" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="BF1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="BG1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="BI1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="BJ1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="BM1" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="BN1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="BO1" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="BP1" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="BQ1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="BX1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="BY1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="BZ1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CA1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="CC1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="CD1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="CE1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CF1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="CH1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="CI1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="CJ1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="CK1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="CM1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="CN1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="CO1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="CQ1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="CR1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="CS1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="CT1" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX2" s="23"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="22"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
+      <c r="CB2" s="20"/>
+      <c r="CC2" s="20"/>
+      <c r="CD2" s="20"/>
+      <c r="CE2" s="20"/>
+      <c r="CF2" s="20"/>
+      <c r="CG2" s="20"/>
+      <c r="CH2" s="20"/>
+      <c r="CI2" s="20"/>
+      <c r="CJ2" s="20"/>
+      <c r="CK2" s="20"/>
+      <c r="CL2" s="20"/>
+      <c r="CM2" s="20"/>
+      <c r="CN2" s="20"/>
+      <c r="CO2" s="20"/>
+      <c r="CP2" s="20"/>
+      <c r="CQ2" s="20"/>
+      <c r="CR2" s="20"/>
+      <c r="CS2" s="20"/>
+      <c r="CT2" s="20"/>
+      <c r="CU2" s="20"/>
+    </row>
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="30"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="22"/>
+      <c r="AN3" s="22"/>
+      <c r="AO3" s="22"/>
+      <c r="AP3" s="22"/>
+      <c r="AQ3" s="22"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="22"/>
+      <c r="AU3" s="22"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="22"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
+      <c r="BN3" s="20"/>
+      <c r="BO3" s="20"/>
+      <c r="BP3" s="20"/>
+      <c r="BQ3" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="BR3" s="20"/>
+      <c r="BS3" s="20"/>
+      <c r="BT3" s="20"/>
+      <c r="BU3" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="BV3" s="20"/>
+      <c r="BW3" s="28"/>
+      <c r="BX3" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="BY3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="BZ3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="CA3" s="20"/>
+      <c r="CB3" s="20"/>
+      <c r="CC3" s="20"/>
+      <c r="CD3" s="20"/>
+      <c r="CE3" s="20"/>
+      <c r="CF3" s="20"/>
+      <c r="CG3" s="20"/>
+      <c r="CH3" s="20"/>
+      <c r="CI3" s="20">
+        <v>25</v>
+      </c>
+      <c r="CJ3" s="20">
+        <v>27</v>
+      </c>
+      <c r="CK3" s="20">
+        <v>15</v>
+      </c>
+      <c r="CL3" s="20">
+        <v>10</v>
+      </c>
+      <c r="CM3" s="20">
+        <v>30</v>
+      </c>
+      <c r="CN3" s="20">
+        <v>35</v>
+      </c>
+      <c r="CO3" s="20">
+        <v>32</v>
+      </c>
+      <c r="CP3" s="20">
+        <v>23</v>
+      </c>
+      <c r="CQ3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="CR3" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="CS3" s="20"/>
+      <c r="CT3" s="20"/>
+      <c r="CU3" s="20"/>
+    </row>
+    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB4" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
+      <c r="AN4" s="20"/>
+      <c r="AO4" s="20"/>
+      <c r="AP4" s="20"/>
+      <c r="AQ4" s="20"/>
+      <c r="AR4" s="20"/>
+      <c r="AS4" s="20"/>
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="20"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="20"/>
+      <c r="BA4" s="20"/>
+      <c r="BB4" s="20"/>
+      <c r="BC4" s="20"/>
+      <c r="BD4" s="20"/>
+      <c r="BE4" s="20"/>
+      <c r="BF4" s="20"/>
+      <c r="BG4" s="20"/>
+      <c r="BH4" s="20"/>
+      <c r="BI4" s="20"/>
+      <c r="BJ4" s="20"/>
+      <c r="BK4" s="20"/>
+      <c r="BL4" s="20"/>
+      <c r="BM4" s="20"/>
+      <c r="BN4" s="20"/>
+      <c r="BO4" s="20"/>
+      <c r="BP4" s="20"/>
+      <c r="BQ4" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="BR4" s="20"/>
+      <c r="BS4" s="20"/>
+      <c r="BT4" s="20"/>
+      <c r="BU4" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="BV4" s="20"/>
+      <c r="BW4" s="20"/>
+      <c r="BX4" s="20"/>
+      <c r="BY4" s="20"/>
+      <c r="BZ4" s="20"/>
+      <c r="CA4" s="20"/>
+      <c r="CB4" s="20"/>
+      <c r="CC4" s="20"/>
+      <c r="CD4" s="20"/>
+      <c r="CE4" s="20"/>
+      <c r="CF4" s="20"/>
+      <c r="CG4" s="20"/>
+      <c r="CH4" s="20"/>
+      <c r="CI4" s="20">
+        <v>12</v>
+      </c>
+      <c r="CJ4" s="20">
+        <v>13</v>
+      </c>
+      <c r="CK4" s="20">
+        <v>15</v>
+      </c>
+      <c r="CL4" s="20">
+        <v>14</v>
+      </c>
+      <c r="CM4" s="20">
+        <v>17</v>
+      </c>
+      <c r="CN4" s="20">
+        <v>18</v>
+      </c>
+      <c r="CO4" s="20">
+        <v>16</v>
+      </c>
+      <c r="CP4" s="20">
+        <v>10</v>
+      </c>
+      <c r="CQ4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="CR4" s="20"/>
+      <c r="CS4" s="20"/>
+      <c r="CT4" s="20"/>
+      <c r="CU4" s="20"/>
+    </row>
+    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="AB5" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC5" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="22"/>
+      <c r="AL5" s="22"/>
+      <c r="AM5" s="22"/>
+      <c r="AN5" s="22"/>
+      <c r="AO5" s="22"/>
+      <c r="AP5" s="22"/>
+      <c r="AQ5" s="22"/>
+      <c r="AR5" s="22"/>
+      <c r="AS5" s="22"/>
+      <c r="AT5" s="22"/>
+      <c r="AU5" s="22"/>
+      <c r="AV5" s="22"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="20"/>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="20"/>
+      <c r="BF5" s="20"/>
+      <c r="BG5" s="20"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="20"/>
+      <c r="BL5" s="20"/>
+      <c r="BM5" s="20"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="20"/>
+      <c r="BP5" s="20"/>
+      <c r="BQ5" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="BR5" s="20"/>
+      <c r="BS5" s="20"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="20"/>
+      <c r="BX5" s="20"/>
+      <c r="BY5" s="20"/>
+      <c r="BZ5" s="20"/>
+      <c r="CA5" s="20"/>
+      <c r="CB5" s="20"/>
+      <c r="CC5" s="20"/>
+      <c r="CD5" s="20"/>
+      <c r="CE5" s="20"/>
+      <c r="CF5" s="20"/>
+      <c r="CG5" s="20"/>
+      <c r="CH5" s="20"/>
+      <c r="CI5" s="20">
+        <v>16</v>
+      </c>
+      <c r="CJ5" s="20">
+        <v>18</v>
+      </c>
+      <c r="CK5" s="20">
+        <v>11</v>
+      </c>
+      <c r="CL5" s="20">
+        <v>12</v>
+      </c>
+      <c r="CM5" s="20">
+        <v>13</v>
+      </c>
+      <c r="CN5" s="20">
+        <v>17</v>
+      </c>
+      <c r="CO5" s="20">
+        <v>15</v>
+      </c>
+      <c r="CP5" s="20">
+        <v>19</v>
+      </c>
+      <c r="CQ5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="CR5" s="20"/>
+      <c r="CS5" s="20"/>
+      <c r="CT5" s="20"/>
+      <c r="CU5" s="20"/>
+    </row>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB6" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC6" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="20"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="20"/>
+      <c r="BF6" s="20"/>
+      <c r="BG6" s="20"/>
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="20"/>
+      <c r="BL6" s="20"/>
+      <c r="BM6" s="20"/>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+      <c r="BP6" s="20"/>
+      <c r="BQ6" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="BR6" s="20"/>
+      <c r="BS6" s="20"/>
+      <c r="BT6" s="20"/>
+      <c r="BU6" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="BV6" s="20"/>
+      <c r="BW6" s="20"/>
+      <c r="BX6" s="20"/>
+      <c r="BY6" s="20"/>
+      <c r="BZ6" s="20"/>
+      <c r="CA6" s="20"/>
+      <c r="CB6" s="20"/>
+      <c r="CC6" s="20"/>
+      <c r="CD6" s="20"/>
+      <c r="CE6" s="20"/>
+      <c r="CF6" s="20"/>
+      <c r="CG6" s="20"/>
+      <c r="CH6" s="20"/>
+      <c r="CI6" s="20">
+        <v>11</v>
+      </c>
+      <c r="CJ6" s="20">
+        <v>14</v>
+      </c>
+      <c r="CK6" s="20">
+        <v>15</v>
+      </c>
+      <c r="CL6" s="20">
+        <v>17</v>
+      </c>
+      <c r="CM6" s="20">
+        <v>19</v>
+      </c>
+      <c r="CN6" s="20">
+        <v>12</v>
+      </c>
+      <c r="CO6" s="20">
+        <v>13</v>
+      </c>
+      <c r="CP6" s="20">
+        <v>16</v>
+      </c>
+      <c r="CQ6" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="CR6" s="20"/>
+      <c r="CS6" s="20"/>
+      <c r="CT6" s="20"/>
+      <c r="CU6" s="20"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BY3" r:id="rId1" xr:uid="{AB1D1A5F-248F-4307-B594-13468C1C9F5B}"/>
+    <hyperlink ref="BZ3" r:id="rId2" xr:uid="{E5985733-2A92-4208-B223-AD8D134C4091}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{6E32348A-82A1-46F2-9343-7AEA69B27A73}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1B6EC-8A60-42BD-BAEF-62942967E41D}">
   <dimension ref="A1:AN13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Category testcase, helper,tetsdata,XML - commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="6_{2DB1CE75-D0E9-488E-88D1-11668EF19B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350F0BAA-A603-4FEE-9E8D-7A02399B8F86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699BA6A9-A235-48BC-9D16-4ACA647225C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Catalog" sheetId="5" r:id="rId5"/>
     <sheet name="TestmonialProductcard" sheetId="7" r:id="rId6"/>
     <sheet name="customer" sheetId="6" r:id="rId7"/>
+    <sheet name="Category" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="324">
   <si>
     <t>DataSet</t>
   </si>
@@ -956,6 +957,48 @@
   </si>
   <si>
     <t>testing3</t>
+  </si>
+  <si>
+    <t>RootCategory</t>
+  </si>
+  <si>
+    <t>Newcategory</t>
+  </si>
+  <si>
+    <t>Newsubcategory</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Updatesubcategory</t>
+  </si>
+  <si>
+    <t>Hydroflask</t>
+  </si>
+  <si>
+    <t>TestRootCategory</t>
+  </si>
+  <si>
+    <t>HFQATestCategory</t>
+  </si>
+  <si>
+    <t>TestSubcategoryHF</t>
+  </si>
+  <si>
+    <t>Shop (ID: 8)</t>
+  </si>
+  <si>
+    <t>OXO</t>
+  </si>
+  <si>
+    <t>OXOQATestCategory</t>
+  </si>
+  <si>
+    <t>TestSubCategoryOXO</t>
+  </si>
+  <si>
+    <t>Shop (ID: 116)</t>
   </si>
 </sst>
 </file>
@@ -1422,62 +1465,62 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" customWidth="1"/>
-    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1597,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1571,7 +1614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1642,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1674,7 +1717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1706,7 +1749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1758,26 +1801,26 @@
       <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.453125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.90625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1968,7 +2011,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2018,7 +2061,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -2070,7 +2113,7 @@
       </c>
       <c r="AO3" s="2"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -2145,7 +2188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2281,7 +2324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2406,7 +2449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2539,7 +2582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -2630,7 +2673,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -2727,7 +2770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2817,9 +2860,9 @@
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3118,7 +3161,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -3256,7 +3299,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3287,9 +3330,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3594,7 +3637,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3660,7 +3703,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3802,7 +3845,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -3867,7 +3910,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>222</v>
       </c>
@@ -3923,7 +3966,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>203</v>
       </c>
@@ -4061,9 +4104,9 @@
       <selection activeCell="DI2" sqref="DI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4383,7 +4426,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4430,7 +4473,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -4465,7 +4508,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -4491,13 +4534,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C75DCD-0AB4-4356-90E0-6B798572C63C}">
   <dimension ref="A1:CU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4796,7 +4839,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4905,7 +4948,7 @@
       <c r="CT2" s="20"/>
       <c r="CU2" s="20"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>290</v>
       </c>
@@ -5038,7 +5081,7 @@
       <c r="CT3" s="20"/>
       <c r="CU3" s="20"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>294</v>
       </c>
@@ -5169,7 +5212,7 @@
       <c r="CT4" s="20"/>
       <c r="CU4" s="20"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>299</v>
       </c>
@@ -5300,7 +5343,7 @@
       <c r="CT5" s="20"/>
       <c r="CU5" s="20"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>304</v>
       </c>
@@ -5449,12 +5492,12 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5576,7 +5619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5593,7 +5636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>246</v>
       </c>
@@ -5634,7 +5677,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -5672,7 +5715,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>265</v>
       </c>
@@ -5680,7 +5723,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -5691,7 +5734,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -5706,7 +5749,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>271</v>
       </c>
@@ -5728,7 +5771,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -5753,7 +5796,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>280</v>
       </c>
@@ -5776,7 +5819,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>284</v>
       </c>
@@ -5830,7 +5873,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>286</v>
       </c>
@@ -5855,7 +5898,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>288</v>
       </c>
@@ -5882,4 +5925,119 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E2C3F0-6842-4C10-80AD-8F3D90A01710}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" t="s">
+        <v>319</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5" t="s">
+        <v>323</v>
+      </c>
+      <c r="J5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hf and oxo pdp validation test case,test data, helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699BA6A9-A235-48BC-9D16-4ACA647225C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="324">
   <si>
     <t>DataSet</t>
   </si>
@@ -1004,7 +1003,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -1458,7 +1457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1784,9 +1783,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{BBA0A981-F568-40C1-AC2C-09553BD71F74}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{FF4C0337-840C-4DD5-8DC3-2B99CB543D05}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{48A24322-C31B-44BB-AF56-D96437544032}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1794,7 +1793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB5A4B-EC66-4209-8F6B-550483823EC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK10"/>
   <sheetViews>
     <sheetView topLeftCell="AG1" workbookViewId="0">
@@ -2825,35 +2824,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{545C81EF-212C-4914-B1CC-38F035FF5397}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{D2391A34-C224-4D1B-AA97-6E45CEB8888F}"/>
-    <hyperlink ref="BA4" r:id="rId3" xr:uid="{90DF9A91-2B57-4701-8133-0E287637405F}"/>
-    <hyperlink ref="AS4" r:id="rId4" xr:uid="{110F003F-F0E4-48E3-9CE4-29321C22F745}"/>
-    <hyperlink ref="Y5" r:id="rId5" xr:uid="{5B81D980-D1F9-47AD-8BF6-1B550950F2C9}"/>
-    <hyperlink ref="AS5" r:id="rId6" xr:uid="{22FF8997-7CDA-4D43-86BB-A68F74B93FB7}"/>
-    <hyperlink ref="R5" r:id="rId7" xr:uid="{34149B8C-AE91-4B93-A719-2B620428B77E}"/>
-    <hyperlink ref="AT5" r:id="rId8" xr:uid="{D40BC6A3-3254-477C-BA79-AB0AE3225BF0}"/>
-    <hyperlink ref="Y6" r:id="rId9" xr:uid="{8D0A20FF-A2B1-4279-8CE5-AC8AC352464A}"/>
-    <hyperlink ref="AS6" r:id="rId10" xr:uid="{F8C69F88-F404-4F8C-AA9A-B134A23981A6}"/>
-    <hyperlink ref="R6" r:id="rId11" xr:uid="{FFA99EE9-509D-4484-945B-7E7EF8C59D67}"/>
-    <hyperlink ref="AT6" r:id="rId12" xr:uid="{B7C67D78-9B1A-47EA-8556-D6F58269B36E}"/>
-    <hyperlink ref="R7" r:id="rId13" xr:uid="{5613E5CF-47A7-44AD-9DBE-FB80C653FCAC}"/>
-    <hyperlink ref="AT7" r:id="rId14" xr:uid="{DF6DEB9F-5DDC-47C5-A87C-F96C16C6D76B}"/>
-    <hyperlink ref="AS7" r:id="rId15" xr:uid="{54C1BDAF-13A1-4751-88C7-DAD09DF38375}"/>
-    <hyperlink ref="Y7" r:id="rId16" xr:uid="{54B6AADA-6FC0-49ED-A1A1-04E4D88FD3CE}"/>
-    <hyperlink ref="AS9" r:id="rId17" xr:uid="{7A7B1448-4BAA-44FA-9FB8-4C9CB7CA30BB}"/>
-    <hyperlink ref="AS10" r:id="rId18" xr:uid="{B2A10DA5-CEB4-4A4E-B85D-0EC7B9DD90CE}"/>
-    <hyperlink ref="AS8" r:id="rId19" xr:uid="{37E9B5E7-E113-4834-B9B6-52B8CD7EDDAB}"/>
-    <hyperlink ref="AT8" r:id="rId20" xr:uid="{0B9952CD-CD69-40E8-8B11-D116CFA2DC80}"/>
-    <hyperlink ref="Y8" r:id="rId21" xr:uid="{26816123-993E-49C8-AC97-793421E97E23}"/>
-    <hyperlink ref="R8" r:id="rId22" xr:uid="{680A5F23-D0BB-40D7-954F-ACF0059C3C3C}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="BA4" r:id="rId3"/>
+    <hyperlink ref="AS4" r:id="rId4"/>
+    <hyperlink ref="Y5" r:id="rId5"/>
+    <hyperlink ref="AS5" r:id="rId6"/>
+    <hyperlink ref="R5" r:id="rId7"/>
+    <hyperlink ref="AT5" r:id="rId8"/>
+    <hyperlink ref="Y6" r:id="rId9"/>
+    <hyperlink ref="AS6" r:id="rId10"/>
+    <hyperlink ref="R6" r:id="rId11"/>
+    <hyperlink ref="AT6" r:id="rId12"/>
+    <hyperlink ref="R7" r:id="rId13"/>
+    <hyperlink ref="AT7" r:id="rId14"/>
+    <hyperlink ref="AS7" r:id="rId15"/>
+    <hyperlink ref="Y7" r:id="rId16"/>
+    <hyperlink ref="AS9" r:id="rId17"/>
+    <hyperlink ref="AS10" r:id="rId18"/>
+    <hyperlink ref="AS8" r:id="rId19"/>
+    <hyperlink ref="AT8" r:id="rId20"/>
+    <hyperlink ref="Y8" r:id="rId21"/>
+    <hyperlink ref="R8" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B278CB69-F3ED-4115-B521-97E3E0FC6D90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3312,18 +3311,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{4ECB1189-452C-417A-A16B-ABA88FA414D9}"/>
-    <hyperlink ref="BY2" r:id="rId2" xr:uid="{3D679BEE-97C8-4868-B708-1A4E8F6C42B4}"/>
-    <hyperlink ref="BZ2" r:id="rId3" xr:uid="{6ADB74A0-C7FE-4B08-9EF3-111224C3CF8B}"/>
-    <hyperlink ref="CG2" r:id="rId4" xr:uid="{06A155BF-8092-479E-9FF6-C50BDB8682C9}"/>
-    <hyperlink ref="B3" r:id="rId5" xr:uid="{A76F3705-53DF-4E1C-9A2A-9DCEC1A82E34}"/>
+    <hyperlink ref="Y2" r:id="rId1"/>
+    <hyperlink ref="BY2" r:id="rId2"/>
+    <hyperlink ref="BZ2" r:id="rId3"/>
+    <hyperlink ref="CG2" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424A69D1-55C8-43D3-BFB0-720A34E1B905}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4082,26 +4081,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DF83D5E4-D7A4-40AE-BADA-7B6F01513272}"/>
-    <hyperlink ref="AH3" r:id="rId2" xr:uid="{BAEF4C00-5796-47C6-AAC0-103BF25B5854}"/>
-    <hyperlink ref="BY3" r:id="rId3" xr:uid="{CA68FB99-4694-4F39-9CC8-C7DC06D07519}"/>
-    <hyperlink ref="Y3" r:id="rId4" xr:uid="{4B76FD30-B042-41B3-B10A-EE82AEE749A0}"/>
-    <hyperlink ref="BZ3" r:id="rId5" xr:uid="{4F54752F-4912-4C7B-81BD-70AB736EC114}"/>
-    <hyperlink ref="CG4" r:id="rId6" xr:uid="{F2C46F32-F6AF-4880-838A-9D5F8D6C20BF}"/>
-    <hyperlink ref="BZ5" r:id="rId7" xr:uid="{034D436D-5CFE-4100-A9A4-36E66EF0A42C}"/>
-    <hyperlink ref="Y6" r:id="rId8" xr:uid="{6B061070-193D-4958-8A43-25D72940BAEF}"/>
-    <hyperlink ref="BY6" r:id="rId9" xr:uid="{45984C68-C2C1-4033-B146-62097928B16E}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="AH3" r:id="rId2"/>
+    <hyperlink ref="BY3" r:id="rId3"/>
+    <hyperlink ref="Y3" r:id="rId4"/>
+    <hyperlink ref="BZ3" r:id="rId5"/>
+    <hyperlink ref="CG4" r:id="rId6"/>
+    <hyperlink ref="BZ5" r:id="rId7"/>
+    <hyperlink ref="Y6" r:id="rId8"/>
+    <hyperlink ref="BY6" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262F1682-39F3-49F0-A5E3-7423827666C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB4"/>
   <sheetViews>
-    <sheetView topLeftCell="CQ1" workbookViewId="0">
-      <selection activeCell="DI2" sqref="DI2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4531,16 +4530,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C75DCD-0AB4-4356-90E0-6B798572C63C}">
-  <dimension ref="A1:CU6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CT6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
+      <selection activeCell="CS1" sqref="CS1:CS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4830,26 +4833,23 @@
         <v>62</v>
       </c>
       <c r="CS1" s="26" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="CT1" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="CU1" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>216</v>
       </c>
+      <c r="D2" s="22"/>
       <c r="E2" s="20"/>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -4946,9 +4946,8 @@
       <c r="CR2" s="20"/>
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
-      <c r="CU2" s="20"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>290</v>
       </c>
@@ -5079,9 +5078,8 @@
       </c>
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
-      <c r="CU3" s="20"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>294</v>
       </c>
@@ -5210,9 +5208,8 @@
       <c r="CR4" s="20"/>
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
-      <c r="CU4" s="20"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>299</v>
       </c>
@@ -5341,9 +5338,8 @@
       <c r="CR5" s="20"/>
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
-      <c r="CU5" s="20"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>304</v>
       </c>
@@ -5472,20 +5468,18 @@
       <c r="CR6" s="20"/>
       <c r="CS6" s="20"/>
       <c r="CT6" s="20"/>
-      <c r="CU6" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BY3" r:id="rId1" xr:uid="{AB1D1A5F-248F-4307-B594-13468C1C9F5B}"/>
-    <hyperlink ref="BZ3" r:id="rId2" xr:uid="{E5985733-2A92-4208-B223-AD8D134C4091}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{6E32348A-82A1-46F2-9343-7AEA69B27A73}"/>
+    <hyperlink ref="BY3" r:id="rId1"/>
+    <hyperlink ref="BZ3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F1B6EC-8A60-42BD-BAEF-62942967E41D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5919,19 +5913,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8607AD4F-E933-4946-AE61-ACEE031DBC7D}"/>
-    <hyperlink ref="AN4" r:id="rId2" xr:uid="{7FB9CA71-95B2-4DE1-B0EC-70F14D79F945}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{7F6153F1-CDB4-48E8-83D0-3D4343E5711E}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="AN4" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E2C3F0-6842-4C10-80AD-8F3D90A01710}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CLP Hero banner - testcase, Helper, testdata, XML commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_E06A04BB7DB357268BFEB4E9612C2A74E9CC4970" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F818CD-072D-47BB-8BB9-C994B0DC5737}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="324">
   <si>
     <t>DataSet</t>
   </si>
@@ -544,9 +545,6 @@
     <t>c-clp-hero</t>
   </si>
   <si>
-    <t>Lotusqa.png</t>
-  </si>
-  <si>
     <t>Edit CLP Hero Banner</t>
   </si>
   <si>
@@ -998,12 +996,15 @@
   </si>
   <si>
     <t>Shop (ID: 116)</t>
+  </si>
+  <si>
+    <t>Description Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -1457,69 +1458,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1783,9 +1784,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1793,454 +1794,482 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AP5" sqref="AP5"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="20"/>
+    <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7265625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.7265625" style="20"/>
+    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7265625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.6328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" style="20"/>
+    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.6328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7265625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7265625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AJ1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AK1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BD1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BF1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BG1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BH1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BI1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BJ1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BK1" s="6" t="s">
+      <c r="BK1" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="3" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="3" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="AN3" s="3" t="s">
+      <c r="AN3" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="AO3" s="2"/>
+      <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AR4" s="2" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AR4" s="22" t="s">
         <v>106</v>
       </c>
       <c r="AS4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="AT4" s="7"/>
-      <c r="AZ4" t="s">
+      <c r="AZ4" s="20" t="s">
         <v>107</v>
       </c>
       <c r="BA4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="BC4">
+      <c r="BC4" s="20">
         <v>25</v>
       </c>
-      <c r="BD4">
+      <c r="BD4" s="20">
         <v>27</v>
       </c>
-      <c r="BE4">
+      <c r="BE4" s="20">
         <v>15</v>
       </c>
-      <c r="BF4">
+      <c r="BF4" s="20">
         <v>10</v>
       </c>
-      <c r="BG4">
+      <c r="BG4" s="20">
         <v>30</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="20">
         <v>35</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="20">
         <v>32</v>
       </c>
-      <c r="BJ4">
+      <c r="BJ4" s="20">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8" t="s">
+      <c r="U5" s="27"/>
+      <c r="V5" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Y5" s="22" t="s">
         <v>124</v>
       </c>
       <c r="Z5" s="9" t="s">
@@ -2249,619 +2278,671 @@
       <c r="AA5" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AB5" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AC5" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="22">
         <v>3</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AE5" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AF5" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AG5" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AH5" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AK5" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AL5" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="AN5" s="2"/>
-      <c r="AO5" t="s">
+      <c r="AN5" s="22"/>
+      <c r="AO5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AP5" s="2" t="s">
+      <c r="AP5" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="AQ5" s="2" t="s">
+      <c r="AQ5" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="AR5" s="2" t="s">
+      <c r="AR5" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="AS5" s="2" t="s">
+      <c r="AS5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AT5" s="2" t="s">
+      <c r="AT5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="BC5">
+      <c r="BC5" s="20">
         <v>25</v>
       </c>
-      <c r="BD5">
+      <c r="BD5" s="20">
         <v>27</v>
       </c>
-      <c r="BE5">
+      <c r="BE5" s="20">
         <v>15</v>
       </c>
-      <c r="BF5">
+      <c r="BF5" s="20">
         <v>10</v>
       </c>
-      <c r="BG5">
+      <c r="BG5" s="20">
         <v>30</v>
       </c>
-      <c r="BH5">
+      <c r="BH5" s="20">
         <v>35</v>
       </c>
-      <c r="BI5">
+      <c r="BI5" s="20">
         <v>32</v>
       </c>
-      <c r="BJ5">
+      <c r="BJ5" s="20">
         <v>23</v>
       </c>
-      <c r="BK5" t="s">
+      <c r="BK5" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="J6" t="s">
+      <c r="E6" s="22"/>
+      <c r="J6" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S6" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8" t="s">
+      <c r="U6" s="27"/>
+      <c r="V6" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="22" t="s">
         <v>141</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="AC6" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AD6" s="2">
+      <c r="AC6" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="AD6" s="22">
         <v>3</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AE6" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AF6" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AG6" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AH6" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AK6" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AL6" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="AN6" s="2"/>
-      <c r="AQ6" s="2" t="s">
+      <c r="AN6" s="22"/>
+      <c r="AQ6" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AR6" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="AS6" s="2" t="s">
+      <c r="AS6" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AT6" s="2" t="s">
+      <c r="AT6" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="BC6">
+      <c r="BC6" s="20">
         <v>25</v>
       </c>
-      <c r="BD6">
+      <c r="BD6" s="20">
         <v>27</v>
       </c>
-      <c r="BE6">
+      <c r="BE6" s="20">
         <v>15</v>
       </c>
-      <c r="BF6">
+      <c r="BF6" s="20">
         <v>10</v>
       </c>
-      <c r="BG6">
+      <c r="BG6" s="20">
         <v>30</v>
       </c>
-      <c r="BH6">
+      <c r="BH6" s="20">
         <v>35</v>
       </c>
-      <c r="BI6">
+      <c r="BI6" s="20">
         <v>32</v>
       </c>
-      <c r="BJ6">
+      <c r="BJ6" s="20">
         <v>23</v>
       </c>
-      <c r="BK6" t="s">
+      <c r="BK6" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" t="s">
+      <c r="I7" s="22"/>
+      <c r="J7" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2" t="s">
+      <c r="N7" s="22"/>
+      <c r="O7" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S7" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2" t="s">
+      <c r="V7" s="22"/>
+      <c r="W7" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="X7" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Y7" s="22" t="s">
         <v>141</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AB7" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2" t="s">
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="AG7" s="2" t="s">
+      <c r="AG7" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AH7" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="AI7" s="2" t="s">
+      <c r="AI7" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2" t="s">
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="AL7" s="2" t="s">
+      <c r="AL7" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AR7" s="2" t="s">
+      <c r="AM7" s="22"/>
+      <c r="AN7" s="22"/>
+      <c r="AO7" s="22"/>
+      <c r="AR7" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="AS7" s="2" t="s">
+      <c r="AS7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AT7" s="2" t="s">
+      <c r="AT7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="AU7" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="AV7" t="s">
+      <c r="AV7" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="AZ7" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="BC7">
+      <c r="BC7" s="20">
         <v>25</v>
       </c>
-      <c r="BD7">
+      <c r="BD7" s="20">
         <v>27</v>
       </c>
-      <c r="BE7">
+      <c r="BE7" s="20">
         <v>15</v>
       </c>
-      <c r="BF7">
+      <c r="BF7" s="20">
         <v>10</v>
       </c>
-      <c r="BG7">
+      <c r="BG7" s="20">
         <v>30</v>
       </c>
-      <c r="BH7">
+      <c r="BH7" s="20">
         <v>35</v>
       </c>
-      <c r="BI7">
+      <c r="BI7" s="20">
         <v>32</v>
       </c>
-      <c r="BJ7">
+      <c r="BJ7" s="20">
         <v>23</v>
       </c>
-      <c r="BK7" t="s">
+      <c r="BK7" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2" t="s">
+      <c r="N8" s="22"/>
+      <c r="O8" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="s">
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="R8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S8" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2" t="s">
+      <c r="V8" s="22"/>
+      <c r="W8" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="X8" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Y8" s="22" t="s">
         <v>141</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AB8" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2" t="s">
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="AG8" s="2" t="s">
+      <c r="AG8" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AH8" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AI8" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2" t="s">
+      <c r="AJ8" s="22"/>
+      <c r="AK8" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="AL8" s="2" t="s">
+      <c r="AL8" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AR8" s="2" t="s">
+      <c r="AM8" s="22"/>
+      <c r="AN8" s="22"/>
+      <c r="AO8" s="22"/>
+      <c r="AR8" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="AS8" s="2" t="s">
+      <c r="AS8" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AT8" s="2" t="s">
+      <c r="AT8" s="22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="K9" s="22"/>
+      <c r="L9" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2" t="s">
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="U9" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2" t="s">
+      <c r="AG9" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="AG9" s="2" t="s">
+      <c r="AH9" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI9" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ9" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AK9" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL9" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM9" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN9" s="22"/>
+      <c r="AO9" s="22"/>
+      <c r="AQ9" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR9" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC9" s="20">
+        <v>25</v>
+      </c>
+      <c r="BD9" s="20">
+        <v>27</v>
+      </c>
+      <c r="BE9" s="20">
+        <v>15</v>
+      </c>
+      <c r="BF9" s="20">
+        <v>10</v>
+      </c>
+      <c r="BG9" s="20">
+        <v>30</v>
+      </c>
+      <c r="BH9" s="20">
+        <v>35</v>
+      </c>
+      <c r="BI9" s="20">
+        <v>32</v>
+      </c>
+      <c r="BJ9" s="20">
+        <v>23</v>
+      </c>
+      <c r="BK9" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="S10" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="T10" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="U10" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z10" s="12"/>
+      <c r="AF10" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG10" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH10" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI10" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ10" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AK10" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL10" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM10" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="AJ9" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2" t="s">
+      <c r="AN10" s="22"/>
+      <c r="AQ10" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR10" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AR9" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS9" s="2" t="s">
+      <c r="AS10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AT9" s="2"/>
-      <c r="BC9">
+      <c r="AT10" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC10" s="20">
         <v>25</v>
       </c>
-      <c r="BD9">
+      <c r="BD10" s="20">
         <v>27</v>
       </c>
-      <c r="BE9">
+      <c r="BE10" s="20">
         <v>15</v>
       </c>
-      <c r="BF9">
+      <c r="BF10" s="20">
         <v>10</v>
       </c>
-      <c r="BG9">
+      <c r="BG10" s="20">
         <v>30</v>
       </c>
-      <c r="BH9">
+      <c r="BH10" s="20">
         <v>35</v>
       </c>
-      <c r="BI9">
+      <c r="BI10" s="20">
         <v>32</v>
       </c>
-      <c r="BJ9">
+      <c r="BJ10" s="20">
         <v>23</v>
       </c>
-      <c r="BK9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J10" t="s">
-        <v>111</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z10" s="12"/>
-      <c r="AN10" s="2"/>
-      <c r="AR10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AT10" s="2"/>
-      <c r="BC10">
-        <v>25</v>
-      </c>
-      <c r="BD10">
-        <v>27</v>
-      </c>
-      <c r="BE10">
-        <v>15</v>
-      </c>
-      <c r="BF10">
-        <v>10</v>
-      </c>
-      <c r="BG10">
-        <v>30</v>
-      </c>
-      <c r="BH10">
-        <v>35</v>
-      </c>
-      <c r="BI10">
-        <v>32</v>
-      </c>
-      <c r="BJ10">
-        <v>23</v>
-      </c>
-      <c r="BK10" t="s">
+      <c r="BK10" s="20" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="BA4" r:id="rId3"/>
-    <hyperlink ref="AS4" r:id="rId4"/>
-    <hyperlink ref="Y5" r:id="rId5"/>
-    <hyperlink ref="AS5" r:id="rId6"/>
-    <hyperlink ref="R5" r:id="rId7"/>
-    <hyperlink ref="AT5" r:id="rId8"/>
-    <hyperlink ref="Y6" r:id="rId9"/>
-    <hyperlink ref="AS6" r:id="rId10"/>
-    <hyperlink ref="R6" r:id="rId11"/>
-    <hyperlink ref="AT6" r:id="rId12"/>
-    <hyperlink ref="R7" r:id="rId13"/>
-    <hyperlink ref="AT7" r:id="rId14"/>
-    <hyperlink ref="AS7" r:id="rId15"/>
-    <hyperlink ref="Y7" r:id="rId16"/>
-    <hyperlink ref="AS9" r:id="rId17"/>
-    <hyperlink ref="AS10" r:id="rId18"/>
-    <hyperlink ref="AS8" r:id="rId19"/>
-    <hyperlink ref="AT8" r:id="rId20"/>
-    <hyperlink ref="Y8" r:id="rId21"/>
-    <hyperlink ref="R8" r:id="rId22"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{F122F0B5-CDB8-4B02-A76A-9928730F7D4B}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1A09C11B-DA7E-4373-B07B-758D09FC1B80}"/>
+    <hyperlink ref="BA4" r:id="rId3" xr:uid="{21935E8F-BE42-4B4F-A679-F5BA6A7DBF84}"/>
+    <hyperlink ref="AS4" r:id="rId4" xr:uid="{3BA37908-0D0B-471A-964D-2E6DAEB8885C}"/>
+    <hyperlink ref="Y5" r:id="rId5" xr:uid="{FF7DBE4B-2E3A-4395-AE85-4306831972F3}"/>
+    <hyperlink ref="AS5" r:id="rId6" xr:uid="{3C5B1BE0-C379-4F2D-97AA-FC4E1EAA804F}"/>
+    <hyperlink ref="R5" r:id="rId7" xr:uid="{8365B64D-1F70-40EB-B4A3-A00254BD4040}"/>
+    <hyperlink ref="AT5" r:id="rId8" xr:uid="{8FB286CF-1A96-457D-ADE7-9A527DE1FEDA}"/>
+    <hyperlink ref="Y6" r:id="rId9" xr:uid="{C6F187F1-6D34-4D9F-8C8F-1A6EB2278438}"/>
+    <hyperlink ref="AS6" r:id="rId10" xr:uid="{98A3D34E-497C-4057-9CC1-01CF0294F682}"/>
+    <hyperlink ref="R6" r:id="rId11" xr:uid="{CC91E832-5B65-40E5-ABDA-8F270B25A190}"/>
+    <hyperlink ref="AT6" r:id="rId12" xr:uid="{796F2406-1AE6-47AB-B8B4-73E7BEFC0768}"/>
+    <hyperlink ref="R7" r:id="rId13" xr:uid="{B2B0E00C-0320-4970-90C1-3429112F9171}"/>
+    <hyperlink ref="AT7" r:id="rId14" xr:uid="{F358D80C-741F-4951-A786-D182A0E24B09}"/>
+    <hyperlink ref="AS7" r:id="rId15" xr:uid="{2861764E-1D8D-42F1-9493-F794A44DB24D}"/>
+    <hyperlink ref="Y7" r:id="rId16" xr:uid="{1DE0D040-8AB9-444D-9AD8-0D5FC95C4DFF}"/>
+    <hyperlink ref="AS9" r:id="rId17" xr:uid="{26E68B64-1352-479C-BC0A-A68F7F8F25D0}"/>
+    <hyperlink ref="AS10" r:id="rId18" xr:uid="{4832032A-E35D-44E9-A707-E9CE84C56900}"/>
+    <hyperlink ref="AS8" r:id="rId19" xr:uid="{6EAAAE19-9513-4739-9165-19F00E2196D4}"/>
+    <hyperlink ref="AT8" r:id="rId20" xr:uid="{46E86EC5-129A-4565-BFCC-976EBF7F44C5}"/>
+    <hyperlink ref="Y8" r:id="rId21" xr:uid="{B8566C4D-3846-4958-AF77-1D6F3533BABA}"/>
+    <hyperlink ref="R8" r:id="rId22" xr:uid="{F84594F0-08FE-426F-9FE7-3AC8E7DD17EF}"/>
+    <hyperlink ref="AT9" r:id="rId23" xr:uid="{828CC311-F952-4017-8956-AFD6EFB8ED6D}"/>
+    <hyperlink ref="AT10" r:id="rId24" xr:uid="{955A94E1-CF15-468B-8E9A-CD653F447FAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2875,25 +2956,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -3010,61 +3091,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -3160,9 +3241,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3171,7 +3252,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -3184,7 +3265,7 @@
         <v>118</v>
       </c>
       <c r="V2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>24</v>
@@ -3211,22 +3292,22 @@
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AV2" s="2"/>
       <c r="AW2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AX2" t="s">
         <v>207</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>208</v>
       </c>
       <c r="AY2" s="2"/>
       <c r="BR2" s="13"/>
       <c r="BS2" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="BT2" s="13" t="s">
         <v>209</v>
-      </c>
-      <c r="BT2" s="13" t="s">
-        <v>210</v>
       </c>
       <c r="BU2" t="s">
         <v>15</v>
@@ -3238,7 +3319,7 @@
         <v>17</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BY2" s="2" t="s">
         <v>18</v>
@@ -3253,13 +3334,13 @@
         <v>123</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CG2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="CH2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CI2">
         <v>12</v>
@@ -3289,16 +3370,16 @@
         <v>13</v>
       </c>
       <c r="CR2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CT2" t="s">
         <v>214</v>
       </c>
-      <c r="CS2" t="s">
-        <v>214</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>215</v>
-      </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3306,32 +3387,32 @@
         <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1"/>
-    <hyperlink ref="BY2" r:id="rId2"/>
-    <hyperlink ref="BZ2" r:id="rId3"/>
-    <hyperlink ref="CG2" r:id="rId4"/>
-    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="BY2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="BZ2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="CG2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3345,25 +3426,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -3480,61 +3561,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -3630,13 +3711,13 @@
         <v>97</v>
       </c>
       <c r="CV1" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="CW1" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="CW1" s="6" t="s">
-        <v>218</v>
-      </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3644,7 +3725,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3702,7 +3783,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3764,7 +3845,7 @@
         <v>125</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>144</v>
@@ -3844,15 +3925,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U4" t="s">
         <v>118</v>
       </c>
       <c r="V4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AE4" t="s">
         <v>107</v>
@@ -3864,10 +3945,10 @@
         <v>160</v>
       </c>
       <c r="AW4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AX4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="CB4" t="s">
         <v>123</v>
@@ -3876,7 +3957,7 @@
         <v>40</v>
       </c>
       <c r="CH4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CI4">
         <v>25</v>
@@ -3906,24 +3987,24 @@
         <v>13</v>
       </c>
       <c r="CT4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>221</v>
+      </c>
+      <c r="U5" t="s">
         <v>222</v>
       </c>
-      <c r="U5" t="s">
+      <c r="AW5" t="s">
         <v>223</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>224</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BX5" t="s">
         <v>225</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>226</v>
       </c>
       <c r="BZ5" s="7" t="s">
         <v>40</v>
@@ -3956,18 +4037,18 @@
         <v>13</v>
       </c>
       <c r="CT5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CU5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="CW5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3976,7 +4057,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4009,22 +4090,22 @@
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AV6" s="2"/>
       <c r="AW6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AX6" t="s">
         <v>207</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>208</v>
       </c>
       <c r="AY6" s="2"/>
       <c r="BR6" s="13"/>
       <c r="BS6" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="BT6" s="13" t="s">
         <v>209</v>
-      </c>
-      <c r="BT6" s="13" t="s">
-        <v>210</v>
       </c>
       <c r="BU6" t="s">
         <v>15</v>
@@ -4036,7 +4117,7 @@
         <v>17</v>
       </c>
       <c r="BX6" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BY6" s="2" t="s">
         <v>18</v>
@@ -4049,7 +4130,7 @@
         <v>27</v>
       </c>
       <c r="CC6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CI6">
         <v>25</v>
@@ -4081,31 +4162,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="AH3" r:id="rId2"/>
-    <hyperlink ref="BY3" r:id="rId3"/>
-    <hyperlink ref="Y3" r:id="rId4"/>
-    <hyperlink ref="BZ3" r:id="rId5"/>
-    <hyperlink ref="CG4" r:id="rId6"/>
-    <hyperlink ref="BZ5" r:id="rId7"/>
-    <hyperlink ref="Y6" r:id="rId8"/>
-    <hyperlink ref="BY6" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="AH3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="BY3" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="Y3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="BZ3" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="CG4" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="BZ5" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="Y6" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="BY6" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:DB4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4119,25 +4200,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -4254,61 +4335,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>87</v>
@@ -4404,28 +4485,28 @@
         <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="CW1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="CY1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="CX1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="DB1" s="1" t="s">
-        <v>233</v>
-      </c>
     </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4433,7 +4514,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
         <v>101</v>
@@ -4442,10 +4523,10 @@
         <v>12</v>
       </c>
       <c r="BR2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BX2" t="s">
         <v>234</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>235</v>
       </c>
       <c r="BY2" t="s">
         <v>146</v>
@@ -4454,71 +4535,71 @@
         <v>147</v>
       </c>
       <c r="CW2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="CX2">
         <v>5</v>
       </c>
       <c r="CY2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="CZ2">
         <v>30</v>
       </c>
       <c r="DA2" t="s">
+        <v>237</v>
+      </c>
+      <c r="DB2" t="s">
         <v>238</v>
       </c>
-      <c r="DB2" t="s">
+    </row>
+    <row r="3" spans="1:106" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AL3" t="s">
         <v>240</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="BR3" t="s">
+        <v>233</v>
+      </c>
+      <c r="BY3" t="s">
         <v>241</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>234</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>242</v>
       </c>
       <c r="BZ3" t="s">
         <v>40</v>
       </c>
       <c r="CW3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="CX3">
         <v>5</v>
       </c>
       <c r="CY3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="CZ3">
         <v>30</v>
       </c>
       <c r="DA3" t="s">
+        <v>237</v>
+      </c>
+      <c r="DB3" t="s">
         <v>238</v>
       </c>
-      <c r="DB3" t="s">
-        <v>239</v>
-      </c>
     </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>242</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>234</v>
+      </c>
+      <c r="BX4" t="s">
         <v>243</v>
       </c>
-      <c r="AW4" t="s">
-        <v>235</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>244</v>
-      </c>
       <c r="BY4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BZ4" t="s">
         <v>40</v>
@@ -4530,20 +4611,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CS1" sqref="CS1:CS1048576"/>
+    <sheetView topLeftCell="CB1" workbookViewId="0">
+      <selection activeCell="CG13" sqref="CG13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4557,25 +4638,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>185</v>
       </c>
       <c r="L1" s="24" t="s">
         <v>3</v>
@@ -4692,61 +4773,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AY1" s="21" t="s">
         <v>85</v>
       </c>
       <c r="AZ1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA1" s="21" t="s">
         <v>187</v>
-      </c>
-      <c r="BA1" s="21" t="s">
-        <v>188</v>
       </c>
       <c r="BB1" s="21" t="s">
         <v>86</v>
       </c>
       <c r="BC1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BD1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>201</v>
-      </c>
-      <c r="BP1" s="21" t="s">
-        <v>202</v>
       </c>
       <c r="BQ1" s="21" t="s">
         <v>87</v>
@@ -4839,7 +4920,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4847,7 +4928,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="20"/>
@@ -4947,9 +5028,9 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -5019,18 +5100,18 @@
       <c r="BO3" s="20"/>
       <c r="BP3" s="20"/>
       <c r="BQ3" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BR3" s="20"/>
       <c r="BS3" s="20"/>
       <c r="BT3" s="20"/>
       <c r="BU3" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BV3" s="20"/>
       <c r="BW3" s="28"/>
       <c r="BX3" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BY3" s="22" t="s">
         <v>18</v>
@@ -5074,14 +5155,14 @@
         <v>13</v>
       </c>
       <c r="CR3" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -5109,13 +5190,13 @@
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
       <c r="AA4" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB4" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AC4" s="20" t="s">
         <v>296</v>
-      </c>
-      <c r="AC4" s="20" t="s">
-        <v>297</v>
       </c>
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
@@ -5157,7 +5238,7 @@
       <c r="BO4" s="20"/>
       <c r="BP4" s="20"/>
       <c r="BQ4" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="BR4" s="20"/>
       <c r="BS4" s="20"/>
@@ -5209,9 +5290,9 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="22"/>
@@ -5239,13 +5320,13 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB5" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="AB5" s="20" t="s">
+      <c r="AC5" s="20" t="s">
         <v>301</v>
-      </c>
-      <c r="AC5" s="20" t="s">
-        <v>302</v>
       </c>
       <c r="AD5" s="22"/>
       <c r="AE5" s="22"/>
@@ -5287,13 +5368,13 @@
       <c r="BO5" s="20"/>
       <c r="BP5" s="20"/>
       <c r="BQ5" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="BR5" s="20"/>
       <c r="BS5" s="20"/>
       <c r="BT5" s="20"/>
       <c r="BU5" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BV5" s="20"/>
       <c r="BW5" s="20"/>
@@ -5339,9 +5420,9 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -5369,13 +5450,13 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="20"/>
       <c r="AA6" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="AB6" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="AB6" s="20" t="s">
+      <c r="AC6" s="20" t="s">
         <v>306</v>
-      </c>
-      <c r="AC6" s="20" t="s">
-        <v>307</v>
       </c>
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
@@ -5417,13 +5498,13 @@
       <c r="BO6" s="20"/>
       <c r="BP6" s="20"/>
       <c r="BQ6" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BR6" s="20"/>
       <c r="BS6" s="20"/>
       <c r="BT6" s="20"/>
       <c r="BU6" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="BV6" s="20"/>
       <c r="BW6" s="20"/>
@@ -5463,7 +5544,7 @@
         <v>16</v>
       </c>
       <c r="CQ6" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="CR6" s="20"/>
       <c r="CS6" s="20"/>
@@ -5471,27 +5552,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BY3" r:id="rId1"/>
-    <hyperlink ref="BZ3" r:id="rId2"/>
+    <hyperlink ref="BY3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="BZ3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5505,25 +5586,25 @@
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -5550,55 +5631,55 @@
         <v>5</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>87</v>
@@ -5613,7 +5694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5630,144 +5711,144 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="T3" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="W3" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>256</v>
       </c>
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="W4" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB4" t="s">
         <v>257</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>258</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="AF4" s="17" t="s">
+      <c r="AG4" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="AG4" s="18" t="s">
+      <c r="AH4" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI4" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="AH4" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="AI4" s="16" t="s">
+      <c r="AN4" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>264</v>
       </c>
-      <c r="AN4" s="2" t="s">
-        <v>242</v>
+      <c r="AJ5" s="17" t="s">
+        <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>265</v>
-      </c>
-      <c r="AJ5" s="17" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="AK6" s="17" t="s">
         <v>267</v>
-      </c>
-      <c r="AK6" s="17" t="s">
-        <v>268</v>
       </c>
       <c r="AM6" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="2"/>
       <c r="L7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AL7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AM7" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" s="2"/>
       <c r="G8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I8" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" t="s">
         <v>272</v>
       </c>
-      <c r="I8" t="s">
-        <v>249</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>273</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>274</v>
-      </c>
-      <c r="L8" t="s">
-        <v>275</v>
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -5777,45 +5858,45 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>279</v>
+      </c>
+      <c r="H10" t="s">
         <v>280</v>
       </c>
-      <c r="H10" t="s">
+      <c r="M10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="N10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="S10" t="s">
         <v>282</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="S10" t="s">
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>284</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -5829,21 +5910,21 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>278</v>
-      </c>
       <c r="O11" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S11" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
@@ -5867,9 +5948,9 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -5879,28 +5960,28 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>
@@ -5913,33 +5994,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="AN4" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="AN4" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5950,16 +6031,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>312</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>313</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>10</v>
@@ -5968,11 +6049,11 @@
         <v>39</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5980,29 +6061,29 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" t="s">
         <v>315</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>316</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>317</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>318</v>
-      </c>
-      <c r="G4" t="s">
-        <v>319</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -6011,24 +6092,24 @@
         <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5" t="s">
         <v>320</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>321</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>322</v>
       </c>
-      <c r="G5" t="s">
-        <v>323</v>
-      </c>
       <c r="J5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Customer group testdata Correction
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B033E971-0D01-46A8-8AF7-330D8FBEC43B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="323">
   <si>
     <t>DataSet</t>
   </si>
@@ -993,6 +993,9 @@
   </si>
   <si>
     <t>tester</t>
+  </si>
+  <si>
+    <t>QA_Test_Updatecustomergroup</t>
   </si>
 </sst>
 </file>
@@ -4611,7 +4614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+    <sheetView topLeftCell="CD1" workbookViewId="0">
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
@@ -5566,8 +5569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5575,6 +5578,8 @@
     <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.453125" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.35">
@@ -5851,7 +5856,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>271</v>
       </c>
@@ -5876,7 +5881,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>275</v>
       </c>
@@ -5887,7 +5892,7 @@
         <v>272</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>277</v>
@@ -5914,11 +5919,11 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>273</v>
+      <c r="M11" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>322</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>277</v>
@@ -5964,10 +5969,12 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="N12" s="3"/>
+      <c r="M12" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>322</v>
+      </c>
       <c r="O12" s="3" t="s">
         <v>282</v>
       </c>

</xml_diff>

<commit_message>
Admin,hero banner code changes,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B033E971-0D01-46A8-8AF7-330D8FBEC43B}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38DCFD74-6A06-42EE-85EF-0112A2144B9C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="324">
   <si>
     <t>DataSet</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>QA_Test_Updatecustomergroup</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/291977948</t>
   </si>
 </sst>
 </file>
@@ -2932,13 +2935,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CU3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.6328125" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3266,8 +3270,8 @@
       <c r="V2" t="s">
         <v>200</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>24</v>
+      <c r="Y2" s="22" t="s">
+        <v>323</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
@@ -3391,10 +3395,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="BY2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="BZ2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="CG2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="BY2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="BZ2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="CG2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="Y2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5569,7 +5573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Category card tiles test data helper changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38DCFD74-6A06-42EE-85EF-0112A2144B9C}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5C997D5-E851-4BC1-87EF-9E25899EA498}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="326">
   <si>
     <t>DataSet</t>
   </si>
@@ -446,559 +446,565 @@
     <t>POP Containers</t>
   </si>
   <si>
+    <t>Test Page</t>
+  </si>
+  <si>
+    <t>#a8d099</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.oxo.com/</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-preprod.oxo.com/</t>
+  </si>
+  <si>
+    <t>PLPBLOCK</t>
+  </si>
+  <si>
+    <t>Thi PLP Block is to configure and validate on the front end</t>
+  </si>
+  <si>
+    <t>plp-block</t>
+  </si>
+  <si>
+    <t>c-plp-cms-block</t>
+  </si>
+  <si>
+    <t>qatest123</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>Screenshot_1.png</t>
+  </si>
+  <si>
+    <t>Screenshot_1_1.png</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Edit PLP Block</t>
+  </si>
+  <si>
+    <t>hot_plp_block</t>
+  </si>
+  <si>
+    <t>type-wrapper</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>QATESTtitle</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEPLPBLOCK</t>
+  </si>
+  <si>
+    <t>Qatest2</t>
+  </si>
+  <si>
+    <t>message_3.png</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>OXOPLPBLOCK</t>
+  </si>
+  <si>
+    <t>qatest124</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>CLPHerobanner</t>
+  </si>
+  <si>
+    <t>Lotus Testing the CLP Hero banner</t>
+  </si>
+  <si>
+    <t>c-clp-hero</t>
+  </si>
+  <si>
+    <t>Edit CLP Hero Banner</t>
+  </si>
+  <si>
+    <t>hot_clp_banner</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>QALOTUSTEST</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVECLPHEROBANNER</t>
+  </si>
+  <si>
+    <t>OXOCLPHerobanner</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>SegmentName</t>
+  </si>
+  <si>
+    <t>taxclass</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>ApplyTo</t>
+  </si>
+  <si>
+    <t>AssignedStatus</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Welcome Email</t>
+  </si>
+  <si>
+    <t>ProDeal</t>
+  </si>
+  <si>
+    <t>Acceptdate</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Phonenumber</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>ordernumber</t>
+  </si>
+  <si>
+    <t>Herobanner</t>
+  </si>
+  <si>
+    <t>QA Testing Hero Banner</t>
+  </si>
+  <si>
+    <t>32 OZ WIDE MOUTH STAINLESS</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>QA test Hero Banner</t>
+  </si>
+  <si>
+    <t>Test Banner</t>
+  </si>
+  <si>
+    <t>HydroFlask</t>
+  </si>
+  <si>
+    <t>Right Alignment</t>
+  </si>
+  <si>
+    <t>qaFlask</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>HYDROFLASK</t>
+  </si>
+  <si>
+    <t>QaTester</t>
+  </si>
+  <si>
+    <t>TestingHydro</t>
+  </si>
+  <si>
+    <t>Amtlmcflmipq1!</t>
+  </si>
+  <si>
+    <t>Sortby</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Copper Brown</t>
+  </si>
+  <si>
+    <t>Categorydetails</t>
+  </si>
+  <si>
+    <t>QATESTING</t>
+  </si>
+  <si>
+    <t>CategoryProducts</t>
+  </si>
+  <si>
+    <t>Bottles &amp; Drinkware</t>
+  </si>
+  <si>
+    <t>HYDROFLASK QA TESTING</t>
+  </si>
+  <si>
+    <t>Qa Testing</t>
+  </si>
+  <si>
+    <t>QATESTINGLOTUSWAVEProductSlider</t>
+  </si>
+  <si>
+    <t>less than</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Updateproductname</t>
+  </si>
+  <si>
+    <t>Stock Status</t>
+  </si>
+  <si>
+    <t>Updateprice</t>
+  </si>
+  <si>
+    <t>updateStock Status</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>QATEST product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 QATEST product </t>
+  </si>
+  <si>
+    <t>Out of Stock</t>
+  </si>
+  <si>
+    <t>In Stock</t>
+  </si>
+  <si>
+    <t>Lowest Price</t>
+  </si>
+  <si>
+    <t>Productupdate</t>
+  </si>
+  <si>
+    <t>Bottles,POP Containers</t>
+  </si>
+  <si>
+    <t>https://mcloud-na-stage.hydroflask.com//</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Home Page (Hydroflask)</t>
+  </si>
+  <si>
+    <t>POP Containers,Cooking &amp; Baking</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>honeywelltest159@gmail.com</t>
+  </si>
+  <si>
+    <t>Hydroflask Website</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>12/5/1995</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Hydroflask Store/Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>7/8/2022</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>844 N colony rd</t>
+  </si>
+  <si>
+    <t>wallingford</t>
+  </si>
+  <si>
+    <t>06492</t>
+  </si>
+  <si>
+    <t>9898989898</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>1256233</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>1526</t>
+  </si>
+  <si>
+    <t>Whishlist</t>
+  </si>
+  <si>
+    <t>32 oz</t>
+  </si>
+  <si>
+    <t>Customer Segment</t>
+  </si>
+  <si>
+    <t>QA Test Test</t>
+  </si>
+  <si>
+    <t>Visitors and Registered Customers</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Test Test</t>
+  </si>
+  <si>
+    <t>CustomerGroup</t>
+  </si>
+  <si>
+    <t>QA Testing Lotuswave</t>
+  </si>
+  <si>
+    <t>QA_Testing_Lotuswave</t>
+  </si>
+  <si>
+    <t>Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>Createcustomergroup</t>
+  </si>
+  <si>
+    <t>Retail Customer</t>
+  </si>
+  <si>
+    <t>You saved the customer group.</t>
+  </si>
+  <si>
+    <t>New Customer Group / Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>UpdatecustomerGroup</t>
+  </si>
+  <si>
+    <t>QA Testing Lotuswave / Customer Groups / Customers / Magento Admin</t>
+  </si>
+  <si>
+    <t>DeleteCustomergroup</t>
+  </si>
+  <si>
+    <t>You deleted the customer group.</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Hydroflask Website,OXO Website</t>
+  </si>
+  <si>
+    <t>TestmonialProductcard</t>
+  </si>
+  <si>
+    <t>W32075</t>
+  </si>
+  <si>
+    <t>#21ffff</t>
+  </si>
+  <si>
+    <t>Qatester</t>
+  </si>
+  <si>
+    <t>Author one</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>4 Stars</t>
+  </si>
+  <si>
+    <t>The product quality is too good</t>
+  </si>
+  <si>
+    <t>W32410</t>
+  </si>
+  <si>
+    <t>Author Two</t>
+  </si>
+  <si>
+    <t>Lotusqa</t>
+  </si>
+  <si>
+    <t>5 Stars</t>
+  </si>
+  <si>
+    <t>Very reasonable Product</t>
+  </si>
+  <si>
+    <t>W32520</t>
+  </si>
+  <si>
+    <t>Author Three</t>
+  </si>
+  <si>
+    <t>Lotuswave</t>
+  </si>
+  <si>
+    <t>1 Star</t>
+  </si>
+  <si>
+    <t>Product price is too High</t>
+  </si>
+  <si>
+    <t>#23ff09</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
+    <t>RootCategory</t>
+  </si>
+  <si>
+    <t>Newcategory</t>
+  </si>
+  <si>
+    <t>Newsubcategory</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Updatesubcategory</t>
+  </si>
+  <si>
+    <t>Hydroflask</t>
+  </si>
+  <si>
+    <t>TestRootCategory</t>
+  </si>
+  <si>
+    <t>HFQATestCategory</t>
+  </si>
+  <si>
+    <t>TestSubcategoryHF</t>
+  </si>
+  <si>
+    <t>Shop (ID: 8)</t>
+  </si>
+  <si>
+    <t>OXO</t>
+  </si>
+  <si>
+    <t>OXOQATestCategory</t>
+  </si>
+  <si>
+    <t>TestSubCategoryOXO</t>
+  </si>
+  <si>
+    <t>Shop (ID: 116)</t>
+  </si>
+  <si>
+    <t>Description Type</t>
+  </si>
+  <si>
+    <t>Lotus</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>QA_Test_Updatecustomergroup</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/291977948</t>
+  </si>
+  <si>
+    <t>ActualCategorydisplay</t>
+  </si>
+  <si>
     <t>POP Container Set</t>
   </si>
   <si>
-    <t>Test Page</t>
-  </si>
-  <si>
-    <t>#a8d099</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-stage.oxo.com/</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-preprod.oxo.com/</t>
-  </si>
-  <si>
-    <t>PLPBLOCK</t>
-  </si>
-  <si>
-    <t>Thi PLP Block is to configure and validate on the front end</t>
-  </si>
-  <si>
-    <t>plp-block</t>
-  </si>
-  <si>
-    <t>c-plp-cms-block</t>
-  </si>
-  <si>
-    <t>qatest123</t>
-  </si>
-  <si>
-    <t>products</t>
-  </si>
-  <si>
-    <t>Screenshot_1.png</t>
-  </si>
-  <si>
-    <t>Screenshot_1_1.png</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
-  <si>
-    <t>Edit PLP Block</t>
-  </si>
-  <si>
-    <t>hot_plp_block</t>
-  </si>
-  <si>
-    <t>type-wrapper</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>QATESTtitle</t>
-  </si>
-  <si>
-    <t>QATESTINGLOTUSWAVEPLPBLOCK</t>
-  </si>
-  <si>
-    <t>Qatest2</t>
-  </si>
-  <si>
-    <t>message_3.png</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>OXOPLPBLOCK</t>
-  </si>
-  <si>
-    <t>qatest124</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
-    <t>CLPHerobanner</t>
-  </si>
-  <si>
-    <t>Lotus Testing the CLP Hero banner</t>
-  </si>
-  <si>
-    <t>c-clp-hero</t>
-  </si>
-  <si>
-    <t>Edit CLP Hero Banner</t>
-  </si>
-  <si>
-    <t>hot_clp_banner</t>
-  </si>
-  <si>
-    <t>H6</t>
-  </si>
-  <si>
-    <t>QALOTUSTEST</t>
-  </si>
-  <si>
-    <t>QATESTINGLOTUSWAVECLPHEROBANNER</t>
-  </si>
-  <si>
-    <t>OXOCLPHerobanner</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>SegmentName</t>
-  </si>
-  <si>
-    <t>taxclass</t>
-  </si>
-  <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>ApplyTo</t>
-  </si>
-  <si>
-    <t>AssignedStatus</t>
-  </si>
-  <si>
-    <t>subtitle</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Welcome Email</t>
-  </si>
-  <si>
-    <t>ProDeal</t>
-  </si>
-  <si>
-    <t>Acceptdate</t>
-  </si>
-  <si>
-    <t>IsEnabled</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Postcode</t>
-  </si>
-  <si>
-    <t>Phonenumber</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>ordernumber</t>
-  </si>
-  <si>
-    <t>Herobanner</t>
-  </si>
-  <si>
-    <t>QA Testing Hero Banner</t>
-  </si>
-  <si>
-    <t>32 OZ WIDE MOUTH STAINLESS</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>QA test Hero Banner</t>
-  </si>
-  <si>
-    <t>Test Banner</t>
-  </si>
-  <si>
-    <t>HydroFlask</t>
-  </si>
-  <si>
-    <t>Right Alignment</t>
-  </si>
-  <si>
-    <t>qaFlask</t>
-  </si>
-  <si>
-    <t>Dark</t>
-  </si>
-  <si>
-    <t>HYDROFLASK</t>
-  </si>
-  <si>
-    <t>QaTester</t>
-  </si>
-  <si>
-    <t>TestingHydro</t>
-  </si>
-  <si>
-    <t>Amtlmcflmipq1!</t>
-  </si>
-  <si>
-    <t>Sortby</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>32 oz Wide Mouth - Copper Brown</t>
-  </si>
-  <si>
-    <t>Categorydetails</t>
-  </si>
-  <si>
-    <t>QATESTING</t>
-  </si>
-  <si>
-    <t>CategoryProducts</t>
-  </si>
-  <si>
-    <t>Bottles &amp; Drinkware</t>
-  </si>
-  <si>
-    <t>HYDROFLASK QA TESTING</t>
-  </si>
-  <si>
-    <t>Qa Testing</t>
-  </si>
-  <si>
-    <t>QATESTINGLOTUSWAVEProductSlider</t>
-  </si>
-  <si>
-    <t>less than</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>Updateproductname</t>
-  </si>
-  <si>
-    <t>Stock Status</t>
-  </si>
-  <si>
-    <t>Updateprice</t>
-  </si>
-  <si>
-    <t>updateStock Status</t>
-  </si>
-  <si>
-    <t>search</t>
-  </si>
-  <si>
-    <t>QATEST product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 QATEST product </t>
-  </si>
-  <si>
-    <t>Out of Stock</t>
-  </si>
-  <si>
-    <t>In Stock</t>
-  </si>
-  <si>
-    <t>Lowest Price</t>
-  </si>
-  <si>
-    <t>Productupdate</t>
-  </si>
-  <si>
-    <t>Bottles,POP Containers</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-stage.hydroflask.com//</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Home Page (Hydroflask)</t>
-  </si>
-  <si>
-    <t>POP Containers,Cooking &amp; Baking</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>qa</t>
-  </si>
-  <si>
-    <t>honeywelltest159@gmail.com</t>
-  </si>
-  <si>
-    <t>Hydroflask Website</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>12/5/1995</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Hydroflask Store/Hydroflask Store View</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>7/8/2022</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>844 N colony rd</t>
-  </si>
-  <si>
-    <t>wallingford</t>
-  </si>
-  <si>
-    <t>06492</t>
-  </si>
-  <si>
-    <t>9898989898</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>Orders</t>
-  </si>
-  <si>
-    <t>1256233</t>
-  </si>
-  <si>
-    <t>Shopping</t>
-  </si>
-  <si>
-    <t>1526</t>
-  </si>
-  <si>
-    <t>Whishlist</t>
-  </si>
-  <si>
-    <t>32 oz</t>
-  </si>
-  <si>
-    <t>Customer Segment</t>
-  </si>
-  <si>
-    <t>QA Test Test</t>
-  </si>
-  <si>
-    <t>Visitors and Registered Customers</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Test Test</t>
-  </si>
-  <si>
-    <t>CustomerGroup</t>
-  </si>
-  <si>
-    <t>QA Testing Lotuswave</t>
-  </si>
-  <si>
-    <t>QA_Testing_Lotuswave</t>
-  </si>
-  <si>
-    <t>Customer Groups / Customers / Magento Admin</t>
-  </si>
-  <si>
-    <t>Createcustomergroup</t>
-  </si>
-  <si>
-    <t>Retail Customer</t>
-  </si>
-  <si>
-    <t>You saved the customer group.</t>
-  </si>
-  <si>
-    <t>New Customer Group / Customer Groups / Customers / Magento Admin</t>
-  </si>
-  <si>
-    <t>UpdatecustomerGroup</t>
-  </si>
-  <si>
-    <t>QA Testing Lotuswave / Customer Groups / Customers / Magento Admin</t>
-  </si>
-  <si>
-    <t>DeleteCustomergroup</t>
-  </si>
-  <si>
-    <t>You deleted the customer group.</t>
-  </si>
-  <si>
-    <t>Websites</t>
-  </si>
-  <si>
-    <t>Hydroflask Website,OXO Website</t>
-  </si>
-  <si>
-    <t>TestmonialProductcard</t>
-  </si>
-  <si>
-    <t>W32075</t>
-  </si>
-  <si>
-    <t>#21ffff</t>
-  </si>
-  <si>
-    <t>Qatester</t>
-  </si>
-  <si>
-    <t>Author one</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>4 Stars</t>
-  </si>
-  <si>
-    <t>The product quality is too good</t>
-  </si>
-  <si>
-    <t>W32410</t>
-  </si>
-  <si>
-    <t>Author Two</t>
-  </si>
-  <si>
-    <t>Lotusqa</t>
-  </si>
-  <si>
-    <t>5 Stars</t>
-  </si>
-  <si>
-    <t>Very reasonable Product</t>
-  </si>
-  <si>
-    <t>W32520</t>
-  </si>
-  <si>
-    <t>Author Three</t>
-  </si>
-  <si>
-    <t>Lotuswave</t>
-  </si>
-  <si>
-    <t>1 Star</t>
-  </si>
-  <si>
-    <t>Product price is too High</t>
-  </si>
-  <si>
-    <t>#23ff09</t>
-  </si>
-  <si>
-    <t>testing3</t>
-  </si>
-  <si>
-    <t>RootCategory</t>
-  </si>
-  <si>
-    <t>Newcategory</t>
-  </si>
-  <si>
-    <t>Newsubcategory</t>
-  </si>
-  <si>
-    <t>Shop</t>
-  </si>
-  <si>
-    <t>Updatesubcategory</t>
-  </si>
-  <si>
-    <t>Hydroflask</t>
-  </si>
-  <si>
-    <t>TestRootCategory</t>
-  </si>
-  <si>
-    <t>HFQATestCategory</t>
-  </si>
-  <si>
-    <t>TestSubcategoryHF</t>
-  </si>
-  <si>
-    <t>Shop (ID: 8)</t>
-  </si>
-  <si>
-    <t>OXO</t>
-  </si>
-  <si>
-    <t>OXOQATestCategory</t>
-  </si>
-  <si>
-    <t>TestSubCategoryOXO</t>
-  </si>
-  <si>
-    <t>Shop (ID: 116)</t>
-  </si>
-  <si>
-    <t>Description Type</t>
-  </si>
-  <si>
-    <t>Lotus</t>
-  </si>
-  <si>
-    <t>tester</t>
-  </si>
-  <si>
-    <t>QA_Test_Updatecustomergroup</t>
-  </si>
-  <si>
-    <t>https://vimeo.com/291977948</t>
+    <t xml:space="preserve">POP </t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1612,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1797,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1822,7 +1828,8 @@
     <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="8.7265625" style="20"/>
     <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.7265625" style="20"/>
+    <col min="27" max="27" width="26.08984375" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="20"/>
     <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="8.7265625" style="20"/>
     <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
@@ -1955,7 +1962,7 @@
         <v>78</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AK1" s="21" t="s">
         <v>80</v>
@@ -2047,7 +2054,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2407,13 +2414,13 @@
         <v>138</v>
       </c>
       <c r="AA6" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB6" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="AB6" s="22" t="s">
-        <v>140</v>
-      </c>
       <c r="AC6" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AD6" s="22">
         <v>3</v>
@@ -2438,16 +2445,16 @@
       </c>
       <c r="AN6" s="22"/>
       <c r="AQ6" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AR6" s="22" t="s">
         <v>133</v>
       </c>
       <c r="AS6" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT6" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="AT6" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="BC6" s="20">
         <v>25</v>
@@ -2479,10 +2486,10 @@
     </row>
     <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>145</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>25</v>
@@ -2495,18 +2502,18 @@
         <v>108</v>
       </c>
       <c r="L7" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>147</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P7" s="22"/>
       <c r="Q7" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R7" s="22" t="s">
         <v>24</v>
@@ -2515,17 +2522,17 @@
         <v>115</v>
       </c>
       <c r="T7" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="U7" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="U7" s="20" t="s">
-        <v>151</v>
       </c>
       <c r="V7" s="22"/>
       <c r="W7" s="22" t="s">
         <v>118</v>
       </c>
       <c r="X7" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y7" s="22" t="s">
         <v>137</v>
@@ -2534,7 +2541,7 @@
         <v>138</v>
       </c>
       <c r="AA7" s="22" t="s">
-        <v>139</v>
+        <v>324</v>
       </c>
       <c r="AB7" s="22" t="s">
         <v>123</v>
@@ -2543,29 +2550,29 @@
       <c r="AD7" s="22"/>
       <c r="AE7" s="22"/>
       <c r="AF7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="AG7" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="AG7" s="22" t="s">
+      <c r="AH7" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="AH7" s="22" t="s">
+      <c r="AI7" s="22" t="s">
         <v>155</v>
-      </c>
-      <c r="AI7" s="22" t="s">
-        <v>156</v>
       </c>
       <c r="AJ7" s="22"/>
       <c r="AK7" s="22" t="s">
         <v>129</v>
       </c>
       <c r="AL7" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AM7" s="22"/>
       <c r="AN7" s="22"/>
       <c r="AO7" s="22"/>
       <c r="AR7" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AS7" s="22" t="s">
         <v>18</v>
@@ -2574,13 +2581,13 @@
         <v>40</v>
       </c>
       <c r="AU7" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="AV7" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="AV7" s="20" t="s">
+      <c r="AZ7" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="AZ7" s="20" t="s">
-        <v>161</v>
       </c>
       <c r="BC7" s="20">
         <v>25</v>
@@ -2612,10 +2619,10 @@
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H8" s="20" t="s">
         <v>25</v>
@@ -2628,18 +2635,18 @@
         <v>108</v>
       </c>
       <c r="L8" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M8" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>147</v>
       </c>
       <c r="N8" s="22"/>
       <c r="O8" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R8" s="22" t="s">
         <v>24</v>
@@ -2652,7 +2659,7 @@
         <v>118</v>
       </c>
       <c r="X8" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y8" s="22" t="s">
         <v>137</v>
@@ -2661,7 +2668,7 @@
         <v>138</v>
       </c>
       <c r="AA8" s="22" t="s">
-        <v>139</v>
+        <v>324</v>
       </c>
       <c r="AB8" s="22" t="s">
         <v>123</v>
@@ -2670,43 +2677,43 @@
       <c r="AD8" s="22"/>
       <c r="AE8" s="22"/>
       <c r="AF8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="AG8" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="AG8" s="22" t="s">
+      <c r="AH8" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="AH8" s="22" t="s">
-        <v>155</v>
-      </c>
       <c r="AI8" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AJ8" s="22"/>
       <c r="AK8" s="22" t="s">
         <v>129</v>
       </c>
       <c r="AL8" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AM8" s="22"/>
       <c r="AN8" s="22"/>
       <c r="AO8" s="22"/>
       <c r="AR8" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AS8" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="AT8" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="AT8" s="22" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>165</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>166</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="20" t="s">
@@ -2714,10 +2721,10 @@
       </c>
       <c r="K9" s="22"/>
       <c r="L9" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
@@ -2728,10 +2735,10 @@
         <v>115</v>
       </c>
       <c r="T9" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="U9" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="U9" s="20" t="s">
-        <v>151</v>
       </c>
       <c r="V9" s="22"/>
       <c r="W9" s="22"/>
@@ -2744,28 +2751,28 @@
       <c r="AD9" s="22"/>
       <c r="AE9" s="22"/>
       <c r="AF9" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="AG9" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="AG9" s="22" t="s">
+      <c r="AH9" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI9" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ9" s="22" t="s">
         <v>169</v>
-      </c>
-      <c r="AH9" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI9" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ9" s="22" t="s">
-        <v>170</v>
       </c>
       <c r="AK9" s="22" t="s">
         <v>129</v>
       </c>
       <c r="AL9" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AM9" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AN9" s="22"/>
       <c r="AO9" s="22"/>
@@ -2773,7 +2780,7 @@
         <v>132</v>
       </c>
       <c r="AR9" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AS9" s="22" t="s">
         <v>18</v>
@@ -2811,66 +2818,66 @@
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>107</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S10" s="22" t="s">
         <v>115</v>
       </c>
       <c r="T10" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="U10" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="U10" s="20" t="s">
-        <v>151</v>
       </c>
       <c r="Z10" s="12"/>
       <c r="AF10" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="AG10" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="AG10" s="22" t="s">
+      <c r="AH10" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI10" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ10" s="22" t="s">
         <v>169</v>
-      </c>
-      <c r="AH10" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI10" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ10" s="22" t="s">
-        <v>170</v>
       </c>
       <c r="AK10" s="22" t="s">
         <v>129</v>
       </c>
       <c r="AL10" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AM10" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AN10" s="22"/>
       <c r="AQ10" s="22" t="s">
         <v>132</v>
       </c>
       <c r="AR10" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AS10" s="22" t="s">
         <v>18</v>
       </c>
       <c r="AT10" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BC10" s="20">
         <v>25</v>
@@ -2935,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2959,25 +2966,25 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -3094,61 +3101,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>85</v>
@@ -3246,7 +3253,7 @@
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3255,7 +3262,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -3268,10 +3275,10 @@
         <v>114</v>
       </c>
       <c r="V2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y2" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
@@ -3282,7 +3289,7 @@
         <v>103</v>
       </c>
       <c r="AG2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -3295,22 +3302,22 @@
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AV2" s="2"/>
       <c r="AW2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX2" t="s">
         <v>202</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>203</v>
       </c>
       <c r="AY2" s="2"/>
       <c r="BR2" s="13"/>
       <c r="BS2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT2" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="BT2" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="BU2" t="s">
         <v>15</v>
@@ -3322,7 +3329,7 @@
         <v>17</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="BY2" s="2" t="s">
         <v>18</v>
@@ -3337,13 +3344,13 @@
         <v>119</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="CG2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="CH2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="CI2">
         <v>12</v>
@@ -3373,24 +3380,24 @@
         <v>13</v>
       </c>
       <c r="CR2" t="s">
+        <v>208</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>208</v>
+      </c>
+      <c r="CT2" t="s">
         <v>209</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>209</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3399,6 +3406,7 @@
     <hyperlink ref="BZ2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
     <hyperlink ref="CG2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
     <hyperlink ref="Y2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{21721A70-E97D-4EE3-8CE3-5AEC0F2AA320}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3431,25 +3439,25 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -3566,61 +3574,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="BB1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>85</v>
@@ -3716,10 +3724,10 @@
         <v>95</v>
       </c>
       <c r="CV1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="CW1" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="CW1" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:101" x14ac:dyDescent="0.35">
@@ -3730,7 +3738,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3841,7 +3849,7 @@
         <v>118</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AH3" s="2" t="s">
         <v>120</v>
@@ -3850,10 +3858,10 @@
         <v>121</v>
       </c>
       <c r="AJ3" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AL3" s="2" t="s">
         <v>124</v>
@@ -3932,28 +3940,28 @@
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U4" t="s">
         <v>114</v>
       </c>
       <c r="V4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AE4" t="s">
         <v>103</v>
       </c>
       <c r="AG4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AR4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AW4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AX4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="CB4" t="s">
         <v>119</v>
@@ -3962,7 +3970,7 @@
         <v>40</v>
       </c>
       <c r="CH4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="CI4">
         <v>25</v>
@@ -3992,24 +4000,24 @@
         <v>13</v>
       </c>
       <c r="CT4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="U5" t="s">
         <v>217</v>
       </c>
-      <c r="U5" t="s">
+      <c r="AW5" t="s">
         <v>218</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>219</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BX5" t="s">
         <v>220</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>221</v>
       </c>
       <c r="BZ5" s="7" t="s">
         <v>40</v>
@@ -4042,18 +4050,18 @@
         <v>13</v>
       </c>
       <c r="CT5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CU5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CW5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -4062,7 +4070,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4095,22 +4103,22 @@
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AV6" s="2"/>
       <c r="AW6" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX6" t="s">
         <v>202</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>203</v>
       </c>
       <c r="AY6" s="2"/>
       <c r="BR6" s="13"/>
       <c r="BS6" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT6" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="BT6" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="BU6" t="s">
         <v>15</v>
@@ -4122,7 +4130,7 @@
         <v>17</v>
       </c>
       <c r="BX6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="BY6" s="2" t="s">
         <v>18</v>
@@ -4135,7 +4143,7 @@
         <v>27</v>
       </c>
       <c r="CC6" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="CI6">
         <v>25</v>
@@ -4182,15 +4190,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DB4"/>
+  <dimension ref="A1:DC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="37" max="37" width="25.90625" customWidth="1"/>
+    <col min="38" max="38" width="28.453125" style="20" customWidth="1"/>
+    <col min="39" max="39" width="31.81640625" customWidth="1"/>
+    <col min="71" max="71" width="28.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:106" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4204,25 +4218,25 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -4302,215 +4316,218 @@
       <c r="AK1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BP1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="CX1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="CX1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="DB1" s="1" t="s">
-        <v>228</v>
-      </c>
     </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4518,94 +4535,97 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F2" t="s">
         <v>97</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>12</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BY2" t="s">
         <v>229</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BZ2" t="s">
+        <v>141</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>142</v>
+      </c>
+      <c r="CX2" t="s">
         <v>230</v>
       </c>
-      <c r="BY2" t="s">
-        <v>142</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>143</v>
-      </c>
-      <c r="CW2" t="s">
+      <c r="CY2">
+        <v>5</v>
+      </c>
+      <c r="CZ2" t="s">
         <v>231</v>
       </c>
-      <c r="CX2">
+      <c r="DA2">
+        <v>30</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>232</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:107" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>235</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>40</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>230</v>
+      </c>
+      <c r="CY3">
         <v>5</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="CZ3" t="s">
+        <v>231</v>
+      </c>
+      <c r="DA3">
+        <v>30</v>
+      </c>
+      <c r="DB3" t="s">
         <v>232</v>
       </c>
-      <c r="CZ2">
-        <v>30</v>
-      </c>
-      <c r="DA2" t="s">
+      <c r="DC3" t="s">
         <v>233</v>
       </c>
-      <c r="DB2" t="s">
-        <v>234</v>
-      </c>
     </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL3" t="s">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>229</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>238</v>
+      </c>
+      <c r="BZ4" t="s">
         <v>236</v>
       </c>
-      <c r="BR3" t="s">
-        <v>229</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>237</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>40</v>
-      </c>
-      <c r="CW3" t="s">
-        <v>231</v>
-      </c>
-      <c r="CX3">
-        <v>5</v>
-      </c>
-      <c r="CY3" t="s">
-        <v>232</v>
-      </c>
-      <c r="CZ3">
-        <v>30</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>233</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>238</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>230</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>239</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>237</v>
-      </c>
-      <c r="BZ4" t="s">
+      <c r="CA4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4642,25 +4662,25 @@
         <v>47</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="24" t="s">
         <v>3</v>
@@ -4777,61 +4797,61 @@
         <v>5</v>
       </c>
       <c r="AX1" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AY1" s="21" t="s">
         <v>83</v>
       </c>
       <c r="AZ1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="BA1" s="21" t="s">
         <v>182</v>
-      </c>
-      <c r="BA1" s="21" t="s">
-        <v>183</v>
       </c>
       <c r="BB1" s="21" t="s">
         <v>84</v>
       </c>
       <c r="BC1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="BD1" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>196</v>
-      </c>
-      <c r="BP1" s="21" t="s">
-        <v>197</v>
       </c>
       <c r="BQ1" s="21" t="s">
         <v>85</v>
@@ -4932,7 +4952,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="20"/>
@@ -5034,7 +5054,7 @@
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -5104,18 +5124,18 @@
       <c r="BO3" s="20"/>
       <c r="BP3" s="20"/>
       <c r="BQ3" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BR3" s="20"/>
       <c r="BS3" s="20"/>
       <c r="BT3" s="20"/>
       <c r="BU3" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BV3" s="20"/>
       <c r="BW3" s="28"/>
       <c r="BX3" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="BY3" s="22" t="s">
         <v>18</v>
@@ -5159,14 +5179,14 @@
         <v>13</v>
       </c>
       <c r="CR3" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
     <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -5194,13 +5214,13 @@
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
       <c r="AA4" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB4" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="AB4" s="20" t="s">
+      <c r="AC4" s="20" t="s">
         <v>291</v>
-      </c>
-      <c r="AC4" s="20" t="s">
-        <v>292</v>
       </c>
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
@@ -5242,7 +5262,7 @@
       <c r="BO4" s="20"/>
       <c r="BP4" s="20"/>
       <c r="BQ4" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BR4" s="20"/>
       <c r="BS4" s="20"/>
@@ -5291,14 +5311,14 @@
         <v>45</v>
       </c>
       <c r="CR4" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="22"/>
@@ -5326,13 +5346,13 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB5" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="AB5" s="20" t="s">
+      <c r="AC5" s="20" t="s">
         <v>296</v>
-      </c>
-      <c r="AC5" s="20" t="s">
-        <v>297</v>
       </c>
       <c r="AD5" s="22"/>
       <c r="AE5" s="22"/>
@@ -5374,13 +5394,13 @@
       <c r="BO5" s="20"/>
       <c r="BP5" s="20"/>
       <c r="BQ5" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="BR5" s="20"/>
       <c r="BS5" s="20"/>
       <c r="BT5" s="20"/>
       <c r="BU5" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BV5" s="20"/>
       <c r="BW5" s="20"/>
@@ -5423,14 +5443,14 @@
         <v>46</v>
       </c>
       <c r="CR5" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
     <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -5458,13 +5478,13 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="20"/>
       <c r="AA6" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB6" s="20" t="s">
         <v>300</v>
       </c>
-      <c r="AB6" s="20" t="s">
+      <c r="AC6" s="20" t="s">
         <v>301</v>
-      </c>
-      <c r="AC6" s="20" t="s">
-        <v>302</v>
       </c>
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
@@ -5506,13 +5526,13 @@
       <c r="BO6" s="20"/>
       <c r="BP6" s="20"/>
       <c r="BQ6" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BR6" s="20"/>
       <c r="BS6" s="20"/>
       <c r="BT6" s="20"/>
       <c r="BU6" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="BV6" s="20"/>
       <c r="BW6" s="20"/>
@@ -5552,7 +5572,7 @@
         <v>16</v>
       </c>
       <c r="CQ6" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="CR6" s="31" t="s">
         <v>13</v>
@@ -5600,25 +5620,25 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -5645,55 +5665,55 @@
         <v>5</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>85</v>
@@ -5716,7 +5736,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5727,97 +5747,97 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="T3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="W3" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="15" t="s">
         <v>250</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>251</v>
       </c>
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="W4" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB4" t="s">
         <v>252</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>253</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="AF4" s="17" t="s">
+      <c r="AG4" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="AG4" s="18" t="s">
+      <c r="AH4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI4" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="AH4" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="AI4" s="16" t="s">
-        <v>259</v>
-      </c>
       <c r="AN4" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ5" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="AJ5" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK6" s="17" t="s">
         <v>262</v>
-      </c>
-      <c r="AK6" s="17" t="s">
-        <v>263</v>
       </c>
       <c r="AM6" s="2" t="s">
         <v>102</v>
@@ -5825,14 +5845,14 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="2"/>
       <c r="L7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AL7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AM7" s="2" t="s">
         <v>102</v>
@@ -5840,29 +5860,29 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" s="2"/>
       <c r="G8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" t="s">
+        <v>243</v>
+      </c>
+      <c r="J8" t="s">
         <v>267</v>
       </c>
-      <c r="I8" t="s">
-        <v>244</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>268</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>269</v>
-      </c>
-      <c r="L8" t="s">
-        <v>270</v>
       </c>
       <c r="AL8" s="13"/>
     </row>
     <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -5872,45 +5892,45 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H10" t="s">
         <v>275</v>
       </c>
-      <c r="H10" t="s">
+      <c r="M10" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="O10" s="3" t="s">
+      <c r="R10" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S10" t="s">
         <v>277</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="S10" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -5924,21 +5944,21 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N11" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S11" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
@@ -5964,7 +5984,7 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -5974,30 +5994,30 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>
@@ -6046,16 +6066,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>307</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>308</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>10</v>
@@ -6064,7 +6084,7 @@
         <v>39</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K1" s="21"/>
     </row>
@@ -6076,29 +6096,29 @@
         <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" t="s">
         <v>310</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>311</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>312</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>313</v>
-      </c>
-      <c r="G4" t="s">
-        <v>314</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -6107,24 +6127,24 @@
         <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" t="s">
         <v>315</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>316</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>317</v>
       </c>
-      <c r="G5" t="s">
-        <v>318</v>
-      </c>
       <c r="J5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Category card tiles test data and helper changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5C997D5-E851-4BC1-87EF-9E25899EA498}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B41E9A-6BF4-492F-B3DB-46B20371795A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
     <t>POP Container Set</t>
   </si>
   <si>
-    <t xml:space="preserve">POP </t>
+    <t>POP</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1804,7 @@
   <dimension ref="A1:BK10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Catalog Price rule testcase, helper, testdata commit.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{04E96F71-5FAE-4792-BC34-1989A6785DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B41E9A-6BF4-492F-B3DB-46B20371795A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225EB76E-E4FC-4468-907F-9B1DD134685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18960" windowHeight="8520" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="TestmonialProductcard" sheetId="7" r:id="rId6"/>
     <sheet name="customer" sheetId="6" r:id="rId7"/>
     <sheet name="Category" sheetId="8" r:id="rId8"/>
+    <sheet name="CatalogPricerule" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="347">
   <si>
     <t>DataSet</t>
   </si>
@@ -1005,6 +1006,69 @@
   </si>
   <si>
     <t>POP</t>
+  </si>
+  <si>
+    <t>RuleName</t>
+  </si>
+  <si>
+    <t>Financecategory</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>HFCategory</t>
+  </si>
+  <si>
+    <t>HFsubcategory</t>
+  </si>
+  <si>
+    <t>OxoCategory</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Oxosubcategory</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Discard subsequent rules</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Catalogpricedetails</t>
+  </si>
+  <si>
+    <t>Qatestcatalogrule</t>
+  </si>
+  <si>
+    <t>5%offcatalogpricerule</t>
+  </si>
+  <si>
+    <t>TRADE</t>
+  </si>
+  <si>
+    <t>Categoryselection</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Coffee &amp; Beverage</t>
+  </si>
+  <si>
+    <t>Coffee &amp; Tea</t>
+  </si>
+  <si>
+    <t>Apply as percentage of original</t>
+  </si>
+  <si>
+    <t>Home Page (OXO)</t>
   </si>
 </sst>
 </file>
@@ -1472,62 +1536,62 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" customWidth="1"/>
-    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1621,7 +1685,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1692,7 +1756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1724,7 +1788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1756,7 +1820,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1803,59 +1867,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="20"/>
-    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7265625" style="20"/>
-    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="20"/>
+    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="20"/>
+    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7109375" style="20"/>
+    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7265625" style="20"/>
-    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7265625" style="20"/>
-    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.08984375" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7265625" style="20"/>
-    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7265625" style="20"/>
-    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.6328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7265625" style="20"/>
-    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7109375" style="20"/>
+    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7109375" style="20"/>
+    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" style="20"/>
+    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7109375" style="20"/>
+    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" style="20"/>
+    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7265625" style="20"/>
-    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7265625" style="20"/>
-    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7265625" style="20"/>
-    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7265625" style="20"/>
+    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="20"/>
+    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7109375" style="20"/>
+    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7109375" style="20"/>
+    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2046,7 +2110,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2160,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -2148,7 +2212,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -2223,7 +2287,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -2359,7 +2423,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -2484,7 +2548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -2617,7 +2681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -2708,7 +2772,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -2816,7 +2880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -2946,13 +3010,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6328125" customWidth="1"/>
-    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="25" max="25" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3251,7 +3315,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -3389,7 +3453,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3420,12 +3484,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.6328125" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3730,7 +3794,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3796,7 +3860,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -3938,7 +4002,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -4003,7 +4067,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -4059,7 +4123,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -4196,15 +4260,15 @@
       <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="37" max="37" width="25.90625" customWidth="1"/>
-    <col min="38" max="38" width="28.453125" style="20" customWidth="1"/>
-    <col min="39" max="39" width="31.81640625" customWidth="1"/>
-    <col min="71" max="71" width="28.1796875" customWidth="1"/>
+    <col min="37" max="37" width="25.85546875" customWidth="1"/>
+    <col min="38" max="38" width="28.42578125" style="20" customWidth="1"/>
+    <col min="39" max="39" width="31.85546875" customWidth="1"/>
+    <col min="71" max="71" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4527,7 +4591,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4574,7 +4638,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -4612,7 +4676,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -4642,13 +4706,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4944,7 +5008,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -5052,7 +5116,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -5184,7 +5248,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -5316,7 +5380,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -5448,7 +5512,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>
@@ -5597,16 +5661,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5728,7 +5792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5745,7 +5809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -5786,7 +5850,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5824,7 +5888,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -5832,7 +5896,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -5843,7 +5907,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -5858,7 +5922,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -5880,7 +5944,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -5905,7 +5969,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -5928,7 +5992,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -5982,7 +6046,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -6009,7 +6073,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -6045,17 +6109,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6088,7 +6152,7 @@
       </c>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6099,12 +6163,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -6130,7 +6194,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -6145,6 +6209,180 @@
       </c>
       <c r="J5" t="s">
         <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EC746B-B379-4F7E-90DE-67DC8F896310}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>341</v>
+      </c>
+      <c r="H4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" t="s">
+        <v>342</v>
+      </c>
+      <c r="J4" t="s">
+        <v>343</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>252</v>
+      </c>
+      <c r="R4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>314</v>
+      </c>
+      <c r="M6" t="s">
+        <v>141</v>
+      </c>
+      <c r="N6" t="s">
+        <v>142</v>
+      </c>
+      <c r="O6" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retail order placement in magneto
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225EB76E-E4FC-4468-907F-9B1DD134685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D339770-7108-4B19-8791-471E2856566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="18960" windowHeight="8520" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="customer" sheetId="6" r:id="rId7"/>
     <sheet name="Category" sheetId="8" r:id="rId8"/>
     <sheet name="CatalogPricerule" sheetId="9" r:id="rId9"/>
+    <sheet name="MagentoOrderplacement" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="370">
   <si>
     <t>DataSet</t>
   </si>
@@ -1069,6 +1070,75 @@
   </si>
   <si>
     <t>Home Page (OXO)</t>
+  </si>
+  <si>
+    <t>streetaddress</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>SKUNumber</t>
+  </si>
+  <si>
+    <t>ExpMonth</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>UpdateBalance</t>
+  </si>
+  <si>
+    <t>rrendla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ackpgkyatnob4!</t>
+  </si>
+  <si>
+    <t>EmailName</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>844 N Colony Rd</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>T20CP110,S18SX001,LW24LW080</t>
+  </si>
+  <si>
+    <t>10/28</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>qatesting.lotuswave@gmail.com</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>RetailOrder</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>lotusqatestmanual.gold6@gmail.com</t>
+  </si>
+  <si>
+    <t>120</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1146,6 +1216,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1200,7 +1276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1249,6 +1325,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1863,6 +1949,502 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0381A9C-D6EB-4082-8DF0-52513B2B3FF7}">
+  <dimension ref="A1:DJ4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:114" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="BI1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="BJ1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="BM1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="BN1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BO1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BQ1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="BR1" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="BS1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="BU1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="BX1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="BY1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CC1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="CD1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="CF1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CH1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CI1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="CJ1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="CK1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="CL1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="CR1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="CS1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="CT1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="CU1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="CV1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="CW1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="CY1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="CZ1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="DA1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DB1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="DC1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="DD1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="DE1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="DF1" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="DG1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="DH1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="DI1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="DJ1" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="BE2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ2" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="CG2" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="CH2" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE2" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="DF2" s="20">
+        <v>5</v>
+      </c>
+      <c r="DG2" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="DH2" s="20">
+        <v>30</v>
+      </c>
+      <c r="DI2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="DJ2" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="BK3" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="BS3" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="BT3" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="BU3" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="BV3" s="20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:114" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>363</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>369</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{D5FD42FE-1162-49F7-BB06-C4DD3D19971D}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{AD0953F4-366F-4C7D-97F5-A323948CC222}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{476CEC24-A5CE-401A-9339-ADB2825BC460}"/>
+    <hyperlink ref="L4" r:id="rId4" xr:uid="{D54C4469-BE0F-41B4-9EDE-A82B0CE0A0A2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK10"/>
@@ -6220,7 +6802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EC746B-B379-4F7E-90DE-67DC8F896310}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Advance pricing test case for magento
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D339770-7108-4B19-8791-471E2856566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9D339770-7108-4B19-8791-471E2856566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C50C2A-53E7-4451-AD6A-0704EAD92E4C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8520" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="375">
   <si>
     <t>DataSet</t>
   </si>
@@ -1139,6 +1139,21 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>AdvancedPricing</t>
+  </si>
+  <si>
+    <t>searchproduct</t>
+  </si>
+  <si>
+    <t>QATestProduct</t>
+  </si>
+  <si>
+    <t>SpecialPrice</t>
+  </si>
+  <si>
+    <t>QATest Product</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0381A9C-D6EB-4082-8DF0-52513B2B3FF7}">
   <dimension ref="A1:DJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -4836,21 +4851,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DC4"/>
+  <dimension ref="A1:DD7"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+    <sheetView tabSelected="1" topLeftCell="CM1" workbookViewId="0">
+      <selection activeCell="DD4" sqref="DD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="37" max="37" width="25.85546875" customWidth="1"/>
     <col min="38" max="38" width="28.42578125" style="20" customWidth="1"/>
     <col min="39" max="39" width="31.85546875" customWidth="1"/>
     <col min="71" max="71" width="28.140625" customWidth="1"/>
+    <col min="107" max="107" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:108" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5172,8 +5189,11 @@
       <c r="DC1" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="DD1" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5220,7 +5240,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -5258,7 +5278,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5273,6 +5293,30 @@
       </c>
       <c r="CA4" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="DD5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="DC6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="DD7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
admin order creation test case, helper, test data commit.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9D339770-7108-4B19-8791-471E2856566E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C50C2A-53E7-4451-AD6A-0704EAD92E4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90355D7-8FC3-4110-A143-4BCC1FBC6D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8520" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="10440" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,11 @@
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
     <sheet name="Catalog" sheetId="5" r:id="rId5"/>
-    <sheet name="TestmonialProductcard" sheetId="7" r:id="rId6"/>
-    <sheet name="customer" sheetId="6" r:id="rId7"/>
-    <sheet name="Category" sheetId="8" r:id="rId8"/>
-    <sheet name="CatalogPricerule" sheetId="9" r:id="rId9"/>
-    <sheet name="MagentoOrderplacement" sheetId="10" r:id="rId10"/>
+    <sheet name="Mogento,orderplacement" sheetId="9" r:id="rId6"/>
+    <sheet name="CartRulePrice" sheetId="10" r:id="rId7"/>
+    <sheet name="TestmonialProductcard" sheetId="7" r:id="rId8"/>
+    <sheet name="customer" sheetId="6" r:id="rId9"/>
+    <sheet name="Category" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="353">
   <si>
     <t>DataSet</t>
   </si>
@@ -1009,151 +1009,85 @@
     <t>POP</t>
   </si>
   <si>
+    <t>rrendla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ackpgkyatnob4!</t>
+  </si>
+  <si>
+    <t>qatesting.lotuswave@gmail.com</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>SKUNumber</t>
+  </si>
+  <si>
+    <t>EmailName</t>
+  </si>
+  <si>
+    <t>T20CP110,S18SX001,LW24LW080</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>streetaddress</t>
+  </si>
+  <si>
+    <t>844 N Colony Rd</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>ExpMonth</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>10/28</t>
+  </si>
+  <si>
     <t>RuleName</t>
   </si>
   <si>
-    <t>Financecategory</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>HFCategory</t>
-  </si>
-  <si>
-    <t>HFsubcategory</t>
-  </si>
-  <si>
-    <t>OxoCategory</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Oxosubcategory</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Discard subsequent rules</t>
-  </si>
-  <si>
-    <t>Apply</t>
-  </si>
-  <si>
-    <t>Catalogpricedetails</t>
-  </si>
-  <si>
-    <t>Qatestcatalogrule</t>
-  </si>
-  <si>
-    <t>5%offcatalogpricerule</t>
+    <t>QA Test 20</t>
+  </si>
+  <si>
+    <t>To apply the cart price</t>
+  </si>
+  <si>
+    <t>Specific Coupon</t>
+  </si>
+  <si>
+    <t>Coupon</t>
   </si>
   <si>
     <t>TRADE</t>
   </si>
   <si>
-    <t>Categoryselection</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>Coffee &amp; Beverage</t>
-  </si>
-  <si>
-    <t>Coffee &amp; Tea</t>
-  </si>
-  <si>
-    <t>Apply as percentage of original</t>
-  </si>
-  <si>
-    <t>Home Page (OXO)</t>
-  </si>
-  <si>
-    <t>streetaddress</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>SKUNumber</t>
-  </si>
-  <si>
-    <t>ExpMonth</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>UpdateBalance</t>
-  </si>
-  <si>
-    <t>rrendla@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Ackpgkyatnob4!</t>
-  </si>
-  <si>
-    <t>EmailName</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>844 N Colony Rd</t>
-  </si>
-  <si>
-    <t>1, 1, 1</t>
-  </si>
-  <si>
-    <t>T20CP110,S18SX001,LW24LW080</t>
-  </si>
-  <si>
-    <t>10/28</t>
-  </si>
-  <si>
-    <t>432</t>
-  </si>
-  <si>
-    <t>4242424242424242</t>
-  </si>
-  <si>
-    <t>qatesting.lotuswave@gmail.com</t>
-  </si>
-  <si>
-    <t>Wallingford</t>
-  </si>
-  <si>
-    <t>RetailOrder</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>lotusqatestmanual.gold6@gmail.com</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>AdvancedPricing</t>
-  </si>
-  <si>
-    <t>searchproduct</t>
-  </si>
-  <si>
-    <t>QATestProduct</t>
-  </si>
-  <si>
-    <t>SpecialPrice</t>
-  </si>
-  <si>
-    <t>QATest Product</t>
+    <t>FinanceCategory</t>
+  </si>
+  <si>
+    <t>Coupon Code</t>
+  </si>
+  <si>
+    <t>GGQA$30</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1097,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1231,12 +1165,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1291,7 +1219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1349,7 +1277,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1965,16 +1892,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0381A9C-D6EB-4082-8DF0-52513B2B3FF7}">
-  <dimension ref="A1:DJ4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1985,477 +1920,88 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>173</v>
+        <v>306</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>348</v>
+        <v>307</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>349</v>
+        <v>10</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>350</v>
+        <v>39</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>351</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z1" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA1" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB1" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC1" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD1" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL1" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM1" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN1" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP1" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ1" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR1" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS1" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="AT1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU1" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV1" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW1" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AY1" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="AZ1" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="BA1" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="BB1" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="BC1" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="BD1" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="BE1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="BF1" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="BG1" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="BH1" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="BI1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="BJ1" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="BK1" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="BL1" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="BM1" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="BN1" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="BO1" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="BP1" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="BQ1" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="BR1" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="BS1" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="BT1" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="BU1" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="BV1" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="BW1" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="BX1" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="BY1" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="BZ1" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="CA1" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB1" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="CC1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="CD1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="CE1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="CF1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="CG1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="CH1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="CI1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="CJ1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="CK1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="CL1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="CN1" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO1" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="CP1" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="CQ1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="CR1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="CS1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="CT1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="CU1" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="CV1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="CW1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="CY1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="CZ1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="DA1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="DB1" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="DC1" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="DD1" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="DE1" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="DF1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="DG1" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="DH1" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="DI1" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="DJ1" s="21" t="s">
-        <v>227</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="M2" s="27"/>
-      <c r="BE2" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="BZ2" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="CF2" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="CG2" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="CH2" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="DE2" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="DF2" s="20">
-        <v>5</v>
-      </c>
-      <c r="DG2" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="DH2" s="20">
-        <v>30</v>
-      </c>
-      <c r="DI2" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="DJ2" s="20" t="s">
-        <v>233</v>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>357</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>361</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>362</v>
-      </c>
-      <c r="K3" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="BK3" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="BS3" s="20" t="s">
-        <v>365</v>
-      </c>
-      <c r="BT3" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="BU3" s="20">
-        <v>9898989898</v>
-      </c>
-      <c r="BV3" s="20" t="s">
-        <v>246</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:114" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>357</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>359</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>360</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>361</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>367</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="M4" s="35" t="s">
-        <v>369</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" t="s">
+        <v>312</v>
+      </c>
+      <c r="G4" t="s">
+        <v>313</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J5" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{D5FD42FE-1162-49F7-BB06-C4DD3D19971D}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{AD0953F4-366F-4C7D-97F5-A323948CC222}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{476CEC24-A5CE-401A-9339-ADB2825BC460}"/>
-    <hyperlink ref="L4" r:id="rId4" xr:uid="{D54C4469-BE0F-41B4-9EDE-A82B0CE0A0A2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4851,23 +4397,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DD7"/>
+  <dimension ref="A1:DC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CM1" workbookViewId="0">
-      <selection activeCell="DD4" sqref="DD4"/>
+    <sheetView topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="37" max="37" width="25.85546875" customWidth="1"/>
     <col min="38" max="38" width="28.42578125" style="20" customWidth="1"/>
     <col min="39" max="39" width="31.85546875" customWidth="1"/>
     <col min="71" max="71" width="28.140625" customWidth="1"/>
-    <col min="107" max="107" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5189,11 +4733,8 @@
       <c r="DC1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="DD1" s="1" t="s">
-        <v>373</v>
-      </c>
     </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5240,7 +4781,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -5278,7 +4819,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5293,30 +4834,6 @@
       </c>
       <c r="CA4" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="DD5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="DC6" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="DD7">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5325,6 +4842,899 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
+  <dimension ref="A1:DI10"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="20"/>
+    <col min="7" max="7" width="9.140625" style="20"/>
+    <col min="8" max="11" width="33" style="20" customWidth="1"/>
+    <col min="12" max="12" width="33" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="72" max="72" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:113" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="BE1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="BF1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="BG1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="BH1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="BI1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BN1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BO1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BP1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="BQ1" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="BR1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="BS1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="BT1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="BU1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="BV1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="BX1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="BY1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="BZ1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CB1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="CC1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="CE1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="CF1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CG1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CH1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="CI1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="CJ1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="CK1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="CL1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="CM1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="CN1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CO1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="CP1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="CQ1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="CR1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="CS1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="CT1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="CU1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="CV1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="CX1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="CY1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="CZ1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DA1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="DB1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="DC1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="DD1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="DE1" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="DF1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="DG1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="DH1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="DI1" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:113" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="BD2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BY2" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="CE2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF2" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="CG2" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="DD2" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="DE2" s="20">
+        <v>5</v>
+      </c>
+      <c r="DF2" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="DG2" s="20">
+        <v>30</v>
+      </c>
+      <c r="DH2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="DI2" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>251</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>336</v>
+      </c>
+      <c r="BS3" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="BT3">
+        <v>9898989898</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="G10" s="29"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{AC56A3CD-87F9-47F3-B4E2-CBD67EBEE8E6}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{70304466-770B-4C05-A0CC-80C67DF26F82}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{AE88654D-CD03-4F51-B9BE-9B1612A867C1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
+  <dimension ref="A1:DN3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:118" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AX1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="BA1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="BG1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BH1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="BM1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="BN1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="BP1" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="BQ1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="BR1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BS1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BT1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BU1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="BV1" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="BX1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="BY1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="BZ1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="CA1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="CB1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="CC1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="CD1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="CE1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="CF1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CG1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="CH1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="CI1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="CJ1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="CK1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CL1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CM1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="CN1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="CO1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="CQ1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="CR1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="CS1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CT1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="CU1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="CV1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="CW1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="CX1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="CY1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="CZ1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="DA1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="DC1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="DD1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="DE1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DF1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="DG1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="DH1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="DI1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="DJ1" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="DK1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="DL1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="DM1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="DN1" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:118" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AX3" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="BY3" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="BZ3" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA3" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C4B9FB17-BB0F-41D0-9C95-4C7FCA804C49}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{5D193D50-B78E-48AE-8445-69A290522922}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
@@ -6279,7 +6689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
@@ -6725,293 +7135,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="K1" s="21"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>309</v>
-      </c>
-      <c r="D4" t="s">
-        <v>310</v>
-      </c>
-      <c r="E4" t="s">
-        <v>311</v>
-      </c>
-      <c r="F4" t="s">
-        <v>312</v>
-      </c>
-      <c r="G4" t="s">
-        <v>313</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>314</v>
-      </c>
-      <c r="E5" t="s">
-        <v>315</v>
-      </c>
-      <c r="F5" t="s">
-        <v>316</v>
-      </c>
-      <c r="G5" t="s">
-        <v>317</v>
-      </c>
-      <c r="J5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EC746B-B379-4F7E-90DE-67DC8F896310}">
-  <dimension ref="A1:R6"/>
-  <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>326</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>330</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>333</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>337</v>
-      </c>
-      <c r="D3" t="s">
-        <v>338</v>
-      </c>
-      <c r="E3" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" t="s">
-        <v>340</v>
-      </c>
-      <c r="G3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>341</v>
-      </c>
-      <c r="H4" t="s">
-        <v>217</v>
-      </c>
-      <c r="I4" t="s">
-        <v>342</v>
-      </c>
-      <c r="J4" t="s">
-        <v>343</v>
-      </c>
-      <c r="K4">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>344</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>252</v>
-      </c>
-      <c r="R4" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>309</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>314</v>
-      </c>
-      <c r="M6" t="s">
-        <v>141</v>
-      </c>
-      <c r="N6" t="s">
-        <v>142</v>
-      </c>
-      <c r="O6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test data update for retail order
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90355D7-8FC3-4110-A143-4BCC1FBC6D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21957BC7-6A3D-46F6-AC8C-BE164C64B549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="10440" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
     <sheet name="Catalog" sheetId="5" r:id="rId5"/>
-    <sheet name="Mogento,orderplacement" sheetId="9" r:id="rId6"/>
-    <sheet name="CartRulePrice" sheetId="10" r:id="rId7"/>
-    <sheet name="TestmonialProductcard" sheetId="7" r:id="rId8"/>
-    <sheet name="customer" sheetId="6" r:id="rId9"/>
-    <sheet name="Category" sheetId="8" r:id="rId10"/>
+    <sheet name="Retailer OrderPlacement" sheetId="11" r:id="rId6"/>
+    <sheet name="Mogento,orderplacement" sheetId="9" r:id="rId7"/>
+    <sheet name="CartRulePrice" sheetId="10" r:id="rId8"/>
+    <sheet name="TestmonialProductcard" sheetId="7" r:id="rId9"/>
+    <sheet name="customer" sheetId="6" r:id="rId10"/>
+    <sheet name="Category" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="358">
   <si>
     <t>DataSet</t>
   </si>
@@ -1088,6 +1089,21 @@
   </si>
   <si>
     <t>GGQA$30</t>
+  </si>
+  <si>
+    <t>UpdateBalance</t>
+  </si>
+  <si>
+    <t>RetailOrder</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>lotusqatestmanual.gold6@gmail.com</t>
+  </si>
+  <si>
+    <t>120</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1165,6 +1181,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1219,7 +1241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1277,6 +1299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1892,6 +1915,454 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AN13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="T3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z3" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I4" t="s">
+        <v>243</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AF4" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI4" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ5" s="17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK6" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="G8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" t="s">
+        <v>243</v>
+      </c>
+      <c r="J8" t="s">
+        <v>267</v>
+      </c>
+      <c r="K8" t="s">
+        <v>268</v>
+      </c>
+      <c r="L8" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL8" s="13"/>
+    </row>
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>274</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19"/>
+      <c r="AM11" s="19"/>
+      <c r="AN11" s="19"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>282</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" t="s">
+        <v>283</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AN4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -4842,11 +5313,507 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
+  <dimension ref="A1:DJ4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:114" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF1" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH1" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="BI1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="BJ1" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="BL1" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="BM1" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="BN1" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="BO1" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="BQ1" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="BR1" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="BS1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="BU1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="BX1" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="BY1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="CC1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="CD1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="CF1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CH1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="CI1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="CJ1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="CK1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="CL1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="CR1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="CS1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="CT1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="CU1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="CV1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="CW1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="CY1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="CZ1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="DA1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DB1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="DC1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="DD1" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="DE1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="DF1" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="DG1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="DH1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="DI1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="DJ1" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="BE2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BZ2" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="CG2" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="CH2" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE2" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="DF2" s="20">
+        <v>5</v>
+      </c>
+      <c r="DG2" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="DH2" s="20">
+        <v>30</v>
+      </c>
+      <c r="DI2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="DJ2" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="BK3" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="BS3" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="BT3" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="BU3" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="BV3" s="20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:114" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>357</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{C53C6307-0E95-43AA-BE0A-AD24F1F87C5A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{CD7D3846-4739-4D8F-8729-8F7437C112E2}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{91CBEDB6-E72E-4BBD-895A-BE1F7FBBAC2E}"/>
+    <hyperlink ref="L4" r:id="rId4" xr:uid="{67370BC4-64DE-4825-91CE-8AFBC1CC9FA7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:DI10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="DQ1" workbookViewId="0">
+      <selection activeCell="EC4" sqref="EC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5309,12 +6276,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,7 +6701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
@@ -6687,452 +7654,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AN13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="T3" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y3" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA3" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I4" t="s">
-        <v>243</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>252</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>253</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="AF4" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="AG4" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="AH4" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="AI4" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>259</v>
-      </c>
-      <c r="AJ5" s="17" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>261</v>
-      </c>
-      <c r="AK6" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>264</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="G8" t="s">
-        <v>266</v>
-      </c>
-      <c r="I8" t="s">
-        <v>243</v>
-      </c>
-      <c r="J8" t="s">
-        <v>267</v>
-      </c>
-      <c r="K8" t="s">
-        <v>268</v>
-      </c>
-      <c r="L8" t="s">
-        <v>269</v>
-      </c>
-      <c r="AL8" s="13"/>
-    </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>270</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>274</v>
-      </c>
-      <c r="H10" t="s">
-        <v>275</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="S10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="N11" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
-      <c r="AC11" s="19"/>
-      <c r="AD11" s="19"/>
-      <c r="AE11" s="19"/>
-      <c r="AF11" s="19"/>
-      <c r="AG11" s="19"/>
-      <c r="AH11" s="19"/>
-      <c r="AI11" s="19"/>
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-      <c r="AL11" s="19"/>
-      <c r="AM11" s="19"/>
-      <c r="AN11" s="19"/>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>280</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>282</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" t="s">
-        <v>283</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="AN4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Catalog price rules sheet in admin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21957BC7-6A3D-46F6-AC8C-BE164C64B549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A752EC63-B999-4723-B2DE-B031217FE4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TestmonialProductcard" sheetId="7" r:id="rId9"/>
     <sheet name="customer" sheetId="6" r:id="rId10"/>
     <sheet name="Category" sheetId="8" r:id="rId11"/>
+    <sheet name="CatalogPricerule" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="377">
   <si>
     <t>DataSet</t>
   </si>
@@ -1104,6 +1105,63 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>Financecategory</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>HFCategory</t>
+  </si>
+  <si>
+    <t>HFsubcategory</t>
+  </si>
+  <si>
+    <t>OxoCategory</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Oxosubcategory</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Discard subsequent rules</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Catalogpricedetails</t>
+  </si>
+  <si>
+    <t>Qatestcatalogrule</t>
+  </si>
+  <si>
+    <t>5%offcatalogpricerule</t>
+  </si>
+  <si>
+    <t>Categoryselection</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Coffee &amp; Beverage</t>
+  </si>
+  <si>
+    <t>Coffee &amp; Tea</t>
+  </si>
+  <si>
+    <t>Apply as percentage of original</t>
+  </si>
+  <si>
+    <t>Home Page (OXO)</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2425,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,6 +2528,162 @@
       </c>
       <c r="J5" t="s">
         <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" t="s">
+        <v>372</v>
+      </c>
+      <c r="J4" t="s">
+        <v>373</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>252</v>
+      </c>
+      <c r="R4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>314</v>
+      </c>
+      <c r="M6" t="s">
+        <v>141</v>
+      </c>
+      <c r="N6" t="s">
+        <v>142</v>
+      </c>
+      <c r="O6" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -5316,7 +5530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:DJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cart price rule test case, helper, testdata commite
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A752EC63-B999-4723-B2DE-B031217FE4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43E5999-20F1-483F-B8C0-3F965E1F99FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="customer" sheetId="6" r:id="rId10"/>
     <sheet name="Category" sheetId="8" r:id="rId11"/>
     <sheet name="CatalogPricerule" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="401">
   <si>
     <t>DataSet</t>
   </si>
@@ -1089,9 +1090,6 @@
     <t>Coupon Code</t>
   </si>
   <si>
-    <t>GGQA$30</t>
-  </si>
-  <si>
     <t>UpdateBalance</t>
   </si>
   <si>
@@ -1162,6 +1160,81 @@
   </si>
   <si>
     <t>Home Page (OXO)</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uses per Coupon</t>
+  </si>
+  <si>
+    <t>Uses per Customer</t>
+  </si>
+  <si>
+    <t>QtyProduct</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
+  </si>
+  <si>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>adaddu@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Aptdqvfjgsvj1!</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>LOTUSQA$20</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Black</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Addressbook</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>GroundShippingmethod</t>
+  </si>
+  <si>
+    <t>Standard Shipping - FedEx Ground (2-5 Business Days)</t>
+  </si>
+  <si>
+    <t>PaymentDetails</t>
+  </si>
+  <si>
+    <t>04/27</t>
+  </si>
+  <si>
+    <t>addproduct</t>
+  </si>
+  <si>
+    <t>OXO ON 9 CUP COFFEE MAKER</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,6 +1318,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1299,7 +1379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1358,6 +1438,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2539,7 +2623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2562,25 +2646,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>363</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>364</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>10</v>
@@ -2592,13 +2676,13 @@
         <v>9</v>
       </c>
       <c r="P1" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>365</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>366</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2614,13 +2698,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D3" t="s">
         <v>368</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>369</v>
-      </c>
-      <c r="E3" t="s">
-        <v>370</v>
       </c>
       <c r="F3" t="s">
         <v>349</v>
@@ -2634,28 +2718,28 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H4" t="s">
         <v>217</v>
       </c>
       <c r="I4" t="s">
+        <v>371</v>
+      </c>
+      <c r="J4" t="s">
         <v>372</v>
-      </c>
-      <c r="J4" t="s">
-        <v>373</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q4" t="s">
         <v>252</v>
       </c>
       <c r="R4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2683,10 +2767,22 @@
         <v>142</v>
       </c>
       <c r="O6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CA6EE1-C0A9-4DD1-ABBA-0E76043F9F34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5574,7 +5670,7 @@
         <v>174</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>175</v>
@@ -5978,7 +6074,7 @@
     </row>
     <row r="4" spans="1:114" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>333</v>
@@ -5999,16 +6095,16 @@
         <v>343</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K4" s="29" t="s">
         <v>342</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="M4" s="35" t="s">
         <v>356</v>
-      </c>
-      <c r="M4" s="35" t="s">
-        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6492,10 +6588,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
-  <dimension ref="A1:DN3"/>
+  <dimension ref="A1:DT10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6504,7 +6600,7 @@
     <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6515,401 +6611,1515 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="L1" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="Q1" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="R1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="W1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AU1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AV1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AY1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AZ1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="BA1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="BB1" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="BC1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="BD1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="BA1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="BB1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="BC1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BQ1" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BR1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BS1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BT1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="BP1" s="21" t="s">
+      <c r="BU1" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BQ1" s="21" t="s">
+      <c r="BV1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="BR1" s="21" t="s">
+      <c r="BW1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="BS1" s="21" t="s">
+      <c r="BX1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BT1" s="21" t="s">
+      <c r="BY1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BU1" s="21" t="s">
+      <c r="BZ1" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="CA1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="BV1" s="21" t="s">
+      <c r="CB1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BW1" s="21" t="s">
+      <c r="CC1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="BX1" s="21" t="s">
+      <c r="CD1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="BY1" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="BZ1" s="21" t="s">
+      <c r="CE1" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="CF1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="CA1" s="21" t="s">
+      <c r="CG1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="CB1" s="21" t="s">
+      <c r="CH1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="CC1" s="21" t="s">
+      <c r="CI1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="CD1" s="21" t="s">
+      <c r="CJ1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="CE1" s="21" t="s">
+      <c r="CK1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="CF1" s="21" t="s">
+      <c r="CL1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CG1" s="21" t="s">
+      <c r="CM1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="CH1" s="21" t="s">
+      <c r="CN1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="CI1" s="21" t="s">
+      <c r="CO1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="CJ1" s="21" t="s">
+      <c r="CP1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="CK1" s="21" t="s">
+      <c r="CQ1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="CL1" s="21" t="s">
+      <c r="CR1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CM1" s="21" t="s">
+      <c r="CS1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CN1" s="21" t="s">
+      <c r="CT1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="CO1" s="21" t="s">
+      <c r="CU1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="CP1" s="21" t="s">
+      <c r="CV1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CQ1" s="21" t="s">
+      <c r="CW1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="CR1" s="21" t="s">
+      <c r="CX1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="CS1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="CT1" s="21" t="s">
+      <c r="CZ1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="CU1" s="21" t="s">
+      <c r="DA1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CV1" s="21" t="s">
+      <c r="DB1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="CW1" s="21" t="s">
+      <c r="DC1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="DD1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="CY1" s="21" t="s">
+      <c r="DE1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="CZ1" s="21" t="s">
+      <c r="DF1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="DA1" s="21" t="s">
+      <c r="DG1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="DB1" s="21" t="s">
+      <c r="DH1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="DC1" s="21" t="s">
+      <c r="DI1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="DD1" s="21" t="s">
+      <c r="DJ1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="DE1" s="21" t="s">
+      <c r="DK1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="DF1" s="21" t="s">
+      <c r="DL1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="DG1" s="21" t="s">
+      <c r="DM1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="DH1" s="21" t="s">
+      <c r="DN1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="DI1" s="21" t="s">
+      <c r="DO1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="DJ1" s="21" t="s">
+      <c r="DP1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="DK1" s="21" t="s">
+      <c r="DQ1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="DL1" s="21" t="s">
+      <c r="DR1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="DM1" s="21" t="s">
+      <c r="DS1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="DN1" s="21" t="s">
+      <c r="DT1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:118" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="C2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D2" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>385</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>326</v>
-      </c>
+      <c r="K2" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="L2" s="29">
+        <v>100</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
+      <c r="CB2" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="CC2" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="CD2" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="CE2" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="CF2" s="20"/>
+      <c r="CG2" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="CH2" s="20"/>
+      <c r="CI2" s="20"/>
+      <c r="CJ2" s="20"/>
+      <c r="CK2" s="20"/>
+      <c r="CL2" s="20"/>
+      <c r="CM2" s="20"/>
+      <c r="CN2" s="20"/>
+      <c r="CO2" s="20"/>
+      <c r="CP2" s="20"/>
+      <c r="CQ2" s="20"/>
+      <c r="CR2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="CS2" s="20"/>
+      <c r="CT2" s="20"/>
+      <c r="CU2" s="20"/>
+      <c r="CV2" s="20"/>
+      <c r="CW2" s="20"/>
+      <c r="CX2" s="20"/>
+      <c r="CY2" s="20"/>
+      <c r="CZ2" s="20"/>
+      <c r="DA2" s="20"/>
+      <c r="DB2" s="20"/>
+      <c r="DC2" s="20"/>
+      <c r="DD2" s="20"/>
+      <c r="DE2" s="20"/>
+      <c r="DF2" s="20"/>
+      <c r="DG2" s="20"/>
+      <c r="DH2" s="20"/>
+      <c r="DI2" s="20"/>
+      <c r="DJ2" s="20"/>
+      <c r="DK2" s="20"/>
+      <c r="DL2" s="20"/>
+      <c r="DM2" s="20"/>
+      <c r="DN2" s="20"/>
+      <c r="DO2" s="20"/>
+      <c r="DP2" s="20"/>
+      <c r="DQ2" s="20"/>
+      <c r="DR2" s="20"/>
+      <c r="DS2" s="20"/>
+      <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:118" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="AX3" s="20" t="s">
+      <c r="BC3" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="BY3" s="20" t="s">
+      <c r="CE3" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="BZ3" s="20" t="s">
+      <c r="CF3" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="CA3" s="20" t="s">
+      <c r="CG3" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="CR3" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="W4" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
+      <c r="AN4" s="20"/>
+      <c r="AO4" s="20"/>
+      <c r="AP4" s="20"/>
+      <c r="AQ4" s="20"/>
+      <c r="AR4" s="20"/>
+      <c r="AS4" s="20"/>
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="20"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="20"/>
+      <c r="BA4" s="20"/>
+      <c r="BB4" s="20"/>
+      <c r="BC4" s="20"/>
+      <c r="BD4" s="20"/>
+      <c r="BE4" s="20"/>
+      <c r="BF4" s="20"/>
+      <c r="BG4" s="20"/>
+      <c r="BH4" s="20"/>
+      <c r="BI4" s="20"/>
+      <c r="BJ4" s="20"/>
+      <c r="BK4" s="20"/>
+      <c r="BL4" s="20"/>
+      <c r="BM4" s="20"/>
+      <c r="BN4" s="20"/>
+      <c r="BO4" s="20"/>
+      <c r="BP4" s="20"/>
+      <c r="BQ4" s="20"/>
+      <c r="BR4" s="20"/>
+      <c r="BS4" s="20"/>
+      <c r="BT4" s="20"/>
+      <c r="BU4" s="20"/>
+      <c r="BV4" s="20"/>
+      <c r="BW4" s="20"/>
+      <c r="BX4" s="20"/>
+      <c r="BY4" s="20"/>
+      <c r="BZ4" s="20"/>
+      <c r="CA4" s="20"/>
+      <c r="CB4" s="20"/>
+      <c r="CC4" s="20"/>
+      <c r="CD4" s="20"/>
+      <c r="CE4" s="20"/>
+      <c r="CF4" s="20"/>
+      <c r="CG4" s="20"/>
+      <c r="CH4" s="20"/>
+      <c r="CI4" s="20"/>
+      <c r="CJ4" s="20"/>
+      <c r="CK4" s="20"/>
+      <c r="CL4" s="20"/>
+      <c r="CM4" s="20"/>
+      <c r="CN4" s="20"/>
+      <c r="CO4" s="20"/>
+      <c r="CP4" s="20"/>
+      <c r="CQ4" s="20"/>
+      <c r="CR4" s="20"/>
+      <c r="CS4" s="20"/>
+      <c r="CT4" s="20"/>
+      <c r="CU4" s="20"/>
+      <c r="CV4" s="20"/>
+      <c r="CW4" s="20"/>
+      <c r="CX4" s="20"/>
+      <c r="CY4" s="20"/>
+      <c r="CZ4" s="20"/>
+      <c r="DA4" s="20"/>
+      <c r="DB4" s="20"/>
+      <c r="DC4" s="20"/>
+      <c r="DD4" s="20"/>
+      <c r="DE4" s="20"/>
+      <c r="DF4" s="20"/>
+      <c r="DG4" s="20"/>
+      <c r="DH4" s="20"/>
+      <c r="DI4" s="20"/>
+      <c r="DJ4" s="20"/>
+      <c r="DK4" s="20"/>
+      <c r="DL4" s="20"/>
+      <c r="DM4" s="20"/>
+      <c r="DN4" s="20"/>
+      <c r="DO4" s="20"/>
+      <c r="DP4" s="20"/>
+      <c r="DQ4" s="20"/>
+      <c r="DR4" s="20"/>
+      <c r="DS4" s="20"/>
+      <c r="DT4" s="20"/>
+    </row>
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="L5" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="S5" s="29"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="20"/>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="20"/>
+      <c r="BF5" s="20"/>
+      <c r="BG5" s="20"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="20"/>
+      <c r="BL5" s="20"/>
+      <c r="BM5" s="20"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="20"/>
+      <c r="BP5" s="20"/>
+      <c r="BQ5" s="20"/>
+      <c r="BR5" s="20"/>
+      <c r="BS5" s="20"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="20"/>
+      <c r="BX5" s="20"/>
+      <c r="BY5" s="20"/>
+      <c r="BZ5" s="20"/>
+      <c r="CA5" s="20"/>
+      <c r="CB5" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="CC5" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="CD5" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="CE5" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="CF5" s="20"/>
+      <c r="CG5" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="CH5" s="20"/>
+      <c r="CI5" s="20"/>
+      <c r="CJ5" s="20"/>
+      <c r="CK5" s="20"/>
+      <c r="CL5" s="20"/>
+      <c r="CM5" s="20"/>
+      <c r="CN5" s="20"/>
+      <c r="CO5" s="20"/>
+      <c r="CP5" s="20"/>
+      <c r="CQ5" s="20"/>
+      <c r="CR5" s="20"/>
+      <c r="CS5" s="20"/>
+      <c r="CT5" s="20"/>
+      <c r="CU5" s="20"/>
+      <c r="CV5" s="20"/>
+      <c r="CW5" s="20"/>
+      <c r="CX5" s="20"/>
+      <c r="CY5" s="20"/>
+      <c r="CZ5" s="20"/>
+      <c r="DA5" s="20"/>
+      <c r="DB5" s="20"/>
+      <c r="DC5" s="20"/>
+      <c r="DD5" s="20"/>
+      <c r="DE5" s="20"/>
+      <c r="DF5" s="20"/>
+      <c r="DG5" s="20"/>
+      <c r="DH5" s="20"/>
+      <c r="DI5" s="20"/>
+      <c r="DJ5" s="20"/>
+      <c r="DK5" s="20"/>
+      <c r="DL5" s="20"/>
+      <c r="DM5" s="20"/>
+      <c r="DN5" s="20"/>
+      <c r="DO5" s="20"/>
+      <c r="DP5" s="20"/>
+      <c r="DQ5" s="20"/>
+      <c r="DR5" s="20"/>
+      <c r="DS5" s="20"/>
+      <c r="DT5" s="20"/>
+    </row>
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="20"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="20"/>
+      <c r="BF6" s="20"/>
+      <c r="BG6" s="20"/>
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="20"/>
+      <c r="BL6" s="20"/>
+      <c r="BM6" s="20"/>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+      <c r="BP6" s="20"/>
+      <c r="BQ6" s="20"/>
+      <c r="BR6" s="20"/>
+      <c r="BS6" s="20"/>
+      <c r="BT6" s="20"/>
+      <c r="BU6" s="20"/>
+      <c r="BV6" s="20"/>
+      <c r="BW6" s="20"/>
+      <c r="BX6" s="20"/>
+      <c r="BY6" s="20"/>
+      <c r="BZ6" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="CA6" s="20"/>
+      <c r="CB6" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="CC6" s="20"/>
+      <c r="CD6" s="20"/>
+      <c r="CE6" s="20"/>
+      <c r="CF6" s="20"/>
+      <c r="CG6" s="20"/>
+      <c r="CH6" s="20"/>
+      <c r="CI6" s="20"/>
+      <c r="CJ6" s="20"/>
+      <c r="CK6" s="20"/>
+      <c r="CL6" s="20"/>
+      <c r="CM6" s="20"/>
+      <c r="CN6" s="20"/>
+      <c r="CO6" s="20"/>
+      <c r="CP6" s="20"/>
+      <c r="CQ6" s="20"/>
+      <c r="CR6" s="20"/>
+      <c r="CS6" s="20"/>
+      <c r="CT6" s="20"/>
+      <c r="CU6" s="20"/>
+      <c r="CV6" s="20"/>
+      <c r="CW6" s="20"/>
+      <c r="CX6" s="20"/>
+      <c r="CY6" s="20"/>
+      <c r="CZ6" s="20"/>
+      <c r="DA6" s="20"/>
+      <c r="DB6" s="20"/>
+      <c r="DC6" s="20"/>
+      <c r="DD6" s="20"/>
+      <c r="DE6" s="20"/>
+      <c r="DF6" s="20"/>
+      <c r="DG6" s="20"/>
+      <c r="DH6" s="20"/>
+      <c r="DI6" s="20"/>
+      <c r="DJ6" s="20"/>
+      <c r="DK6" s="20"/>
+      <c r="DL6" s="20"/>
+      <c r="DM6" s="20"/>
+      <c r="DN6" s="20"/>
+      <c r="DO6" s="20"/>
+      <c r="DP6" s="20"/>
+      <c r="DQ6" s="20"/>
+      <c r="DR6" s="20"/>
+      <c r="DS6" s="20"/>
+      <c r="DT6" s="20"/>
+    </row>
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="V7" s="20">
+        <v>432</v>
+      </c>
+      <c r="W7" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
+      <c r="BE7" s="20"/>
+      <c r="BF7" s="20"/>
+      <c r="BG7" s="20"/>
+      <c r="BH7" s="20"/>
+      <c r="BI7" s="20"/>
+      <c r="BJ7" s="20"/>
+      <c r="BK7" s="20"/>
+      <c r="BL7" s="20"/>
+      <c r="BM7" s="20"/>
+      <c r="BN7" s="20"/>
+      <c r="BO7" s="20"/>
+      <c r="BP7" s="20"/>
+      <c r="BQ7" s="20"/>
+      <c r="BR7" s="20"/>
+      <c r="BS7" s="20"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="20"/>
+      <c r="BW7" s="20"/>
+      <c r="BX7" s="20"/>
+      <c r="BY7" s="20"/>
+      <c r="BZ7" s="20"/>
+      <c r="CA7" s="20"/>
+      <c r="CB7" s="20"/>
+      <c r="CC7" s="20"/>
+      <c r="CD7" s="20"/>
+      <c r="CE7" s="20"/>
+      <c r="CF7" s="20"/>
+      <c r="CG7" s="20"/>
+      <c r="CH7" s="20"/>
+      <c r="CI7" s="20"/>
+      <c r="CJ7" s="20"/>
+      <c r="CK7" s="20"/>
+      <c r="CL7" s="20"/>
+      <c r="CM7" s="20"/>
+      <c r="CN7" s="20"/>
+      <c r="CO7" s="20"/>
+      <c r="CP7" s="20"/>
+      <c r="CQ7" s="20"/>
+      <c r="CR7" s="20"/>
+      <c r="CS7" s="20"/>
+      <c r="CT7" s="20"/>
+      <c r="CU7" s="20"/>
+      <c r="CV7" s="20"/>
+      <c r="CW7" s="20"/>
+      <c r="CX7" s="20"/>
+      <c r="CY7" s="20"/>
+      <c r="CZ7" s="20"/>
+      <c r="DA7" s="20"/>
+      <c r="DB7" s="20"/>
+      <c r="DC7" s="20"/>
+      <c r="DD7" s="20"/>
+      <c r="DE7" s="20"/>
+      <c r="DF7" s="20"/>
+      <c r="DG7" s="20"/>
+      <c r="DH7" s="20"/>
+      <c r="DI7" s="20"/>
+      <c r="DJ7" s="20"/>
+      <c r="DK7" s="20"/>
+      <c r="DL7" s="20"/>
+      <c r="DM7" s="20"/>
+      <c r="DN7" s="20"/>
+      <c r="DO7" s="20"/>
+      <c r="DP7" s="20"/>
+      <c r="DQ7" s="20"/>
+      <c r="DR7" s="20"/>
+      <c r="DS7" s="20"/>
+      <c r="DT7" s="20"/>
+    </row>
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="20"/>
+      <c r="AN8" s="20"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
+      <c r="BB8" s="20"/>
+      <c r="BC8" s="20"/>
+      <c r="BD8" s="20"/>
+      <c r="BE8" s="20"/>
+      <c r="BF8" s="20"/>
+      <c r="BG8" s="20"/>
+      <c r="BH8" s="20"/>
+      <c r="BI8" s="20"/>
+      <c r="BJ8" s="20"/>
+      <c r="BK8" s="20"/>
+      <c r="BL8" s="20"/>
+      <c r="BM8" s="20"/>
+      <c r="BN8" s="20"/>
+      <c r="BO8" s="20"/>
+      <c r="BP8" s="20"/>
+      <c r="BQ8" s="20"/>
+      <c r="BR8" s="20"/>
+      <c r="BS8" s="20"/>
+      <c r="BT8" s="20"/>
+      <c r="BU8" s="20"/>
+      <c r="BV8" s="20"/>
+      <c r="BW8" s="20"/>
+      <c r="BX8" s="20"/>
+      <c r="BY8" s="20"/>
+      <c r="BZ8" s="20"/>
+      <c r="CA8" s="20"/>
+      <c r="CB8" s="20"/>
+      <c r="CC8" s="20"/>
+      <c r="CD8" s="20"/>
+      <c r="CE8" s="20"/>
+      <c r="CF8" s="20"/>
+      <c r="CG8" s="20"/>
+      <c r="CH8" s="20"/>
+      <c r="CI8" s="20"/>
+      <c r="CJ8" s="20"/>
+      <c r="CK8" s="20"/>
+      <c r="CL8" s="20"/>
+      <c r="CM8" s="20"/>
+      <c r="CN8" s="20"/>
+      <c r="CO8" s="20"/>
+      <c r="CP8" s="20"/>
+      <c r="CQ8" s="20"/>
+      <c r="CR8" s="20"/>
+      <c r="CS8" s="20"/>
+      <c r="CT8" s="20"/>
+      <c r="CU8" s="20"/>
+      <c r="CV8" s="20"/>
+      <c r="CW8" s="20"/>
+      <c r="CX8" s="20"/>
+      <c r="CY8" s="20"/>
+      <c r="CZ8" s="20"/>
+      <c r="DA8" s="20"/>
+      <c r="DB8" s="20"/>
+      <c r="DC8" s="20"/>
+      <c r="DD8" s="20"/>
+      <c r="DE8" s="20"/>
+      <c r="DF8" s="20"/>
+      <c r="DG8" s="20"/>
+      <c r="DH8" s="20"/>
+      <c r="DI8" s="20"/>
+      <c r="DJ8" s="20"/>
+      <c r="DK8" s="20"/>
+      <c r="DL8" s="20"/>
+      <c r="DM8" s="20"/>
+      <c r="DN8" s="20"/>
+      <c r="DO8" s="20"/>
+      <c r="DP8" s="20"/>
+      <c r="DQ8" s="20"/>
+      <c r="DR8" s="20"/>
+      <c r="DS8" s="20"/>
+      <c r="DT8" s="20"/>
+    </row>
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="20"/>
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20"/>
+      <c r="AZ9" s="20"/>
+      <c r="BA9" s="20"/>
+      <c r="BB9" s="20"/>
+      <c r="BC9" s="20"/>
+      <c r="BD9" s="20"/>
+      <c r="BE9" s="20"/>
+      <c r="BF9" s="20"/>
+      <c r="BG9" s="20"/>
+      <c r="BH9" s="20"/>
+      <c r="BI9" s="20"/>
+      <c r="BJ9" s="20"/>
+      <c r="BK9" s="20"/>
+      <c r="BL9" s="20"/>
+      <c r="BM9" s="20"/>
+      <c r="BN9" s="20"/>
+      <c r="BO9" s="20"/>
+      <c r="BP9" s="20"/>
+      <c r="BQ9" s="20"/>
+      <c r="BR9" s="20"/>
+      <c r="BS9" s="20"/>
+      <c r="BT9" s="20"/>
+      <c r="BU9" s="20"/>
+      <c r="BV9" s="20"/>
+      <c r="BW9" s="20"/>
+      <c r="BX9" s="20"/>
+      <c r="BY9" s="20"/>
+      <c r="BZ9" s="20"/>
+      <c r="CA9" s="20"/>
+      <c r="CB9" s="20"/>
+      <c r="CC9" s="20"/>
+      <c r="CD9" s="20"/>
+      <c r="CE9" s="20"/>
+      <c r="CF9" s="20"/>
+      <c r="CG9" s="20"/>
+      <c r="CH9" s="20"/>
+      <c r="CI9" s="20"/>
+      <c r="CJ9" s="20"/>
+      <c r="CK9" s="20"/>
+      <c r="CL9" s="20"/>
+      <c r="CM9" s="20"/>
+      <c r="CN9" s="20"/>
+      <c r="CO9" s="20"/>
+      <c r="CP9" s="20"/>
+      <c r="CQ9" s="20"/>
+      <c r="CR9" s="20"/>
+      <c r="CS9" s="20"/>
+      <c r="CT9" s="20"/>
+      <c r="CU9" s="20"/>
+      <c r="CV9" s="20"/>
+      <c r="CW9" s="20"/>
+      <c r="CX9" s="20"/>
+      <c r="CY9" s="20"/>
+      <c r="CZ9" s="20"/>
+      <c r="DA9" s="20"/>
+      <c r="DB9" s="20"/>
+      <c r="DC9" s="20"/>
+      <c r="DD9" s="20"/>
+      <c r="DE9" s="20"/>
+      <c r="DF9" s="20"/>
+      <c r="DG9" s="20"/>
+      <c r="DH9" s="20"/>
+      <c r="DI9" s="20"/>
+      <c r="DJ9" s="20"/>
+      <c r="DK9" s="20"/>
+      <c r="DL9" s="20"/>
+      <c r="DM9" s="20"/>
+      <c r="DN9" s="20"/>
+      <c r="DO9" s="20"/>
+      <c r="DP9" s="20"/>
+      <c r="DQ9" s="20"/>
+      <c r="DR9" s="20"/>
+      <c r="DS9" s="20"/>
+      <c r="DT9" s="20"/>
+    </row>
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="20"/>
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="20"/>
+      <c r="AW10" s="20"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="20"/>
+      <c r="AZ10" s="20"/>
+      <c r="BA10" s="20"/>
+      <c r="BB10" s="20"/>
+      <c r="BC10" s="20"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="20"/>
+      <c r="BF10" s="20"/>
+      <c r="BG10" s="20"/>
+      <c r="BH10" s="20"/>
+      <c r="BI10" s="20"/>
+      <c r="BJ10" s="20"/>
+      <c r="BK10" s="20"/>
+      <c r="BL10" s="20"/>
+      <c r="BM10" s="20"/>
+      <c r="BN10" s="20"/>
+      <c r="BO10" s="20"/>
+      <c r="BP10" s="20"/>
+      <c r="BQ10" s="20"/>
+      <c r="BR10" s="20"/>
+      <c r="BS10" s="20"/>
+      <c r="BT10" s="20"/>
+      <c r="BU10" s="20"/>
+      <c r="BV10" s="20"/>
+      <c r="BW10" s="20"/>
+      <c r="BX10" s="20"/>
+      <c r="BY10" s="20"/>
+      <c r="BZ10" s="20"/>
+      <c r="CA10" s="20"/>
+      <c r="CB10" s="20"/>
+      <c r="CC10" s="20"/>
+      <c r="CD10" s="20"/>
+      <c r="CE10" s="20"/>
+      <c r="CF10" s="20"/>
+      <c r="CG10" s="20"/>
+      <c r="CH10" s="20"/>
+      <c r="CI10" s="20"/>
+      <c r="CJ10" s="20"/>
+      <c r="CK10" s="20"/>
+      <c r="CL10" s="20"/>
+      <c r="CM10" s="20"/>
+      <c r="CN10" s="20"/>
+      <c r="CO10" s="20"/>
+      <c r="CP10" s="20"/>
+      <c r="CQ10" s="20"/>
+      <c r="CR10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="CS10" s="20"/>
+      <c r="CT10" s="20"/>
+      <c r="CU10" s="20"/>
+      <c r="CV10" s="20"/>
+      <c r="CW10" s="20"/>
+      <c r="CX10" s="20"/>
+      <c r="CY10" s="20"/>
+      <c r="CZ10" s="20"/>
+      <c r="DA10" s="20"/>
+      <c r="DB10" s="20"/>
+      <c r="DC10" s="20"/>
+      <c r="DD10" s="20"/>
+      <c r="DE10" s="20"/>
+      <c r="DF10" s="20"/>
+      <c r="DG10" s="20"/>
+      <c r="DH10" s="20"/>
+      <c r="DI10" s="20"/>
+      <c r="DJ10" s="20"/>
+      <c r="DK10" s="20"/>
+      <c r="DL10" s="20"/>
+      <c r="DM10" s="20"/>
+      <c r="DN10" s="20"/>
+      <c r="DO10" s="20"/>
+      <c r="DP10" s="20"/>
+      <c r="DQ10" s="20"/>
+      <c r="DR10" s="20"/>
+      <c r="DS10" s="20"/>
+      <c r="DT10" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{C4B9FB17-BB0F-41D0-9C95-4C7FCA804C49}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{5D193D50-B78E-48AE-8445-69A290522922}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0F4D727E-2335-43BE-863D-37226A5E2D36}"/>
+    <hyperlink ref="CG3" r:id="rId2" xr:uid="{F057FAC8-0A57-4D6D-A9D0-DE791A21EBC0}"/>
+    <hyperlink ref="CF3" r:id="rId3" xr:uid="{AE3ED39A-666B-4E61-8DB3-2B6C76B58E1D}"/>
+    <hyperlink ref="CR3" r:id="rId4" xr:uid="{A4708C70-4900-4C39-B150-20BAAEBFBA53}"/>
+    <hyperlink ref="CR2" r:id="rId5" xr:uid="{3A3E797F-0206-4012-9009-9813395840D8}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{B5FCC387-F56C-4A93-A380-0DAA3732B74C}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{B092573B-9361-4BEF-88D6-65CF0E39C980}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{0FE5CD64-EACD-4A80-9A06-BCBBEAAED9C7}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{5D471A0C-E64A-46B2-8D41-DE60BD921291}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{9C87F5C9-9F4E-4856-A5CB-B00741632FE8}"/>
+    <hyperlink ref="D6" r:id="rId11" xr:uid="{5CEF3D62-AF1A-4151-A457-4D8F820085BB}"/>
+    <hyperlink ref="D5" r:id="rId12" xr:uid="{554881D9-889D-4E28-8CFC-7A88786BEBF7}"/>
+    <hyperlink ref="CR10" r:id="rId13" xr:uid="{CECF781A-1973-4855-B511-F61368BE1D65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Advance pricing excel admin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43E5999-20F1-483F-B8C0-3F965E1F99FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6A2018-5320-4CB9-BC5C-902325F2F2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="customer" sheetId="6" r:id="rId10"/>
     <sheet name="Category" sheetId="8" r:id="rId11"/>
     <sheet name="CatalogPricerule" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="406">
   <si>
     <t>DataSet</t>
   </si>
@@ -1235,6 +1234,21 @@
   </si>
   <si>
     <t>OXO ON 9 CUP COFFEE MAKER</t>
+  </si>
+  <si>
+    <t>searchproduct</t>
+  </si>
+  <si>
+    <t>QATest Product</t>
+  </si>
+  <si>
+    <t>SpecialPrice</t>
+  </si>
+  <si>
+    <t>AdvancedPricing</t>
+  </si>
+  <si>
+    <t>QATestProduct</t>
   </si>
 </sst>
 </file>
@@ -2508,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,18 +2785,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CA6EE1-C0A9-4DD1-ABBA-0E76043F9F34}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5178,21 +5180,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DC4"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView topLeftCell="BR1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="37" max="37" width="25.85546875" customWidth="1"/>
-    <col min="38" max="38" width="28.42578125" style="20" customWidth="1"/>
-    <col min="39" max="39" width="31.85546875" customWidth="1"/>
-    <col min="71" max="71" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5217,305 +5222,68 @@
       <c r="H1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>177</v>
+      <c r="I1" s="21" t="s">
+        <v>323</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>56</v>
+        <v>223</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>58</v>
+        <v>224</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>225</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>59</v>
+        <v>226</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>60</v>
+        <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL1" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>227</v>
+        <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5528,93 +5296,117 @@
       <c r="F2" t="s">
         <v>97</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="N2" t="s">
         <v>228</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="O2" t="s">
         <v>229</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="P2" t="s">
         <v>141</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="Q2" t="s">
         <v>142</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="V2" t="s">
         <v>230</v>
       </c>
-      <c r="CY2">
+      <c r="W2">
         <v>5</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="X2" t="s">
         <v>231</v>
       </c>
-      <c r="DA2">
+      <c r="Y2">
         <v>30</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="Z2" t="s">
         <v>232</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="AA2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
-      <c r="AL3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="J3" t="s">
         <v>235</v>
       </c>
-      <c r="BS3" t="s">
+      <c r="N3" t="s">
         <v>228</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="P3" t="s">
         <v>236</v>
       </c>
-      <c r="CA3" t="s">
+      <c r="Q3" t="s">
         <v>40</v>
       </c>
-      <c r="CX3" t="s">
+      <c r="V3" t="s">
         <v>230</v>
       </c>
-      <c r="CY3">
+      <c r="W3">
         <v>5</v>
       </c>
-      <c r="CZ3" t="s">
+      <c r="X3" t="s">
         <v>231</v>
       </c>
-      <c r="DA3">
+      <c r="Y3">
         <v>30</v>
       </c>
-      <c r="DB3" t="s">
+      <c r="Z3" t="s">
         <v>232</v>
       </c>
-      <c r="DC3" t="s">
+      <c r="AA3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="K4" t="s">
         <v>229</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="O4" t="s">
         <v>238</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="P4" t="s">
         <v>236</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="Q4" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>404</v>
+      </c>
+      <c r="AB6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>405</v>
+      </c>
+      <c r="AB7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6590,8 +6382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Magento group product order placement-Testcase,Testdata,helper-commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6A2018-5320-4CB9-BC5C-902325F2F2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFCBFB5-6427-4CE7-A9A7-4BFAD7082B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="425">
   <si>
     <t>DataSet</t>
   </si>
@@ -1249,6 +1249,63 @@
   </si>
   <si>
     <t>QATestProduct</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>lotusqatestmanual.gold2@gmail.com</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>OXO Store View</t>
+  </si>
+  <si>
+    <t>HFWebsite</t>
+  </si>
+  <si>
+    <t>OXOWebsite</t>
+  </si>
+  <si>
+    <t>HFGroupproduct</t>
+  </si>
+  <si>
+    <t>hf-group</t>
+  </si>
+  <si>
+    <t>storepage</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>spanem@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>hJTROzDump6@</t>
+  </si>
+  <si>
+    <t>Create New Order for test lotus in Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>Create New Order in OXO Store View</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>You need to choose options for your item.</t>
+  </si>
+  <si>
+    <t>'10/28</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1456,6 +1513,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5182,7 +5240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -5912,25 +5970,31 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
-  <dimension ref="A1:DI10"/>
+  <dimension ref="A1:DM10"/>
   <sheetViews>
-    <sheetView topLeftCell="DQ1" workbookViewId="0">
-      <selection activeCell="EC4" sqref="EC4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="20"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="20"/>
-    <col min="8" max="11" width="33" style="20" customWidth="1"/>
-    <col min="12" max="12" width="33" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="72" max="72" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="33" style="20" customWidth="1"/>
+    <col min="13" max="13" width="33" customWidth="1"/>
+    <col min="14" max="14" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:117" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5953,374 +6017,387 @@
         <v>329</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="O1" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AU1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AV1" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AY1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="AZ1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="BA1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="BB1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="BC1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="BD1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="BA1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="BB1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="BC1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BQ1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BR1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BS1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BP1" s="21" t="s">
+      <c r="BT1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="BQ1" s="21" t="s">
+      <c r="BU1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BR1" s="21" t="s">
+      <c r="BV1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="BS1" s="21" t="s">
+      <c r="BW1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="BT1" s="21" t="s">
+      <c r="BX1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="BU1" s="21" t="s">
+      <c r="BY1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="BV1" s="21" t="s">
+      <c r="BZ1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="BW1" s="21" t="s">
+      <c r="CA1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="BX1" s="21" t="s">
+      <c r="CB1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="BY1" s="21" t="s">
+      <c r="CC1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="BZ1" s="21" t="s">
+      <c r="CD1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="CA1" s="21" t="s">
+      <c r="CE1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CB1" s="21" t="s">
+      <c r="CF1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="CC1" s="21" t="s">
+      <c r="CG1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="CD1" s="21" t="s">
+      <c r="CH1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="CE1" s="21" t="s">
+      <c r="CI1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="CF1" s="21" t="s">
+      <c r="CJ1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="CG1" s="21" t="s">
+      <c r="CK1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CH1" s="21" t="s">
+      <c r="CL1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CI1" s="21" t="s">
+      <c r="CM1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="CJ1" s="21" t="s">
+      <c r="CN1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="CK1" s="21" t="s">
+      <c r="CO1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CL1" s="21" t="s">
+      <c r="CP1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="CM1" s="21" t="s">
+      <c r="CQ1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="CN1" s="21" t="s">
+      <c r="CR1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="CO1" s="21" t="s">
+      <c r="CS1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="CP1" s="21" t="s">
+      <c r="CT1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CQ1" s="21" t="s">
+      <c r="CU1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="CR1" s="21" t="s">
+      <c r="CV1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="CS1" s="21" t="s">
+      <c r="CW1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="CT1" s="21" t="s">
+      <c r="CX1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="CU1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="CV1" s="21" t="s">
+      <c r="CZ1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="CW1" s="21" t="s">
+      <c r="DA1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="DB1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="CY1" s="21" t="s">
+      <c r="DC1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="CZ1" s="21" t="s">
+      <c r="DD1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="DA1" s="21" t="s">
+      <c r="DE1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="DB1" s="21" t="s">
+      <c r="DF1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="DC1" s="21" t="s">
+      <c r="DG1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="DD1" s="21" t="s">
+      <c r="DH1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="DE1" s="21" t="s">
+      <c r="DI1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="DF1" s="21" t="s">
+      <c r="DJ1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="DG1" s="21" t="s">
+      <c r="DK1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="DH1" s="21" t="s">
+      <c r="DL1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="DI1" s="21" t="s">
+      <c r="DM1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:113" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:117" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>326</v>
-      </c>
-      <c r="BD2" s="20" t="s">
+      <c r="BH2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="BY2" s="20" t="s">
+      <c r="CC2" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="CE2" s="20" t="s">
+      <c r="CI2" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="CF2" s="20" t="s">
+      <c r="CJ2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="CG2" s="20" t="s">
+      <c r="CK2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="DD2" s="20" t="s">
+      <c r="DH2" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="DE2" s="20">
+      <c r="DI2" s="20">
         <v>5</v>
       </c>
-      <c r="DF2" s="20" t="s">
+      <c r="DJ2" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="DG2" s="20">
+      <c r="DK2" s="20">
         <v>30</v>
       </c>
-      <c r="DH2" s="20" t="s">
+      <c r="DL2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="DI2" s="20" t="s">
+      <c r="DM2" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>406</v>
       </c>
       <c r="D3" t="s">
         <v>333</v>
@@ -6334,46 +6411,83 @@
       <c r="G3" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>343</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="33" t="s">
+        <v>424</v>
+      </c>
+      <c r="L3" s="34">
+        <v>432</v>
+      </c>
+      <c r="M3" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="BJ3" t="s">
+      <c r="N3" t="s">
+        <v>407</v>
+      </c>
+      <c r="BN3" t="s">
         <v>251</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="BT3" s="29"/>
+      <c r="BV3" t="s">
         <v>336</v>
       </c>
-      <c r="BS3" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="BT3">
+      <c r="BW3">
+        <v>6492</v>
+      </c>
+      <c r="BX3">
         <v>9898989898</v>
       </c>
-      <c r="BU3" t="s">
+      <c r="BY3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>411</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>412</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>413</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="O6" t="s">
+        <v>422</v>
+      </c>
+      <c r="P6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:117" x14ac:dyDescent="0.25">
       <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{AC56A3CD-87F9-47F3-B4E2-CBD67EBEE8E6}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{70304466-770B-4C05-A0CC-80C67DF26F82}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{AE88654D-CD03-4F51-B9BE-9B1612A867C1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Flush magneto cache method admin
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFCBFB5-6427-4CE7-A9A7-4BFAD7082B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF1E5C-F0F8-4C8A-BF8B-ADBB70C0559A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="17280" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="428">
   <si>
     <t>DataSet</t>
   </si>
@@ -1306,6 +1306,15 @@
   </si>
   <si>
     <t>'10/28</t>
+  </si>
+  <si>
+    <t>FlushMagento</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>Flush Magento Cache</t>
   </si>
 </sst>
 </file>
@@ -1795,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1865,7 @@
     <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1932,12 +1941,15 @@
       <c r="Y1" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="Z1" s="26" t="s">
+        <v>426</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -1950,7 +1962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2053,7 +2065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2085,7 +2097,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2115,6 +2127,14 @@
       </c>
       <c r="Y6" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2122,9 +2142,10 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{FE45A353-2970-40A1-8263-26DCFE88D323}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3991,7 +4012,7 @@
   <dimension ref="A1:CU3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,8 +5993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:DM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Admin Ordercreation 29, 31 - Testcases,TestData, helper,XMl file Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF1E5C-F0F8-4C8A-BF8B-ADBB70C0559A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F69D62C-3A04-481F-8186-7F52111F1BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="17280" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="431">
   <si>
     <t>DataSet</t>
   </si>
@@ -1315,6 +1315,15 @@
   </si>
   <si>
     <t>Flush Magento Cache</t>
+  </si>
+  <si>
+    <t>OXOGroupproduct</t>
+  </si>
+  <si>
+    <t>Baking Group</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -5993,26 +6002,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:DM10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="33" style="20" customWidth="1"/>
-    <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="14" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="33" style="20" customWidth="1"/>
+    <col min="14" max="14" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39" style="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="72" width="9.140625" style="20"/>
+    <col min="73" max="73" width="11" style="20" bestFit="1" customWidth="1"/>
+    <col min="74" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:117" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -6368,7 +6378,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:117" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6417,16 +6427,16 @@
       </c>
     </row>
     <row r="3" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="20" t="s">
         <v>333</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G3" s="20" t="s">
@@ -6445,28 +6455,28 @@
       <c r="M3" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="BN3" t="s">
+      <c r="BN3" s="20" t="s">
         <v>251</v>
       </c>
       <c r="BT3" s="29"/>
-      <c r="BV3" t="s">
+      <c r="BV3" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="BW3">
+      <c r="BW3" s="20">
         <v>6492</v>
       </c>
-      <c r="BX3">
+      <c r="BX3" s="20">
         <v>9898989898</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="BY3" s="20" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="20" t="s">
         <v>411</v>
       </c>
       <c r="H4" s="20" t="s">
@@ -6477,7 +6487,7 @@
       </c>
     </row>
     <row r="5" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="20" t="s">
         <v>412</v>
       </c>
       <c r="H5" s="20" t="s">
@@ -6488,7 +6498,7 @@
       </c>
     </row>
     <row r="6" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="20" t="s">
         <v>413</v>
       </c>
       <c r="G6" s="20">
@@ -6497,11 +6507,25 @@
       <c r="J6" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="20" t="s">
         <v>422</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="20" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:117" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Admin orderplacements - testcases 2, Testdata, XML File, Helper - Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BDCA10-3A10-407C-8185-263D856FEBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DC82F5-628B-4D1C-899E-A89294C3F7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9480" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="440">
   <si>
     <t>DataSet</t>
   </si>
@@ -1318,6 +1318,39 @@
   </si>
   <si>
     <t>1,2</t>
+  </si>
+  <si>
+    <t>OXOProducts</t>
+  </si>
+  <si>
+    <t>SKUNumberoxosimple</t>
+  </si>
+  <si>
+    <t>oxoQuantity</t>
+  </si>
+  <si>
+    <t>SKUNumberoxoconfigurable</t>
+  </si>
+  <si>
+    <t>SKUNumberoxobundle</t>
+  </si>
+  <si>
+    <t>32480</t>
+  </si>
+  <si>
+    <t>61132200B</t>
+  </si>
+  <si>
+    <t>oxo-13-piece-grilling-set</t>
+  </si>
+  <si>
+    <t>SKUnumb</t>
+  </si>
+  <si>
+    <t>Choosecolor</t>
+  </si>
+  <si>
+    <t>Tot Navy</t>
   </si>
 </sst>
 </file>
@@ -5996,10 +6029,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6012,14 +6045,14 @@
     <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="33" style="20" customWidth="1"/>
-    <col min="14" max="14" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="20"/>
+    <col min="9" max="19" width="33" style="20" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6051,91 +6084,109 @@
         <v>330</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>438</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6145,45 +6196,45 @@
       <c r="C2" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="20" t="s">
+      <c r="S2" s="27"/>
+      <c r="T2" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="W2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AM2" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="AH2" s="20">
+      <c r="AN2" s="20">
         <v>5</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AO2" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="AJ2" s="20">
+      <c r="AP2" s="20">
         <v>30</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AR2" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>406</v>
       </c>
@@ -6203,35 +6254,41 @@
       <c r="J3" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="L3" s="34">
+      <c r="R3" s="34">
         <v>432</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="S3" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="T3" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="Z3" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="AA3" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="V3" s="20">
+      <c r="AB3" s="20">
         <v>6492</v>
       </c>
-      <c r="W3" s="20">
+      <c r="AC3" s="20">
         <v>9898989898</v>
       </c>
-      <c r="X3" s="20" t="s">
+      <c r="AD3" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>411</v>
       </c>
@@ -6247,11 +6304,11 @@
       <c r="I4" s="20" t="s">
         <v>418</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="T4" s="20" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>412</v>
       </c>
@@ -6267,11 +6324,11 @@
       <c r="I5" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="T5" s="20" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>413</v>
       </c>
@@ -6287,17 +6344,17 @@
       <c r="J6" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="T6" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="U6" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="V6" s="20" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>426</v>
       </c>
@@ -6313,14 +6370,37 @@
       <c r="J7" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="T7" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="U7" s="20" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="O8" s="20">
+        <v>61132300</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>

</xml_diff>

<commit_message>
Retail Order custom price update Automation for HYF
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DC82F5-628B-4D1C-899E-A89294C3F7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B3F891-9841-488B-8721-9E093E33D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9480" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="446">
   <si>
     <t>DataSet</t>
   </si>
@@ -1351,6 +1351,24 @@
   </si>
   <si>
     <t>Tot Navy</t>
+  </si>
+  <si>
+    <t>HighPriceOverride</t>
+  </si>
+  <si>
+    <t>LowPriceOverride</t>
+  </si>
+  <si>
+    <t>highprice</t>
+  </si>
+  <si>
+    <t>lowprice</t>
+  </si>
+  <si>
+    <t>50.99</t>
+  </si>
+  <si>
+    <t>12.95</t>
   </si>
 </sst>
 </file>
@@ -5533,15 +5551,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:DJ4"/>
+  <dimension ref="A1:DM6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="9.140625" style="20"/>
+    <col min="16" max="16" width="9.140625" style="20"/>
+    <col min="18" max="18" width="9.140625" style="20"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:114" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:117" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5582,310 +5605,319 @@
         <v>352</v>
       </c>
       <c r="N1" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="21" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="R1" s="21" t="s">
+        <v>443</v>
+      </c>
+      <c r="S1" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AU1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AV1" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="AY1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="AZ1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="BA1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="BB1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="BC1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BA1" s="21" t="s">
+      <c r="BD1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="BB1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BQ1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BR1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BP1" s="21" t="s">
+      <c r="BS1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BQ1" s="21" t="s">
+      <c r="BT1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="BR1" s="21" t="s">
+      <c r="BU1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BS1" s="21" t="s">
+      <c r="BV1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="BT1" s="21" t="s">
+      <c r="BW1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="BU1" s="21" t="s">
+      <c r="BX1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="BV1" s="21" t="s">
+      <c r="BY1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="BW1" s="21" t="s">
+      <c r="BZ1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="BX1" s="21" t="s">
+      <c r="CA1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="BY1" s="21" t="s">
+      <c r="CB1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="BZ1" s="21" t="s">
+      <c r="CC1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="CA1" s="21" t="s">
+      <c r="CD1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="CB1" s="21" t="s">
+      <c r="CE1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CC1" s="21" t="s">
+      <c r="CF1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="CD1" s="21" t="s">
+      <c r="CG1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="CE1" s="21" t="s">
+      <c r="CH1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="CF1" s="21" t="s">
+      <c r="CI1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="CG1" s="21" t="s">
+      <c r="CJ1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="CH1" s="21" t="s">
+      <c r="CK1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CI1" s="21" t="s">
+      <c r="CL1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CJ1" s="21" t="s">
+      <c r="CM1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="CK1" s="21" t="s">
+      <c r="CN1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="CL1" s="21" t="s">
+      <c r="CO1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="21" t="s">
+      <c r="CP1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="21" t="s">
+      <c r="CQ1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="21" t="s">
+      <c r="CR1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="21" t="s">
+      <c r="CS1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="21" t="s">
+      <c r="CT1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CR1" s="21" t="s">
+      <c r="CU1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="CS1" s="21" t="s">
+      <c r="CV1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="CT1" s="21" t="s">
+      <c r="CW1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="CU1" s="21" t="s">
+      <c r="CX1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="CV1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="CW1" s="21" t="s">
+      <c r="CZ1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="DA1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="CY1" s="21" t="s">
+      <c r="DB1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="CZ1" s="21" t="s">
+      <c r="DC1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="DA1" s="21" t="s">
+      <c r="DD1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="DB1" s="21" t="s">
+      <c r="DE1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="DC1" s="21" t="s">
+      <c r="DF1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="DD1" s="21" t="s">
+      <c r="DG1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="DE1" s="21" t="s">
+      <c r="DH1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="DF1" s="21" t="s">
+      <c r="DI1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="DG1" s="21" t="s">
+      <c r="DJ1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="DH1" s="21" t="s">
+      <c r="DK1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="DI1" s="21" t="s">
+      <c r="DL1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="DJ1" s="21" t="s">
+      <c r="DM1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:117" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -5899,41 +5931,42 @@
         <v>326</v>
       </c>
       <c r="M2" s="27"/>
-      <c r="BE2" s="20" t="s">
+      <c r="N2" s="27"/>
+      <c r="BH2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="20" t="s">
+      <c r="CC2" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="CF2" s="20" t="s">
+      <c r="CI2" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="CG2" s="20" t="s">
+      <c r="CJ2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="CH2" s="20" t="s">
+      <c r="CK2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="DE2" s="20" t="s">
+      <c r="DH2" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="DF2" s="20">
+      <c r="DI2" s="20">
         <v>5</v>
       </c>
-      <c r="DG2" s="20" t="s">
+      <c r="DJ2" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="DH2" s="20">
+      <c r="DK2" s="20">
         <v>30</v>
       </c>
-      <c r="DI2" s="20" t="s">
+      <c r="DL2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="DJ2" s="20" t="s">
+      <c r="DM2" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:114" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:117" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>331</v>
       </c>
@@ -5965,23 +5998,24 @@
         <v>328</v>
       </c>
       <c r="M3" s="7"/>
-      <c r="BK3" s="20" t="s">
+      <c r="N3" s="7"/>
+      <c r="BN3" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="BS3" s="20" t="s">
+      <c r="BV3" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="BT3" s="29" t="s">
+      <c r="BW3" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="BU3" s="20">
+      <c r="BX3" s="20">
         <v>9898989898</v>
       </c>
-      <c r="BV3" s="20" t="s">
+      <c r="BY3" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:114" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:117" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>353</v>
       </c>
@@ -6014,6 +6048,25 @@
       </c>
       <c r="M4" s="35" t="s">
         <v>356</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>440</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:117" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R6" s="29" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -6031,7 +6084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Admin-33 testcase,helper,testdata - commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B3F891-9841-488B-8721-9E093E33D7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F7DD68-7F9D-45BA-A635-F421447B7893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="451">
   <si>
     <t>DataSet</t>
   </si>
@@ -1014,9 +1014,6 @@
     <t>rrendla@helenoftroy.com</t>
   </si>
   <si>
-    <t>Ackpgkyatnob4!</t>
-  </si>
-  <si>
     <t>qatesting.lotuswave@gmail.com</t>
   </si>
   <si>
@@ -1369,6 +1366,24 @@
   </si>
   <si>
     <t>12.95</t>
+  </si>
+  <si>
+    <t>OXO Website</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>32480,11234000</t>
+  </si>
+  <si>
+    <t>222 concord valley ave</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ahezcphlkbjh2!</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1577,6 +1592,8 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1996,7 +2013,7 @@
         <v>38</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -2185,10 +2202,10 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Z7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -2787,31 +2804,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>360</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>362</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>363</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>10</v>
@@ -2823,13 +2840,13 @@
         <v>9</v>
       </c>
       <c r="P1" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>364</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>365</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2845,16 +2862,16 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D3" t="s">
         <v>367</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>368</v>
       </c>
-      <c r="E3" t="s">
-        <v>369</v>
-      </c>
       <c r="F3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G3" t="s">
         <v>114</v>
@@ -2865,28 +2882,28 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H4" t="s">
         <v>217</v>
       </c>
       <c r="I4" t="s">
+        <v>370</v>
+      </c>
+      <c r="J4" t="s">
         <v>371</v>
-      </c>
-      <c r="J4" t="s">
-        <v>372</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Q4" t="s">
         <v>252</v>
       </c>
       <c r="R4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2914,7 +2931,7 @@
         <v>142</v>
       </c>
       <c r="O6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -4540,7 +4557,7 @@
   <dimension ref="A1:CW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,7 +5432,7 @@
         <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -5522,15 +5539,15 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>400</v>
+      </c>
+      <c r="AA5" t="s">
         <v>401</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AB6">
         <v>20</v>
@@ -5538,7 +5555,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AB7">
         <v>10</v>
@@ -5551,20 +5568,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:DM6"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="9.140625" style="20"/>
-    <col min="16" max="16" width="9.140625" style="20"/>
-    <col min="18" max="18" width="9.140625" style="20"/>
+    <col min="1" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="20"/>
+    <col min="12" max="12" width="35.7109375" style="20" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" style="20" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="20" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5578,503 +5602,336 @@
         <v>47</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>173</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>330</v>
-      </c>
       <c r="I1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>340</v>
-      </c>
       <c r="K1" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>174</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>176</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>48</v>
+        <v>191</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>49</v>
+        <v>192</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="AF1" s="21" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="AG1" s="21" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="AH1" s="21" t="s">
-        <v>58</v>
+        <v>223</v>
       </c>
       <c r="AI1" s="21" t="s">
-        <v>23</v>
+        <v>212</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="AK1" s="21" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="AM1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO1" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP1" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ1" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR1" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS1" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT1" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU1" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AV1" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="AW1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AX1" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY1" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="AZ1" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA1" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB1" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="BC1" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="BD1" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="BE1" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF1" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="BG1" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="BH1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="BI1" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="BJ1" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK1" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="BL1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="BM1" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="BN1" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="BO1" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="BP1" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="BQ1" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="BR1" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="BS1" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="BT1" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="BU1" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="BV1" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="BW1" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="BX1" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="BY1" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="BZ1" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="CA1" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="CB1" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="CC1" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="CD1" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="CE1" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="CG1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="CH1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="CI1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="CJ1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="CK1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="CL1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="CM1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="CN1" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="CO1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="CP1" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="CQ1" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="CR1" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="CS1" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="CT1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="CU1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="CV1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="CW1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="CX1" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="CY1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="CZ1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="DB1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="DC1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="DD1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="DE1" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="DF1" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="DG1" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="DH1" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="DI1" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="DJ1" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="DK1" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="DL1" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="DM1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:117" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>326</v>
+        <v>449</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>327</v>
+        <v>450</v>
       </c>
       <c r="L2" s="27" t="s">
         <v>326</v>
       </c>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
-      <c r="BH2" s="20" t="s">
+      <c r="S2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="CC2" s="20" t="s">
+      <c r="AA2" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="CI2" s="20" t="s">
+      <c r="AC2" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="CJ2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="CK2" s="20" t="s">
+      <c r="AE2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="DH2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="DI2" s="20">
+      <c r="AI2" s="20">
         <v>5</v>
       </c>
-      <c r="DJ2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="DK2" s="20">
+      <c r="AK2" s="20">
         <v>30</v>
       </c>
-      <c r="DL2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="DM2" s="20" t="s">
+      <c r="AM2" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:117" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J3" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="K3" s="34" t="s">
-        <v>342</v>
-      </c>
       <c r="L3" s="7" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="BN3" s="20" t="s">
+      <c r="V3" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="BV3" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="BW3" s="29" t="s">
+      <c r="W3" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="X3" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="BX3" s="20">
+      <c r="Y3" s="20">
         <v>9898989898</v>
       </c>
-      <c r="BY3" s="20" t="s">
+      <c r="Z3" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:117" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H4" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>408</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="I4" s="33" t="s">
-        <v>343</v>
-      </c>
-      <c r="J4" s="29" t="s">
+      <c r="E5" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>447</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="K4" s="29" t="s">
-        <v>342</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="M4" s="35" t="s">
-        <v>356</v>
-      </c>
-      <c r="N4" s="35" t="s">
+      <c r="M5" s="35"/>
+      <c r="N5" s="35" t="s">
         <v>409</v>
       </c>
+      <c r="O5" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="V5" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="W5" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="X5" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="Z5" s="20" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="5" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="R7" s="29" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>441</v>
-      </c>
-      <c r="R6" s="29" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{C53C6307-0E95-43AA-BE0A-AD24F1F87C5A}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{CD7D3846-4739-4D8F-8729-8F7437C112E2}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{91CBEDB6-E72E-4BBD-895A-BE1F7FBBAC2E}"/>
-    <hyperlink ref="L4" r:id="rId4" xr:uid="{67370BC4-64DE-4825-91CE-8AFBC1CC9FA7}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{54FAA365-3D1D-44D9-8E39-98E81F5CACCC}"/>
+    <hyperlink ref="L4" r:id="rId2" xr:uid="{666C0A42-77E9-4DD7-B2F5-7206CD34949B}"/>
+    <hyperlink ref="L5:L6" r:id="rId3" display="lotusqatestmanual.gold6@gmail.com" xr:uid="{08C579EF-AAE8-4E97-9AF1-C8FBB3408B8C}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{8D7DB33B-F951-4ACD-8F6C-8B16C8E96059}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{767DBD81-D7A1-4868-A8FE-FB9631371DC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6119,58 +5976,58 @@
         <v>47</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>173</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>330</v>
-      </c>
       <c r="K1" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>433</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>432</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>431</v>
-      </c>
       <c r="Q1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="R1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="R1" s="21" t="s">
-        <v>340</v>
-      </c>
       <c r="S1" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="T1" s="21" t="s">
         <v>174</v>
       </c>
       <c r="U1" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>416</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>417</v>
       </c>
       <c r="W1" s="21" t="s">
         <v>5</v>
@@ -6289,23 +6146,23 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I3" s="32"/>
       <c r="J3" s="33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K3" s="33"/>
       <c r="L3" s="33"/>
@@ -6314,22 +6171,22 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="R3" s="34">
         <v>432</v>
       </c>
       <c r="S3" s="40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Z3" s="20" t="s">
         <v>251</v>
       </c>
       <c r="AA3" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AB3" s="20">
         <v>6492</v>
@@ -6343,7 +6200,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>241</v>
@@ -6352,18 +6209,18 @@
         <v>289</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>241</v>
@@ -6372,18 +6229,18 @@
         <v>289</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>241</v>
@@ -6395,21 +6252,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="U6" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="V6" s="20" t="s">
         <v>420</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>241</v>
@@ -6421,36 +6278,36 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="U7" s="20" t="s">
         <v>427</v>
-      </c>
-      <c r="T7" s="20" t="s">
-        <v>407</v>
-      </c>
-      <c r="U7" s="20" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K8" s="29" t="s">
+        <v>433</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>434</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>436</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>435</v>
-      </c>
       <c r="N8" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
@@ -6490,61 +6347,61 @@
         <v>174</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J1" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>351</v>
-      </c>
       <c r="L1" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>379</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>380</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="R1" s="21" t="s">
         <v>173</v>
       </c>
       <c r="S1" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="T1" s="21" t="s">
-        <v>330</v>
-      </c>
       <c r="U1" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="V1" s="21" t="s">
-        <v>340</v>
-      </c>
       <c r="W1" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>175</v>
@@ -6709,7 +6566,7 @@
         <v>188</v>
       </c>
       <c r="BZ1" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="CA1" s="21" t="s">
         <v>189</v>
@@ -6724,7 +6581,7 @@
         <v>192</v>
       </c>
       <c r="CE1" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="CF1" s="21" t="s">
         <v>194</v>
@@ -6855,46 +6712,46 @@
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>384</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="E2" s="36" t="s">
+      <c r="G2" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>385</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>349</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>386</v>
       </c>
       <c r="L2" s="29">
         <v>100</v>
       </c>
       <c r="M2" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>387</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="O2" s="29" t="s">
-        <v>389</v>
-      </c>
       <c r="P2" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="20" t="s">
@@ -6962,10 +6819,10 @@
       <c r="BZ2" s="20"/>
       <c r="CA2" s="20"/>
       <c r="CB2" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="CC2" s="20" t="s">
         <v>335</v>
-      </c>
-      <c r="CC2" s="20" t="s">
-        <v>336</v>
       </c>
       <c r="CD2" s="29" t="s">
         <v>256</v>
@@ -7047,7 +6904,7 @@
       <c r="C4" s="20"/>
       <c r="E4" s="37"/>
       <c r="F4" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="22"/>
@@ -7060,18 +6917,18 @@
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
       <c r="S4" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
       <c r="V4" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
@@ -7176,44 +7033,44 @@
     </row>
     <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>394</v>
-      </c>
       <c r="D5" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="M5" s="20" t="s">
         <v>335</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>336</v>
       </c>
       <c r="N5" s="20"/>
       <c r="O5" s="20" t="s">
         <v>251</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q5" s="29" t="s">
         <v>257</v>
@@ -7283,10 +7140,10 @@
       <c r="BZ5" s="20"/>
       <c r="CA5" s="20"/>
       <c r="CB5" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="CC5" s="20" t="s">
         <v>335</v>
-      </c>
-      <c r="CC5" s="20" t="s">
-        <v>336</v>
       </c>
       <c r="CD5" s="29" t="s">
         <v>256</v>
@@ -7340,18 +7197,18 @@
     </row>
     <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E6" s="7"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
@@ -7420,11 +7277,11 @@
       <c r="BX6" s="20"/>
       <c r="BY6" s="20"/>
       <c r="BZ6" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="CA6" s="20"/>
       <c r="CB6" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="CC6" s="20"/>
       <c r="CD6" s="20"/>
@@ -7473,7 +7330,7 @@
     </row>
     <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -7490,13 +7347,13 @@
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="38" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="V7" s="20">
         <v>432</v>
       </c>
       <c r="W7" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
@@ -7602,14 +7459,14 @@
     </row>
     <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -7727,15 +7584,15 @@
     </row>
     <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -7748,7 +7605,7 @@
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
       <c r="S9" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>

</xml_diff>

<commit_message>
Retail Ordre 34, 35 testcase commit - Testcase, testdata, helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA7A182-BB3D-4B29-B14D-AD1966CC5EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3982F28-1B94-41FB-9A68-4368F6AB038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="9720" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="461">
   <si>
     <t>DataSet</t>
   </si>
@@ -1383,13 +1383,37 @@
     <t>7.0</t>
   </si>
   <si>
-    <t>32480,11234001</t>
-  </si>
-  <si>
     <t>10/27</t>
   </si>
   <si>
     <t>431</t>
+  </si>
+  <si>
+    <t>40.99,50.99</t>
+  </si>
+  <si>
+    <t>6.99,7.59</t>
+  </si>
+  <si>
+    <t>10/29</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>10/30</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>skatipelli@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ahezcphlkbjh3!</t>
+  </si>
+  <si>
+    <t>6.99,8.99</t>
   </si>
 </sst>
 </file>
@@ -4563,7 +4587,7 @@
   <dimension ref="A1:CW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5577,13 +5601,15 @@
   <dimension ref="A1:AM7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="20"/>
+    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
     <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
@@ -5654,7 +5680,7 @@
         <v>5</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="U1" s="21" t="s">
         <v>83</v>
@@ -5718,17 +5744,17 @@
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>97</v>
+      <c r="B2" s="7" t="s">
+        <v>458</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>210</v>
+        <v>459</v>
       </c>
       <c r="I2" s="33" t="s">
+        <v>450</v>
+      </c>
+      <c r="J2" s="33" t="s">
         <v>451</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>452</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>341</v>
@@ -5900,6 +5926,12 @@
       <c r="O5" s="20" t="s">
         <v>445</v>
       </c>
+      <c r="P5" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>453</v>
+      </c>
       <c r="V5" s="20" t="s">
         <v>251</v>
       </c>
@@ -5923,6 +5955,15 @@
       <c r="H6" s="42" t="s">
         <v>447</v>
       </c>
+      <c r="I6" s="33" t="s">
+        <v>454</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>341</v>
+      </c>
       <c r="L6" s="7" t="s">
         <v>354</v>
       </c>
@@ -5934,6 +5975,9 @@
       </c>
       <c r="P6" s="29" t="s">
         <v>443</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -5941,7 +5985,16 @@
         <v>440</v>
       </c>
       <c r="H7" s="42" t="s">
-        <v>450</v>
+        <v>447</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>341</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>354</v>
@@ -5951,6 +6004,9 @@
       </c>
       <c r="R7" s="29" t="s">
         <v>444</v>
+      </c>
+      <c r="T7" s="29" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -5959,6 +6015,7 @@
     <hyperlink ref="L2" r:id="rId1" xr:uid="{54FAA365-3D1D-44D9-8E39-98E81F5CACCC}"/>
     <hyperlink ref="L4" r:id="rId2" xr:uid="{666C0A42-77E9-4DD7-B2F5-7206CD34949B}"/>
     <hyperlink ref="L3" r:id="rId3" xr:uid="{8D7DB33B-F951-4ACD-8F6C-8B16C8E96059}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{719A4B45-4D21-4E72-B0DC-31316B521FAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7889,7 +7946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CT6"/>
   <sheetViews>
-    <sheetView topLeftCell="CD1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Warranty testcases commit - Helper, Testcases, Test Data, XML file commit.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F3982F28-1B94-41FB-9A68-4368F6AB038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F354F1E-0050-43D2-B03F-88A898986692}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70256C-EECA-4601-B6A4-017EA65DDF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="458">
   <si>
     <t>DataSet</t>
   </si>
@@ -1053,15 +1053,9 @@
     <t>CVV</t>
   </si>
   <si>
-    <t>432</t>
-  </si>
-  <si>
     <t>4242424242424242</t>
   </si>
   <si>
-    <t>10/28</t>
-  </si>
-  <si>
     <t>RuleName</t>
   </si>
   <si>
@@ -1092,15 +1086,9 @@
     <t>RetailOrder</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>lotusqatestmanual.gold6@gmail.com</t>
   </si>
   <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>Financecategory</t>
   </si>
   <si>
@@ -1356,52 +1344,67 @@
     <t>lowprice</t>
   </si>
   <si>
-    <t>50.99</t>
-  </si>
-  <si>
-    <t>12.95</t>
-  </si>
-  <si>
     <t>OXO Website</t>
   </si>
   <si>
     <t>3,4</t>
   </si>
   <si>
-    <t>32480,11234000</t>
-  </si>
-  <si>
     <t>222 concord valley ave</t>
   </si>
   <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>10/27</t>
-  </si>
-  <si>
-    <t>431</t>
-  </si>
-  <si>
     <t>40.99,50.99</t>
   </si>
   <si>
     <t>6.99,7.59</t>
   </si>
   <si>
-    <t>10/29</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>10/30</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
     <t>6.99,8.99</t>
+  </si>
+  <si>
+    <t>Lotus$mk2022</t>
+  </si>
+  <si>
+    <t>Ackpgkyatnob4!</t>
+  </si>
+  <si>
+    <t>HFProducts</t>
+  </si>
+  <si>
+    <t>2, 2</t>
+  </si>
+  <si>
+    <t>T20CP110,S18SX001</t>
+  </si>
+  <si>
+    <t>T20CP110</t>
+  </si>
+  <si>
+    <t>S18SX</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>S18SX464</t>
+  </si>
+  <si>
+    <t>CustomPrice</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>ProductQuantity</t>
+  </si>
+  <si>
+    <t>39.99,0</t>
+  </si>
+  <si>
+    <t>Warrentyorder</t>
+  </si>
+  <si>
+    <t>0.00,0.00</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1612,6 +1615,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1899,62 +1908,62 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.6640625" customWidth="1"/>
-    <col min="12" max="12" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2031,10 +2040,10 @@
         <v>38</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2122,7 +2131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2154,7 +2163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2218,12 +2227,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="Z7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2246,16 +2255,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2377,7 +2386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2394,7 +2403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -2435,7 +2444,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -2473,7 +2482,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -2492,7 +2501,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -2529,7 +2538,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -2554,7 +2563,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -2631,7 +2640,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -2658,7 +2667,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -2694,17 +2703,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2746,7 @@
       </c>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2748,12 +2757,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -2779,7 +2788,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -2805,13 +2814,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2822,31 +2831,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>358</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>361</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>362</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>10</v>
@@ -2858,16 +2867,16 @@
         <v>9</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2875,21 +2884,21 @@
         <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G3" t="s">
         <v>114</v>
@@ -2898,33 +2907,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H4" t="s">
         <v>217</v>
       </c>
       <c r="I4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="Q4" t="s">
         <v>252</v>
       </c>
       <c r="R4" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>309</v>
       </c>
@@ -2938,7 +2947,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>314</v>
       </c>
@@ -2949,7 +2958,7 @@
         <v>142</v>
       </c>
       <c r="O6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2965,55 +2974,55 @@
       <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="20"/>
-    <col min="5" max="5" width="49.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.6640625" style="20"/>
-    <col min="10" max="10" width="13.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" style="20"/>
+    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="20"/>
+    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7109375" style="20"/>
+    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.6640625" style="20"/>
-    <col min="18" max="18" width="42.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.6640625" style="20"/>
-    <col min="26" max="26" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.109375" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.6640625" style="20"/>
-    <col min="29" max="29" width="37.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.6640625" style="20"/>
-    <col min="32" max="32" width="18.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" style="20"/>
-    <col min="36" max="36" width="15.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7109375" style="20"/>
+    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7109375" style="20"/>
+    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" style="20"/>
+    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7109375" style="20"/>
+    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" style="20"/>
+    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.6640625" style="20"/>
-    <col min="42" max="42" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.6640625" style="20"/>
-    <col min="44" max="44" width="37.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.6640625" style="20"/>
-    <col min="52" max="52" width="9.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.6640625" style="20"/>
+    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="20"/>
+    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7109375" style="20"/>
+    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7109375" style="20"/>
+    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3204,7 +3213,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -3254,7 +3263,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -3306,7 +3315,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -3381,7 +3390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -3642,7 +3651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -3775,7 +3784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -3866,7 +3875,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -3974,7 +3983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -4104,13 +4113,13 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="25" max="25" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="25" max="25" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4409,7 +4418,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -4547,7 +4556,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4578,12 +4587,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4888,7 +4897,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4954,7 +4963,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -5096,7 +5105,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -5161,7 +5170,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -5354,20 +5363,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.88671875" customWidth="1"/>
-    <col min="14" max="14" width="28.109375" customWidth="1"/>
-    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5450,10 +5459,10 @@
         <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5500,7 +5509,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -5538,7 +5547,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5555,25 +5564,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="AA5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AB6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AB7">
         <v>10</v>
@@ -5586,30 +5595,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:AM7"/>
+  <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="20"/>
-    <col min="5" max="5" width="15.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="20"/>
-    <col min="8" max="8" width="16.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.109375" style="20"/>
-    <col min="12" max="12" width="35.6640625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" style="20" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="20"/>
+    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="20"/>
+    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5632,161 +5642,185 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="K1" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>351</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>405</v>
-      </c>
-      <c r="O1" s="21" t="s">
+      <c r="S1" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="Q1" s="21" t="s">
+      <c r="W1" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="X1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="R1" s="21" t="s">
-        <v>440</v>
-      </c>
-      <c r="S1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>97</v>
+      <c r="B2" s="7" t="s">
+        <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>448</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>449</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>326</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
-      <c r="S2" s="20" t="s">
+      <c r="O2" s="44">
+        <v>44861</v>
+      </c>
+      <c r="P2" s="20">
+        <v>431</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="Z2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="20" t="s">
+      <c r="AH2" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AO2" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="AI2" s="20">
+      <c r="AP2" s="20">
         <v>5</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="AK2" s="20">
+      <c r="AR2" s="20">
         <v>30</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AS2" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="AM2" s="20" t="s">
+      <c r="AT2" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -5802,42 +5836,47 @@
       <c r="G3" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="K3" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>354</v>
-      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="V3" s="20" t="s">
+      <c r="O3" s="45">
+        <v>44862</v>
+      </c>
+      <c r="P3" s="20">
+        <v>432</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="AA3" s="29"/>
+      <c r="AC3" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="AD3" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="X3" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y3" s="20">
+      <c r="AE3" s="20">
+        <v>6492</v>
+      </c>
+      <c r="AF3" s="20">
         <v>9898989898</v>
       </c>
-      <c r="Z3" s="20" t="s">
+      <c r="AG3" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>332</v>
@@ -5851,159 +5890,298 @@
       <c r="G4" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="J4" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="I4" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>353</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="M4" s="35" t="s">
-        <v>355</v>
-      </c>
-      <c r="N4" s="35" t="s">
-        <v>406</v>
-      </c>
-      <c r="O4" s="41" t="s">
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="43">
+        <v>44862</v>
+      </c>
+      <c r="P4" s="41">
+        <v>123</v>
+      </c>
+      <c r="Q4" s="41">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R4" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="S4" s="20">
+        <v>120</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="V4" s="20" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>444</v>
-      </c>
-      <c r="H5" s="42" t="s">
+        <v>438</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="33">
+        <v>3248011234000</v>
+      </c>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="43">
+        <v>44862</v>
+      </c>
+      <c r="P5" s="20">
+        <v>123</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="S5" s="29"/>
+      <c r="T5" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="U5" s="29"/>
+      <c r="V5" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="W5" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y5" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA5" s="29"/>
+      <c r="AC5" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD5" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>6492</v>
+      </c>
+      <c r="AF5" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="AG5" s="20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="33">
+        <v>3248011234000</v>
+      </c>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="7"/>
+      <c r="O6" s="43">
+        <v>44863</v>
+      </c>
+      <c r="P6" s="20">
+        <v>124</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="S6" s="29"/>
+      <c r="T6" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="V6" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="W6" s="29">
+        <v>50.99</v>
+      </c>
+      <c r="Y6" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="AA6" s="20" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="33">
+        <v>3248011234000</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="7"/>
+      <c r="O7" s="46">
+        <v>44864</v>
+      </c>
+      <c r="P7" s="20">
+        <v>125</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="S7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="W7" s="29">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="20">
+        <v>12.95</v>
+      </c>
+      <c r="AA7" s="20" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>445</v>
       </c>
-      <c r="I5" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>353</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35" t="s">
-        <v>407</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>443</v>
-      </c>
-      <c r="P5" s="29" t="s">
+      <c r="G8" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="H8" s="20">
+        <v>3</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>450</v>
       </c>
-      <c r="R5" s="29" t="s">
+      <c r="N8" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="V5" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="W5" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="X5" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y5" s="20">
-        <v>9898989898</v>
-      </c>
-      <c r="Z5" s="20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>445</v>
-      </c>
-      <c r="I6" s="33" t="s">
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>452</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="W9" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="AA9" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="K6" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="N6" s="35" t="s">
-        <v>407</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>443</v>
-      </c>
-      <c r="P6" s="29" t="s">
-        <v>441</v>
-      </c>
-      <c r="T6" s="29" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>445</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>454</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>455</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>341</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="P7" s="29" t="s">
-        <v>447</v>
-      </c>
-      <c r="R7" s="29" t="s">
-        <v>442</v>
-      </c>
-      <c r="T7" s="29" t="s">
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="H10" s="20">
+        <v>3</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="O10" s="35"/>
+      <c r="R10" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="T10" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="U10" s="20" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>456</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="O11" s="46">
+        <v>44862</v>
+      </c>
+      <c r="P11" s="20">
+        <v>123</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R11" s="20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="H12" s="20">
+        <v>3</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="K12" s="20">
+        <v>32480</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="N12" s="20">
+        <v>61132300</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{54FAA365-3D1D-44D9-8E39-98E81F5CACCC}"/>
-    <hyperlink ref="L4" r:id="rId2" xr:uid="{666C0A42-77E9-4DD7-B2F5-7206CD34949B}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{8D7DB33B-F951-4ACD-8F6C-8B16C8E96059}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6012,28 +6190,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="20"/>
-    <col min="8" max="8" width="20.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.109375" style="20"/>
+    <col min="23" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6056,31 +6234,31 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="L1" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>429</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>435</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>434</v>
-      </c>
       <c r="P1" s="21" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>338</v>
@@ -6095,10 +6273,10 @@
         <v>174</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="W1" s="21" t="s">
         <v>5</v>
@@ -6167,15 +6345,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>97</v>
+      <c r="B2" s="7" t="s">
+        <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>210</v>
+        <v>444</v>
       </c>
       <c r="S2" s="27"/>
       <c r="T2" s="20" t="s">
@@ -6215,9 +6393,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>332</v>
@@ -6242,16 +6420,16 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="R3" s="34">
         <v>432</v>
       </c>
       <c r="S3" s="40" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="Z3" s="20" t="s">
         <v>251</v>
@@ -6269,9 +6447,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>241</v>
@@ -6280,18 +6458,18 @@
         <v>289</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>415</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>241</v>
@@ -6300,18 +6478,18 @@
         <v>289</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>241</v>
@@ -6323,21 +6501,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>241</v>
@@ -6349,43 +6527,47 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="M8" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="N8" s="20" t="s">
         <v>432</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>436</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{86970EF5-12C7-4C5A-B822-15F786ADCB58}"/>
+    <hyperlink ref="T4" r:id="rId2" xr:uid="{CADB4D26-6B28-40F8-9311-CFDB38B3EC21}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6398,13 +6580,13 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.44140625" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.88671875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6418,37 +6600,37 @@
         <v>174</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>349</v>
-      </c>
       <c r="K1" s="21" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="P1" s="21" t="s">
         <v>47</v>
@@ -6637,7 +6819,7 @@
         <v>188</v>
       </c>
       <c r="BZ1" s="21" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="CA1" s="21" t="s">
         <v>189</v>
@@ -6652,7 +6834,7 @@
         <v>192</v>
       </c>
       <c r="CE1" s="21" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="CF1" s="21" t="s">
         <v>194</v>
@@ -6778,7 +6960,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6792,34 +6974,34 @@
         <v>327</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>348</v>
-      </c>
       <c r="K2" s="20" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="L2" s="29">
         <v>100</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="P2" s="20" t="s">
         <v>332</v>
@@ -6947,7 +7129,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -6967,7 +7149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -6975,7 +7157,7 @@
       <c r="C4" s="20"/>
       <c r="E4" s="37"/>
       <c r="F4" s="20" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="22"/>
@@ -6988,18 +7170,18 @@
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
       <c r="S4" s="29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
       <c r="V4" s="20" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
@@ -7102,15 +7284,15 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>327</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>327</v>
@@ -7118,7 +7300,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>332</v>
@@ -7266,9 +7448,9 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -7279,7 +7461,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
@@ -7348,7 +7530,7 @@
       <c r="BX6" s="20"/>
       <c r="BY6" s="20"/>
       <c r="BZ6" s="20" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="CA6" s="20"/>
       <c r="CB6" s="20" t="s">
@@ -7399,9 +7581,9 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -7418,13 +7600,13 @@
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="38" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="V7" s="20">
         <v>432</v>
       </c>
       <c r="W7" s="29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
@@ -7528,16 +7710,16 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -7653,17 +7835,17 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -7676,7 +7858,7 @@
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
       <c r="S9" s="29" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
@@ -7784,7 +7966,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>314</v>
       </c>
@@ -7936,13 +8118,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8238,7 +8420,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8346,7 +8528,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -8478,7 +8660,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -8610,7 +8792,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -8742,7 +8924,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>

</xml_diff>

<commit_message>
Admin herobanner updated code test case,helper,Testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70256C-EECA-4601-B6A4-017EA65DDF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5719B4-FF47-4B22-918A-46D2CF55D083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8760" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="460">
   <si>
     <t>DataSet</t>
   </si>
@@ -1405,6 +1405,12 @@
   </si>
   <si>
     <t>0.00,0.00</t>
+  </si>
+  <si>
+    <t>adaddu@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Aptdqvfjgsvj1!</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1911,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,10 +2974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BK10"/>
+  <dimension ref="A1:BK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,11 +3223,11 @@
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>97</v>
+      <c r="B2" s="7" t="s">
+        <v>458</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>210</v>
+        <v>459</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -4074,6 +4080,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR11" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
@@ -4100,6 +4114,7 @@
     <hyperlink ref="R8" r:id="rId21" xr:uid="{F84594F0-08FE-426F-9FE7-3AC8E7DD17EF}"/>
     <hyperlink ref="AT9" r:id="rId22" xr:uid="{828CC311-F952-4017-8956-AFD6EFB8ED6D}"/>
     <hyperlink ref="AT10" r:id="rId23" xr:uid="{955A94E1-CF15-468B-8E9A-CD653F447FAF}"/>
+    <hyperlink ref="B2" r:id="rId24" xr:uid="{AEF8F750-637D-4EDA-B0E2-DA08676E6BD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4107,19 +4122,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CU3"/>
+  <dimension ref="A1:CV4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="25" max="25" width="27.140625" customWidth="1"/>
+    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:100" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4195,230 +4211,233 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CJ1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="CJ1" s="5" t="s">
+      <c r="CK1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CL1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CM1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CN1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CO1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CP1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="CQ1" s="6" t="s">
+      <c r="CR1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="CR1" s="6" t="s">
+      <c r="CS1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="CS1" s="6" t="s">
+      <c r="CT1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="CT1" s="6" t="s">
+      <c r="CU1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="CU1" s="6" t="s">
+      <c r="CV1" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -4447,18 +4466,18 @@
       <c r="Y2" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="Z2" s="2"/>
+      <c r="Z2" s="22"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" t="s">
+      <c r="AE2" s="2"/>
+      <c r="AF2" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>151</v>
       </c>
-      <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
@@ -4468,95 +4487,96 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
-      <c r="AR2" t="s">
+      <c r="AR2" s="2"/>
+      <c r="AS2" t="s">
         <v>200</v>
       </c>
-      <c r="AV2" s="2"/>
-      <c r="AW2" t="s">
+      <c r="AW2" s="2"/>
+      <c r="AX2" t="s">
         <v>201</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>202</v>
       </c>
-      <c r="AY2" s="2"/>
-      <c r="BR2" s="13"/>
-      <c r="BS2" s="13" t="s">
+      <c r="AZ2" s="2"/>
+      <c r="BS2" s="13"/>
+      <c r="BT2" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="BT2" s="13" t="s">
+      <c r="BU2" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
         <v>15</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
         <v>16</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
         <v>17</v>
       </c>
-      <c r="BX2" s="3" t="s">
+      <c r="BY2" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="BY2" s="2" t="s">
+      <c r="BZ2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CA2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CB2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="CB2" s="3" t="s">
+      <c r="CC2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="CC2" s="3" t="s">
+      <c r="CD2" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="CG2" s="7" t="s">
+      <c r="CH2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>207</v>
       </c>
-      <c r="CI2">
+      <c r="CJ2">
         <v>12</v>
       </c>
-      <c r="CJ2">
+      <c r="CK2">
         <v>13</v>
       </c>
-      <c r="CK2">
+      <c r="CL2">
         <v>14</v>
       </c>
-      <c r="CL2">
+      <c r="CM2">
         <v>15</v>
       </c>
-      <c r="CM2">
+      <c r="CN2">
         <v>16</v>
       </c>
-      <c r="CN2">
+      <c r="CO2">
         <v>11</v>
       </c>
-      <c r="CO2">
+      <c r="CP2">
         <v>17</v>
       </c>
-      <c r="CP2">
+      <c r="CQ2">
         <v>10</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CR2" t="s">
         <v>13</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>208</v>
       </c>
       <c r="CS2" t="s">
         <v>208</v>
       </c>
       <c r="CT2" t="s">
+        <v>208</v>
+      </c>
+      <c r="CU2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4564,14 +4584,22 @@
         <v>97</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>210</v>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BY2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="BZ2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="CG2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="BZ2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="CA2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="CH2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
     <hyperlink ref="Y2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{21721A70-E97D-4EE3-8CE3-5AEC0F2AA320}"/>
   </hyperlinks>
@@ -5597,7 +5625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Admin herobanner correction test case,testdata,helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5719B4-FF47-4B22-918A-46D2CF55D083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785E4D84-802E-4E4B-B647-5D7D4FDA1D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="458">
   <si>
     <t>DataSet</t>
   </si>
@@ -1405,12 +1405,6 @@
   </si>
   <si>
     <t>0.00,0.00</t>
-  </si>
-  <si>
-    <t>adaddu@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Aptdqvfjgsvj1!</t>
   </si>
 </sst>
 </file>
@@ -2976,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3223,11 +3217,11 @@
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>458</v>
+      <c r="B2" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -4114,7 +4108,7 @@
     <hyperlink ref="R8" r:id="rId21" xr:uid="{F84594F0-08FE-426F-9FE7-3AC8E7DD17EF}"/>
     <hyperlink ref="AT9" r:id="rId22" xr:uid="{828CC311-F952-4017-8956-AFD6EFB8ED6D}"/>
     <hyperlink ref="AT10" r:id="rId23" xr:uid="{955A94E1-CF15-468B-8E9A-CD653F447FAF}"/>
-    <hyperlink ref="B2" r:id="rId24" xr:uid="{AEF8F750-637D-4EDA-B0E2-DA08676E6BD2}"/>
+    <hyperlink ref="B2" r:id="rId24" xr:uid="{55834C34-228F-4546-8A89-3FCFBF356F71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4124,8 +4118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Admin Advance pricing corrected code ,testcase, testdata,helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD966D99-9FB4-4457-8B69-1A88B1A1B4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FB34E969-67ED-4E6C-BFEB-FBC45A5C4490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E630C084-8666-4905-A97F-2E3C2CF16DF1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="463">
   <si>
     <t>DataSet</t>
   </si>
@@ -1170,244 +1170,256 @@
     <t>1</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Black</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Addressbook</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>GroundShippingmethod</t>
+  </si>
+  <si>
+    <t>Standard Shipping - FedEx Ground (2-5 Business Days)</t>
+  </si>
+  <si>
+    <t>PaymentDetails</t>
+  </si>
+  <si>
+    <t>04/27</t>
+  </si>
+  <si>
+    <t>addproduct</t>
+  </si>
+  <si>
+    <t>OXO ON 9 CUP COFFEE MAKER</t>
+  </si>
+  <si>
+    <t>searchproduct</t>
+  </si>
+  <si>
+    <t>QATest Product</t>
+  </si>
+  <si>
+    <t>SpecialPrice</t>
+  </si>
+  <si>
+    <t>AdvancedPricing</t>
+  </si>
+  <si>
+    <t>QATestProduct</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>lotusqatestmanual.gold2@gmail.com</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>OXO Store View</t>
+  </si>
+  <si>
+    <t>HFWebsite</t>
+  </si>
+  <si>
+    <t>OXOWebsite</t>
+  </si>
+  <si>
+    <t>HFGroupproduct</t>
+  </si>
+  <si>
+    <t>hf-group</t>
+  </si>
+  <si>
+    <t>storepage</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Create New Order for test lotus in Hydroflask Store View</t>
+  </si>
+  <si>
+    <t>Create New Order in OXO Store View</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>You need to choose options for your item.</t>
+  </si>
+  <si>
+    <t>'10/28</t>
+  </si>
+  <si>
+    <t>FlushMagento</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>Flush Magento Cache</t>
+  </si>
+  <si>
+    <t>OXOGroupproduct</t>
+  </si>
+  <si>
+    <t>Baking Group</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>OXOProducts</t>
+  </si>
+  <si>
+    <t>SKUNumberoxosimple</t>
+  </si>
+  <si>
+    <t>oxoQuantity</t>
+  </si>
+  <si>
+    <t>SKUNumberoxoconfigurable</t>
+  </si>
+  <si>
+    <t>SKUNumberoxobundle</t>
+  </si>
+  <si>
+    <t>32480</t>
+  </si>
+  <si>
+    <t>61132200B</t>
+  </si>
+  <si>
+    <t>oxo-13-piece-grilling-set</t>
+  </si>
+  <si>
+    <t>SKUnumb</t>
+  </si>
+  <si>
+    <t>Choosecolor</t>
+  </si>
+  <si>
+    <t>Tot Navy</t>
+  </si>
+  <si>
+    <t>HighPriceOverride</t>
+  </si>
+  <si>
+    <t>LowPriceOverride</t>
+  </si>
+  <si>
+    <t>highprice</t>
+  </si>
+  <si>
+    <t>lowprice</t>
+  </si>
+  <si>
+    <t>OXO Website</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>222 concord valley ave</t>
+  </si>
+  <si>
+    <t>40.99,50.99</t>
+  </si>
+  <si>
+    <t>6.99,7.59</t>
+  </si>
+  <si>
+    <t>6.99,8.99</t>
+  </si>
+  <si>
+    <t>Lotus$mk2022</t>
+  </si>
+  <si>
+    <t>Ackpgkyatnob4!</t>
+  </si>
+  <si>
+    <t>HFProducts</t>
+  </si>
+  <si>
+    <t>2, 2</t>
+  </si>
+  <si>
+    <t>T20CP110,S18SX001</t>
+  </si>
+  <si>
+    <t>T20CP110</t>
+  </si>
+  <si>
+    <t>S18SX</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>S18SX464</t>
+  </si>
+  <si>
+    <t>CustomPrice</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>ProductQuantity</t>
+  </si>
+  <si>
+    <t>39.99,0</t>
+  </si>
+  <si>
+    <t>Warrentyorder</t>
+  </si>
+  <si>
+    <t>0.00,0.00</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>spanem@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>hJTROzDump6@</t>
+  </si>
+  <si>
+    <t>10 QATEST product</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
     <t>LOTUSQA$20</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>&gt;2</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>32 oz Wide Mouth - Black</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Addressbook</t>
-  </si>
-  <si>
-    <t>Lotuswave@123</t>
-  </si>
-  <si>
-    <t>GroundShippingmethod</t>
-  </si>
-  <si>
-    <t>Standard Shipping - FedEx Ground (2-5 Business Days)</t>
-  </si>
-  <si>
-    <t>PaymentDetails</t>
-  </si>
-  <si>
-    <t>04/27</t>
-  </si>
-  <si>
-    <t>addproduct</t>
-  </si>
-  <si>
-    <t>OXO ON 9 CUP COFFEE MAKER</t>
-  </si>
-  <si>
-    <t>searchproduct</t>
-  </si>
-  <si>
-    <t>QATest Product</t>
-  </si>
-  <si>
-    <t>SpecialPrice</t>
-  </si>
-  <si>
-    <t>AdvancedPricing</t>
-  </si>
-  <si>
-    <t>QATestProduct</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>lotusqatestmanual.gold2@gmail.com</t>
-  </si>
-  <si>
-    <t>Store</t>
-  </si>
-  <si>
-    <t>Hydroflask Store View</t>
-  </si>
-  <si>
-    <t>OXO Store View</t>
-  </si>
-  <si>
-    <t>HFWebsite</t>
-  </si>
-  <si>
-    <t>OXOWebsite</t>
-  </si>
-  <si>
-    <t>HFGroupproduct</t>
-  </si>
-  <si>
-    <t>hf-group</t>
-  </si>
-  <si>
-    <t>storepage</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Create New Order for test lotus in Hydroflask Store View</t>
-  </si>
-  <si>
-    <t>Create New Order in OXO Store View</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7</t>
-  </si>
-  <si>
-    <t>You need to choose options for your item.</t>
-  </si>
-  <si>
-    <t>'10/28</t>
-  </si>
-  <si>
-    <t>FlushMagento</t>
-  </si>
-  <si>
-    <t>cache</t>
-  </si>
-  <si>
-    <t>Flush Magento Cache</t>
-  </si>
-  <si>
-    <t>OXOGroupproduct</t>
-  </si>
-  <si>
-    <t>Baking Group</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>OXOProducts</t>
-  </si>
-  <si>
-    <t>SKUNumberoxosimple</t>
-  </si>
-  <si>
-    <t>oxoQuantity</t>
-  </si>
-  <si>
-    <t>SKUNumberoxoconfigurable</t>
-  </si>
-  <si>
-    <t>SKUNumberoxobundle</t>
-  </si>
-  <si>
-    <t>32480</t>
-  </si>
-  <si>
-    <t>61132200B</t>
-  </si>
-  <si>
-    <t>oxo-13-piece-grilling-set</t>
-  </si>
-  <si>
-    <t>SKUnumb</t>
-  </si>
-  <si>
-    <t>Choosecolor</t>
-  </si>
-  <si>
-    <t>Tot Navy</t>
-  </si>
-  <si>
-    <t>HighPriceOverride</t>
-  </si>
-  <si>
-    <t>LowPriceOverride</t>
-  </si>
-  <si>
-    <t>highprice</t>
-  </si>
-  <si>
-    <t>lowprice</t>
-  </si>
-  <si>
-    <t>OXO Website</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>222 concord valley ave</t>
-  </si>
-  <si>
-    <t>40.99,50.99</t>
-  </si>
-  <si>
-    <t>6.99,7.59</t>
-  </si>
-  <si>
-    <t>6.99,8.99</t>
-  </si>
-  <si>
-    <t>Lotus$mk2022</t>
-  </si>
-  <si>
-    <t>Ackpgkyatnob4!</t>
-  </si>
-  <si>
-    <t>HFProducts</t>
-  </si>
-  <si>
-    <t>2, 2</t>
-  </si>
-  <si>
-    <t>T20CP110,S18SX001</t>
-  </si>
-  <si>
-    <t>T20CP110</t>
-  </si>
-  <si>
-    <t>S18SX</t>
-  </si>
-  <si>
-    <t>Indigo</t>
-  </si>
-  <si>
-    <t>S18SX464</t>
-  </si>
-  <si>
-    <t>CustomPrice</t>
-  </si>
-  <si>
-    <t>0,0</t>
-  </si>
-  <si>
-    <t>ProductQuantity</t>
-  </si>
-  <si>
-    <t>39.99,0</t>
-  </si>
-  <si>
-    <t>Warrentyorder</t>
-  </si>
-  <si>
-    <t>0.00,0.00</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1624,6 +1636,9 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1911,62 +1926,62 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2043,10 +2058,10 @@
         <v>38</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2134,7 +2149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2166,7 +2181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2198,7 +2213,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2230,12 +2245,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -2258,16 +2273,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2406,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -2447,7 +2462,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -2485,7 +2500,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -2493,7 +2508,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -2519,7 +2534,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -2541,7 +2556,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -2566,7 +2581,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -2589,7 +2604,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -2643,7 +2658,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -2670,7 +2685,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -2706,17 +2721,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2764,7 @@
       </c>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2760,12 +2775,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -2791,7 +2806,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -2815,156 +2830,422 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="48" t="s">
         <v>355</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="48" t="s">
         <v>356</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="48" t="s">
         <v>359</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="48" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="S1" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>395</v>
+      </c>
+      <c r="U1" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="49" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="47" t="s">
         <v>362</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47" t="s">
         <v>363</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="47" t="s">
         <v>346</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="P3">
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
         <v>365</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="47" t="s">
         <v>366</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="47" t="s">
         <v>367</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="47">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="47" t="s">
         <v>368</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="47" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="47" t="s">
         <v>309</v>
       </c>
-      <c r="M5" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="47" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="47" t="s">
         <v>314</v>
       </c>
-      <c r="M6" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="47" t="s">
         <v>370</v>
       </c>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="47"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47">
+        <v>10</v>
+      </c>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47">
+        <v>20</v>
+      </c>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47" t="s">
+        <v>460</v>
+      </c>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="N10" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47" t="s">
+        <v>461</v>
+      </c>
+      <c r="W10" s="47"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47" t="s">
+        <v>228</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{56FC7C01-14F8-404B-9BA6-55321738E0FD}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{3E5BA075-C023-462E-ABE1-8ACCFCA37358}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2977,55 +3258,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="20"/>
-    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="20"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="20"/>
+    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" style="20"/>
-    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7109375" style="20"/>
-    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="20"/>
-    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7109375" style="20"/>
-    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" style="20"/>
-    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7265625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="20"/>
+    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7265625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" style="20"/>
+    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="20"/>
-    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7109375" style="20"/>
-    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7109375" style="20"/>
-    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7109375" style="20"/>
+    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7265625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7265625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3216,7 +3497,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -3224,7 +3505,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -3266,7 +3547,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -3318,7 +3599,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -3393,7 +3674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -3529,7 +3810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -3654,7 +3935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -3787,7 +4068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -3878,7 +4159,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -3986,7 +4267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -4077,7 +4358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -4125,14 +4406,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="25" max="25" width="27.140625" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:100" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4209,7 +4490,7 @@
         <v>23</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>59</v>
@@ -4434,7 +4715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -4573,7 +4854,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4581,15 +4862,15 @@
         <v>97</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z4" s="20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -4612,12 +4893,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4922,7 +5203,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4988,7 +5269,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -5130,7 +5411,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -5195,7 +5476,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -5251,7 +5532,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -5384,24 +5665,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5484,19 +5765,17 @@
         <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>443</v>
-      </c>
+      <c r="C2" s="20"/>
       <c r="F2" t="s">
         <v>97</v>
       </c>
@@ -5534,7 +5813,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -5572,7 +5851,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5589,28 +5868,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA5" t="s">
         <v>394</v>
       </c>
-      <c r="AA5" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB6" s="29" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>397</v>
       </c>
-      <c r="AB6" s="29" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>398</v>
-      </c>
       <c r="AB7" s="29" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -5622,29 +5901,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView topLeftCell="S4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="20"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="20"/>
-    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="20"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5667,25 +5946,25 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O1" s="21" t="s">
         <v>338</v>
@@ -5703,22 +5982,22 @@
         <v>349</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="V1" s="21" t="s">
         <v>181</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>176</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Z1" s="21" t="s">
         <v>5</v>
@@ -5784,7 +6063,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -5792,7 +6071,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
@@ -5845,7 +6124,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -5899,7 +6178,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>350</v>
       </c>
@@ -5938,27 +6217,27 @@
         <v>120</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="V4" s="20" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
@@ -5983,17 +6262,17 @@
       </c>
       <c r="S5" s="29"/>
       <c r="T5" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="U5" s="29"/>
       <c r="V5" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="W5" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="Y5" s="20" t="s">
         <v>440</v>
-      </c>
-      <c r="Y5" s="20" t="s">
-        <v>441</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AC5" s="20" t="s">
@@ -6012,9 +6291,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
@@ -6038,24 +6317,24 @@
       </c>
       <c r="S6" s="29"/>
       <c r="T6" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="W6" s="29">
         <v>50.99</v>
       </c>
       <c r="Y6" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AA6" s="20" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
@@ -6086,54 +6365,54 @@
         <v>12.95</v>
       </c>
       <c r="AA7" s="20" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>445</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>446</v>
       </c>
       <c r="H8" s="20">
         <v>3</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>447</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="M8" s="20" t="s">
         <v>449</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="N8" s="20" t="s">
         <v>450</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>451</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="W9" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA9" s="20" t="s">
         <v>452</v>
       </c>
-      <c r="W9" s="29" t="s">
-        <v>457</v>
-      </c>
-      <c r="AA9" s="20" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>241</v>
@@ -6147,24 +6426,24 @@
       <c r="M10" s="7"/>
       <c r="O10" s="35"/>
       <c r="R10" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="T10" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>160</v>
@@ -6182,24 +6461,24 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H12" s="20">
         <v>3</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K12" s="20">
         <v>32480</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N12" s="20">
         <v>61132300</v>
@@ -6215,28 +6494,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AV10" sqref="AV10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="20"/>
+    <col min="23" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6259,31 +6538,31 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>423</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>426</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>425</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>431</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>430</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>424</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>338</v>
@@ -6298,10 +6577,10 @@
         <v>174</v>
       </c>
       <c r="U1" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>409</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>410</v>
       </c>
       <c r="W1" s="21" t="s">
         <v>5</v>
@@ -6370,7 +6649,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6378,7 +6657,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S2" s="27"/>
       <c r="T2" s="20" t="s">
@@ -6418,9 +6697,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>332</v>
@@ -6445,7 +6724,7 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R3" s="34">
         <v>432</v>
@@ -6454,7 +6733,7 @@
         <v>340</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Z3" s="20" t="s">
         <v>251</v>
@@ -6472,9 +6751,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>241</v>
@@ -6483,18 +6762,18 @@
         <v>289</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>241</v>
@@ -6503,18 +6782,18 @@
         <v>289</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>241</v>
@@ -6526,21 +6805,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="U6" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="V6" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="V6" s="20" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>241</v>
@@ -6552,39 +6831,39 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="U7" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="T7" s="20" t="s">
-        <v>400</v>
-      </c>
-      <c r="U7" s="20" t="s">
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>422</v>
-      </c>
       <c r="K8" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>428</v>
-      </c>
       <c r="N8" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -6601,17 +6880,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DT11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6967,7 +7246,7 @@
         <v>222</v>
       </c>
       <c r="DO1" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="DP1" s="21" t="s">
         <v>212</v>
@@ -6985,15 +7264,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>210</v>
+      <c r="C2" s="7" t="s">
+        <v>442</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>327</v>
@@ -7014,19 +7293,19 @@
         <v>346</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>379</v>
+        <v>462</v>
       </c>
       <c r="L2" s="29">
         <v>100</v>
       </c>
       <c r="M2" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>380</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>381</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>382</v>
       </c>
       <c r="P2" s="20" t="s">
         <v>332</v>
@@ -7154,7 +7433,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -7174,7 +7453,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -7182,7 +7461,7 @@
       <c r="C4" s="20"/>
       <c r="E4" s="37"/>
       <c r="F4" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="22"/>
@@ -7195,18 +7474,18 @@
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
       <c r="S4" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
       <c r="V4" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W4" s="29" t="s">
         <v>378</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
@@ -7309,15 +7588,15 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>327</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>327</v>
@@ -7325,7 +7604,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>332</v>
@@ -7473,9 +7752,9 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -7486,7 +7765,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
@@ -7555,7 +7834,7 @@
       <c r="BX6" s="20"/>
       <c r="BY6" s="20"/>
       <c r="BZ6" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="CA6" s="20"/>
       <c r="CB6" s="20" t="s">
@@ -7606,9 +7885,9 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -7625,7 +7904,7 @@
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="38" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="V7" s="20">
         <v>432</v>
@@ -7735,7 +8014,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>357</v>
       </c>
@@ -7744,7 +8023,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20" t="s">
-        <v>379</v>
+        <v>462</v>
       </c>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -7860,17 +8139,17 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -7883,7 +8162,7 @@
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
       <c r="S9" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
@@ -7991,7 +8270,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>314</v>
       </c>
@@ -8116,7 +8395,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -8133,6 +8412,7 @@
     <hyperlink ref="D6" r:id="rId10" xr:uid="{5CEF3D62-AF1A-4151-A457-4D8F820085BB}"/>
     <hyperlink ref="D5" r:id="rId11" xr:uid="{554881D9-889D-4E28-8CFC-7A88786BEBF7}"/>
     <hyperlink ref="CR10" r:id="rId12" xr:uid="{CECF781A-1973-4855-B511-F61368BE1D65}"/>
+    <hyperlink ref="C2" r:id="rId13" display="Lotuswave@123" xr:uid="{FDFAA4EF-FAD1-4829-B9DD-838905824080}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8146,13 +8426,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8448,7 +8728,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8556,7 +8836,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -8688,7 +8968,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -8820,7 +9100,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -8952,7 +9232,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>

</xml_diff>

<commit_message>
Admin promotion cartrule testcase helper,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{FB34E969-67ED-4E6C-BFEB-FBC45A5C4490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D751765D-E997-429C-A9A6-3A24F7ED9B35}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{FB34E969-67ED-4E6C-BFEB-FBC45A5C4490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{396D50A4-0D00-4AE2-ACED-8677706115AC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="464">
   <si>
     <t>DataSet</t>
   </si>
@@ -1167,12 +1167,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>&gt;2</t>
   </si>
   <si>
@@ -1203,9 +1197,6 @@
     <t>PaymentDetails</t>
   </si>
   <si>
-    <t>04/27</t>
-  </si>
-  <si>
     <t>addproduct</t>
   </si>
   <si>
@@ -1429,6 +1420,9 @@
   </si>
   <si>
     <t>Magentocache</t>
+  </si>
+  <si>
+    <t>Fixed amount discount</t>
   </si>
 </sst>
 </file>
@@ -1935,62 +1929,62 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2067,10 +2061,10 @@
         <v>38</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2087,7 +2081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2158,7 +2152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2222,7 +2216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2254,12 +2248,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Z7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2282,16 +2276,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2430,7 +2424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -2471,7 +2465,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -2509,7 +2503,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -2517,7 +2511,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -2543,7 +2537,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -2565,7 +2559,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -2590,7 +2584,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -2613,7 +2607,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -2667,7 +2661,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -2694,7 +2688,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -2726,26 +2720,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2777,27 +2771,27 @@
         <v>308</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -2823,7 +2817,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -2846,12 +2840,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -2867,9 +2861,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2922,7 @@
         <v>86</v>
       </c>
       <c r="T1" s="48" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="U1" s="48" t="s">
         <v>223</v>
@@ -2940,15 +2934,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -2975,7 +2969,7 @@
       <c r="V2" s="47"/>
       <c r="W2" s="47"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>362</v>
       </c>
@@ -3012,7 +3006,7 @@
       <c r="V3" s="47"/>
       <c r="W3" s="47"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>365</v>
       </c>
@@ -3053,7 +3047,7 @@
       <c r="V4" s="47"/>
       <c r="W4" s="47"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>309</v>
       </c>
@@ -3086,7 +3080,7 @@
       <c r="V5" s="47"/>
       <c r="W5" s="47"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>314</v>
       </c>
@@ -3119,9 +3113,9 @@
       <c r="V6" s="47"/>
       <c r="W6" s="47"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
@@ -3148,9 +3142,9 @@
       <c r="V7" s="47"/>
       <c r="W7" s="47"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
@@ -3177,7 +3171,7 @@
       <c r="V8" s="47"/>
       <c r="W8" s="47"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -3203,12 +3197,12 @@
       </c>
       <c r="T9" s="47"/>
       <c r="U9" s="47" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="V9" s="47"/>
       <c r="W9" s="47"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -3239,13 +3233,13 @@
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="W10" s="47"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -3289,55 +3283,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="20"/>
-    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="20"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="20"/>
+    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" style="20"/>
-    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7109375" style="20"/>
-    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="20"/>
-    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7109375" style="20"/>
-    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" style="20"/>
-    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7265625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="20"/>
+    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7265625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" style="20"/>
+    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="20"/>
-    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7109375" style="20"/>
-    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7109375" style="20"/>
-    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7109375" style="20"/>
+    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7265625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7265625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3528,7 +3522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -3536,7 +3530,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -3578,7 +3572,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -3630,7 +3624,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -3705,7 +3699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -3841,7 +3835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -3966,7 +3960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -4099,7 +4093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -4190,7 +4184,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -4298,7 +4292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -4389,7 +4383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -4437,14 +4431,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="25" max="25" width="27.140625" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:100" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4521,7 +4515,7 @@
         <v>23</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>59</v>
@@ -4746,7 +4740,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -4885,7 +4879,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4893,15 +4887,15 @@
         <v>97</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Z4" s="20" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -4924,12 +4918,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5234,7 +5228,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5300,7 +5294,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -5442,7 +5436,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -5507,7 +5501,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -5563,7 +5557,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -5700,20 +5694,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5796,10 +5790,10 @@
         <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5844,7 +5838,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -5882,7 +5876,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -5899,28 +5893,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>390</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>393</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB6" s="29" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>396</v>
-      </c>
-      <c r="AB6" s="29" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>397</v>
-      </c>
       <c r="AB7" s="29" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -5936,25 +5930,25 @@
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="20"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="20"/>
-    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="20"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -5977,25 +5971,25 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="O1" s="21" t="s">
         <v>338</v>
@@ -6013,22 +6007,22 @@
         <v>349</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="V1" s="21" t="s">
         <v>181</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>176</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="Z1" s="21" t="s">
         <v>5</v>
@@ -6094,7 +6088,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6102,7 +6096,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
@@ -6155,7 +6149,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -6209,7 +6203,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>350</v>
       </c>
@@ -6248,27 +6242,27 @@
         <v>120</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="V4" s="20" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
@@ -6293,17 +6287,17 @@
       </c>
       <c r="S5" s="29"/>
       <c r="T5" s="20" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="U5" s="29"/>
       <c r="V5" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="W5" s="20" t="s">
         <v>436</v>
       </c>
-      <c r="W5" s="20" t="s">
-        <v>439</v>
-      </c>
       <c r="Y5" s="20" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AC5" s="20" t="s">
@@ -6322,9 +6316,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
@@ -6348,24 +6342,24 @@
       </c>
       <c r="S6" s="29"/>
       <c r="T6" s="20" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="W6" s="29">
         <v>50.99</v>
       </c>
       <c r="Y6" s="20" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="AA6" s="20" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
@@ -6396,54 +6390,54 @@
         <v>12.95</v>
       </c>
       <c r="AA7" s="20" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>444</v>
-      </c>
       <c r="G8" s="20" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H8" s="20">
         <v>3</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="N8" s="20" t="s">
         <v>447</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>450</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="W9" s="29" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AA9" s="20" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>241</v>
@@ -6457,24 +6451,24 @@
       <c r="M10" s="7"/>
       <c r="O10" s="35"/>
       <c r="R10" s="20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="T10" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>160</v>
@@ -6492,24 +6486,24 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H12" s="20">
         <v>3</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K12" s="20">
         <v>32480</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="N12" s="20">
         <v>61132300</v>
@@ -6529,24 +6523,24 @@
       <selection activeCell="AV10" sqref="AV10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="20"/>
+    <col min="23" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6569,31 +6563,31 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>422</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>425</v>
-      </c>
       <c r="M1" s="21" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>338</v>
@@ -6608,10 +6602,10 @@
         <v>174</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="W1" s="21" t="s">
         <v>5</v>
@@ -6680,7 +6674,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -6688,7 +6682,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="S2" s="27"/>
       <c r="T2" s="20" t="s">
@@ -6728,9 +6722,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>332</v>
@@ -6755,7 +6749,7 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R3" s="34">
         <v>432</v>
@@ -6764,7 +6758,7 @@
         <v>340</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="Z3" s="20" t="s">
         <v>251</v>
@@ -6782,9 +6776,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>241</v>
@@ -6793,18 +6787,18 @@
         <v>289</v>
       </c>
       <c r="H4" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>407</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
         <v>401</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>404</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>241</v>
@@ -6813,18 +6807,18 @@
         <v>289</v>
       </c>
       <c r="H5" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
         <v>402</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>411</v>
-      </c>
-      <c r="T5" s="20" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>405</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>241</v>
@@ -6836,21 +6830,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="U6" s="20" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>241</v>
@@ -6862,39 +6856,39 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="L8" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="N8" s="20" t="s">
         <v>428</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>427</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>431</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -6911,17 +6905,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DT11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -6938,364 +6933,364 @@
         <v>359</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>372</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>373</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>333</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="AB1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="Z1" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AC1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AK1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AM1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="21" t="s">
+      <c r="AN1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AM1" s="21" t="s">
+      <c r="AO1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AN1" s="21" t="s">
+      <c r="AP1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="21" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AP1" s="21" t="s">
+      <c r="AR1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AQ1" s="21" t="s">
+      <c r="AS1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AR1" s="21" t="s">
+      <c r="AT1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" s="21" t="s">
+      <c r="AU1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AV1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="AU1" s="21" t="s">
+      <c r="AW1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AV1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AW1" s="21" t="s">
+      <c r="AY1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AX1" s="21" t="s">
+      <c r="AZ1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AY1" s="21" t="s">
+      <c r="BA1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" s="21" t="s">
+      <c r="BB1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="BA1" s="21" t="s">
+      <c r="BC1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="21" t="s">
+      <c r="BD1" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="BC1" s="21" t="s">
+      <c r="BE1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="BD1" s="21" t="s">
+      <c r="BF1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BG1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="BF1" s="21" t="s">
+      <c r="BH1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="BG1" s="21" t="s">
+      <c r="BI1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="BH1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BK1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BJ1" s="21" t="s">
+      <c r="BL1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="BK1" s="21" t="s">
+      <c r="BM1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="BL1" s="21" t="s">
+      <c r="BN1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="21" t="s">
+      <c r="BO1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="BN1" s="21" t="s">
+      <c r="BP1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="BO1" s="21" t="s">
+      <c r="BQ1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="BP1" s="21" t="s">
+      <c r="BR1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="BQ1" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="BR1" s="21" t="s">
+      <c r="BS1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="BS1" s="21" t="s">
+      <c r="BT1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="BT1" s="21" t="s">
+      <c r="BU1" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="BU1" s="21" t="s">
+      <c r="BV1" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BV1" s="21" t="s">
+      <c r="BW1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="BW1" s="21" t="s">
+      <c r="BX1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="BX1" s="21" t="s">
+      <c r="BY1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="BY1" s="21" t="s">
+      <c r="BZ1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BZ1" s="21" t="s">
+      <c r="CA1" s="21" t="s">
         <v>376</v>
       </c>
-      <c r="CA1" s="21" t="s">
+      <c r="CB1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="CB1" s="21" t="s">
+      <c r="CC1" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="CC1" s="21" t="s">
+      <c r="CD1" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="CD1" s="21" t="s">
+      <c r="CE1" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="CE1" s="21" t="s">
+      <c r="CF1" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="CF1" s="21" t="s">
+      <c r="CG1" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="CG1" s="21" t="s">
+      <c r="CH1" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="CH1" s="21" t="s">
+      <c r="CI1" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="CI1" s="21" t="s">
+      <c r="CJ1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="21" t="s">
+      <c r="CK1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="21" t="s">
+      <c r="CL1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="21" t="s">
+      <c r="CM1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="21" t="s">
+      <c r="CN1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="CN1" s="21" t="s">
+      <c r="CO1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="CO1" s="21" t="s">
+      <c r="CP1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="CP1" s="21" t="s">
+      <c r="CQ1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="CQ1" s="21" t="s">
+      <c r="CR1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="CR1" s="21" t="s">
+      <c r="CS1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CS1" s="21" t="s">
+      <c r="CT1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CT1" s="21" t="s">
+      <c r="CU1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="CU1" s="21" t="s">
+      <c r="CV1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="CV1" s="21" t="s">
+      <c r="CW1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CW1" s="21" t="s">
+      <c r="CX1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="CX1" s="21" t="s">
+      <c r="CY1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="CY1" s="21" t="s">
+      <c r="CZ1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="CZ1" s="21" t="s">
+      <c r="DA1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="DA1" s="21" t="s">
+      <c r="DB1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="DB1" s="21" t="s">
+      <c r="DC1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="DC1" s="21" t="s">
+      <c r="DD1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="DD1" s="21" t="s">
+      <c r="DE1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="DE1" s="21" t="s">
+      <c r="DF1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="DF1" s="21" t="s">
+      <c r="DG1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="DG1" s="21" t="s">
+      <c r="DH1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="DH1" s="21" t="s">
+      <c r="DI1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="DI1" s="21" t="s">
+      <c r="DJ1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="DJ1" s="21" t="s">
+      <c r="DK1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="DK1" s="21" t="s">
+      <c r="DL1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="DL1" s="21" t="s">
+      <c r="DM1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="DM1" s="21" t="s">
+      <c r="DN1" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="DN1" s="21" t="s">
+      <c r="DO1" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="DO1" s="21" t="s">
-        <v>395</v>
-      </c>
       <c r="DP1" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="DQ1" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="DQ1" s="21" t="s">
+      <c r="DR1" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="DR1" s="21" t="s">
+      <c r="DS1" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="DS1" s="21" t="s">
+      <c r="DT1" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="DT1" s="21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7303,51 +7298,58 @@
         <v>97</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="36">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" s="20">
+        <v>20</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="O2" s="29">
+        <v>100</v>
+      </c>
+      <c r="P2" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>462</v>
-      </c>
-      <c r="L2" s="29">
-        <v>100</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>379</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>380</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>381</v>
-      </c>
-      <c r="P2" s="20" t="s">
+      <c r="R2" s="20">
+        <v>20</v>
+      </c>
+      <c r="S2" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="T2" s="20"/>
+      <c r="U2" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
       <c r="X2" s="20"/>
@@ -7406,23 +7408,23 @@
       <c r="BY2" s="20"/>
       <c r="BZ2" s="20"/>
       <c r="CA2" s="20"/>
-      <c r="CB2" s="20" t="s">
+      <c r="CB2" s="20"/>
+      <c r="CC2" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="CC2" s="20" t="s">
+      <c r="CD2" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="CD2" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="CE2" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="20" t="s">
+      <c r="CE2" s="29">
+        <v>6492</v>
+      </c>
+      <c r="CF2" s="20">
+        <v>9898989898</v>
+      </c>
+      <c r="CG2" s="20"/>
+      <c r="CH2" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="CH2" s="20"/>
       <c r="CI2" s="20"/>
       <c r="CJ2" s="20"/>
       <c r="CK2" s="20"/>
@@ -7432,10 +7434,10 @@
       <c r="CO2" s="20"/>
       <c r="CP2" s="20"/>
       <c r="CQ2" s="20"/>
-      <c r="CR2" s="7" t="s">
+      <c r="CR2" s="7"/>
+      <c r="CS2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
       <c r="CU2" s="20"/>
       <c r="CV2" s="20"/>
@@ -7464,37 +7466,37 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="BC3" s="20" t="s">
+      <c r="BE3" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="CE3" s="20" t="s">
+      <c r="CF3" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="CF3" s="7" t="s">
+      <c r="CG3" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="CG3" s="7" t="s">
+      <c r="CH3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="CR3" s="7" t="s">
+      <c r="CR3" s="7"/>
+      <c r="CS3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="E4" s="37"/>
-      <c r="F4" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>380</v>
+      </c>
       <c r="J4" s="22"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
@@ -7504,23 +7506,23 @@
       <c r="P4" s="20"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
-      <c r="S4" s="29" t="s">
-        <v>383</v>
-      </c>
+      <c r="S4" s="29"/>
       <c r="T4" s="20"/>
       <c r="U4" s="20"/>
-      <c r="V4" s="20" t="s">
+      <c r="V4" s="20">
+        <v>3</v>
+      </c>
+      <c r="W4" s="29"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="Z4" s="20">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="W4" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="X4" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
       <c r="AC4" s="20"/>
       <c r="AD4" s="20"/>
@@ -7619,56 +7621,55 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>327</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>327</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="23" t="s">
-        <v>386</v>
-      </c>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="23"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="K5" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="L5" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="M5" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>335</v>
       </c>
       <c r="N5" s="20"/>
       <c r="O5" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="S5" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="Q5" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="R5" s="20" t="s">
+      <c r="T5" s="38">
+        <v>9898989898</v>
+      </c>
+      <c r="U5" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="20"/>
       <c r="V5" s="20"/>
       <c r="W5" s="20"/>
       <c r="X5" s="20"/>
@@ -7727,23 +7728,23 @@
       <c r="BY5" s="20"/>
       <c r="BZ5" s="20"/>
       <c r="CA5" s="20"/>
-      <c r="CB5" s="20" t="s">
+      <c r="CB5" s="20"/>
+      <c r="CC5" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="CC5" s="20" t="s">
+      <c r="CD5" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="CD5" s="29" t="s">
-        <v>256</v>
-      </c>
       <c r="CE5" s="20">
+        <v>6492</v>
+      </c>
+      <c r="CF5" s="20">
         <v>9898989898</v>
       </c>
-      <c r="CF5" s="20"/>
-      <c r="CG5" s="20" t="s">
+      <c r="CG5" s="20"/>
+      <c r="CH5" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="CH5" s="20"/>
       <c r="CI5" s="20"/>
       <c r="CJ5" s="20"/>
       <c r="CK5" s="20"/>
@@ -7783,9 +7784,9 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -7795,12 +7796,12 @@
       <c r="E6" s="7"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="20" t="s">
-        <v>388</v>
-      </c>
+      <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+      <c r="N6" s="20" t="s">
+        <v>386</v>
+      </c>
       <c r="O6" s="20"/>
       <c r="P6" s="28"/>
       <c r="Q6" s="39"/>
@@ -7864,14 +7865,14 @@
       <c r="BW6" s="20"/>
       <c r="BX6" s="20"/>
       <c r="BY6" s="20"/>
-      <c r="BZ6" s="20" t="s">
-        <v>388</v>
-      </c>
-      <c r="CA6" s="20"/>
-      <c r="CB6" s="20" t="s">
+      <c r="BZ6" s="20"/>
+      <c r="CA6" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="CB6" s="20"/>
+      <c r="CC6" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="CC6" s="20"/>
       <c r="CD6" s="20"/>
       <c r="CE6" s="20"/>
       <c r="CF6" s="20"/>
@@ -7916,9 +7917,9 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -7934,18 +7935,18 @@
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
-      <c r="U7" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="V7" s="20">
+      <c r="U7" s="38"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="46">
+        <v>44678</v>
+      </c>
+      <c r="Y7" s="20">
         <v>432</v>
       </c>
-      <c r="W7" s="29" t="s">
+      <c r="Z7" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
       <c r="AC7" s="20"/>
@@ -8045,7 +8046,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>357</v>
       </c>
@@ -8053,12 +8054,12 @@
       <c r="C8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="20" t="s">
-        <v>462</v>
-      </c>
+      <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="N8" s="20" t="s">
+        <v>459</v>
+      </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
@@ -8170,20 +8171,18 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
-      <c r="F9" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>389</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -8192,12 +8191,12 @@
       <c r="P9" s="20"/>
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
-      <c r="S9" s="29" t="s">
-        <v>383</v>
-      </c>
+      <c r="S9" s="29"/>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
+      <c r="V9" s="20">
+        <v>3</v>
+      </c>
       <c r="W9" s="20"/>
       <c r="X9" s="20"/>
       <c r="Y9" s="20"/>
@@ -8301,7 +8300,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>314</v>
       </c>
@@ -8394,10 +8393,10 @@
       <c r="CO10" s="20"/>
       <c r="CP10" s="20"/>
       <c r="CQ10" s="20"/>
-      <c r="CR10" s="7" t="s">
+      <c r="CR10" s="7"/>
+      <c r="CS10" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="CS10" s="20"/>
       <c r="CT10" s="20"/>
       <c r="CU10" s="20"/>
       <c r="CV10" s="20"/>
@@ -8426,25 +8425,10 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="CG3" r:id="rId1" xr:uid="{F057FAC8-0A57-4D6D-A9D0-DE791A21EBC0}"/>
-    <hyperlink ref="CF3" r:id="rId2" xr:uid="{AE3ED39A-666B-4E61-8DB3-2B6C76B58E1D}"/>
-    <hyperlink ref="CR3" r:id="rId3" xr:uid="{A4708C70-4900-4C39-B150-20BAAEBFBA53}"/>
-    <hyperlink ref="CR2" r:id="rId4" xr:uid="{3A3E797F-0206-4012-9009-9813395840D8}"/>
-    <hyperlink ref="J5" r:id="rId5" xr:uid="{B5FCC387-F56C-4A93-A380-0DAA3732B74C}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{B092573B-9361-4BEF-88D6-65CF0E39C980}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{0FE5CD64-EACD-4A80-9A06-BCBBEAAED9C7}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{5D471A0C-E64A-46B2-8D41-DE60BD921291}"/>
-    <hyperlink ref="D2" r:id="rId9" xr:uid="{9C87F5C9-9F4E-4856-A5CB-B00741632FE8}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{5CEF3D62-AF1A-4151-A457-4D8F820085BB}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{554881D9-889D-4E28-8CFC-7A88786BEBF7}"/>
-    <hyperlink ref="CR10" r:id="rId12" xr:uid="{CECF781A-1973-4855-B511-F61368BE1D65}"/>
-    <hyperlink ref="C2" r:id="rId13" display="Lotuswave@123" xr:uid="{FDFAA4EF-FAD1-4829-B9DD-838905824080}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8457,13 +8441,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8759,7 +8743,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8867,7 +8851,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -8999,7 +8983,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -9131,7 +9115,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -9263,7 +9247,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>

</xml_diff>

<commit_message>
value prop banner padding for main page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32729DFB-48C7-449A-9E1E-60B9D8B7FB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E749EE9-8777-49D6-B67B-42780FDBBFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="469">
   <si>
     <t>DataSet</t>
   </si>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2088,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>210</v>
+        <v>439</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2165,7 +2165,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>13</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,11 +3382,11 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>210</v>
+      <c r="C2" s="47" t="s">
+        <v>439</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3682,6 +3682,7 @@
   <hyperlinks>
     <hyperlink ref="AN4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{1DD4B60C-4B72-4846-B416-B7E0F6E43969}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3828,8 +3829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5400,7 @@
   <dimension ref="A1:CV4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6662,7 +6663,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6768,10 +6769,12 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="47" t="s">
+        <v>439</v>
+      </c>
       <c r="F2" t="s">
         <v>97</v>
       </c>
@@ -6889,6 +6892,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9DE1F5FC-059F-415C-99B9-8B77C7014EF2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6897,7 +6903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
@@ -9408,8 +9414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43BF1809-245A-40C2-A8A3-0C31646D517C}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
verifying the Advance pricing test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E749EE9-8777-49D6-B67B-42780FDBBFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BC9520-B501-4EE6-A24B-8F30D348E79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="475">
   <si>
     <t>DataSet</t>
   </si>
@@ -1439,6 +1439,24 @@
   </si>
   <si>
     <t>This Promo content is to configure and validate on the front end</t>
+  </si>
+  <si>
+    <t>Stockstatus</t>
+  </si>
+  <si>
+    <t>Instock</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>QtyPrice</t>
+  </si>
+  <si>
+    <t>QtyPrice1</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -3827,15 +3845,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="23" max="23" width="9.140625" style="47"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3903,10 +3924,34 @@
         <v>5</v>
       </c>
       <c r="W1" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="X1" s="48" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y1" s="48" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z1" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB1" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="AC1" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD1" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="AE1" s="48" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
@@ -3939,9 +3984,9 @@
         <v>230</v>
       </c>
       <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="47"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>362</v>
       </c>
@@ -3976,9 +4021,9 @@
       <c r="T3" s="47"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="47"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>365</v>
       </c>
@@ -4017,9 +4062,9 @@
       <c r="T4" s="47"/>
       <c r="U4" s="47"/>
       <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="47"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>309</v>
       </c>
@@ -4050,9 +4095,9 @@
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
       <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="47"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>314</v>
       </c>
@@ -4083,9 +4128,9 @@
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
       <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="47"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>393</v>
       </c>
@@ -4112,9 +4157,23 @@
       </c>
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W7" s="47">
+        <v>1</v>
+      </c>
+      <c r="X7" s="47"/>
+      <c r="AA7" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB7" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC7" s="47">
+        <v>10</v>
+      </c>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>394</v>
       </c>
@@ -4141,9 +4200,23 @@
       </c>
       <c r="U8" s="47"/>
       <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W8" s="47">
+        <v>2</v>
+      </c>
+      <c r="X8" s="47"/>
+      <c r="AA8" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47" t="s">
+        <v>357</v>
+      </c>
+      <c r="AE8" s="47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4172,9 +4245,9 @@
         <v>457</v>
       </c>
       <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="47"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4207,9 +4280,9 @@
       <c r="V10" s="47" t="s">
         <v>458</v>
       </c>
-      <c r="W10" s="47"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="47"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>390</v>
       </c>
@@ -4234,8 +4307,24 @@
       <c r="T11" s="47"/>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
-      <c r="W11" s="47" t="s">
+      <c r="X11" s="47" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="Y12" s="47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>469</v>
+      </c>
+      <c r="Z13" s="47" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
29 admin Testcase correction -Testdata commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BC9520-B501-4EE6-A24B-8F30D348E79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A5FFF5-0952-4457-93C5-D901614F7B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -1282,12 +1282,6 @@
     <t>OXOGroupproduct</t>
   </si>
   <si>
-    <t>Baking Group</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>OXOProducts</t>
   </si>
   <si>
@@ -1457,6 +1451,12 @@
   </si>
   <si>
     <t>percentage</t>
+  </si>
+  <si>
+    <t>POP Mini Square Containers</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
   </si>
 </sst>
 </file>
@@ -2106,7 +2106,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3404,7 +3404,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3770,10 +3770,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3832,7 +3832,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K6" s="47" t="s">
         <v>414</v>
@@ -3847,7 +3847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3924,7 +3924,7 @@
         <v>5</v>
       </c>
       <c r="W1" s="48" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="X1" s="48" t="s">
         <v>227</v>
@@ -3933,22 +3933,22 @@
         <v>371</v>
       </c>
       <c r="Z1" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="AB1" s="48" t="s">
         <v>470</v>
-      </c>
-      <c r="AA1" s="48" t="s">
-        <v>470</v>
-      </c>
-      <c r="AB1" s="48" t="s">
-        <v>472</v>
       </c>
       <c r="AC1" s="48" t="s">
         <v>212</v>
       </c>
       <c r="AD1" s="48" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="AE1" s="48" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -3956,10 +3956,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="T9" s="47"/>
       <c r="U9" s="47" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="V9" s="47"/>
       <c r="X9" s="47"/>
@@ -4278,7 +4278,7 @@
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="X10" s="47"/>
     </row>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z13" s="47" t="s">
         <v>232</v>
@@ -4591,7 +4591,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -5948,7 +5948,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6862,7 +6862,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F2" t="s">
         <v>97</v>
@@ -6969,7 +6969,7 @@
         <v>393</v>
       </c>
       <c r="AB6" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -7037,25 +7037,25 @@
         <v>328</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>421</v>
-      </c>
       <c r="M1" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="O1" s="21" t="s">
         <v>338</v>
@@ -7082,13 +7082,13 @@
         <v>181</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>176</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="Z1" s="21" t="s">
         <v>5</v>
@@ -7162,7 +7162,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
@@ -7322,13 +7322,13 @@
         <v>332</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
@@ -7357,13 +7357,13 @@
       </c>
       <c r="U5" s="29"/>
       <c r="V5" s="20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W5" s="20" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="Y5" s="20" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AC5" s="20" t="s">
@@ -7384,7 +7384,7 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
@@ -7411,21 +7411,21 @@
         <v>399</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W6" s="29">
         <v>50.99</v>
       </c>
       <c r="Y6" s="20" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AA6" s="20" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
@@ -7456,15 +7456,15 @@
         <v>12.95</v>
       </c>
       <c r="AA7" s="20" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H8" s="20">
         <v>3</v>
@@ -7473,32 +7473,32 @@
         <v>381</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="L8" s="20" t="s">
         <v>443</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="M8" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="N8" s="20" t="s">
         <v>445</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>447</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="W9" s="29" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AA9" s="20" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
@@ -7528,13 +7528,13 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>332</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>160</v>
@@ -7554,7 +7554,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H12" s="20">
         <v>3</v>
@@ -7566,10 +7566,10 @@
         <v>32480</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="N12" s="20">
         <v>61132300</v>
@@ -7585,8 +7585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AV10" sqref="AV10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7638,22 +7638,22 @@
         <v>329</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>421</v>
-      </c>
       <c r="N1" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>338</v>
@@ -7748,7 +7748,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="S2" s="27"/>
       <c r="T2" s="20" t="s">
@@ -7922,30 +7922,30 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>416</v>
+        <v>473</v>
       </c>
       <c r="T7" s="20" t="s">
         <v>396</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>417</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K8" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="L8" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>425</v>
-      </c>
       <c r="M8" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
@@ -8364,7 +8364,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>327</v>
@@ -8373,7 +8373,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>283</v>
@@ -8395,7 +8395,7 @@
         <v>346</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="O2" s="29">
         <v>100</v>
@@ -9124,7 +9124,7 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
@@ -9592,7 +9592,7 @@
         <v>5</v>
       </c>
       <c r="AB1" s="48" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="AC1" s="48" t="s">
         <v>56</v>
@@ -9618,10 +9618,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -9638,7 +9638,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -9813,13 +9813,13 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA8" s="47" t="s">
+        <v>465</v>
+      </c>
+      <c r="AE8" s="47" t="s">
         <v>466</v>
-      </c>
-      <c r="AA8" s="47" t="s">
-        <v>467</v>
-      </c>
-      <c r="AE8" s="47" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Admin herobanner updated code, testcase, test data ,helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A5FFF5-0952-4457-93C5-D901614F7B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16032E3-8716-4AF3-BF53-4AE5D0F6BDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="482">
   <si>
     <t>DataSet</t>
   </si>
@@ -1457,6 +1457,27 @@
   </si>
   <si>
     <t>1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>VideoB</t>
+  </si>
+  <si>
+    <t>tilte2</t>
+  </si>
+  <si>
+    <t>prodURL</t>
+  </si>
+  <si>
+    <t>24 oz Standard Mouth</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/665626770</t>
+  </si>
+  <si>
+    <t>QA clonetest Hero Banner</t>
+  </si>
+  <si>
+    <t>https://mcloud-na.hydroflask.com/</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1676,6 +1697,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1963,62 +1999,62 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2134,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2115,7 +2151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2186,7 +2222,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2218,7 +2254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2250,7 +2286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2282,7 +2318,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -2310,13 +2346,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2648,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2720,7 +2756,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2852,7 +2888,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -2984,7 +3020,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -3116,7 +3152,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>
@@ -3265,16 +3301,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3413,7 +3449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3454,7 +3490,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3492,7 +3528,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3500,7 +3536,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3511,7 +3547,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3526,7 +3562,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3548,7 +3584,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3573,7 +3609,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3596,7 +3632,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3650,7 +3686,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3677,7 +3713,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3714,22 +3750,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3765,7 +3801,7 @@
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3776,12 +3812,12 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -3807,7 +3843,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -3830,7 +3866,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>460</v>
       </c>
@@ -3851,12 +3887,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="23" max="23" width="9.140625" style="47"/>
+    <col min="23" max="23" width="9.1796875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3951,7 +3987,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
@@ -3986,7 +4022,7 @@
       <c r="V2" s="47"/>
       <c r="X2" s="47"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>362</v>
       </c>
@@ -4023,7 +4059,7 @@
       <c r="V3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>365</v>
       </c>
@@ -4064,7 +4100,7 @@
       <c r="V4" s="47"/>
       <c r="X4" s="47"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>309</v>
       </c>
@@ -4097,7 +4133,7 @@
       <c r="V5" s="47"/>
       <c r="X5" s="47"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>314</v>
       </c>
@@ -4130,7 +4166,7 @@
       <c r="V6" s="47"/>
       <c r="X6" s="47"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>393</v>
       </c>
@@ -4173,7 +4209,7 @@
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>394</v>
       </c>
@@ -4216,7 +4252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4247,7 +4283,7 @@
       <c r="V9" s="47"/>
       <c r="X9" s="47"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4282,7 +4318,7 @@
       </c>
       <c r="X10" s="47"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>390</v>
       </c>
@@ -4311,7 +4347,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="47" t="s">
         <v>328</v>
       </c>
@@ -4319,7 +4355,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="47" t="s">
         <v>467</v>
       </c>
@@ -4344,55 +4380,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="20"/>
-    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="20"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="20"/>
+    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" style="20"/>
-    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7109375" style="20"/>
-    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="20"/>
-    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7109375" style="20"/>
-    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" style="20"/>
-    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7265625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="20"/>
+    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7265625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" style="20"/>
+    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="20"/>
-    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7109375" style="20"/>
-    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7109375" style="20"/>
-    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7109375" style="20"/>
+    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7265625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7265625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4583,7 +4619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4633,7 +4669,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4685,7 +4721,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4760,7 +4796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4896,7 +4932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5021,7 +5057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5154,7 +5190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5245,7 +5281,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5353,7 +5389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5444,7 +5480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5486,486 +5522,742 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CV4"/>
+  <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="25" max="25" width="27.140625" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="Z1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AA1" s="51" t="s">
         <v>413</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="51" t="s">
+        <v>476</v>
+      </c>
+      <c r="AZ1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="51" t="s">
         <v>181</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BT1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BU1" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BW1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BY1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BZ1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CA1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CB1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CC1" s="51" t="s">
+        <v>477</v>
+      </c>
+      <c r="CD1" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CE1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CF1" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CG1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CH1" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CI1" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CJ1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CK1" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CL1" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="CJ1" s="5" t="s">
+      <c r="CM1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CN1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CO1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CP1" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CQ1" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CR1" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CS1" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CT1" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="CR1" s="6" t="s">
+      <c r="CU1" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="CS1" s="6" t="s">
+      <c r="CV1" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="CT1" s="6" t="s">
+      <c r="CW1" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="CU1" s="6" t="s">
+      <c r="CX1" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="CV1" s="6" t="s">
+      <c r="CY1" s="56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52" t="s">
         <v>198</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" t="s">
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" t="s">
+      <c r="P2" s="52"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="V2" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y2" s="22" t="s">
+      <c r="V2" s="50" t="s">
+        <v>478</v>
+      </c>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="57" t="s">
+        <v>479</v>
+      </c>
+      <c r="Z2" s="52" t="s">
         <v>322</v>
       </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" t="s">
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" t="s">
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="52"/>
+      <c r="AM2" s="52"/>
+      <c r="AN2" s="52"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
+      <c r="AR2" s="52"/>
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="AW2" s="2"/>
-      <c r="AX2" t="s">
+      <c r="AU2" s="50"/>
+      <c r="AV2" s="50"/>
+      <c r="AW2" s="50"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="52" t="s">
+        <v>480</v>
+      </c>
+      <c r="AZ2" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BA2" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="AZ2" s="2"/>
-      <c r="BS2" s="13"/>
-      <c r="BT2" s="13" t="s">
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="50"/>
+      <c r="BD2" s="50"/>
+      <c r="BE2" s="50"/>
+      <c r="BF2" s="50"/>
+      <c r="BG2" s="50"/>
+      <c r="BH2" s="50"/>
+      <c r="BI2" s="50"/>
+      <c r="BJ2" s="50"/>
+      <c r="BK2" s="50"/>
+      <c r="BL2" s="50"/>
+      <c r="BM2" s="50"/>
+      <c r="BN2" s="50"/>
+      <c r="BO2" s="50"/>
+      <c r="BP2" s="50"/>
+      <c r="BQ2" s="50"/>
+      <c r="BR2" s="50"/>
+      <c r="BS2" s="50"/>
+      <c r="BT2" s="50"/>
+      <c r="BU2" s="58"/>
+      <c r="BV2" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="BU2" s="13" t="s">
+      <c r="BW2" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BX2" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BY2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BZ2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="BY2" s="3" t="s">
+      <c r="CA2" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CB2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CC2" s="52" t="s">
+        <v>481</v>
+      </c>
+      <c r="CD2" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="CB2" s="3" t="s">
+      <c r="CE2" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="CC2" s="3" t="s">
+      <c r="CF2" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="CD2" s="3" t="s">
+      <c r="CG2" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="CH2" s="7" t="s">
+      <c r="CH2" s="50"/>
+      <c r="CI2" s="50"/>
+      <c r="CJ2" s="50"/>
+      <c r="CK2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CL2" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="CJ2">
+      <c r="CM2" s="50">
         <v>12</v>
       </c>
-      <c r="CK2">
+      <c r="CN2" s="50">
         <v>13</v>
       </c>
-      <c r="CL2">
+      <c r="CO2" s="50">
         <v>14</v>
       </c>
-      <c r="CM2">
+      <c r="CP2" s="50">
         <v>15</v>
       </c>
-      <c r="CN2">
+      <c r="CQ2" s="50">
         <v>16</v>
       </c>
-      <c r="CO2">
+      <c r="CR2" s="50">
         <v>11</v>
       </c>
-      <c r="CP2">
+      <c r="CS2" s="50">
         <v>17</v>
       </c>
-      <c r="CQ2">
+      <c r="CT2" s="50">
         <v>10</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CU2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CV2" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CW2" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CX2" s="50" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="CY2" s="50"/>
+    </row>
+    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="50" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="4" spans="1:100" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50"/>
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AP3" s="50"/>
+      <c r="AQ3" s="50"/>
+      <c r="AR3" s="50"/>
+      <c r="AS3" s="50"/>
+      <c r="AT3" s="50"/>
+      <c r="AU3" s="50"/>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="50"/>
+      <c r="AX3" s="50"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="50"/>
+      <c r="BA3" s="50"/>
+      <c r="BB3" s="50"/>
+      <c r="BC3" s="50"/>
+      <c r="BD3" s="50"/>
+      <c r="BE3" s="50"/>
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="50"/>
+      <c r="BH3" s="50"/>
+      <c r="BI3" s="50"/>
+      <c r="BJ3" s="50"/>
+      <c r="BK3" s="50"/>
+      <c r="BL3" s="50"/>
+      <c r="BM3" s="50"/>
+      <c r="BN3" s="50"/>
+      <c r="BO3" s="50"/>
+      <c r="BP3" s="50"/>
+      <c r="BQ3" s="50"/>
+      <c r="BR3" s="50"/>
+      <c r="BS3" s="50"/>
+      <c r="BT3" s="50"/>
+      <c r="BU3" s="50"/>
+      <c r="BV3" s="50"/>
+      <c r="BW3" s="50"/>
+      <c r="BX3" s="50"/>
+      <c r="BY3" s="50"/>
+      <c r="BZ3" s="50"/>
+      <c r="CA3" s="50"/>
+      <c r="CB3" s="50"/>
+      <c r="CC3" s="50"/>
+      <c r="CD3" s="50"/>
+      <c r="CE3" s="50"/>
+      <c r="CF3" s="50"/>
+      <c r="CG3" s="50"/>
+      <c r="CH3" s="50"/>
+      <c r="CI3" s="50"/>
+      <c r="CJ3" s="50"/>
+      <c r="CK3" s="50"/>
+      <c r="CL3" s="50"/>
+      <c r="CM3" s="50"/>
+      <c r="CN3" s="50"/>
+      <c r="CO3" s="50"/>
+      <c r="CP3" s="50"/>
+      <c r="CQ3" s="50"/>
+      <c r="CR3" s="50"/>
+      <c r="CS3" s="50"/>
+      <c r="CT3" s="50"/>
+      <c r="CU3" s="50"/>
+      <c r="CV3" s="50"/>
+      <c r="CW3" s="50"/>
+      <c r="CX3" s="50"/>
+      <c r="CY3" s="50"/>
+    </row>
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="50" t="s">
         <v>412</v>
       </c>
-      <c r="Z4" s="20" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50" t="s">
         <v>414</v>
       </c>
+      <c r="AB4" s="50"/>
+      <c r="AC4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="50"/>
+      <c r="AG4" s="50"/>
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="50"/>
+      <c r="AJ4" s="50"/>
+      <c r="AK4" s="50"/>
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="50"/>
+      <c r="AN4" s="50"/>
+      <c r="AO4" s="50"/>
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="50"/>
+      <c r="AR4" s="50"/>
+      <c r="AS4" s="50"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
+      <c r="AZ4" s="50"/>
+      <c r="BA4" s="50"/>
+      <c r="BB4" s="50"/>
+      <c r="BC4" s="50"/>
+      <c r="BD4" s="50"/>
+      <c r="BE4" s="50"/>
+      <c r="BF4" s="50"/>
+      <c r="BG4" s="50"/>
+      <c r="BH4" s="50"/>
+      <c r="BI4" s="50"/>
+      <c r="BJ4" s="50"/>
+      <c r="BK4" s="50"/>
+      <c r="BL4" s="50"/>
+      <c r="BM4" s="50"/>
+      <c r="BN4" s="50"/>
+      <c r="BO4" s="50"/>
+      <c r="BP4" s="50"/>
+      <c r="BQ4" s="50"/>
+      <c r="BR4" s="50"/>
+      <c r="BS4" s="50"/>
+      <c r="BT4" s="50"/>
+      <c r="BU4" s="50"/>
+      <c r="BV4" s="50"/>
+      <c r="BW4" s="50"/>
+      <c r="BX4" s="50"/>
+      <c r="BY4" s="50"/>
+      <c r="BZ4" s="50"/>
+      <c r="CA4" s="50"/>
+      <c r="CB4" s="50"/>
+      <c r="CC4" s="50"/>
+      <c r="CD4" s="50"/>
+      <c r="CE4" s="50"/>
+      <c r="CF4" s="50"/>
+      <c r="CG4" s="50"/>
+      <c r="CH4" s="50"/>
+      <c r="CI4" s="50"/>
+      <c r="CJ4" s="50"/>
+      <c r="CK4" s="50"/>
+      <c r="CL4" s="50"/>
+      <c r="CM4" s="50"/>
+      <c r="CN4" s="50"/>
+      <c r="CO4" s="50"/>
+      <c r="CP4" s="50"/>
+      <c r="CQ4" s="50"/>
+      <c r="CR4" s="50"/>
+      <c r="CS4" s="50"/>
+      <c r="CT4" s="50"/>
+      <c r="CU4" s="50"/>
+      <c r="CV4" s="50"/>
+      <c r="CW4" s="50"/>
+      <c r="CX4" s="50"/>
+      <c r="CY4" s="50"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BZ2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="CA2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="CH2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="Y2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
+    <hyperlink ref="CB2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="CD2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="CK2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="Z2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{21721A70-E97D-4EE3-8CE3-5AEC0F2AA320}"/>
+    <hyperlink ref="CC2" r:id="rId6" xr:uid="{80112893-C12E-403E-A8BC-5798F689F083}"/>
+    <hyperlink ref="Y2" r:id="rId7" xr:uid="{62DC118F-1CA7-43F0-B74E-A134C0ADFC5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5979,12 +6271,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6289,7 +6581,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6355,7 +6647,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6497,7 +6789,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6562,7 +6854,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6618,7 +6910,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -6755,20 +7047,20 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6854,7 +7146,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6901,7 +7193,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -6939,7 +7231,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -6956,7 +7248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>390</v>
       </c>
@@ -6964,7 +7256,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>393</v>
       </c>
@@ -6972,7 +7264,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>394</v>
       </c>
@@ -6996,25 +7288,25 @@
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="20"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="20"/>
-    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="20"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7154,7 +7446,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7215,7 +7507,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -7269,7 +7561,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>350</v>
       </c>
@@ -7314,7 +7606,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>401</v>
       </c>
@@ -7382,7 +7674,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>427</v>
       </c>
@@ -7423,7 +7715,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>428</v>
       </c>
@@ -7459,7 +7751,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>439</v>
       </c>
@@ -7490,7 +7782,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>446</v>
       </c>
@@ -7501,7 +7793,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>400</v>
       </c>
@@ -7526,7 +7818,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>450</v>
       </c>
@@ -7552,7 +7844,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>416</v>
       </c>
@@ -7585,28 +7877,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="20"/>
+    <col min="23" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7740,7 +8032,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7788,7 +8080,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>395</v>
       </c>
@@ -7842,7 +8134,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>400</v>
       </c>
@@ -7862,7 +8154,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>401</v>
       </c>
@@ -7882,7 +8174,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>402</v>
       </c>
@@ -7908,7 +8200,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>415</v>
       </c>
@@ -7931,7 +8223,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>416</v>
       </c>
@@ -7954,7 +8246,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -7975,14 +8267,14 @@
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8356,7 +8648,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8532,7 +8824,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8553,7 +8845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -8687,7 +8979,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>383</v>
       </c>
@@ -8850,7 +9142,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>385</v>
       </c>
@@ -8983,7 +9275,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>387</v>
       </c>
@@ -9112,7 +9404,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>357</v>
       </c>
@@ -9237,7 +9529,7 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>388</v>
       </c>
@@ -9366,7 +9658,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>314</v>
       </c>
@@ -9491,7 +9783,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9507,9 +9799,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9613,7 +9905,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9627,7 +9919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9707,7 +9999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -9739,7 +10031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -9771,7 +10063,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -9803,7 +10095,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -9811,7 +10103,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>464</v>
       </c>
@@ -9822,7 +10114,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin cart rule price updated code test case, helper, test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16032E3-8716-4AF3-BF53-4AE5D0F6BDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3058704E-FFD1-42CD-84DB-DC1BC4DEF561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="8520" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="485">
   <si>
     <t>DataSet</t>
   </si>
@@ -1478,6 +1478,15 @@
   </si>
   <si>
     <t>https://mcloud-na.hydroflask.com/</t>
+  </si>
+  <si>
+    <t>https://mcloud-na.oxo.com/</t>
+  </si>
+  <si>
+    <t>###############################################################################################################################################################################################################################################################</t>
+  </si>
+  <si>
+    <t>8-Cup Coffee Maker</t>
   </si>
 </sst>
 </file>
@@ -1999,62 +2008,62 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" customWidth="1"/>
-    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2222,7 +2231,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2318,7 +2327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -2346,13 +2355,13 @@
       <selection activeCell="CO12" sqref="CO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2648,7 +2657,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2756,7 +2765,7 @@
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2888,7 +2897,7 @@
       <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>288</v>
       </c>
@@ -3020,7 +3029,7 @@
       <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>293</v>
       </c>
@@ -3152,7 +3161,7 @@
       <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>298</v>
       </c>
@@ -3301,16 +3310,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3449,7 +3458,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3490,7 +3499,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3536,7 +3545,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3547,7 +3556,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3562,7 +3571,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3584,7 +3593,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3609,7 +3618,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3632,7 +3641,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3686,7 +3695,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3713,7 +3722,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3750,22 +3759,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3801,7 +3810,7 @@
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3812,12 +3821,12 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -3843,7 +3852,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -3866,7 +3875,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>460</v>
       </c>
@@ -3887,12 +3896,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="23" max="23" width="9.1796875" style="47"/>
+    <col min="23" max="23" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3987,7 +3996,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
@@ -4022,7 +4031,7 @@
       <c r="V2" s="47"/>
       <c r="X2" s="47"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>362</v>
       </c>
@@ -4059,7 +4068,7 @@
       <c r="V3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>365</v>
       </c>
@@ -4100,7 +4109,7 @@
       <c r="V4" s="47"/>
       <c r="X4" s="47"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>309</v>
       </c>
@@ -4133,7 +4142,7 @@
       <c r="V5" s="47"/>
       <c r="X5" s="47"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>314</v>
       </c>
@@ -4166,7 +4175,7 @@
       <c r="V6" s="47"/>
       <c r="X6" s="47"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>393</v>
       </c>
@@ -4209,7 +4218,7 @@
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>394</v>
       </c>
@@ -4252,7 +4261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4283,7 +4292,7 @@
       <c r="V9" s="47"/>
       <c r="X9" s="47"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4318,7 +4327,7 @@
       </c>
       <c r="X10" s="47"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>390</v>
       </c>
@@ -4347,7 +4356,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>328</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>467</v>
       </c>
@@ -4380,55 +4389,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="20"/>
-    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7265625" style="20"/>
-    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="20"/>
+    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="20"/>
+    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7109375" style="20"/>
+    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7265625" style="20"/>
-    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7265625" style="20"/>
-    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7265625" style="20"/>
-    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7265625" style="20"/>
-    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7265625" style="20"/>
-    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7109375" style="20"/>
+    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7109375" style="20"/>
+    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" style="20"/>
+    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7109375" style="20"/>
+    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" style="20"/>
+    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7265625" style="20"/>
-    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7265625" style="20"/>
-    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7265625" style="20"/>
-    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7265625" style="20"/>
+    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="20"/>
+    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7109375" style="20"/>
+    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7109375" style="20"/>
+    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4619,7 +4628,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4669,7 +4678,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4721,7 +4730,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4796,7 +4805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4932,7 +4941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5057,7 +5066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5190,7 +5199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5281,7 +5290,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5389,7 +5398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5480,7 +5489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5524,18 +5533,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
+    <sheetView topLeftCell="BS1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="25" max="25" width="27.1796875" customWidth="1"/>
-    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="25" max="25" width="27.140625" customWidth="1"/>
+    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5846,7 +5855,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
@@ -6029,7 +6038,7 @@
       </c>
       <c r="CY2" s="50"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
@@ -6140,7 +6149,7 @@
       <c r="CX3" s="50"/>
       <c r="CY3" s="50"/>
     </row>
-    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>412</v>
       </c>
@@ -6271,12 +6280,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6581,7 +6590,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6647,7 +6656,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6789,7 +6798,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6854,7 +6863,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6910,7 +6919,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -7047,20 +7056,20 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.81640625" customWidth="1"/>
-    <col min="14" max="14" width="28.1796875" customWidth="1"/>
-    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7146,7 +7155,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7193,7 +7202,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -7231,7 +7240,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -7248,7 +7257,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>390</v>
       </c>
@@ -7256,7 +7265,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>393</v>
       </c>
@@ -7264,7 +7273,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>394</v>
       </c>
@@ -7288,25 +7297,25 @@
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="20"/>
-    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.1796875" style="20"/>
-    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="20"/>
+    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7446,7 +7455,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7507,7 +7516,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -7561,7 +7570,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>350</v>
       </c>
@@ -7606,7 +7615,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>401</v>
       </c>
@@ -7674,7 +7683,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>427</v>
       </c>
@@ -7715,7 +7724,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>428</v>
       </c>
@@ -7751,7 +7760,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>439</v>
       </c>
@@ -7782,7 +7791,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>446</v>
       </c>
@@ -7793,7 +7802,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>400</v>
       </c>
@@ -7818,7 +7827,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>450</v>
       </c>
@@ -7844,7 +7853,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>416</v>
       </c>
@@ -7881,24 +7890,24 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="20"/>
+    <col min="23" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8032,7 +8041,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8080,7 +8089,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>395</v>
       </c>
@@ -8134,7 +8143,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>400</v>
       </c>
@@ -8154,7 +8163,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>401</v>
       </c>
@@ -8174,7 +8183,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>402</v>
       </c>
@@ -8200,7 +8209,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>415</v>
       </c>
@@ -8223,7 +8232,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>416</v>
       </c>
@@ -8246,7 +8255,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -8263,18 +8272,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DT11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8561,7 +8570,7 @@
         <v>9</v>
       </c>
       <c r="CR1" s="21" t="s">
-        <v>10</v>
+        <v>477</v>
       </c>
       <c r="CS1" s="21" t="s">
         <v>39</v>
@@ -8648,15 +8657,15 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>97</v>
+        <v>326</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>327</v>
@@ -8792,7 +8801,9 @@
       <c r="CO2" s="20"/>
       <c r="CP2" s="20"/>
       <c r="CQ2" s="20"/>
-      <c r="CR2" s="7"/>
+      <c r="CR2" s="7" t="s">
+        <v>482</v>
+      </c>
       <c r="CS2" s="20" t="s">
         <v>142</v>
       </c>
@@ -8824,7 +8835,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8840,12 +8851,14 @@
       <c r="CH3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="CR3" s="7"/>
+      <c r="CR3" s="7" t="s">
+        <v>481</v>
+      </c>
       <c r="CS3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -8979,7 +8992,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>383</v>
       </c>
@@ -9022,8 +9035,8 @@
       <c r="S5" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="T5" s="38">
-        <v>9898989898</v>
+      <c r="T5" s="38" t="s">
+        <v>483</v>
       </c>
       <c r="U5" s="20" t="s">
         <v>160</v>
@@ -9142,7 +9155,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>385</v>
       </c>
@@ -9275,7 +9288,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>387</v>
       </c>
@@ -9404,7 +9417,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>357</v>
       </c>
@@ -9529,14 +9542,14 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>388</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="I9" s="20" t="s">
-        <v>389</v>
+        <v>484</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>389</v>
@@ -9658,7 +9671,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>314</v>
       </c>
@@ -9751,7 +9764,9 @@
       <c r="CO10" s="20"/>
       <c r="CP10" s="20"/>
       <c r="CQ10" s="20"/>
-      <c r="CR10" s="7"/>
+      <c r="CR10" s="7" t="s">
+        <v>482</v>
+      </c>
       <c r="CS10" s="20" t="s">
         <v>142</v>
       </c>
@@ -9783,7 +9798,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9799,9 +9814,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9905,7 +9920,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9919,7 +9934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9999,7 +10014,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -10031,7 +10046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10063,7 +10078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -10095,7 +10110,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -10103,7 +10118,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>464</v>
       </c>
@@ -10114,7 +10129,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin testimonails updated code testcase,testdata,helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55E606-EE1C-4C99-8697-317B7B753197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952CE6BA-D94B-4D8D-A60D-250561EF4B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="487">
   <si>
     <t>DataSet</t>
   </si>
@@ -1490,6 +1490,9 @@
   </si>
   <si>
     <t>24 oz Standard Mouth - Seagrass</t>
+  </si>
+  <si>
+    <t>Testmonialqa</t>
   </si>
 </sst>
 </file>
@@ -2011,62 +2014,62 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" customWidth="1"/>
-    <col min="12" max="12" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.7265625" customWidth="1"/>
+    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>410</v>
       </c>
@@ -2352,19 +2355,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CT6"/>
+  <dimension ref="A1:CU6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="78" max="78" width="8.7265625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2596,71 +2600,74 @@
       <c r="BY1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="BZ1" s="21" t="s">
+      <c r="BZ1" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="CA1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CA1" s="21" t="s">
+      <c r="CB1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CB1" s="21" t="s">
+      <c r="CC1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="CC1" s="21" t="s">
+      <c r="CD1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="CD1" s="21" t="s">
+      <c r="CE1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="CE1" s="21" t="s">
+      <c r="CF1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="CF1" s="21" t="s">
+      <c r="CG1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="CG1" s="21" t="s">
+      <c r="CH1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="CH1" s="21" t="s">
+      <c r="CI1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="CI1" s="25" t="s">
+      <c r="CJ1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="CJ1" s="25" t="s">
+      <c r="CK1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="CK1" s="25" t="s">
+      <c r="CL1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="CL1" s="25" t="s">
+      <c r="CM1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="CM1" s="25" t="s">
+      <c r="CN1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="CN1" s="25" t="s">
+      <c r="CO1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="CO1" s="25" t="s">
+      <c r="CP1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="CP1" s="25" t="s">
+      <c r="CQ1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="CQ1" s="26" t="s">
+      <c r="CR1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="CR1" s="26" t="s">
+      <c r="CS1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="CS1" s="26" t="s">
+      <c r="CT1" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="CT1" s="26" t="s">
+      <c r="CU1" s="26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2753,6 @@
       <c r="BW2" s="20"/>
       <c r="BX2" s="20"/>
       <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
       <c r="CA2" s="20"/>
       <c r="CB2" s="20"/>
       <c r="CC2" s="20"/>
@@ -2767,8 +2773,9 @@
       <c r="CR2" s="20"/>
       <c r="CS2" s="20"/>
       <c r="CT2" s="20"/>
-    </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="CU2" s="20"/>
+    </row>
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2788,7 +2795,7 @@
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
@@ -2858,10 +2865,12 @@
       <c r="BY3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="BZ3" s="22" t="s">
+      <c r="BZ3" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="CA3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="CA3" s="20"/>
       <c r="CB3" s="20"/>
       <c r="CC3" s="20"/>
       <c r="CD3" s="20"/>
@@ -2869,40 +2878,41 @@
       <c r="CF3" s="20"/>
       <c r="CG3" s="20"/>
       <c r="CH3" s="20"/>
-      <c r="CI3" s="20">
+      <c r="CI3" s="20"/>
+      <c r="CJ3" s="20">
         <v>25</v>
       </c>
-      <c r="CJ3" s="20">
+      <c r="CK3" s="20">
         <v>27</v>
       </c>
-      <c r="CK3" s="20">
+      <c r="CL3" s="20">
         <v>15</v>
       </c>
-      <c r="CL3" s="20">
+      <c r="CM3" s="20">
         <v>10</v>
       </c>
-      <c r="CM3" s="20">
+      <c r="CN3" s="20">
         <v>30</v>
       </c>
-      <c r="CN3" s="20">
+      <c r="CO3" s="20">
         <v>35</v>
       </c>
-      <c r="CO3" s="20">
+      <c r="CP3" s="20">
         <v>32</v>
       </c>
-      <c r="CP3" s="20">
+      <c r="CQ3" s="20">
         <v>23</v>
       </c>
-      <c r="CQ3" s="20" t="s">
+      <c r="CR3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="CR3" s="20" t="s">
+      <c r="CS3" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="CS3" s="20"/>
       <c r="CT3" s="20"/>
-    </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="CU3" s="20"/>
+    </row>
+    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>287</v>
       </c>
@@ -2992,7 +3002,6 @@
       <c r="BW4" s="20"/>
       <c r="BX4" s="20"/>
       <c r="BY4" s="20"/>
-      <c r="BZ4" s="20"/>
       <c r="CA4" s="20"/>
       <c r="CB4" s="20"/>
       <c r="CC4" s="20"/>
@@ -3001,40 +3010,41 @@
       <c r="CF4" s="20"/>
       <c r="CG4" s="20"/>
       <c r="CH4" s="20"/>
-      <c r="CI4" s="20">
+      <c r="CI4" s="20"/>
+      <c r="CJ4" s="20">
         <v>12</v>
       </c>
-      <c r="CJ4" s="20">
+      <c r="CK4" s="20">
         <v>13</v>
       </c>
-      <c r="CK4" s="20">
+      <c r="CL4" s="20">
         <v>15</v>
       </c>
-      <c r="CL4" s="20">
+      <c r="CM4" s="20">
         <v>14</v>
       </c>
-      <c r="CM4" s="20">
+      <c r="CN4" s="20">
         <v>17</v>
       </c>
-      <c r="CN4" s="20">
+      <c r="CO4" s="20">
         <v>18</v>
       </c>
-      <c r="CO4" s="20">
+      <c r="CP4" s="20">
         <v>16</v>
       </c>
-      <c r="CP4" s="20">
+      <c r="CQ4" s="20">
         <v>10</v>
       </c>
-      <c r="CQ4" s="20" t="s">
+      <c r="CR4" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="CR4" s="20" t="s">
+      <c r="CS4" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="CS4" s="20"/>
       <c r="CT4" s="20"/>
-    </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="CU4" s="20"/>
+    </row>
+    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>291</v>
       </c>
@@ -3124,7 +3134,6 @@
       <c r="BW5" s="20"/>
       <c r="BX5" s="20"/>
       <c r="BY5" s="20"/>
-      <c r="BZ5" s="20"/>
       <c r="CA5" s="20"/>
       <c r="CB5" s="20"/>
       <c r="CC5" s="20"/>
@@ -3133,40 +3142,41 @@
       <c r="CF5" s="20"/>
       <c r="CG5" s="20"/>
       <c r="CH5" s="20"/>
-      <c r="CI5" s="20">
+      <c r="CI5" s="20"/>
+      <c r="CJ5" s="20">
         <v>16</v>
       </c>
-      <c r="CJ5" s="20">
+      <c r="CK5" s="20">
         <v>18</v>
       </c>
-      <c r="CK5" s="20">
+      <c r="CL5" s="20">
         <v>11</v>
       </c>
-      <c r="CL5" s="20">
+      <c r="CM5" s="20">
         <v>12</v>
       </c>
-      <c r="CM5" s="20">
+      <c r="CN5" s="20">
         <v>13</v>
       </c>
-      <c r="CN5" s="20">
+      <c r="CO5" s="20">
         <v>17</v>
       </c>
-      <c r="CO5" s="20">
+      <c r="CP5" s="20">
         <v>15</v>
       </c>
-      <c r="CP5" s="20">
+      <c r="CQ5" s="20">
         <v>19</v>
       </c>
-      <c r="CQ5" s="20" t="s">
+      <c r="CR5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="CR5" s="31" t="s">
+      <c r="CS5" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="CS5" s="20"/>
       <c r="CT5" s="20"/>
-    </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="CU5" s="20"/>
+    </row>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>296</v>
       </c>
@@ -3256,7 +3266,6 @@
       <c r="BW6" s="20"/>
       <c r="BX6" s="20"/>
       <c r="BY6" s="20"/>
-      <c r="BZ6" s="20"/>
       <c r="CA6" s="20"/>
       <c r="CB6" s="20"/>
       <c r="CC6" s="20"/>
@@ -3265,44 +3274,46 @@
       <c r="CF6" s="20"/>
       <c r="CG6" s="20"/>
       <c r="CH6" s="20"/>
-      <c r="CI6" s="20">
+      <c r="CI6" s="20"/>
+      <c r="CJ6" s="20">
         <v>11</v>
       </c>
-      <c r="CJ6" s="20">
+      <c r="CK6" s="20">
         <v>14</v>
       </c>
-      <c r="CK6" s="20">
+      <c r="CL6" s="20">
         <v>15</v>
       </c>
-      <c r="CL6" s="20">
+      <c r="CM6" s="20">
         <v>17</v>
       </c>
-      <c r="CM6" s="20">
+      <c r="CN6" s="20">
         <v>19</v>
       </c>
-      <c r="CN6" s="20">
+      <c r="CO6" s="20">
         <v>12</v>
       </c>
-      <c r="CO6" s="20">
+      <c r="CP6" s="20">
         <v>13</v>
       </c>
-      <c r="CP6" s="20">
+      <c r="CQ6" s="20">
         <v>16</v>
       </c>
-      <c r="CQ6" s="20" t="s">
+      <c r="CR6" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="CR6" s="31" t="s">
+      <c r="CS6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="CS6" s="20"/>
       <c r="CT6" s="20"/>
+      <c r="CU6" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="BY3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="BZ3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="CA3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{44992E42-E8EB-4F33-8E2F-6CF0F11139FC}"/>
+    <hyperlink ref="BZ3" r:id="rId4" xr:uid="{75C44558-18F5-4CFE-8606-47F5AA70D99B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3316,16 +3327,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3447,7 +3458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3464,7 +3475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3505,7 +3516,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3543,7 +3554,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3551,7 +3562,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3562,7 +3573,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3577,7 +3588,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3599,7 +3610,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3624,7 +3635,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3647,7 +3658,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3701,7 +3712,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3728,7 +3739,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3765,22 +3776,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3816,7 +3827,7 @@
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3827,12 +3838,12 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3858,7 +3869,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3881,7 +3892,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -3902,12 +3913,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="23" max="23" width="9.140625" style="47"/>
+    <col min="23" max="23" width="9.1796875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -4002,7 +4013,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
@@ -4037,7 +4048,7 @@
       <c r="V2" s="47"/>
       <c r="X2" s="47"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>360</v>
       </c>
@@ -4074,7 +4085,7 @@
       <c r="V3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>363</v>
       </c>
@@ -4115,7 +4126,7 @@
       <c r="V4" s="47"/>
       <c r="X4" s="47"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>307</v>
       </c>
@@ -4148,7 +4159,7 @@
       <c r="V5" s="47"/>
       <c r="X5" s="47"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>312</v>
       </c>
@@ -4181,7 +4192,7 @@
       <c r="V6" s="47"/>
       <c r="X6" s="47"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>391</v>
       </c>
@@ -4224,7 +4235,7 @@
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>392</v>
       </c>
@@ -4267,7 +4278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4298,7 +4309,7 @@
       <c r="V9" s="47"/>
       <c r="X9" s="47"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4333,7 +4344,7 @@
       </c>
       <c r="X10" s="47"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>388</v>
       </c>
@@ -4362,7 +4373,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="47" t="s">
         <v>326</v>
       </c>
@@ -4370,7 +4381,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="47" t="s">
         <v>465</v>
       </c>
@@ -4395,55 +4406,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="20"/>
-    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="20"/>
-    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="20"/>
+    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" style="20"/>
-    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7109375" style="20"/>
-    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="20"/>
-    <col min="29" max="29" width="37.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7109375" style="20"/>
-    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" style="20"/>
-    <col min="36" max="36" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.7265625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="20"/>
+    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.7265625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" style="20"/>
+    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="20"/>
-    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7109375" style="20"/>
-    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7109375" style="20"/>
-    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7109375" style="20"/>
+    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7265625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.7265625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.7265625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4634,7 +4645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4684,7 +4695,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4736,7 +4747,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4811,7 +4822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4947,7 +4958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5072,7 +5083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5205,7 +5216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5296,7 +5307,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5404,7 +5415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5495,7 +5506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5539,19 +5550,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="CC1" sqref="CC1:CC1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.140625" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="22" max="22" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5862,7 +5873,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
@@ -6045,7 +6056,7 @@
       </c>
       <c r="CY2" s="50"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
@@ -6156,7 +6167,7 @@
       <c r="CX3" s="50"/>
       <c r="CY3" s="50"/>
     </row>
-    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50" t="s">
         <v>410</v>
       </c>
@@ -6287,12 +6298,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6597,7 +6608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6663,7 +6674,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6805,7 +6816,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6870,7 +6881,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6926,7 +6937,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -7063,20 +7074,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7162,7 +7173,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7209,7 +7220,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -7247,7 +7258,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -7264,7 +7275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -7272,7 +7283,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -7280,7 +7291,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -7304,25 +7315,25 @@
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="20"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="20"/>
-    <col min="13" max="13" width="35.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.28515625" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="20"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7462,7 +7473,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7523,7 +7534,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>328</v>
       </c>
@@ -7577,7 +7588,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>348</v>
       </c>
@@ -7622,7 +7633,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -7690,7 +7701,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>425</v>
       </c>
@@ -7731,7 +7742,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>426</v>
       </c>
@@ -7767,7 +7778,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>437</v>
       </c>
@@ -7798,7 +7809,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>444</v>
       </c>
@@ -7809,7 +7820,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>398</v>
       </c>
@@ -7834,7 +7845,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>448</v>
       </c>
@@ -7860,7 +7871,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>414</v>
       </c>
@@ -7897,24 +7908,24 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="20"/>
-    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="20"/>
+    <col min="23" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8048,7 +8059,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8096,7 +8107,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>393</v>
       </c>
@@ -8150,7 +8161,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>398</v>
       </c>
@@ -8170,7 +8181,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -8190,7 +8201,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>400</v>
       </c>
@@ -8216,7 +8227,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>413</v>
       </c>
@@ -8239,7 +8250,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>414</v>
       </c>
@@ -8262,7 +8273,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -8283,14 +8294,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8664,7 +8675,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8842,7 +8853,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8865,7 +8876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -8999,7 +9010,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>381</v>
       </c>
@@ -9162,7 +9173,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>383</v>
       </c>
@@ -9295,7 +9306,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>385</v>
       </c>
@@ -9424,7 +9435,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>355</v>
       </c>
@@ -9549,7 +9560,7 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>386</v>
       </c>
@@ -9678,7 +9689,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>312</v>
       </c>
@@ -9805,7 +9816,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9821,9 +9832,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9927,7 +9938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9941,7 +9952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10021,7 +10032,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -10053,7 +10064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10085,7 +10096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -10117,7 +10128,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>410</v>
       </c>
@@ -10125,7 +10136,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>462</v>
       </c>
@@ -10136,7 +10147,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin herobanner updated helper,testcase,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952CE6BA-D94B-4D8D-A60D-250561EF4B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633576CD-CF07-4DDD-87BC-9490F020EBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -1489,10 +1489,10 @@
     <t>W20BTS</t>
   </si>
   <si>
-    <t>24 oz Standard Mouth - Seagrass</t>
-  </si>
-  <si>
     <t>Testmonialqa</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Laguna</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+    <sheetView topLeftCell="BL1" workbookViewId="0">
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
@@ -2795,7 +2795,7 @@
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
@@ -5550,8 +5550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="CC1" sqref="CC1:CC1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5904,7 +5904,7 @@
         <v>114</v>
       </c>
       <c r="V2" s="50" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="W2" s="50"/>
       <c r="X2" s="50"/>

</xml_diff>

<commit_message>
Admin order placement testcases correction-Helper,testdata,testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633576CD-CF07-4DDD-87BC-9490F020EBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6EA0B3-C6C9-48DC-AF49-D61782C1E1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11412" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -1237,9 +1237,6 @@
     <t>HFGroupproduct</t>
   </si>
   <si>
-    <t>hf-group</t>
-  </si>
-  <si>
     <t>storepage</t>
   </si>
   <si>
@@ -1493,6 +1490,9 @@
   </si>
   <si>
     <t>32 oz Wide Mouth - Laguna</t>
+  </si>
+  <si>
+    <t>Test_Grouped</t>
   </si>
 </sst>
 </file>
@@ -2014,62 +2014,62 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7265625" customWidth="1"/>
-    <col min="12" max="12" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.77734375" customWidth="1"/>
+    <col min="12" max="12" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.77734375" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2146,10 +2146,10 @@
         <v>38</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2166,7 +2166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2333,12 +2333,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -2361,14 +2361,14 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
-    <col min="78" max="78" width="8.7265625" style="50"/>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1"/>
+    <col min="78" max="78" width="8.77734375" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>10</v>
       </c>
       <c r="BZ1" s="51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="CA1" s="21" t="s">
         <v>39</v>
@@ -2667,7 +2667,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="20"/>
@@ -2775,7 +2775,7 @@
       <c r="CT2" s="20"/>
       <c r="CU2" s="20"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
@@ -2860,13 +2860,13 @@
       <c r="BV3" s="20"/>
       <c r="BW3" s="28"/>
       <c r="BX3" s="22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="BY3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="BZ3" s="52" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CA3" s="52" t="s">
         <v>40</v>
@@ -2912,7 +2912,7 @@
       <c r="CT3" s="20"/>
       <c r="CU3" s="20"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>287</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="BO4" s="20"/>
       <c r="BP4" s="20"/>
       <c r="BQ4" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="BR4" s="20"/>
       <c r="BS4" s="20"/>
@@ -3044,7 +3044,7 @@
       <c r="CT4" s="20"/>
       <c r="CU4" s="20"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>291</v>
       </c>
@@ -3176,7 +3176,7 @@
       <c r="CT5" s="20"/>
       <c r="CU5" s="20"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>296</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="BO6" s="20"/>
       <c r="BP6" s="20"/>
       <c r="BQ6" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="BR6" s="20"/>
       <c r="BS6" s="20"/>
@@ -3327,16 +3327,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3475,7 +3475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3776,22 +3776,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3823,27 +3823,27 @@
         <v>306</v>
       </c>
       <c r="K1" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" t="s">
         <v>456</v>
       </c>
-      <c r="C2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3892,12 +3892,12 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3913,12 +3913,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="23" max="23" width="9.1796875" style="47"/>
+    <col min="23" max="23" width="9.21875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>5</v>
       </c>
       <c r="W1" s="48" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="X1" s="48" t="s">
         <v>227</v>
@@ -3995,33 +3995,33 @@
         <v>369</v>
       </c>
       <c r="Z1" s="48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AA1" s="48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AB1" s="48" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AC1" s="48" t="s">
         <v>212</v>
       </c>
       <c r="AD1" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="AE1" s="48" t="s">
         <v>469</v>
       </c>
-      <c r="AE1" s="48" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="49" t="s">
+        <v>450</v>
+      </c>
+      <c r="C2" s="49" t="s">
         <v>451</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>452</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -4048,7 +4048,7 @@
       <c r="V2" s="47"/>
       <c r="X2" s="47"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>360</v>
       </c>
@@ -4085,7 +4085,7 @@
       <c r="V3" s="47"/>
       <c r="X3" s="47"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>363</v>
       </c>
@@ -4126,7 +4126,7 @@
       <c r="V4" s="47"/>
       <c r="X4" s="47"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>307</v>
       </c>
@@ -4159,7 +4159,7 @@
       <c r="V5" s="47"/>
       <c r="X5" s="47"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>312</v>
       </c>
@@ -4192,7 +4192,7 @@
       <c r="V6" s="47"/>
       <c r="X6" s="47"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>391</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>392</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4304,12 +4304,12 @@
       </c>
       <c r="T9" s="47"/>
       <c r="U9" s="47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="V9" s="47"/>
       <c r="X9" s="47"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4340,11 +4340,11 @@
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X10" s="47"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>388</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
         <v>326</v>
       </c>
@@ -4381,9 +4381,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Z13" s="47" t="s">
         <v>232</v>
@@ -4406,55 +4406,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="20"/>
-    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7265625" style="20"/>
-    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="20"/>
+    <col min="1" max="1" width="17.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="20"/>
+    <col min="5" max="5" width="49.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.77734375" style="20"/>
+    <col min="10" max="10" width="13.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.7265625" style="20"/>
-    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.7265625" style="20"/>
-    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.7265625" style="20"/>
-    <col min="29" max="29" width="37.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.7265625" style="20"/>
-    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.7265625" style="20"/>
-    <col min="36" max="36" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.77734375" style="20"/>
+    <col min="18" max="18" width="42.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.77734375" style="20"/>
+    <col min="26" max="26" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.21875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.77734375" style="20"/>
+    <col min="29" max="29" width="37.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.77734375" style="20"/>
+    <col min="32" max="32" width="18.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.77734375" style="20"/>
+    <col min="36" max="36" width="15.21875" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.7265625" style="20"/>
-    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.7265625" style="20"/>
-    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.7265625" style="20"/>
-    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.7265625" style="20"/>
+    <col min="38" max="38" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.77734375" style="20"/>
+    <col min="42" max="42" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.77734375" style="20"/>
+    <col min="44" max="44" width="37.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.77734375" style="20"/>
+    <col min="52" max="52" width="9.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.77734375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -4695,7 +4695,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5550,19 +5550,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="22" max="22" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.1796875" customWidth="1"/>
-    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.21875" customWidth="1"/>
+    <col min="26" max="26" width="27.21875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5636,13 +5636,13 @@
         <v>58</v>
       </c>
       <c r="Y1" s="51" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Z1" s="51" t="s">
         <v>23</v>
       </c>
       <c r="AA1" s="51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AB1" s="51" t="s">
         <v>59</v>
@@ -5714,7 +5714,7 @@
         <v>82</v>
       </c>
       <c r="AY1" s="51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AZ1" s="51" t="s">
         <v>5</v>
@@ -5804,7 +5804,7 @@
         <v>10</v>
       </c>
       <c r="CC1" s="51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="CD1" s="51" t="s">
         <v>39</v>
@@ -5873,7 +5873,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
@@ -5904,12 +5904,12 @@
         <v>114</v>
       </c>
       <c r="V2" s="50" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="W2" s="50"/>
       <c r="X2" s="50"/>
       <c r="Y2" s="57" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Z2" s="52" t="s">
         <v>320</v>
@@ -5945,7 +5945,7 @@
       <c r="AW2" s="50"/>
       <c r="AX2" s="52"/>
       <c r="AY2" s="52" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AZ2" s="50" t="s">
         <v>201</v>
@@ -5995,7 +5995,7 @@
         <v>18</v>
       </c>
       <c r="CC2" s="52" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CD2" s="52" t="s">
         <v>40</v>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="CY2" s="50"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D3" s="50"/>
       <c r="E3" s="50"/>
@@ -6167,9 +6167,9 @@
       <c r="CX3" s="50"/>
       <c r="CY3" s="50"/>
     </row>
-    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
@@ -6197,7 +6197,7 @@
       <c r="Y4" s="50"/>
       <c r="Z4" s="50"/>
       <c r="AA4" s="50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AB4" s="50"/>
       <c r="AC4" s="50"/>
@@ -6298,12 +6298,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6674,7 +6674,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -7074,20 +7074,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.81640625" customWidth="1"/>
-    <col min="14" max="14" width="28.1796875" customWidth="1"/>
-    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.77734375" customWidth="1"/>
+    <col min="14" max="14" width="28.21875" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F2" t="s">
         <v>97</v>
@@ -7220,7 +7220,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -7283,15 +7283,15 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>391</v>
       </c>
       <c r="AB6" s="29" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -7315,25 +7315,25 @@
       <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="20"/>
-    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.1796875" style="20"/>
-    <col min="13" max="13" width="35.7265625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.26953125" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="20.21875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" style="20"/>
+    <col min="5" max="5" width="15.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.21875" style="20"/>
+    <col min="8" max="8" width="16.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.21875" style="20"/>
+    <col min="13" max="13" width="35.77734375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.21875" style="20" customWidth="1"/>
+    <col min="19" max="16384" width="9.21875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7356,25 +7356,25 @@
         <v>326</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>327</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O1" s="21" t="s">
         <v>336</v>
@@ -7395,19 +7395,19 @@
         <v>395</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="V1" s="21" t="s">
         <v>181</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>176</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="Z1" s="21" t="s">
         <v>5</v>
@@ -7473,7 +7473,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>324</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
@@ -7534,7 +7534,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>328</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>348</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -7641,13 +7641,13 @@
         <v>330</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
@@ -7676,13 +7676,13 @@
       </c>
       <c r="U5" s="29"/>
       <c r="V5" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W5" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y5" s="20" t="s">
         <v>432</v>
-      </c>
-      <c r="Y5" s="20" t="s">
-        <v>433</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AC5" s="20" t="s">
@@ -7701,9 +7701,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
@@ -7730,21 +7730,21 @@
         <v>397</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W6" s="29">
         <v>50.99</v>
       </c>
       <c r="Y6" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AA6" s="20" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
@@ -7775,15 +7775,15 @@
         <v>12.95</v>
       </c>
       <c r="AA7" s="20" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>437</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>438</v>
       </c>
       <c r="H8" s="20">
         <v>3</v>
@@ -7792,35 +7792,35 @@
         <v>379</v>
       </c>
       <c r="J8" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>439</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="M8" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="N8" s="20" t="s">
         <v>442</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>443</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="W9" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA9" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="W9" s="29" t="s">
-        <v>449</v>
-      </c>
-      <c r="AA9" s="20" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>398</v>
       </c>
@@ -7842,18 +7842,18 @@
         <v>396</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>330</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>160</v>
@@ -7871,9 +7871,9 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H12" s="20">
         <v>3</v>
@@ -7885,10 +7885,10 @@
         <v>32480</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N12" s="20">
         <v>61132300</v>
@@ -7904,28 +7904,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" style="20"/>
+    <col min="8" max="8" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="20"/>
+    <col min="23" max="16384" width="9.21875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7951,28 +7951,28 @@
         <v>395</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>327</v>
       </c>
       <c r="K1" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>415</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>416</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>336</v>
@@ -7987,10 +7987,10 @@
         <v>174</v>
       </c>
       <c r="U1" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>403</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>404</v>
       </c>
       <c r="W1" s="21" t="s">
         <v>5</v>
@@ -8059,7 +8059,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>324</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S2" s="27"/>
       <c r="T2" s="20" t="s">
@@ -8107,7 +8107,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>393</v>
       </c>
@@ -8134,7 +8134,7 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R3" s="34">
         <v>432</v>
@@ -8161,7 +8161,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>398</v>
       </c>
@@ -8175,13 +8175,13 @@
         <v>396</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -8195,13 +8195,13 @@
         <v>397</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="T5" s="20" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>400</v>
       </c>
@@ -8215,21 +8215,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>401</v>
+        <v>486</v>
       </c>
       <c r="T6" s="20" t="s">
         <v>394</v>
       </c>
       <c r="U6" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="V6" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="V6" s="20" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>241</v>
@@ -8241,30 +8241,30 @@
         <v>1</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="T7" s="20" t="s">
         <v>394</v>
       </c>
       <c r="U7" s="20" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K8" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>421</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>420</v>
-      </c>
       <c r="N8" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O8" s="20">
         <v>61132300</v>
@@ -8273,7 +8273,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -8294,14 +8294,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.77734375" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>9</v>
       </c>
       <c r="CR1" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="CS1" s="21" t="s">
         <v>39</v>
@@ -8675,7 +8675,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>324</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>325</v>
@@ -8692,7 +8692,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>283</v>
@@ -8714,7 +8714,7 @@
         <v>344</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O2" s="29">
         <v>100</v>
@@ -8820,7 +8820,7 @@
       <c r="CP2" s="20"/>
       <c r="CQ2" s="20"/>
       <c r="CR2" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="CS2" s="20" t="s">
         <v>142</v>
@@ -8853,7 +8853,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8870,13 +8870,13 @@
         <v>40</v>
       </c>
       <c r="CR3" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CS3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -9010,7 +9010,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>381</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>330</v>
       </c>
       <c r="T5" s="38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="U5" s="20" t="s">
         <v>160</v>
@@ -9173,7 +9173,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>383</v>
       </c>
@@ -9306,7 +9306,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>385</v>
       </c>
@@ -9435,7 +9435,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>355</v>
       </c>
@@ -9447,7 +9447,7 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
@@ -9560,14 +9560,14 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>386</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="I9" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>387</v>
@@ -9689,7 +9689,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>312</v>
       </c>
@@ -9783,7 +9783,7 @@
       <c r="CP10" s="20"/>
       <c r="CQ10" s="20"/>
       <c r="CR10" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="CS10" s="20" t="s">
         <v>142</v>
@@ -9816,7 +9816,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9832,9 +9832,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9911,13 +9911,13 @@
         <v>38</v>
       </c>
       <c r="Z1" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AA1" s="48" t="s">
         <v>5</v>
       </c>
       <c r="AB1" s="48" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AC1" s="48" t="s">
         <v>56</v>
@@ -9938,21 +9938,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C2" t="s">
         <v>451</v>
-      </c>
-      <c r="C2" t="s">
-        <v>452</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -10032,7 +10032,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -10128,26 +10128,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z7" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>461</v>
+      </c>
+      <c r="AA8" s="47" t="s">
         <v>462</v>
       </c>
-      <c r="AA8" s="47" t="s">
+      <c r="AE8" s="47" t="s">
         <v>463</v>
       </c>
-      <c r="AE8" s="47" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin retail order placement code correction-Testdat
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6EA0B3-C6C9-48DC-AF49-D61782C1E1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F429AD95-04BC-421F-A0E0-77DA66FB0CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11412" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="489">
   <si>
     <t>DataSet</t>
   </si>
@@ -1493,6 +1493,12 @@
   </si>
   <si>
     <t>Test_Grouped</t>
+  </si>
+  <si>
+    <t>32480,11234000</t>
+  </si>
+  <si>
+    <t>59.99,19.99</t>
   </si>
 </sst>
 </file>
@@ -7311,8 +7317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7330,7 +7336,9 @@
     <col min="14" max="14" width="18.44140625" style="20" customWidth="1"/>
     <col min="15" max="15" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="18.21875" style="20" customWidth="1"/>
-    <col min="19" max="16384" width="9.21875" style="20"/>
+    <col min="19" max="22" width="9.21875" style="20"/>
+    <col min="23" max="23" width="11.5546875" style="20" customWidth="1"/>
+    <col min="24" max="16384" width="9.21875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -7633,7 +7641,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -7651,8 +7659,8 @@
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="42"/>
-      <c r="J5" s="33">
-        <v>3248011234000</v>
+      <c r="J5" s="33" t="s">
+        <v>487</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
@@ -7701,14 +7709,14 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>424</v>
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
-      <c r="J6" s="33">
-        <v>3248011234000</v>
+      <c r="J6" s="33" t="s">
+        <v>487</v>
       </c>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
@@ -7732,8 +7740,8 @@
       <c r="V6" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="W6" s="29">
-        <v>50.99</v>
+      <c r="W6" s="29" t="s">
+        <v>488</v>
       </c>
       <c r="Y6" s="20" t="s">
         <v>446</v>
@@ -7742,14 +7750,14 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>425</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
-      <c r="J7" s="33">
-        <v>3248011234000</v>
+      <c r="J7" s="33" t="s">
+        <v>487</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
@@ -7904,7 +7912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Admin updated excel and helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F429AD95-04BC-421F-A0E0-77DA66FB0CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0374187F-AA2F-4BEB-B8E6-4C451DAAB371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="489">
   <si>
     <t>DataSet</t>
   </si>
@@ -2020,62 +2020,62 @@
       <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.77734375" customWidth="1"/>
-    <col min="12" max="12" width="54.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.81640625" customWidth="1"/>
+    <col min="12" max="12" width="54.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.81640625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -2367,14 +2367,14 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1"/>
-    <col min="78" max="78" width="8.77734375" style="50"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="78" max="78" width="8.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="CT2" s="20"/>
       <c r="CU2" s="20"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="CT3" s="20"/>
       <c r="CU3" s="20"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>287</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="CT4" s="20"/>
       <c r="CU4" s="20"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>291</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="CT5" s="20"/>
       <c r="CU5" s="20"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>296</v>
       </c>
@@ -3333,16 +3333,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3522,7 +3522,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3718,7 +3718,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3782,22 +3782,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3844,12 +3844,12 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -3913,18 +3913,21 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="23" max="23" width="9.21875" style="47"/>
+    <col min="2" max="2" width="47.81640625" customWidth="1"/>
+    <col min="13" max="13" width="44.6328125" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="50"/>
+    <col min="24" max="24" width="9.1796875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -3964,70 +3967,73 @@
       <c r="M1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="O1" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="P1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="Q1" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="R1" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="S1" s="48" t="s">
         <v>359</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="U1" s="48" t="s">
         <v>390</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="W1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>466</v>
       </c>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48" t="s">
         <v>369</v>
-      </c>
-      <c r="Z1" s="48" t="s">
-        <v>465</v>
       </c>
       <c r="AA1" s="48" t="s">
         <v>465</v>
       </c>
       <c r="AB1" s="48" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC1" s="48" t="s">
         <v>467</v>
       </c>
-      <c r="AC1" s="48" t="s">
+      <c r="AD1" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="AD1" s="48" t="s">
+      <c r="AE1" s="48" t="s">
         <v>468</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AF1" s="48" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>450</v>
+      <c r="B2" s="57" t="s">
+        <v>97</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -4039,22 +4045,22 @@
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
       <c r="O2" s="47"/>
       <c r="P2" s="47"/>
       <c r="Q2" s="47"/>
       <c r="R2" s="47"/>
-      <c r="S2" s="47" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>228</v>
       </c>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>230</v>
       </c>
-      <c r="V2" s="47"/>
-      <c r="X2" s="47"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W2" s="47"/>
+      <c r="Y2" s="47"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>360</v>
       </c>
@@ -4078,20 +4084,20 @@
       <c r="K3" s="47"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
       <c r="O3" s="47"/>
-      <c r="P3" s="47">
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47">
         <v>0</v>
       </c>
-      <c r="Q3" s="47"/>
       <c r="R3" s="47"/>
       <c r="S3" s="47"/>
       <c r="T3" s="47"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
-      <c r="X3" s="47"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W3" s="47"/>
+      <c r="Y3" s="47"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
         <v>363</v>
       </c>
@@ -4117,22 +4123,22 @@
         <v>366</v>
       </c>
       <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
       <c r="O4" s="47"/>
       <c r="P4" s="47"/>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="S4" s="47" t="s">
         <v>367</v>
       </c>
-      <c r="S4" s="47"/>
       <c r="T4" s="47"/>
       <c r="U4" s="47"/>
       <c r="V4" s="47"/>
-      <c r="X4" s="47"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W4" s="47"/>
+      <c r="Y4" s="47"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
         <v>307</v>
       </c>
@@ -4147,25 +4153,28 @@
       <c r="J5" s="47"/>
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
-      <c r="M5" s="47" t="s">
+      <c r="M5" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="N5" s="57" t="s">
+        <v>477</v>
+      </c>
+      <c r="O5" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="47" t="s">
+      <c r="P5" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="P5" s="47"/>
       <c r="Q5" s="47"/>
       <c r="R5" s="47"/>
       <c r="S5" s="47"/>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
       <c r="V5" s="47"/>
-      <c r="X5" s="47"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W5" s="47"/>
+      <c r="Y5" s="47"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>312</v>
       </c>
@@ -4180,25 +4189,28 @@
       <c r="J6" s="47"/>
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
-      <c r="M6" s="47" t="s">
+      <c r="M6" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="57" t="s">
+        <v>478</v>
+      </c>
+      <c r="O6" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="47" t="s">
+      <c r="P6" s="47" t="s">
         <v>368</v>
       </c>
-      <c r="P6" s="47"/>
       <c r="Q6" s="47"/>
       <c r="R6" s="47"/>
       <c r="S6" s="47"/>
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
       <c r="V6" s="47"/>
-      <c r="X6" s="47"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W6" s="47"/>
+      <c r="Y6" s="47"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" s="47" t="s">
         <v>391</v>
       </c>
@@ -4214,34 +4226,34 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
       <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
       <c r="O7" s="47"/>
       <c r="P7" s="47"/>
       <c r="Q7" s="47"/>
       <c r="R7" s="47"/>
       <c r="S7" s="47"/>
-      <c r="T7" s="47">
+      <c r="T7" s="47"/>
+      <c r="U7" s="47">
         <v>10</v>
       </c>
-      <c r="U7" s="47"/>
       <c r="V7" s="47"/>
-      <c r="W7" s="47">
+      <c r="W7" s="47"/>
+      <c r="X7" s="47">
         <v>1</v>
       </c>
-      <c r="X7" s="47"/>
-      <c r="AA7" s="47" t="s">
+      <c r="Y7" s="47"/>
+      <c r="AB7" s="47" t="s">
         <v>244</v>
       </c>
-      <c r="AB7" s="47" t="s">
+      <c r="AC7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="47">
+      <c r="AD7" s="47">
         <v>10</v>
       </c>
-      <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF7" s="47"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="47" t="s">
         <v>392</v>
       </c>
@@ -4257,34 +4269,34 @@
       <c r="K8" s="47"/>
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
       <c r="O8" s="47"/>
       <c r="P8" s="47"/>
       <c r="Q8" s="47"/>
       <c r="R8" s="47"/>
       <c r="S8" s="47"/>
-      <c r="T8" s="47">
+      <c r="T8" s="47"/>
+      <c r="U8" s="47">
         <v>20</v>
       </c>
-      <c r="U8" s="47"/>
       <c r="V8" s="47"/>
-      <c r="W8" s="47">
+      <c r="W8" s="47"/>
+      <c r="X8" s="47">
         <v>2</v>
       </c>
-      <c r="X8" s="47"/>
-      <c r="AA8" s="47" t="s">
+      <c r="Y8" s="47"/>
+      <c r="AB8" s="47" t="s">
         <v>244</v>
       </c>
-      <c r="AB8" s="47"/>
       <c r="AC8" s="47"/>
-      <c r="AD8" s="47" t="s">
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="AE8" s="47">
+      <c r="AF8" s="47">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4300,22 +4312,22 @@
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
       <c r="O9" s="47"/>
       <c r="P9" s="47"/>
       <c r="Q9" s="47"/>
       <c r="R9" s="47"/>
-      <c r="S9" s="47" t="s">
+      <c r="S9" s="47"/>
+      <c r="T9" s="47" t="s">
         <v>228</v>
       </c>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47" t="s">
+      <c r="U9" s="47"/>
+      <c r="V9" s="47" t="s">
         <v>452</v>
       </c>
-      <c r="V9" s="47"/>
-      <c r="X9" s="47"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="W9" s="47"/>
+      <c r="Y9" s="47"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4330,27 +4342,30 @@
       <c r="J10" s="47"/>
       <c r="K10" s="47"/>
       <c r="L10" s="47"/>
-      <c r="M10" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="N10" s="47" t="s">
+      <c r="M10" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="57" t="s">
+        <v>477</v>
+      </c>
+      <c r="O10" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="47" t="s">
+      <c r="P10" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="P10" s="47"/>
       <c r="Q10" s="47"/>
       <c r="R10" s="47"/>
       <c r="S10" s="47"/>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
-      <c r="V10" s="47" t="s">
+      <c r="V10" s="47"/>
+      <c r="W10" s="47" t="s">
         <v>453</v>
       </c>
-      <c r="X10" s="47"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="Y10" s="47"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>388</v>
       </c>
@@ -4366,7 +4381,6 @@
       <c r="K11" s="47"/>
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
       <c r="O11" s="47"/>
       <c r="P11" s="47"/>
       <c r="Q11" s="47"/>
@@ -4375,30 +4389,38 @@
       <c r="T11" s="47"/>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
-      <c r="X11" s="47" t="s">
+      <c r="W11" s="47"/>
+      <c r="Y11" s="47" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="Y12" s="47">
+      <c r="N12" s="50"/>
+      <c r="Z12" s="47">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="Z13" s="47" t="s">
+      <c r="N13" s="50"/>
+      <c r="AA13" s="47" t="s">
         <v>232</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{56FC7C01-14F8-404B-9BA6-55321738E0FD}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{3E5BA075-C023-462E-ABE1-8ACCFCA37358}"/>
+    <hyperlink ref="M5" r:id="rId2" xr:uid="{01CEA421-2E8E-4152-818D-7A1E87447EB6}"/>
+    <hyperlink ref="N5" r:id="rId3" xr:uid="{D7DAD218-128F-4387-8E33-93E5524ACF59}"/>
+    <hyperlink ref="M6" r:id="rId4" xr:uid="{7A468824-E13D-4C09-B78B-F15BD4621476}"/>
+    <hyperlink ref="N6" r:id="rId5" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
+    <hyperlink ref="M10" r:id="rId6" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
+    <hyperlink ref="N10" r:id="rId7" xr:uid="{05DB7605-785C-4F54-9C95-FDDA7B131849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4412,55 +4434,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="20"/>
-    <col min="5" max="5" width="49.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.77734375" style="20"/>
-    <col min="10" max="10" width="13.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="20"/>
+    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" style="20"/>
+    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.77734375" style="20"/>
-    <col min="18" max="18" width="42.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.77734375" style="20"/>
-    <col min="26" max="26" width="16.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.21875" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.77734375" style="20"/>
-    <col min="29" max="29" width="37.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.77734375" style="20"/>
-    <col min="32" max="32" width="18.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.77734375" style="20"/>
-    <col min="36" max="36" width="15.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.81640625" style="20"/>
+    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.81640625" style="20"/>
+    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.81640625" style="20"/>
+    <col min="29" max="29" width="37.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.81640625" style="20"/>
+    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.81640625" style="20"/>
+    <col min="36" max="36" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" style="20"/>
-    <col min="42" max="42" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.77734375" style="20"/>
-    <col min="44" max="44" width="37.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.77734375" style="20"/>
-    <col min="52" max="52" width="9.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.77734375" style="20"/>
+    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.81640625" style="20"/>
+    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.81640625" style="20"/>
+    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.81640625" style="20"/>
+    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.81640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4651,7 +4673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4701,7 +4723,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4753,7 +4775,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4828,7 +4850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4964,7 +4986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5089,7 +5111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5222,7 +5244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5313,7 +5335,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5421,7 +5443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5512,7 +5534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5560,15 +5582,15 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.21875" customWidth="1"/>
-    <col min="26" max="26" width="27.21875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="22" max="22" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.1796875" customWidth="1"/>
+    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5879,7 +5901,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
@@ -6062,7 +6084,7 @@
       </c>
       <c r="CY2" s="50"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
@@ -6173,7 +6195,7 @@
       <c r="CX3" s="50"/>
       <c r="CY3" s="50"/>
     </row>
-    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50" t="s">
         <v>409</v>
       </c>
@@ -6304,12 +6326,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6614,7 +6636,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6680,7 +6702,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6822,7 +6844,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6887,7 +6909,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6943,7 +6965,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -7080,20 +7102,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.77734375" customWidth="1"/>
-    <col min="14" max="14" width="28.21875" customWidth="1"/>
-    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7179,7 +7201,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7226,7 +7248,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -7264,7 +7286,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -7281,7 +7303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -7289,7 +7311,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -7297,7 +7319,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -7317,31 +7339,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="20"/>
-    <col min="5" max="5" width="15.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.21875" style="20"/>
-    <col min="8" max="8" width="16.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.21875" style="20"/>
-    <col min="13" max="13" width="35.77734375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.21875" style="20" customWidth="1"/>
-    <col min="19" max="22" width="9.21875" style="20"/>
-    <col min="23" max="23" width="11.5546875" style="20" customWidth="1"/>
-    <col min="24" max="16384" width="9.21875" style="20"/>
+    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="20"/>
+    <col min="5" max="5" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="35.81640625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.1796875" style="20" customWidth="1"/>
+    <col min="19" max="22" width="9.1796875" style="20"/>
+    <col min="23" max="23" width="11.54296875" style="20" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7481,7 +7503,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7542,7 +7564,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>328</v>
       </c>
@@ -7596,7 +7618,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>348</v>
       </c>
@@ -7641,7 +7663,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -7709,7 +7731,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>424</v>
       </c>
@@ -7750,7 +7772,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>425</v>
       </c>
@@ -7786,7 +7808,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>436</v>
       </c>
@@ -7817,7 +7839,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>443</v>
       </c>
@@ -7828,7 +7850,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>398</v>
       </c>
@@ -7853,7 +7875,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>447</v>
       </c>
@@ -7879,7 +7901,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>413</v>
       </c>
@@ -7916,24 +7938,24 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" style="20"/>
-    <col min="8" max="8" width="20.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="20"/>
+    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.21875" style="20"/>
+    <col min="23" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8067,7 +8089,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8115,7 +8137,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>393</v>
       </c>
@@ -8169,7 +8191,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>398</v>
       </c>
@@ -8189,7 +8211,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -8209,7 +8231,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>400</v>
       </c>
@@ -8235,7 +8257,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>412</v>
       </c>
@@ -8258,7 +8280,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>413</v>
       </c>
@@ -8281,7 +8303,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -8302,14 +8324,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.44140625" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.77734375" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8683,7 +8705,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8861,7 +8883,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8884,7 +8906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -9018,7 +9040,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>381</v>
       </c>
@@ -9181,7 +9203,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>383</v>
       </c>
@@ -9314,7 +9336,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>385</v>
       </c>
@@ -9443,7 +9465,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>355</v>
       </c>
@@ -9568,7 +9590,7 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>386</v>
       </c>
@@ -9697,7 +9719,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>312</v>
       </c>
@@ -9824,7 +9846,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9840,9 +9862,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9946,7 +9968,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9960,7 +9982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10040,7 +10062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -10072,7 +10094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10104,7 +10126,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -10136,7 +10158,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -10144,7 +10166,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -10155,7 +10177,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
testdata for value prop banner
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0374187F-AA2F-4BEB-B8E6-4C451DAAB371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60BAAD7-9748-4194-80F9-8D3D45BC409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="490">
   <si>
     <t>DataSet</t>
   </si>
@@ -1499,6 +1499,9 @@
   </si>
   <si>
     <t>59.99,19.99</t>
+  </si>
+  <si>
+    <t>Qatestvalueprop</t>
   </si>
 </sst>
 </file>
@@ -2014,68 +2017,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.81640625" customWidth="1"/>
-    <col min="12" max="12" width="54.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="255.81640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.85546875" style="50" customWidth="1"/>
+    <col min="14" max="14" width="54.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2112,50 +2116,53 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2172,7 +2179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2198,152 +2205,155 @@
         <v>17</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>41</v>
+        <v>489</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="N3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>25</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>27</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>15</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>10</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>30</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>35</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>32</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>23</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>25</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>27</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>15</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>30</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>35</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>32</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>23</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>12</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>32</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>22</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>12</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>23</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>20</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>32</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>21</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>32</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>34</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>54</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>21</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>13</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>5</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>12</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>409</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>411</v>
       </c>
     </row>
@@ -2353,9 +2363,11 @@
     <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{FE45A353-2970-40A1-8263-26DCFE88D323}"/>
+    <hyperlink ref="N3" r:id="rId4" xr:uid="{1E9C7ABE-9AD4-433A-93D8-0847C3C7692F}"/>
+    <hyperlink ref="M3" r:id="rId5" xr:uid="{B47EF309-D0F6-4854-B6A3-925061D1D767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2367,14 +2379,14 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
-    <col min="78" max="78" width="8.81640625" style="50"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="78" max="78" width="8.85546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2685,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -2781,7 +2793,7 @@
       <c r="CT2" s="20"/>
       <c r="CU2" s="20"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>284</v>
       </c>
@@ -2918,7 +2930,7 @@
       <c r="CT3" s="20"/>
       <c r="CU3" s="20"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>287</v>
       </c>
@@ -3050,7 +3062,7 @@
       <c r="CT4" s="20"/>
       <c r="CU4" s="20"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>291</v>
       </c>
@@ -3182,7 +3194,7 @@
       <c r="CT5" s="20"/>
       <c r="CU5" s="20"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>296</v>
       </c>
@@ -3333,16 +3345,16 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3464,7 +3476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3481,7 +3493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3522,7 +3534,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3560,7 +3572,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3568,7 +3580,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3579,7 +3591,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3594,7 +3606,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3616,7 +3628,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3641,7 +3653,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3664,7 +3676,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3718,7 +3730,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3745,7 +3757,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3782,22 +3794,22 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3833,7 +3845,7 @@
       </c>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3844,12 +3856,12 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3875,7 +3887,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3898,7 +3910,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -3915,19 +3927,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.81640625" customWidth="1"/>
-    <col min="13" max="13" width="44.6328125" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="50"/>
-    <col min="24" max="24" width="9.1796875" style="47"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="13" max="13" width="44.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="50"/>
+    <col min="24" max="24" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -4025,7 +4037,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
@@ -4060,7 +4072,7 @@
       <c r="W2" s="47"/>
       <c r="Y2" s="47"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>360</v>
       </c>
@@ -4097,7 +4109,7 @@
       <c r="W3" s="47"/>
       <c r="Y3" s="47"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>363</v>
       </c>
@@ -4138,7 +4150,7 @@
       <c r="W4" s="47"/>
       <c r="Y4" s="47"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>307</v>
       </c>
@@ -4174,7 +4186,7 @@
       <c r="W5" s="47"/>
       <c r="Y5" s="47"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>312</v>
       </c>
@@ -4210,7 +4222,7 @@
       <c r="W6" s="47"/>
       <c r="Y6" s="47"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>391</v>
       </c>
@@ -4253,7 +4265,7 @@
       <c r="AE7" s="47"/>
       <c r="AF7" s="47"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>392</v>
       </c>
@@ -4296,7 +4308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>234</v>
       </c>
@@ -4327,7 +4339,7 @@
       <c r="W9" s="47"/>
       <c r="Y9" s="47"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>237</v>
       </c>
@@ -4365,7 +4377,7 @@
       </c>
       <c r="Y10" s="47"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>388</v>
       </c>
@@ -4394,7 +4406,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>326</v>
       </c>
@@ -4403,7 +4415,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>464</v>
       </c>
@@ -4434,55 +4446,55 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" style="20"/>
-    <col min="5" max="5" width="49.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" style="20"/>
-    <col min="10" max="10" width="13.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="20"/>
+    <col min="1" max="1" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="20"/>
+    <col min="5" max="5" width="49.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" style="20"/>
+    <col min="10" max="10" width="13.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="20"/>
     <col min="15" max="15" width="83" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.81640625" style="20"/>
-    <col min="18" max="18" width="42.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="8.81640625" style="20"/>
-    <col min="26" max="26" width="16.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.1796875" style="20" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" style="20"/>
-    <col min="29" max="29" width="37.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="8.81640625" style="20"/>
-    <col min="32" max="32" width="18.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.81640625" style="20"/>
-    <col min="36" max="36" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.85546875" style="20"/>
+    <col min="18" max="18" width="42.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="8.85546875" style="20"/>
+    <col min="26" max="26" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" style="20" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="20"/>
+    <col min="29" max="29" width="37.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.85546875" style="20"/>
+    <col min="32" max="32" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.85546875" style="20"/>
+    <col min="36" max="36" width="15.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" style="20" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.81640625" style="20"/>
-    <col min="42" max="42" width="46.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.81640625" style="20"/>
-    <col min="44" max="44" width="37.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="8.81640625" style="20"/>
-    <col min="52" max="52" width="9.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.81640625" style="20"/>
+    <col min="38" max="38" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.85546875" style="20"/>
+    <col min="42" max="42" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.85546875" style="20"/>
+    <col min="44" max="44" width="37.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="49" max="51" width="8.85546875" style="20"/>
+    <col min="52" max="52" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4673,7 +4685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4723,7 +4735,7 @@
       <c r="AN2" s="22"/>
       <c r="AO2" s="22"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
@@ -4775,7 +4787,7 @@
       </c>
       <c r="AO3" s="22"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
@@ -4850,7 +4862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -4986,7 +4998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>134</v>
       </c>
@@ -5111,7 +5123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>143</v>
       </c>
@@ -5244,7 +5256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>161</v>
       </c>
@@ -5335,7 +5347,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>164</v>
       </c>
@@ -5443,7 +5455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>172</v>
       </c>
@@ -5534,7 +5546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
@@ -5582,15 +5594,15 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="22" max="22" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.1796875" customWidth="1"/>
-    <col min="26" max="26" width="27.1796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.140625" customWidth="1"/>
+    <col min="26" max="26" width="27.140625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
@@ -5901,7 +5913,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>197</v>
       </c>
@@ -6084,7 +6096,7 @@
       </c>
       <c r="CY2" s="50"/>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>11</v>
       </c>
@@ -6195,7 +6207,7 @@
       <c r="CX3" s="50"/>
       <c r="CY3" s="50"/>
     </row>
-    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:103" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>409</v>
       </c>
@@ -6326,12 +6338,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6636,7 +6648,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6702,7 +6714,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6844,7 +6856,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6909,7 +6921,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6965,7 +6977,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -7102,20 +7114,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="31.81640625" customWidth="1"/>
-    <col min="14" max="14" width="28.1796875" customWidth="1"/>
-    <col min="22" max="22" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7201,7 +7213,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7248,7 +7260,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -7286,7 +7298,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -7303,7 +7315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -7311,7 +7323,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -7319,7 +7331,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -7343,27 +7355,27 @@
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="20"/>
-    <col min="5" max="5" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="16.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
-    <col min="10" max="12" width="9.1796875" style="20"/>
-    <col min="13" max="13" width="35.81640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.1796875" style="20" customWidth="1"/>
-    <col min="19" max="22" width="9.1796875" style="20"/>
-    <col min="23" max="23" width="11.54296875" style="20" customWidth="1"/>
-    <col min="24" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="20.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="20"/>
+    <col min="5" max="5" width="15.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="16.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="20" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="20"/>
+    <col min="13" max="13" width="35.85546875" style="20" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.140625" style="20" customWidth="1"/>
+    <col min="19" max="22" width="9.140625" style="20"/>
+    <col min="23" max="23" width="11.5703125" style="20" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -7503,7 +7515,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -7564,7 +7576,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>328</v>
       </c>
@@ -7618,7 +7630,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>348</v>
       </c>
@@ -7663,7 +7675,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -7731,7 +7743,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>424</v>
       </c>
@@ -7772,7 +7784,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>425</v>
       </c>
@@ -7808,7 +7820,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>436</v>
       </c>
@@ -7839,7 +7851,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>443</v>
       </c>
@@ -7850,7 +7862,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>398</v>
       </c>
@@ -7875,7 +7887,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>447</v>
       </c>
@@ -7901,7 +7913,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>413</v>
       </c>
@@ -7938,24 +7950,24 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="20"/>
-    <col min="8" max="8" width="20.81640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="20"/>
+    <col min="8" max="8" width="20.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" style="20" customWidth="1"/>
-    <col min="20" max="20" width="34.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" style="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="20"/>
+    <col min="23" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8089,7 +8101,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8137,7 +8149,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>393</v>
       </c>
@@ -8191,7 +8203,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>398</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>399</v>
       </c>
@@ -8231,7 +8243,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>400</v>
       </c>
@@ -8257,7 +8269,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>412</v>
       </c>
@@ -8280,7 +8292,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>413</v>
       </c>
@@ -8303,7 +8315,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
     </row>
@@ -8324,14 +8336,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.453125" style="20" customWidth="1"/>
-    <col min="5" max="8" width="20.81640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="20" customWidth="1"/>
+    <col min="5" max="8" width="20.85546875" style="20" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:124" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -8705,7 +8717,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -8883,7 +8895,7 @@
       <c r="DS2" s="20"/>
       <c r="DT2" s="20"/>
     </row>
-    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:124" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>237</v>
       </c>
@@ -8906,7 +8918,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
@@ -9040,7 +9052,7 @@
       <c r="DS4" s="20"/>
       <c r="DT4" s="20"/>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>381</v>
       </c>
@@ -9203,7 +9215,7 @@
       <c r="DS5" s="20"/>
       <c r="DT5" s="20"/>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>383</v>
       </c>
@@ -9336,7 +9348,7 @@
       <c r="DS6" s="20"/>
       <c r="DT6" s="20"/>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>385</v>
       </c>
@@ -9465,7 +9477,7 @@
       <c r="DS7" s="20"/>
       <c r="DT7" s="20"/>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>355</v>
       </c>
@@ -9590,7 +9602,7 @@
       <c r="DS8" s="20"/>
       <c r="DT8" s="20"/>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>386</v>
       </c>
@@ -9719,7 +9731,7 @@
       <c r="DS9" s="20"/>
       <c r="DT9" s="20"/>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>312</v>
       </c>
@@ -9846,7 +9858,7 @@
       <c r="DS10" s="20"/>
       <c r="DT10" s="20"/>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
       <c r="DO11" s="29"/>
     </row>
   </sheetData>
@@ -9862,9 +9874,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -9968,7 +9980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -9982,7 +9994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10062,7 +10074,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -10094,7 +10106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10126,7 +10138,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -10158,7 +10170,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -10166,7 +10178,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -10177,7 +10189,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
RMA retail order magneto
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60BAAD7-9748-4194-80F9-8D3D45BC409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF054189-C384-4DF0-9919-5419292BBBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="customer" sheetId="6" r:id="rId11"/>
     <sheet name="Category" sheetId="8" r:id="rId12"/>
     <sheet name="CatalogPricerule" sheetId="12" r:id="rId13"/>
+    <sheet name="Retailer RMA" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="495">
   <si>
     <t>DataSet</t>
   </si>
@@ -1502,6 +1503,21 @@
   </si>
   <si>
     <t>Qatestvalueprop</t>
+  </si>
+  <si>
+    <t>Avayujipqhf1!</t>
+  </si>
+  <si>
+    <t>avayugundla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Shipping method</t>
+  </si>
+  <si>
+    <t>FedEx Ground</t>
+  </si>
+  <si>
+    <t>Add New Address</t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -3341,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,8 +3806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3927,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4433,6 +4449,304 @@
     <hyperlink ref="N6" r:id="rId5" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
     <hyperlink ref="M10" r:id="rId6" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
     <hyperlink ref="N10" r:id="rId7" xr:uid="{05DB7605-785C-4F54-9C95-FDDA7B131849}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42566712-9BDD-4411-A327-58B0705D2B5D}">
+  <dimension ref="A1:AL3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>331</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>327</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>337</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>335</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>347</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>395</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>492</v>
+      </c>
+      <c r="P1" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q1" s="51" t="s">
+        <v>426</v>
+      </c>
+      <c r="R1" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="T1" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="V1" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="W1" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="X1" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y1" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z1" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA1" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB1" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD1" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF1" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG1" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH1" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI1" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ1" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK1" s="51" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL1" s="51" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>491</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>490</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="44">
+        <v>44861</v>
+      </c>
+      <c r="J2" s="50">
+        <v>431</v>
+      </c>
+      <c r="K2" s="50">
+        <v>4242424242424240</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>324</v>
+      </c>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC2" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD2" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH2" s="50">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="AJ2" s="50">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL2" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="I3" s="43">
+        <v>44862</v>
+      </c>
+      <c r="J3" s="41">
+        <v>123</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="M3" s="50">
+        <v>120</v>
+      </c>
+      <c r="N3" s="50" t="s">
+        <v>396</v>
+      </c>
+      <c r="O3" s="50" t="s">
+        <v>493</v>
+      </c>
+      <c r="P3" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50" t="s">
+        <v>494</v>
+      </c>
+      <c r="V3" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="W3" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="X3" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y3" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50"/>
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5A837F4D-E595-47D8-8D66-3EB4633C1B39}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{2E9605E1-24A5-4113-8434-6DB9E01E6161}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7351,8 +7665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView topLeftCell="X4" workbookViewId="0">
+      <selection sqref="A1:AT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Admin 16 testcase code changes-Helper,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DCC810-78D0-4AC1-ACDC-8B6CBF699712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB7843E-BD92-4F4E-B8D7-C129512C12A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9720" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -3809,8 +3809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3946,15 +3946,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="13" max="13" width="44.5703125" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="50"/>
+    <col min="14" max="14" width="41.140625" style="50" customWidth="1"/>
     <col min="24" max="24" width="9.140625" style="47"/>
   </cols>
   <sheetData>
@@ -4060,11 +4060,11 @@
       <c r="A2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="57" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>434</v>
+      <c r="B2" s="50" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>456</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
@@ -4445,13 +4445,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{56FC7C01-14F8-404B-9BA6-55321738E0FD}"/>
-    <hyperlink ref="M5" r:id="rId2" xr:uid="{01CEA421-2E8E-4152-818D-7A1E87447EB6}"/>
-    <hyperlink ref="N5" r:id="rId3" xr:uid="{D7DAD218-128F-4387-8E33-93E5524ACF59}"/>
-    <hyperlink ref="M6" r:id="rId4" xr:uid="{7A468824-E13D-4C09-B78B-F15BD4621476}"/>
-    <hyperlink ref="N6" r:id="rId5" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
-    <hyperlink ref="M10" r:id="rId6" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
-    <hyperlink ref="N10" r:id="rId7" xr:uid="{05DB7605-785C-4F54-9C95-FDDA7B131849}"/>
+    <hyperlink ref="M5" r:id="rId1" xr:uid="{01CEA421-2E8E-4152-818D-7A1E87447EB6}"/>
+    <hyperlink ref="N5" r:id="rId2" xr:uid="{D7DAD218-128F-4387-8E33-93E5524ACF59}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{7A468824-E13D-4C09-B78B-F15BD4621476}"/>
+    <hyperlink ref="N6" r:id="rId4" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
+    <hyperlink ref="M10" r:id="rId5" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
+    <hyperlink ref="N10" r:id="rId6" xr:uid="{05DB7605-785C-4F54-9C95-FDDA7B131849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4461,7 +4460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42566712-9BDD-4411-A327-58B0705D2B5D}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testdata and Store selector method changes for Admin testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8553783-8DF0-4560-ABB0-D44CC5F657E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3C4548-E89D-4E92-AB2C-AA6095B7EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="500">
   <si>
     <t>DataSet</t>
   </si>
@@ -1530,6 +1530,9 @@
   </si>
   <si>
     <t>TL-W40BTS-120,SFS001,SSSFX</t>
+  </si>
+  <si>
+    <t>Store_Selection</t>
   </si>
 </sst>
 </file>
@@ -7446,7 +7449,7 @@
   <dimension ref="A1:AR10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7810,6 +7813,14 @@
       </c>
       <c r="P8" s="17" t="s">
         <v>379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>499</v>
+      </c>
+      <c r="H9" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Admin Testcase retail order for gobal
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3C4548-E89D-4E92-AB2C-AA6095B7EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86DF4DA-5A12-413F-A682-CC33FCBD8C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="503">
   <si>
     <t>DataSet</t>
   </si>
@@ -1533,6 +1533,15 @@
   </si>
   <si>
     <t>Store_Selection</t>
+  </si>
+  <si>
+    <t>HYFWebsite</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>S18SX001,LW24LW080</t>
   </si>
 </sst>
 </file>
@@ -2018,62 +2027,62 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.88671875" customWidth="1"/>
+    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.88671875" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2156,7 +2165,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2173,7 +2182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2279,7 +2288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -2373,14 +2382,13 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="78" max="78" width="8.85546875"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2679,7 +2687,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2754,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -2829,7 +2837,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2879,7 +2887,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -2970,7 +2978,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -3039,16 +3047,16 @@
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3170,7 +3178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3187,7 +3195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3228,7 +3236,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3266,7 +3274,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3274,7 +3282,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3285,7 +3293,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3300,7 +3308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3322,7 +3330,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3347,7 +3355,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3370,7 +3378,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3424,7 +3432,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3451,7 +3459,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3488,22 +3496,22 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3547,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3550,12 +3558,12 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3581,7 +3589,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3604,7 +3612,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -3625,14 +3633,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="13" max="13" width="44.5703125" customWidth="1"/>
-    <col min="14" max="14" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+    <col min="13" max="13" width="44.5546875" customWidth="1"/>
+    <col min="14" max="14" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3747,7 +3755,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -3767,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>363</v>
       </c>
@@ -3793,7 +3801,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -3810,7 +3818,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3827,7 +3835,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -3847,7 +3855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -3867,7 +3875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3878,7 +3886,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -3898,7 +3906,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>388</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -3914,7 +3922,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>464</v>
       </c>
@@ -3943,22 +3951,22 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="48.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4071,7 +4079,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4125,7 +4133,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -4202,43 +4210,43 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" customWidth="1"/>
-    <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.109375" customWidth="1"/>
+    <col min="29" max="29" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4429,7 +4437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4479,7 +4487,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -4531,7 +4539,7 @@
       </c>
       <c r="AO3" s="2"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4606,7 +4614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -4742,7 +4750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -4867,7 +4875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5000,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -5091,7 +5099,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -5199,7 +5207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -5290,7 +5298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5338,14 +5346,14 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5656,7 +5664,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -5804,7 +5812,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -5815,7 +5823,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>409</v>
       </c>
@@ -5845,12 +5853,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6155,7 +6163,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6221,7 +6229,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6363,7 +6371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6428,7 +6436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6484,7 +6492,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -6621,20 +6629,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="14" max="14" width="28.109375" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6720,7 +6728,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6767,7 +6775,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -6805,7 +6813,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -6822,7 +6830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6830,7 +6838,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -6838,7 +6846,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -6858,26 +6866,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView topLeftCell="X4" workbookViewId="0">
-      <selection sqref="A1:AT12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.140625" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.109375" customWidth="1"/>
+    <col min="23" max="23" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7017,7 +7025,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7078,7 +7086,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -7112,8 +7120,8 @@
       <c r="Q3">
         <v>4242424242424240</v>
       </c>
-      <c r="R3" t="s">
-        <v>349</v>
+      <c r="R3" s="7" t="s">
+        <v>491</v>
       </c>
       <c r="AA3" s="17"/>
       <c r="AC3" t="s">
@@ -7132,9 +7140,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>348</v>
+        <v>500</v>
       </c>
       <c r="D4" t="s">
         <v>330</v>
@@ -7146,10 +7154,10 @@
         <v>160</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>334</v>
+        <v>501</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>329</v>
+        <v>502</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
@@ -7164,11 +7172,8 @@
       <c r="Q4" s="29">
         <v>4242424242424240</v>
       </c>
-      <c r="R4" s="29" t="s">
-        <v>349</v>
-      </c>
-      <c r="S4">
-        <v>120</v>
+      <c r="R4" s="7" t="s">
+        <v>491</v>
       </c>
       <c r="T4" t="s">
         <v>396</v>
@@ -7176,8 +7181,23 @@
       <c r="V4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="AC4" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE4" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF4">
+        <v>9898989898</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7211,8 +7231,8 @@
       <c r="Q5">
         <v>4242424242424240</v>
       </c>
-      <c r="R5" t="s">
-        <v>349</v>
+      <c r="R5" s="7" t="s">
+        <v>491</v>
       </c>
       <c r="S5" s="17"/>
       <c r="T5" t="s">
@@ -7235,8 +7255,8 @@
       <c r="AD5" t="s">
         <v>333</v>
       </c>
-      <c r="AE5">
-        <v>6492</v>
+      <c r="AE5" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="AF5">
         <v>9898989898</v>
@@ -7245,7 +7265,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>424</v>
       </c>
@@ -7286,7 +7306,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>425</v>
       </c>
@@ -7322,7 +7342,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>436</v>
       </c>
@@ -7353,7 +7373,7 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>443</v>
       </c>
@@ -7364,7 +7384,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>398</v>
       </c>
@@ -7389,7 +7409,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>447</v>
       </c>
@@ -7415,7 +7435,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>413</v>
       </c>
@@ -7440,6 +7460,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="R3" r:id="rId1" xr:uid="{78410139-3F4D-4B6F-9F04-D94F482B4A40}"/>
+    <hyperlink ref="R5" r:id="rId2" xr:uid="{C0F1BA52-3CB2-47A4-B221-25770F0B26EB}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{9B481B38-4CD2-49A3-A338-E5214B346491}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7448,26 +7473,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7601,7 +7626,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7649,7 +7674,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -7703,7 +7728,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>398</v>
       </c>
@@ -7723,7 +7748,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7743,7 +7768,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>400</v>
       </c>
@@ -7769,7 +7794,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -7792,7 +7817,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -7815,7 +7840,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>499</v>
       </c>
@@ -7823,7 +7848,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
@@ -7844,14 +7869,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="8" width="20.88671875" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8225,7 +8250,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8305,7 +8330,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -8328,7 +8353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8352,7 +8377,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>381</v>
       </c>
@@ -8415,7 +8440,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>383</v>
       </c>
@@ -8436,7 +8461,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>385</v>
       </c>
@@ -8452,7 +8477,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -8460,7 +8485,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>386</v>
       </c>
@@ -8475,7 +8500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>312</v>
       </c>
@@ -8486,7 +8511,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
       <c r="DO11" s="17"/>
     </row>
   </sheetData>
@@ -8502,9 +8527,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8608,7 +8633,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8622,7 +8647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8702,7 +8727,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -8734,7 +8759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -8766,7 +8791,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -8798,7 +8823,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -8806,7 +8831,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -8817,7 +8842,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Assert condition chnge for admin testcase Signin method
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86DF4DA-5A12-413F-A682-CC33FCBD8C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E86DF4DA-5A12-413F-A682-CC33FCBD8C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{305FDFE0-BB9A-4538-9842-A78D817E0DB6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14685" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="503">
   <si>
     <t>DataSet</t>
   </si>
@@ -2027,62 +2027,62 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.88671875" customWidth="1"/>
-    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -2382,13 +2382,13 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -3047,16 +3047,16 @@
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3236,7 +3236,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3496,22 +3496,22 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3558,12 +3558,12 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -3633,14 +3633,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.88671875" customWidth="1"/>
-    <col min="13" max="13" width="44.5546875" customWidth="1"/>
-    <col min="14" max="14" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="13" max="13" width="44.5703125" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>363</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>388</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>464</v>
       </c>
@@ -3951,22 +3951,22 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -4210,43 +4210,43 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.109375" customWidth="1"/>
-    <col min="29" max="29" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" customWidth="1"/>
+    <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.44140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4487,7 +4487,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="AO3" s="2"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5346,14 +5346,14 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>409</v>
       </c>
@@ -5853,12 +5853,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6229,7 +6229,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -6629,20 +6629,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" customWidth="1"/>
-    <col min="10" max="10" width="31.88671875" customWidth="1"/>
-    <col min="14" max="14" width="28.109375" customWidth="1"/>
-    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -6866,26 +6866,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="13" max="13" width="35.88671875" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.109375" customWidth="1"/>
-    <col min="23" max="23" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="35.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>500</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>424</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>425</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>436</v>
       </c>
@@ -7373,7 +7373,7 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>443</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>398</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>447</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>413</v>
       </c>
@@ -7473,26 +7473,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" customWidth="1"/>
-    <col min="20" max="20" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>398</v>
       </c>
@@ -7744,11 +7744,14 @@
       <c r="I4" t="s">
         <v>404</v>
       </c>
+      <c r="J4" s="21" t="s">
+        <v>498</v>
+      </c>
       <c r="T4" s="7" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7768,7 +7771,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>400</v>
       </c>
@@ -7794,7 +7797,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -7817,7 +7820,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -7840,7 +7843,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>499</v>
       </c>
@@ -7848,7 +7851,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
@@ -7869,14 +7872,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="8" width="20.88671875" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="8" width="20.85546875" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8250,7 +8253,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8330,7 +8333,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -8353,7 +8356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8377,7 +8380,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>381</v>
       </c>
@@ -8440,7 +8443,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>383</v>
       </c>
@@ -8461,7 +8464,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>385</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>386</v>
       </c>
@@ -8500,7 +8503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>312</v>
       </c>
@@ -8511,7 +8514,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
       <c r="DO11" s="17"/>
     </row>
   </sheetData>
@@ -8527,9 +8530,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8647,7 +8650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8727,7 +8730,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -8759,7 +8762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -8791,7 +8794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -8823,7 +8826,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -8831,7 +8834,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -8842,7 +8845,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin 35 testcase updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E57782-B8C6-4896-826E-25FE4616DD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="10230" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="529">
   <si>
     <t>DataSet</t>
   </si>
@@ -1340,9 +1340,6 @@
     <t>Lotus$mk2022</t>
   </si>
   <si>
-    <t>Ackpgkyatnob4!</t>
-  </si>
-  <si>
     <t>HFProducts</t>
   </si>
   <si>
@@ -1499,9 +1496,6 @@
     <t>32480,11234000</t>
   </si>
   <si>
-    <t>59.99,19.99</t>
-  </si>
-  <si>
     <t>Qatestvalueprop</t>
   </si>
   <si>
@@ -1557,6 +1551,75 @@
   </si>
   <si>
     <t>Drybar_PageTitle</t>
+  </si>
+  <si>
+    <t>rbogi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Ramya@1234</t>
+  </si>
+  <si>
+    <t>3118700,11234000</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>GRASUSWebsite</t>
+  </si>
+  <si>
+    <t>OXOSKU</t>
+  </si>
+  <si>
+    <t>HFSKU</t>
+  </si>
+  <si>
+    <t>OSPSKU</t>
+  </si>
+  <si>
+    <t>DRYSKU</t>
+  </si>
+  <si>
+    <t>TT32PS474,S18SX001</t>
+  </si>
+  <si>
+    <t>10005241,10006005</t>
+  </si>
+  <si>
+    <t>900-2230-1,900-2225-4</t>
+  </si>
+  <si>
+    <t>DRYStore</t>
+  </si>
+  <si>
+    <t>OSPStore</t>
+  </si>
+  <si>
+    <t>HFStore</t>
+  </si>
+  <si>
+    <t>OXOStore</t>
+  </si>
+  <si>
+    <t>Drybar Store View</t>
+  </si>
+  <si>
+    <t>Osprey US English</t>
+  </si>
+  <si>
+    <t>DRYWebsite</t>
+  </si>
+  <si>
+    <t>OSPWebsite</t>
+  </si>
+  <si>
+    <t>Drybar Website</t>
+  </si>
+  <si>
+    <t>Osprey US</t>
+  </si>
+  <si>
+    <t>araikanti@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -2045,66 +2108,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.88671875" customWidth="1"/>
+    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.88671875" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2205,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>39</v>
@@ -2187,7 +2250,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2204,7 +2267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2230,13 +2293,13 @@
         <v>17</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>40</v>
@@ -2278,7 +2341,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2310,7 +2373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2342,7 +2405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2374,7 +2437,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -2404,14 +2467,13 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="78" max="78" width="8.85546875"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2644,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="CA1" s="1" t="s">
         <v>39</v>
@@ -2710,7 +2772,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2777,13 +2839,13 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>284</v>
       </c>
       <c r="L3" s="2"/>
       <c r="Q3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2818,13 +2880,13 @@
       </c>
       <c r="BW3" s="10"/>
       <c r="BX3" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="BY3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="BZ3" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="CA3" s="2" t="s">
         <v>40</v>
@@ -2860,7 +2922,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2874,7 +2936,7 @@
         <v>290</v>
       </c>
       <c r="BQ4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="BU4" s="2" t="s">
         <v>132</v>
@@ -2910,7 +2972,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -3001,7 +3063,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -3015,7 +3077,7 @@
         <v>299</v>
       </c>
       <c r="BQ6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="BU6" s="2" t="s">
         <v>300</v>
@@ -3070,16 +3132,16 @@
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3201,7 +3263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3218,7 +3280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3259,7 +3321,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3297,7 +3359,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3305,7 +3367,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3316,7 +3378,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3331,7 +3393,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3353,7 +3415,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3378,7 +3440,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3401,7 +3463,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3455,7 +3517,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3482,7 +3544,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3519,22 +3581,22 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3570,23 +3632,23 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" t="s">
         <v>455</v>
       </c>
-      <c r="C2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3612,7 +3674,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3635,9 +3697,9 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K6" t="s">
         <v>411</v>
@@ -3652,30 +3714,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="13" max="13" width="44.5703125" customWidth="1"/>
-    <col min="14" max="16" width="41.140625" customWidth="1"/>
-    <col min="17" max="17" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+    <col min="13" max="13" width="44.5546875" customWidth="1"/>
+    <col min="14" max="16" width="41.109375" customWidth="1"/>
+    <col min="17" max="17" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3716,13 +3778,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>39</v>
@@ -3752,7 +3814,7 @@
         <v>5</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>227</v>
@@ -3761,42 +3823,42 @@
         <v>369</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>270</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>212</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" t="s">
         <v>455</v>
       </c>
-      <c r="C2" t="s">
-        <v>456</v>
-      </c>
       <c r="V2" s="35" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="X2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -3816,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>363</v>
       </c>
@@ -3842,7 +3904,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -3861,7 +3923,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3869,7 +3931,7 @@
         <v>141</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -3880,7 +3942,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -3900,7 +3962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -3920,7 +3982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3928,10 +3990,10 @@
         <v>228</v>
       </c>
       <c r="X9" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -3942,10 +4004,10 @@
         <v>40</v>
       </c>
       <c r="O10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="Q10" t="s">
         <v>40</v>
@@ -3954,21 +4016,21 @@
         <v>238</v>
       </c>
       <c r="Y10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>388</v>
       </c>
       <c r="Z11" s="35" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="AA11" s="35" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -3976,30 +4038,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AC13" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="V14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="W14">
         <v>10</v>
       </c>
       <c r="X14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4022,22 +4084,22 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="48.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4081,7 +4143,7 @@
         <v>395</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>181</v>
@@ -4150,15 +4212,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="32">
@@ -4183,7 +4245,7 @@
         <v>229</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AF2" t="s">
         <v>230</v>
@@ -4204,7 +4266,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -4242,13 +4304,13 @@
         <v>396</v>
       </c>
       <c r="O3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="P3" t="s">
         <v>243</v>
       </c>
       <c r="U3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="V3" t="s">
         <v>333</v>
@@ -4281,43 +4343,43 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" customWidth="1"/>
-    <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.109375" customWidth="1"/>
+    <col min="29" max="29" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4508,7 +4570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4558,7 +4620,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -4610,7 +4672,7 @@
       </c>
       <c r="AO3" s="2"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4685,7 +4747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -4821,7 +4883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -4946,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5079,7 +5141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -5170,7 +5232,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -5278,7 +5340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -5369,7 +5431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5413,18 +5475,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CY4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5498,7 +5560,7 @@
         <v>58</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>23</v>
@@ -5576,7 +5638,7 @@
         <v>82</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>5</v>
@@ -5666,7 +5728,7 @@
         <v>10</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="CD1" s="1" t="s">
         <v>39</v>
@@ -5735,7 +5797,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -5759,10 +5821,10 @@
         <v>114</v>
       </c>
       <c r="V2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>320</v>
@@ -5794,7 +5856,7 @@
       </c>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AZ2" t="s">
         <v>201</v>
@@ -5826,7 +5888,7 @@
         <v>18</v>
       </c>
       <c r="CC2" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="CD2" s="2" t="s">
         <v>40</v>
@@ -5883,7 +5945,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -5894,7 +5956,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>409</v>
       </c>
@@ -5924,12 +5986,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6234,7 +6296,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6300,7 +6362,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6442,7 +6504,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6507,7 +6569,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6563,7 +6625,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -6700,20 +6762,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="14" max="14" width="28.109375" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6799,7 +6861,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6846,7 +6908,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -6884,7 +6946,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -6901,7 +6963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6909,15 +6971,15 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>391</v>
       </c>
       <c r="AB6" s="17" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -6935,28 +6997,34 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:AT12"/>
+  <dimension ref="A1:BF12"/>
   <sheetViews>
-    <sheetView topLeftCell="X4" workbookViewId="0">
-      <selection sqref="A1:AT12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.140625" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="18.109375" customWidth="1"/>
+    <col min="23" max="23" width="11.5546875" customWidth="1"/>
+    <col min="47" max="49" width="30.44140625" customWidth="1"/>
+    <col min="51" max="53" width="18.6640625" customWidth="1"/>
+    <col min="54" max="54" width="16.44140625" customWidth="1"/>
+    <col min="55" max="55" width="17.109375" customWidth="1"/>
+    <col min="56" max="56" width="16" customWidth="1"/>
+    <col min="57" max="57" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6979,7 +7047,7 @@
         <v>326</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>415</v>
@@ -7095,16 +7163,52 @@
       <c r="AT1" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU1" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C2" t="s">
-        <v>435</v>
+        <v>506</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>507</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
@@ -7156,8 +7260,12 @@
       <c r="AT2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="21"/>
+      <c r="AX2" s="21"/>
+    </row>
+    <row r="3" spans="1:58" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -7210,8 +7318,12 @@
       <c r="AG3" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+      <c r="AU3" s="21"/>
+      <c r="AV3" s="21"/>
+      <c r="AW3" s="21"/>
+      <c r="AX3" s="21"/>
+    </row>
+    <row r="4" spans="1:58" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -7255,10 +7367,23 @@
       <c r="V4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="AU4" s="21"/>
+      <c r="AV4" s="21"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="21"/>
+      <c r="BB4" t="s">
+        <v>396</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>526</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>399</v>
+        <v>510</v>
       </c>
       <c r="D5" t="s">
         <v>330</v>
@@ -7275,7 +7400,7 @@
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="21" t="s">
-        <v>487</v>
+        <v>508</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
@@ -7290,8 +7415,8 @@
       <c r="Q5">
         <v>4242424242424240</v>
       </c>
-      <c r="R5" t="s">
-        <v>349</v>
+      <c r="R5" s="7" t="s">
+        <v>528</v>
       </c>
       <c r="S5" s="17"/>
       <c r="T5" t="s">
@@ -7301,8 +7426,8 @@
       <c r="V5" t="s">
         <v>428</v>
       </c>
-      <c r="W5" t="s">
-        <v>431</v>
+      <c r="W5" s="17" t="s">
+        <v>509</v>
       </c>
       <c r="Y5" t="s">
         <v>432</v>
@@ -7323,15 +7448,51 @@
       <c r="AG5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="AU5" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="AV5" s="21" t="s">
+        <v>515</v>
+      </c>
+      <c r="AW5" s="21" t="s">
+        <v>516</v>
+      </c>
+      <c r="AX5" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="AY5" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="AZ5" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="BA5" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>397</v>
+      </c>
+      <c r="BC5" s="17" t="s">
+        <v>526</v>
+      </c>
+      <c r="BD5" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="BE5" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>424</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
@@ -7356,23 +7517,36 @@
         <v>428</v>
       </c>
       <c r="W6" s="17" t="s">
-        <v>488</v>
+        <v>509</v>
       </c>
       <c r="Y6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AA6" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="AU6" s="21"/>
+      <c r="AV6" s="21"/>
+      <c r="AW6" s="21"/>
+      <c r="AX6" s="21"/>
+      <c r="AY6" s="17"/>
+      <c r="AZ6" s="17"/>
+      <c r="BA6" s="17"/>
+      <c r="BB6" t="s">
+        <v>397</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>425</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
@@ -7400,13 +7574,23 @@
       <c r="AA7" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU7" s="21"/>
+      <c r="AV7" s="21"/>
+      <c r="AW7" s="21"/>
+      <c r="AX7" s="21"/>
+      <c r="AY7" s="17"/>
+      <c r="AZ7" s="17"/>
+      <c r="BA7" s="17"/>
+      <c r="BC7" s="17"/>
+      <c r="BD7" s="17"/>
+      <c r="BE7" s="17"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>435</v>
+      </c>
+      <c r="G8" t="s">
         <v>436</v>
-      </c>
-      <c r="G8" t="s">
-        <v>437</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -7415,35 +7599,35 @@
         <v>379</v>
       </c>
       <c r="J8" t="s">
+        <v>437</v>
+      </c>
+      <c r="K8" t="s">
         <v>438</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>439</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>440</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>441</v>
-      </c>
-      <c r="N8" t="s">
-        <v>442</v>
       </c>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>442</v>
+      </c>
+      <c r="W9" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="AA9" t="s">
         <v>443</v>
       </c>
-      <c r="W9" s="17" t="s">
-        <v>448</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>398</v>
       </c>
@@ -7467,10 +7651,13 @@
       <c r="U10" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="BB10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D11" t="s">
         <v>330</v>
@@ -7494,7 +7681,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>413</v>
       </c>
@@ -7519,6 +7706,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{73C9E29E-98A4-4FB1-9749-39723AE24DE5}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{3BCCFF1E-72A1-48D2-9EB3-32FE566289D6}"/>
+    <hyperlink ref="R5" r:id="rId3" xr:uid="{AAD3F1DA-E08F-4F81-8FC2-43761D991A76}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7527,26 +7719,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR10"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7680,15 +7872,15 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="S2" s="8"/>
       <c r="T2" t="s">
@@ -7728,7 +7920,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -7746,7 +7938,7 @@
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="21" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -7782,7 +7974,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>398</v>
       </c>
@@ -7802,7 +7994,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7822,7 +8014,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>400</v>
       </c>
@@ -7836,7 +8028,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="T6" t="s">
         <v>394</v>
@@ -7848,7 +8040,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -7862,16 +8054,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="T7" t="s">
         <v>394</v>
       </c>
       <c r="U7" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -7894,15 +8086,15 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H9" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
     </row>
@@ -7919,18 +8111,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6850E244-5F78-40CC-8B1C-BFED15554E14}">
   <dimension ref="A1:DT11"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="8" width="20.88671875" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8217,7 +8409,7 @@
         <v>9</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>39</v>
@@ -8304,15 +8496,15 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>324</v>
+        <v>506</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>435</v>
+        <v>507</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>325</v>
@@ -8321,7 +8513,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G2" t="s">
         <v>283</v>
@@ -8342,7 +8534,7 @@
         <v>344</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="O2" s="17">
         <v>100</v>
@@ -8378,13 +8570,13 @@
         <v>251</v>
       </c>
       <c r="CR2" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CS2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -8401,13 +8593,13 @@
         <v>40</v>
       </c>
       <c r="CR3" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="CS3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8431,7 +8623,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>381</v>
       </c>
@@ -8473,7 +8665,7 @@
         <v>330</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="U5" t="s">
         <v>160</v>
@@ -8494,7 +8686,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>383</v>
       </c>
@@ -8515,7 +8707,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>385</v>
       </c>
@@ -8531,20 +8723,20 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>355</v>
       </c>
       <c r="N8" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>386</v>
       </c>
       <c r="I9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J9" t="s">
         <v>387</v>
@@ -8554,21 +8746,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>312</v>
       </c>
       <c r="CR10" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CS10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
       <c r="DO11" s="17"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6F88B7CB-0100-41A9-9C9F-6497BE92D740}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{C7BB2632-04D3-45FE-B954-C8330330E816}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8581,9 +8777,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8666,7 +8862,7 @@
         <v>5</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>56</v>
@@ -8687,21 +8883,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" t="s">
         <v>450</v>
-      </c>
-      <c r="C2" t="s">
-        <v>451</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8712,7 +8908,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -8781,7 +8977,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -8813,7 +9009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -8845,7 +9041,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -8877,7 +9073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -8885,18 +9081,18 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>460</v>
+      </c>
+      <c r="AA8" t="s">
         <v>461</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AE8" t="s">
         <v>462</v>
       </c>
-      <c r="AE8" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Admin 003 Testcase testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BF89C7F-CE08-47E8-B756-7A0251A8B85C}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E3E19E8-7FC6-421D-AA11-7DA85AB7824C}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2355" windowWidth="21600" windowHeight="11325" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="519">
   <si>
     <t>DataSet</t>
   </si>
@@ -1587,6 +1587,9 @@
   </si>
   <si>
     <t>OSP-EMEA_Store</t>
+  </si>
+  <si>
+    <t>Hydroflask Website,OXO Website,Osprey US,Drybar Website</t>
   </si>
 </sst>
 </file>
@@ -3107,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3116,6 +3119,7 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="56" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3531,7 +3535,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" t="s">
-        <v>283</v>
+        <v>518</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>
@@ -7568,7 +7572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F259D-AD55-4F7C-B532-04C9DE6174AC}">
   <dimension ref="A1:AR14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Admin 03 testcase testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E3E19E8-7FC6-421D-AA11-7DA85AB7824C}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CB7027-0E04-4BBE-B6D6-EF3399D5F275}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3119,7 +3119,7 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
22 magento testcase changes for all websites
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{CEB50112-8E2C-4B04-8806-6FAE7B4F1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CB7027-0E04-4BBE-B6D6-EF3399D5F275}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB2B28C-12D3-4DEF-B13A-1920A8763D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="522">
   <si>
     <t>DataSet</t>
   </si>
@@ -1590,6 +1590,15 @@
   </si>
   <si>
     <t>Hydroflask Website,OXO Website,Osprey US,Drybar Website</t>
+  </si>
+  <si>
+    <t>HYFWebsite</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>S18SX001,LW24LW080</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1802,6 +1811,18 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1818,10 +1839,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3110,7 +3127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -6980,10 +6997,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:AT12"/>
+  <dimension ref="A1:AT13"/>
   <sheetViews>
-    <sheetView topLeftCell="X4" workbookViewId="0">
-      <selection sqref="A1:AT12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +7014,10 @@
     <col min="13" max="13" width="35.85546875" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
     <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="18.140625" customWidth="1"/>
+    <col min="16" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7301,77 +7321,103 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>399</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="5" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="E5" t="s">
-        <v>430</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>429</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="21" t="s">
-        <v>487</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="31">
+      <c r="G5" s="39" t="s">
+        <v>520</v>
+      </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="43">
         <v>44862</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="42">
         <v>123</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="42">
         <v>4242424242424240</v>
       </c>
-      <c r="R5" t="s">
-        <v>349</v>
-      </c>
-      <c r="S5" s="17"/>
-      <c r="T5" t="s">
-        <v>397</v>
-      </c>
-      <c r="U5" s="17"/>
-      <c r="V5" t="s">
-        <v>428</v>
-      </c>
-      <c r="W5" t="s">
-        <v>431</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>432</v>
-      </c>
-      <c r="AA5" s="17"/>
-      <c r="AC5" t="s">
+      <c r="R5" s="38" t="s">
+        <v>491</v>
+      </c>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="AE5">
-        <v>6492</v>
-      </c>
-      <c r="AF5">
+      <c r="AE5" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF5" s="37">
         <v>9898989898</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" s="37" t="s">
         <v>246</v>
       </c>
+      <c r="AH5" s="37"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="37"/>
+      <c r="AO5" s="37"/>
+      <c r="AP5" s="37"/>
+      <c r="AQ5" s="37"/>
+      <c r="AR5" s="37"/>
+      <c r="AS5" s="37"/>
+      <c r="AT5" s="37"/>
     </row>
     <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>399</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>430</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>429</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -7381,38 +7427,53 @@
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="7"/>
+      <c r="N6" s="23"/>
       <c r="O6" s="31">
-        <v>44863</v>
+        <v>44862</v>
       </c>
       <c r="P6">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q6">
         <v>4242424242424240</v>
       </c>
-      <c r="R6" t="s">
-        <v>349</v>
+      <c r="R6" s="45" t="s">
+        <v>491</v>
       </c>
       <c r="S6" s="17"/>
       <c r="T6" t="s">
         <v>397</v>
       </c>
+      <c r="U6" s="17"/>
       <c r="V6" t="s">
         <v>428</v>
       </c>
-      <c r="W6" s="17" t="s">
-        <v>488</v>
+      <c r="W6" t="s">
+        <v>431</v>
       </c>
       <c r="Y6" t="s">
-        <v>446</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>431</v>
+        <v>432</v>
+      </c>
+      <c r="AA6" s="17"/>
+      <c r="AC6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE6">
+        <v>6492</v>
+      </c>
+      <c r="AF6">
+        <v>9898989898</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
@@ -7422,11 +7483,11 @@
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="7"/>
-      <c r="O7" s="34">
-        <v>44864</v>
+      <c r="O7" s="31">
+        <v>44863</v>
       </c>
       <c r="P7">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q7">
         <v>4242424242424240</v>
@@ -7435,135 +7496,180 @@
         <v>349</v>
       </c>
       <c r="S7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="W7" s="17">
+      <c r="T7" t="s">
+        <v>397</v>
+      </c>
+      <c r="V7" t="s">
+        <v>428</v>
+      </c>
+      <c r="W7" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>425</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="7"/>
+      <c r="O8" s="34">
+        <v>44864</v>
+      </c>
+      <c r="P8">
+        <v>125</v>
+      </c>
+      <c r="Q8">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R8" t="s">
+        <v>349</v>
+      </c>
+      <c r="S8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="W8" s="17">
         <v>7</v>
       </c>
-      <c r="Y7">
+      <c r="Y8">
         <v>12.95</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA8" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>436</v>
-      </c>
-      <c r="G8" t="s">
-        <v>437</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="J8" t="s">
-        <v>438</v>
-      </c>
-      <c r="K8" t="s">
-        <v>439</v>
-      </c>
-      <c r="L8" t="s">
-        <v>440</v>
-      </c>
-      <c r="M8" t="s">
-        <v>441</v>
-      </c>
-      <c r="N8" t="s">
-        <v>442</v>
-      </c>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>443</v>
-      </c>
-      <c r="W9" s="17" t="s">
-        <v>448</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>444</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="G9" t="s">
+        <v>437</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="J9" t="s">
+        <v>438</v>
+      </c>
+      <c r="K9" t="s">
+        <v>439</v>
+      </c>
+      <c r="L9" t="s">
+        <v>440</v>
+      </c>
+      <c r="M9" t="s">
+        <v>441</v>
+      </c>
+      <c r="N9" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>398</v>
-      </c>
-      <c r="D10" t="s">
-        <v>241</v>
-      </c>
-      <c r="F10" t="s">
-        <v>288</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="M10" s="7"/>
-      <c r="O10" s="23"/>
-      <c r="R10" t="s">
-        <v>394</v>
-      </c>
-      <c r="T10" t="s">
-        <v>396</v>
-      </c>
-      <c r="U10" t="s">
-        <v>404</v>
+        <v>443</v>
+      </c>
+      <c r="W10" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="D11" t="s">
-        <v>330</v>
-      </c>
-      <c r="E11" t="s">
-        <v>430</v>
+        <v>241</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
-      </c>
-      <c r="O11" s="34">
-        <v>44862</v>
-      </c>
-      <c r="P11">
-        <v>123</v>
-      </c>
-      <c r="Q11">
-        <v>4242424242424240</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="O11" s="23"/>
       <c r="R11" t="s">
-        <v>349</v>
+        <v>394</v>
+      </c>
+      <c r="T11" t="s">
+        <v>396</v>
+      </c>
+      <c r="U11" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>447</v>
+      </c>
+      <c r="D12" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12" t="s">
+        <v>430</v>
+      </c>
+      <c r="F12" t="s">
+        <v>160</v>
+      </c>
+      <c r="O12" s="34">
+        <v>44862</v>
+      </c>
+      <c r="P12">
+        <v>123</v>
+      </c>
+      <c r="Q12">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R12" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>413</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I13" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>32480</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>419</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>423</v>
       </c>
-      <c r="N12">
+      <c r="N13">
         <v>61132300</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="R5" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="R6" r:id="rId2" xr:uid="{D744BE2B-C64A-4C73-8428-F9F807BCE02C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
helper and excel changes for Admin testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB2B28C-12D3-4DEF-B13A-1920A8763D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C42C58-20A8-4F98-80D6-4A7C2F959ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="530">
   <si>
     <t>DataSet</t>
   </si>
@@ -1599,6 +1599,30 @@
   </si>
   <si>
     <t>S18SX001,LW24LW080</t>
+  </si>
+  <si>
+    <t>DRYWebsite</t>
+  </si>
+  <si>
+    <t>900-3785-1,900-2230-1</t>
+  </si>
+  <si>
+    <t>Drybar Website</t>
+  </si>
+  <si>
+    <t>OpsreyUSWebsite</t>
+  </si>
+  <si>
+    <t>Osprey US</t>
+  </si>
+  <si>
+    <t>10004460,10005241</t>
+  </si>
+  <si>
+    <t>Osprey US English</t>
+  </si>
+  <si>
+    <t>habogi@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -1755,7 +1779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1811,18 +1835,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2110,62 +2122,62 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.88671875" customWidth="1"/>
+    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.88671875" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2265,7 +2277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2339,7 +2351,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2403,7 +2415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2435,7 +2447,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -2465,14 +2477,13 @@
       <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="78" max="78" width="8.85546875"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2771,7 +2782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2838,7 +2849,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -2921,7 +2932,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2971,7 +2982,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -3062,7 +3073,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -3131,17 +3142,17 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="38.33203125" customWidth="1"/>
     <col min="13" max="14" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3280,7 +3291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3321,7 +3332,7 @@
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -3359,7 +3370,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -3367,7 +3378,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -3378,7 +3389,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -3393,7 +3404,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>265</v>
       </c>
@@ -3415,7 +3426,7 @@
       </c>
       <c r="AL8" s="13"/>
     </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>270</v>
       </c>
@@ -3440,7 +3451,7 @@
       </c>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -3463,7 +3474,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>278</v>
       </c>
@@ -3517,7 +3528,7 @@
       <c r="AM11" s="19"/>
       <c r="AN11" s="19"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>280</v>
       </c>
@@ -3544,7 +3555,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>282</v>
       </c>
@@ -3581,22 +3592,22 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3632,7 +3643,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3643,12 +3654,12 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -3674,7 +3685,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -3697,7 +3708,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>457</v>
       </c>
@@ -3718,26 +3729,26 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="13" max="13" width="44.5703125" customWidth="1"/>
-    <col min="14" max="16" width="41.140625" customWidth="1"/>
-    <col min="17" max="17" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+    <col min="13" max="13" width="44.5546875" customWidth="1"/>
+    <col min="14" max="16" width="41.109375" customWidth="1"/>
+    <col min="17" max="17" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3841,7 +3852,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3858,7 +3869,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -3878,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>363</v>
       </c>
@@ -3904,7 +3915,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -3923,7 +3934,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3942,7 +3953,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -3962,7 +3973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -3982,7 +3993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3993,7 +4004,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -4019,7 +4030,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>388</v>
       </c>
@@ -4030,7 +4041,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -4038,7 +4049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>464</v>
       </c>
@@ -4046,7 +4057,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>500</v>
       </c>
@@ -4084,22 +4095,22 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="48.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4223,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4266,7 +4277,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -4343,43 +4354,43 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" customWidth="1"/>
-    <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.109375" customWidth="1"/>
+    <col min="29" max="29" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="49.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4570,7 +4581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4620,7 +4631,7 @@
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -4672,7 +4683,7 @@
       </c>
       <c r="AO3" s="2"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4747,7 +4758,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -4883,7 +4894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -5008,7 +5019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5141,7 +5152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -5232,7 +5243,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -5340,7 +5351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -5431,7 +5442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5479,14 +5490,14 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5797,7 +5808,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -5945,7 +5956,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -5956,7 +5967,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>409</v>
       </c>
@@ -5986,12 +5997,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6296,7 +6307,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6362,7 +6373,7 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:101" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -6504,7 +6515,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -6569,7 +6580,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -6625,7 +6636,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>197</v>
       </c>
@@ -6762,20 +6773,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="14" max="14" width="28.109375" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6861,7 +6872,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -6908,7 +6919,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>234</v>
       </c>
@@ -6946,7 +6957,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>237</v>
       </c>
@@ -6963,7 +6974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6971,7 +6982,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -6979,7 +6990,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -6997,31 +7008,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:AT13"/>
+  <dimension ref="A1:AT15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.109375" customWidth="1"/>
+    <col min="18" max="18" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7161,7 +7172,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7222,7 +7233,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -7276,7 +7287,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -7321,108 +7332,81 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>519</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37" t="s">
+    <row r="5" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>522</v>
+      </c>
+      <c r="D5" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" t="s">
         <v>332</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="40" t="s">
-        <v>521</v>
-      </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="43">
+      <c r="J5" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="31">
         <v>44862</v>
       </c>
-      <c r="P5" s="42">
+      <c r="P5" s="29">
         <v>123</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="Q5" s="29">
         <v>4242424242424240</v>
       </c>
-      <c r="R5" s="38" t="s">
-        <v>491</v>
-      </c>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37" t="s">
-        <v>396</v>
-      </c>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="37"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37" t="s">
+      <c r="R5" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="T5" t="s">
+        <v>508</v>
+      </c>
+      <c r="V5" t="s">
+        <v>524</v>
+      </c>
+      <c r="AC5" t="s">
         <v>251</v>
       </c>
-      <c r="AD5" s="37" t="s">
+      <c r="AD5" t="s">
         <v>333</v>
       </c>
-      <c r="AE5" s="39" t="s">
+      <c r="AE5" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="AF5" s="37">
+      <c r="AF5">
         <v>9898989898</v>
       </c>
-      <c r="AG5" s="37" t="s">
+      <c r="AG5" t="s">
         <v>246</v>
       </c>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="37"/>
-      <c r="AL5" s="37"/>
-      <c r="AM5" s="37"/>
-      <c r="AN5" s="37"/>
-      <c r="AO5" s="37"/>
-      <c r="AP5" s="37"/>
-      <c r="AQ5" s="37"/>
-      <c r="AR5" s="37"/>
-      <c r="AS5" s="37"/>
-      <c r="AT5" s="37"/>
-    </row>
-    <row r="6" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>399</v>
-      </c>
-      <c r="D6" s="44" t="s">
+        <v>525</v>
+      </c>
+      <c r="D6" t="s">
         <v>330</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>430</v>
-      </c>
-      <c r="F6" s="44" t="s">
+      <c r="E6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F6" t="s">
         <v>160</v>
       </c>
-      <c r="G6" s="46" t="s">
-        <v>429</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="G6" s="17" t="s">
+        <v>520</v>
+      </c>
       <c r="J6" s="21" t="s">
-        <v>487</v>
+        <v>527</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
@@ -7431,38 +7415,29 @@
       <c r="O6" s="31">
         <v>44862</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="29">
         <v>123</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="29">
         <v>4242424242424240</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="S6" s="17"/>
       <c r="T6" t="s">
-        <v>397</v>
-      </c>
-      <c r="U6" s="17"/>
+        <v>528</v>
+      </c>
       <c r="V6" t="s">
-        <v>428</v>
-      </c>
-      <c r="W6" t="s">
-        <v>431</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>432</v>
-      </c>
-      <c r="AA6" s="17"/>
+        <v>526</v>
+      </c>
       <c r="AC6" t="s">
         <v>251</v>
       </c>
       <c r="AD6" t="s">
         <v>333</v>
       </c>
-      <c r="AE6">
-        <v>6492</v>
+      <c r="AE6" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="AF6">
         <v>9898989898</v>
@@ -7471,50 +7446,78 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>424</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+        <v>519</v>
+      </c>
+      <c r="D7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" t="s">
+        <v>332</v>
+      </c>
+      <c r="F7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>520</v>
+      </c>
       <c r="J7" s="21" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="7"/>
+      <c r="N7" s="23"/>
       <c r="O7" s="31">
-        <v>44863</v>
-      </c>
-      <c r="P7">
-        <v>124</v>
-      </c>
-      <c r="Q7">
+        <v>44862</v>
+      </c>
+      <c r="P7" s="29">
+        <v>123</v>
+      </c>
+      <c r="Q7" s="29">
         <v>4242424242424240</v>
       </c>
-      <c r="R7" t="s">
-        <v>349</v>
-      </c>
-      <c r="S7" s="17"/>
+      <c r="R7" s="7" t="s">
+        <v>491</v>
+      </c>
       <c r="T7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="V7" t="s">
-        <v>428</v>
-      </c>
-      <c r="W7" s="17" t="s">
-        <v>488</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>446</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE7" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF7">
+        <v>9898989898</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>399</v>
+      </c>
+      <c r="D8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" t="s">
+        <v>430</v>
+      </c>
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>429</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
@@ -7524,151 +7527,250 @@
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="7"/>
-      <c r="O8" s="34">
-        <v>44864</v>
+      <c r="N8" s="23"/>
+      <c r="O8" s="31">
+        <v>44862</v>
       </c>
       <c r="P8">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q8">
         <v>4242424242424240</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="S8" s="17"/>
+      <c r="T8" t="s">
+        <v>397</v>
+      </c>
+      <c r="U8" s="17"/>
+      <c r="V8" t="s">
+        <v>428</v>
+      </c>
+      <c r="W8" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA8" s="17"/>
+      <c r="AC8" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE8">
+        <v>6492</v>
+      </c>
+      <c r="AF8">
+        <v>9898989898</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="7"/>
+      <c r="O9" s="31">
+        <v>44863</v>
+      </c>
+      <c r="P9">
+        <v>124</v>
+      </c>
+      <c r="Q9">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R9" t="s">
         <v>349</v>
       </c>
-      <c r="S8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="W8" s="17">
+      <c r="S9" s="17"/>
+      <c r="T9" t="s">
+        <v>397</v>
+      </c>
+      <c r="V9" t="s">
+        <v>428</v>
+      </c>
+      <c r="W9" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="7"/>
+      <c r="O10" s="34">
+        <v>44864</v>
+      </c>
+      <c r="P10">
+        <v>125</v>
+      </c>
+      <c r="Q10">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R10" t="s">
+        <v>349</v>
+      </c>
+      <c r="S10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="W10" s="17">
         <v>7</v>
       </c>
-      <c r="Y8">
+      <c r="Y10">
         <v>12.95</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA10" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>436</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G11" t="s">
         <v>437</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="J9" t="s">
-        <v>438</v>
-      </c>
-      <c r="K9" t="s">
-        <v>439</v>
-      </c>
-      <c r="L9" t="s">
-        <v>440</v>
-      </c>
-      <c r="M9" t="s">
-        <v>441</v>
-      </c>
-      <c r="N9" t="s">
-        <v>442</v>
-      </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>443</v>
-      </c>
-      <c r="W10" s="17" t="s">
-        <v>448</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" t="s">
-        <v>241</v>
-      </c>
-      <c r="F11" t="s">
-        <v>288</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
-      <c r="M11" s="7"/>
-      <c r="O11" s="23"/>
-      <c r="R11" t="s">
-        <v>394</v>
-      </c>
-      <c r="T11" t="s">
-        <v>396</v>
-      </c>
-      <c r="U11" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="I11" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="J11" t="s">
+        <v>438</v>
+      </c>
+      <c r="K11" t="s">
+        <v>439</v>
+      </c>
+      <c r="L11" t="s">
+        <v>440</v>
+      </c>
+      <c r="M11" t="s">
+        <v>441</v>
+      </c>
+      <c r="N11" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>447</v>
-      </c>
-      <c r="D12" t="s">
-        <v>330</v>
-      </c>
-      <c r="E12" t="s">
-        <v>430</v>
-      </c>
-      <c r="F12" t="s">
-        <v>160</v>
-      </c>
-      <c r="O12" s="34">
-        <v>44862</v>
-      </c>
-      <c r="P12">
-        <v>123</v>
-      </c>
-      <c r="Q12">
-        <v>4242424242424240</v>
-      </c>
-      <c r="R12" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+      <c r="W12" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>413</v>
+        <v>398</v>
+      </c>
+      <c r="D13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F13" t="s">
+        <v>288</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="M13" s="7"/>
+      <c r="O13" s="23"/>
+      <c r="R13" t="s">
+        <v>394</v>
+      </c>
+      <c r="T13" t="s">
+        <v>396</v>
+      </c>
+      <c r="U13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>447</v>
+      </c>
+      <c r="D14" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F14" t="s">
+        <v>160</v>
+      </c>
+      <c r="O14" s="34">
+        <v>44862</v>
+      </c>
+      <c r="P14">
+        <v>123</v>
+      </c>
+      <c r="Q14">
+        <v>4242424242424240</v>
+      </c>
+      <c r="R14" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>413</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>32480</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L15" t="s">
         <v>419</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M15" t="s">
         <v>423</v>
       </c>
-      <c r="N13">
+      <c r="N15">
         <v>61132300</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="R5" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="R6" r:id="rId2" xr:uid="{D744BE2B-C64A-4C73-8428-F9F807BCE02C}"/>
+    <hyperlink ref="R7" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="R8" r:id="rId2" xr:uid="{D744BE2B-C64A-4C73-8428-F9F807BCE02C}"/>
+    <hyperlink ref="R5" r:id="rId3" xr:uid="{D38FF484-E094-4F39-B9D2-7417DAADB5CF}"/>
+    <hyperlink ref="R6" r:id="rId4" xr:uid="{F2137B4D-3C10-4FC2-9D27-5E884C325C05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7682,22 +7784,22 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="19" width="33" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7831,7 +7933,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7879,7 +7981,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -7933,7 +8035,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>398</v>
       </c>
@@ -7953,7 +8055,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>399</v>
       </c>
@@ -7973,7 +8075,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>400</v>
       </c>
@@ -7999,7 +8101,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -8022,7 +8124,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -8045,7 +8147,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>498</v>
       </c>
@@ -8053,7 +8155,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>513</v>
       </c>
@@ -8067,7 +8169,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>514</v>
       </c>
@@ -8081,7 +8183,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>515</v>
       </c>
@@ -8095,7 +8197,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>516</v>
       </c>
@@ -8109,7 +8211,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>517</v>
       </c>
@@ -8132,14 +8234,14 @@
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="8" width="20.85546875" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="8" width="20.88671875" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:124" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8513,7 +8615,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8593,7 +8695,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>237</v>
       </c>
@@ -8616,7 +8718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -8640,7 +8742,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>381</v>
       </c>
@@ -8703,7 +8805,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>383</v>
       </c>
@@ -8724,7 +8826,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>385</v>
       </c>
@@ -8740,7 +8842,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>355</v>
       </c>
@@ -8748,7 +8850,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>386</v>
       </c>
@@ -8763,7 +8865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>312</v>
       </c>
@@ -8774,7 +8876,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.3">
       <c r="DO11" s="17"/>
     </row>
   </sheetData>
@@ -8790,9 +8892,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8896,7 +8998,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8910,7 +9012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8990,7 +9092,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -9022,7 +9124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -9054,7 +9156,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -9086,7 +9188,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -9094,7 +9196,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>461</v>
       </c>
@@ -9105,7 +9207,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
doller symbol changes for the admin testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C42C58-20A8-4F98-80D6-4A7C2F959ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925DF5DD-5A0D-4CF7-8EE7-AFB70E846208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="532">
   <si>
     <t>DataSet</t>
   </si>
@@ -1623,6 +1623,12 @@
   </si>
   <si>
     <t>habogi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -7008,10 +7014,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:AT15"/>
+  <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7032,7 +7038,7 @@
     <col min="23" max="23" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7133,46 +7139,49 @@
         <v>194</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7202,38 +7211,38 @@
       <c r="Z2" t="s">
         <v>12</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>228</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>229</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>141</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>142</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>230</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>5</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>231</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>30</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>232</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -7287,7 +7296,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -7332,7 +7341,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>522</v>
       </c>
@@ -7388,8 +7397,11 @@
       <c r="AG5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AH5" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>525</v>
       </c>
@@ -7445,8 +7457,11 @@
       <c r="AG6" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AH6" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>519</v>
       </c>
@@ -7502,8 +7517,11 @@
       <c r="AG7" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AH7" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>399</v>
       </c>
@@ -7570,8 +7588,11 @@
       <c r="AG8" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AH8" s="17" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>424</v>
       </c>
@@ -7612,7 +7633,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>425</v>
       </c>
@@ -7648,7 +7669,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>436</v>
       </c>
@@ -7679,7 +7700,7 @@
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>443</v>
       </c>
@@ -7690,7 +7711,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>398</v>
       </c>
@@ -7715,7 +7736,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>447</v>
       </c>
@@ -7741,7 +7762,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>413</v>
       </c>

</xml_diff>

<commit_message>
Content Page Validation Test Case 011
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Admin/GoldAdminTestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE55AE8A-BA6C-43C1-80B4-219C6DAA6CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A602121-56C8-49E4-B6E9-2FB7047F51B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23880" windowHeight="10170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valueprop" sheetId="1" r:id="rId1"/>
     <sheet name="Cardtile,PLP,CLP" sheetId="2" r:id="rId2"/>
-    <sheet name="Herobanner" sheetId="3" r:id="rId3"/>
+    <sheet name="Content" sheetId="3" r:id="rId3"/>
     <sheet name="ProductSlider" sheetId="4" r:id="rId4"/>
     <sheet name="Catalog" sheetId="5" r:id="rId5"/>
     <sheet name="Retailer OrderPlacement" sheetId="11" r:id="rId6"/>
@@ -22,6 +22,7 @@
     <sheet name="Category" sheetId="8" r:id="rId12"/>
     <sheet name="CatalogPricerule" sheetId="12" r:id="rId13"/>
     <sheet name="Retailer RMA" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="531">
   <si>
     <t>DataSet</t>
   </si>
@@ -1340,6 +1341,9 @@
     <t>Lotus$mk2022</t>
   </si>
   <si>
+    <t>Ackpgkyatnob4!</t>
+  </si>
+  <si>
     <t>HFProducts</t>
   </si>
   <si>
@@ -1487,15 +1491,15 @@
     <t>Testmonialqa</t>
   </si>
   <si>
-    <t>32 oz Wide Mouth - Laguna</t>
-  </si>
-  <si>
     <t>Test_Grouped</t>
   </si>
   <si>
     <t>32480,11234000</t>
   </si>
   <si>
+    <t>59.99,19.99</t>
+  </si>
+  <si>
     <t>Qatestvalueprop</t>
   </si>
   <si>
@@ -1517,40 +1521,70 @@
     <t>https://hydroflask-sandbox.kustomerapp.com/login</t>
   </si>
   <si>
-    <t>vnarra@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>&lt;i&lt;3k@1999</t>
-  </si>
-  <si>
-    <t>TL-W40BTS-120,SFS001,SSSFX</t>
-  </si>
-  <si>
-    <t>Store_Selection</t>
-  </si>
-  <si>
-    <t>QA Testing</t>
-  </si>
-  <si>
-    <t>Drybar</t>
-  </si>
-  <si>
-    <t>https://mcloud-na-preprod.drybar.com/</t>
-  </si>
-  <si>
-    <t>Drybar | Premium Hair Care Created for the Perfect Blowout</t>
-  </si>
-  <si>
-    <t>10 QA Test Dry</t>
-  </si>
-  <si>
-    <t>QA Testing Dry</t>
-  </si>
-  <si>
-    <t>Drybar_PreProd_URL</t>
-  </si>
-  <si>
-    <t>Drybar_PageTitle</t>
+    <t xml:space="preserve">HerobannerImage </t>
+  </si>
+  <si>
+    <t>Contact us</t>
+  </si>
+  <si>
+    <t>QAButton</t>
+  </si>
+  <si>
+    <t>qacontent</t>
+  </si>
+  <si>
+    <t>OxoProduct</t>
+  </si>
+  <si>
+    <t>Daylite® Sling</t>
+  </si>
+  <si>
+    <t>Detox Dry Shampoo Original Scent Jumbo Size</t>
+  </si>
+  <si>
+    <t>Daylite™ Waist</t>
+  </si>
+  <si>
+    <t>Steel Pizza Wheel</t>
+  </si>
+  <si>
+    <t>OXOSKU</t>
+  </si>
+  <si>
+    <t>HYFSKU</t>
+  </si>
+  <si>
+    <t>OSPSKU</t>
+  </si>
+  <si>
+    <t>DBSKU</t>
+  </si>
+  <si>
+    <t>900-1030-4,900-2895-1,900-1385-1</t>
+  </si>
+  <si>
+    <t>HydroflaskProduct</t>
+  </si>
+  <si>
+    <t>OspreyProduct</t>
+  </si>
+  <si>
+    <t>DrybarProduct</t>
+  </si>
+  <si>
+    <t>OspreyEMEAProduct</t>
+  </si>
+  <si>
+    <t>32 oz Wide Mouth - Seagrass</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>This is CLP Banner</t>
+  </si>
+  <si>
+    <t>qatestTitle</t>
   </si>
   <si>
     <t>rbogi@helenoftroy.com</t>
@@ -1559,109 +1593,40 @@
     <t>Ramya@1234</t>
   </si>
   <si>
-    <t>3118700,11234000</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>GRASUSWebsite</t>
-  </si>
-  <si>
-    <t>OXOSKU</t>
-  </si>
-  <si>
-    <t>HFSKU</t>
-  </si>
-  <si>
-    <t>OSPSKU</t>
-  </si>
-  <si>
-    <t>DRYSKU</t>
-  </si>
-  <si>
-    <t>TT32PS474,S18SX001</t>
-  </si>
-  <si>
-    <t>10005241,10006005</t>
-  </si>
-  <si>
-    <t>900-2230-1,900-2225-4</t>
-  </si>
-  <si>
-    <t>DRYStore</t>
-  </si>
-  <si>
-    <t>OSPStore</t>
-  </si>
-  <si>
-    <t>HFStore</t>
-  </si>
-  <si>
-    <t>OXOStore</t>
-  </si>
-  <si>
-    <t>Drybar Store View</t>
-  </si>
-  <si>
-    <t>Osprey US English</t>
-  </si>
-  <si>
-    <t>DRYWebsite</t>
-  </si>
-  <si>
-    <t>OSPWebsite</t>
-  </si>
-  <si>
-    <t>Drybar Website</t>
-  </si>
-  <si>
-    <t>Osprey US</t>
-  </si>
-  <si>
-    <t>araikanti@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>Shipping</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>mmarella@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Mysur#134</t>
-  </si>
-  <si>
-    <t>Drybar Website,OXO Website</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4/28</t>
-  </si>
-  <si>
-    <t>432</t>
-  </si>
-  <si>
-    <t>preprod</t>
-  </si>
-  <si>
-    <t>DRYBAR</t>
-  </si>
-  <si>
-    <t>The Lemon Bar Paddle Brush</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>Standard (5 - 7 Business Days)</t>
+    <t>Lotuswave Software Solutions Private Ltd. CLP Hero Banner</t>
+  </si>
+  <si>
+    <t>QA Testing Hero Banner. Lotuswave Software Solutions Private Ltd</t>
+  </si>
+  <si>
+    <t>Card Tile Block is for testing. Lotuswave Software Solutions Private Ltd</t>
+  </si>
+  <si>
+    <t>category_navigation</t>
+  </si>
+  <si>
+    <t>image3</t>
+  </si>
+  <si>
+    <t>image4</t>
+  </si>
+  <si>
+    <t>PRESS2_2.jpg</t>
+  </si>
+  <si>
+    <t>History_LP_SBS_5.jpg</t>
+  </si>
+  <si>
+    <t>Customizer-Banner-Desktop-2x.jpg</t>
+  </si>
+  <si>
+    <t>TT32PS678,W32BFS,TT40PS752</t>
+  </si>
+  <si>
+    <t>DAYLTPLUSS21,TALON26S21,SOJOURN22F23</t>
+  </si>
+  <si>
+    <t>8717000,11235900,8710100</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1636,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1752,18 +1717,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF303030"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1818,7 +1771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1872,8 +1825,7 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2157,7 +2109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -2254,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>39</v>
@@ -2342,13 +2294,13 @@
         <v>17</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>40</v>
@@ -2520,6 +2472,7 @@
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="78" max="78" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2755,7 +2708,7 @@
         <v>10</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="CA1" s="1" t="s">
         <v>39</v>
@@ -2894,7 +2847,7 @@
       </c>
       <c r="L3" s="2"/>
       <c r="Q3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2929,13 +2882,13 @@
       </c>
       <c r="BW3" s="10"/>
       <c r="BX3" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="BY3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="BZ3" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="CA3" s="2" t="s">
         <v>40</v>
@@ -2985,7 +2938,7 @@
         <v>290</v>
       </c>
       <c r="BQ4" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="BU4" s="2" t="s">
         <v>132</v>
@@ -3126,7 +3079,7 @@
         <v>299</v>
       </c>
       <c r="BQ6" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="BU6" s="2" t="s">
         <v>300</v>
@@ -3686,10 +3639,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3748,7 +3701,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="K6" t="s">
         <v>411</v>
@@ -3761,32 +3714,20 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770B1097-B001-484C-95E3-0CE3DFB81BB0}">
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="13" max="13" width="44.5703125" customWidth="1"/>
-    <col min="14" max="16" width="41.140625" customWidth="1"/>
-    <col min="17" max="17" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3827,87 +3768,81 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>505</v>
+        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>504</v>
+        <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>39</v>
+        <v>357</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>9</v>
+        <v>358</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>358</v>
+        <v>86</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>359</v>
+        <v>390</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>86</v>
+        <v>223</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>390</v>
+        <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>223</v>
+        <v>466</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>5</v>
+        <v>227</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>369</v>
+        <v>270</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>270</v>
+        <v>212</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
-      </c>
-      <c r="V2" s="35" t="s">
-        <v>498</v>
-      </c>
-      <c r="X2" t="s">
+        <v>456</v>
+      </c>
+      <c r="T2" t="s">
+        <v>228</v>
+      </c>
+      <c r="V2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>360</v>
       </c>
@@ -3923,11 +3858,11 @@
       <c r="G3" t="s">
         <v>114</v>
       </c>
-      <c r="S3">
+      <c r="Q3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>363</v>
       </c>
@@ -3946,33 +3881,31 @@
       <c r="L4" t="s">
         <v>366</v>
       </c>
-      <c r="T4" t="s">
+      <c r="R4" t="s">
         <v>252</v>
       </c>
-      <c r="U4" t="s">
+      <c r="S4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>307</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="P5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3980,146 +3913,118 @@
         <v>141</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" t="s">
+        <v>478</v>
+      </c>
+      <c r="O6" t="s">
         <v>142</v>
       </c>
-      <c r="R6" t="s">
+      <c r="P6" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>391</v>
       </c>
-      <c r="W7">
+      <c r="U7">
         <v>10</v>
       </c>
-      <c r="Z7">
+      <c r="X7">
         <v>1</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AB7" t="s">
         <v>244</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AC7" t="s">
         <v>17</v>
       </c>
-      <c r="AF7">
+      <c r="AD7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>392</v>
       </c>
-      <c r="W8">
+      <c r="U8">
         <v>20</v>
       </c>
-      <c r="Z8">
+      <c r="X8">
         <v>2</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AB8" t="s">
         <v>244</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AE8" t="s">
         <v>355</v>
       </c>
-      <c r="AH8">
+      <c r="AF8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>234</v>
       </c>
+      <c r="T9" t="s">
+        <v>228</v>
+      </c>
       <c r="V9" t="s">
-        <v>228</v>
-      </c>
-      <c r="X9" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>237</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="O10" t="s">
         <v>40</v>
       </c>
-      <c r="O10" t="s">
-        <v>501</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="P10" t="s">
         <v>238</v>
       </c>
-      <c r="Y10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="W10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>388</v>
       </c>
-      <c r="Z11" s="35" t="s">
-        <v>498</v>
-      </c>
-      <c r="AA11" s="35" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="Y11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>326</v>
       </c>
-      <c r="AB12">
+      <c r="Z12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>463</v>
-      </c>
-      <c r="AC13" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA13" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>499</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="V14" t="s">
-        <v>503</v>
-      </c>
-      <c r="W14">
-        <v>10</v>
-      </c>
-      <c r="X14" t="s">
-        <v>502</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M5" r:id="rId1" xr:uid="{01CEA421-2E8E-4152-818D-7A1E87447EB6}"/>
-    <hyperlink ref="M6" r:id="rId2" xr:uid="{7A468824-E13D-4C09-B78B-F15BD4621476}"/>
-    <hyperlink ref="N6" r:id="rId3" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
-    <hyperlink ref="M10" r:id="rId4" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
-    <hyperlink ref="P10" r:id="rId5" xr:uid="{933C8FD1-C89E-45F3-A409-5845C2648897}"/>
+    <hyperlink ref="N5" r:id="rId2" xr:uid="{D7DAD218-128F-4387-8E33-93E5524ACF59}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{7A468824-E13D-4C09-B78B-F15BD4621476}"/>
+    <hyperlink ref="N6" r:id="rId4" xr:uid="{749F65AE-9E9B-496A-9C27-5BF63FAD954A}"/>
+    <hyperlink ref="M10" r:id="rId5" xr:uid="{74EE04EC-FBFA-4ABB-89F7-C42507901B71}"/>
+    <hyperlink ref="N10" r:id="rId6" xr:uid="{05DB7605-785C-4F54-9C95-FDDA7B131849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4192,7 +4097,7 @@
         <v>395</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>181</v>
@@ -4266,10 +4171,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
         <v>489</v>
-      </c>
-      <c r="C2" t="s">
-        <v>488</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="32">
@@ -4294,7 +4199,7 @@
         <v>229</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AF2" t="s">
         <v>230</v>
@@ -4353,13 +4258,13 @@
         <v>396</v>
       </c>
       <c r="O3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="P3" t="s">
         <v>243</v>
       </c>
       <c r="U3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="V3" t="s">
         <v>333</v>
@@ -4384,12 +4289,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B939B710-87C9-437F-98E2-7A51873973A9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4400,13 +4317,14 @@
     <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="47.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="83" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.7109375" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" customWidth="1"/>
+    <col min="21" max="21" width="31.140625" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" customWidth="1"/>
     <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="26.140625" customWidth="1"/>
     <col min="29" max="29" width="37.140625" bestFit="1" customWidth="1"/>
@@ -4414,7 +4332,7 @@
     <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="44.28515625" customWidth="1"/>
     <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -5522,20 +5440,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:CY4"/>
+  <dimension ref="A1:DO9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="70.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1"/>
     <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="27.140625" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" customWidth="1"/>
+    <col min="32" max="32" width="22.85546875" customWidth="1"/>
+    <col min="33" max="33" width="34.7109375" customWidth="1"/>
+    <col min="34" max="35" width="25.5703125" customWidth="1"/>
+    <col min="36" max="36" width="21.42578125" customWidth="1"/>
+    <col min="38" max="38" width="24.28515625" customWidth="1"/>
+    <col min="43" max="43" width="22.85546875" customWidth="1"/>
+    <col min="46" max="46" width="21" customWidth="1"/>
+    <col min="49" max="49" width="18.5703125" customWidth="1"/>
+    <col min="50" max="50" width="23.140625" customWidth="1"/>
+    <col min="51" max="51" width="20.28515625" customWidth="1"/>
+    <col min="52" max="52" width="22.7109375" customWidth="1"/>
+    <col min="55" max="55" width="23.42578125" customWidth="1"/>
+    <col min="56" max="56" width="23" customWidth="1"/>
+    <col min="82" max="82" width="18.85546875" customWidth="1"/>
+    <col min="83" max="83" width="54.42578125" customWidth="1"/>
+    <col min="84" max="84" width="39.7109375" customWidth="1"/>
+    <col min="85" max="85" width="54" customWidth="1"/>
+    <col min="87" max="87" width="15.7109375" customWidth="1"/>
+    <col min="92" max="92" width="55.85546875" customWidth="1"/>
+    <col min="93" max="93" width="26.7109375" customWidth="1"/>
+    <col min="107" max="107" width="13.140625" customWidth="1"/>
+    <col min="109" max="109" width="19" customWidth="1"/>
+    <col min="110" max="110" width="22.5703125" customWidth="1"/>
+    <col min="111" max="111" width="23.28515625" customWidth="1"/>
+    <col min="112" max="112" width="24.85546875" customWidth="1"/>
+    <col min="113" max="113" width="18.28515625" customWidth="1"/>
+    <col min="114" max="114" width="20.85546875" customWidth="1"/>
+    <col min="115" max="115" width="17.5703125" customWidth="1"/>
+    <col min="116" max="116" width="20.5703125" customWidth="1"/>
+    <col min="117" max="117" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:119" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5609,7 +5563,7 @@
         <v>58</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>23</v>
@@ -5633,222 +5587,270 @@
         <v>63</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="BC1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="CC1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="CG1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CP1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CR1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CS1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CT1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="CR1" s="5" t="s">
+      <c r="CU1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="CS1" s="5" t="s">
+      <c r="CV1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="CT1" s="5" t="s">
+      <c r="CW1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="CU1" s="6" t="s">
+      <c r="CX1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="CV1" s="6" t="s">
+      <c r="CY1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="CW1" s="6" t="s">
+      <c r="CZ1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="CX1" s="6" t="s">
+      <c r="DA1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="CY1" s="6" t="s">
+      <c r="DB1" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+      <c r="DC1" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="DD1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="DE1" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="DF1" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="DG1" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="DH1" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="DI1" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="DJ1" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="DK1" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="DL1" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="DM1" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="DN1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="DO1" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>514</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5856,8 +5858,8 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>198</v>
+      <c r="L2" s="35" t="s">
+        <v>520</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -5870,10 +5872,10 @@
         <v>114</v>
       </c>
       <c r="V2" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>320</v>
@@ -5884,15 +5886,15 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
-      <c r="AG2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AL2" t="s">
         <v>151</v>
       </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
@@ -5900,112 +5902,118 @@
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
-      <c r="AT2" t="s">
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" t="s">
         <v>200</v>
       </c>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="BC2" t="s">
         <v>201</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BD2" t="s">
         <v>202</v>
       </c>
-      <c r="BB2" s="2"/>
-      <c r="BU2" s="13"/>
-      <c r="BV2" s="13" t="s">
+      <c r="BE2" s="2"/>
+      <c r="BX2" s="13"/>
+      <c r="BY2" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="BW2" s="13" t="s">
+      <c r="BZ2" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CA2" t="s">
         <v>15</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CB2" t="s">
         <v>16</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CC2" t="s">
         <v>17</v>
       </c>
-      <c r="CA2" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CD2" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="CH2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="CI2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="CJ2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="CN2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="CC2" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="CD2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="CE2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="CF2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="CG2" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="CK2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="CL2" t="s">
+      <c r="CO2" t="s">
         <v>207</v>
       </c>
-      <c r="CM2">
+      <c r="CP2">
         <v>12</v>
       </c>
-      <c r="CN2">
+      <c r="CQ2">
         <v>13</v>
       </c>
-      <c r="CO2">
+      <c r="CR2">
         <v>14</v>
       </c>
-      <c r="CP2">
+      <c r="CS2">
         <v>15</v>
       </c>
-      <c r="CQ2">
+      <c r="CT2">
         <v>16</v>
       </c>
-      <c r="CR2">
+      <c r="CU2">
         <v>11</v>
       </c>
-      <c r="CS2">
+      <c r="CV2">
         <v>17</v>
       </c>
-      <c r="CT2">
+      <c r="CW2">
         <v>10</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CX2" t="s">
         <v>13</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CY2" t="s">
         <v>208</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CZ2" t="s">
         <v>208</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="DA2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+      <c r="DC2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:119" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>409</v>
       </c>
@@ -6013,17 +6021,240 @@
         <v>411</v>
       </c>
     </row>
+    <row r="5" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>495</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>497</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>202</v>
+      </c>
+      <c r="CB6" s="7"/>
+      <c r="CD6" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="CE6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF6" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="CG6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="CN6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="CP6">
+        <v>55</v>
+      </c>
+      <c r="DB6" t="s">
+        <v>212</v>
+      </c>
+      <c r="DD6" t="s">
+        <v>114</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:119" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>497</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>151</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>202</v>
+      </c>
+      <c r="CD7" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="CE7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF7" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="CG7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="CI7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="CN7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="DC7" t="s">
+        <v>312</v>
+      </c>
+      <c r="DD7" t="s">
+        <v>114</v>
+      </c>
+      <c r="DE7" t="s">
+        <v>503</v>
+      </c>
+      <c r="DF7" s="20" t="s">
+        <v>513</v>
+      </c>
+      <c r="DG7" t="s">
+        <v>500</v>
+      </c>
+      <c r="DH7" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="DI7" t="s">
+        <v>502</v>
+      </c>
+      <c r="DJ7" s="22" t="s">
+        <v>530</v>
+      </c>
+      <c r="DK7" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="DL7" s="22" t="s">
+        <v>529</v>
+      </c>
+      <c r="DM7" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="DN7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" t="s">
+        <v>519</v>
+      </c>
+      <c r="S8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>527</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>526</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>525</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>167</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>129</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>515</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>15</v>
+      </c>
+      <c r="CD8" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="CG8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DC8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" t="s">
+        <v>521</v>
+      </c>
+      <c r="S9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>522</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>497</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>516</v>
+      </c>
+      <c r="CD9" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="CG9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DC9" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="CB2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="CD2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="CK2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="CE2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="CG2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="CN2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
     <hyperlink ref="Z2" r:id="rId4" xr:uid="{43AE1D6B-A8FC-477C-83DE-DA74A954CCEF}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{21721A70-E97D-4EE3-8CE3-5AEC0F2AA320}"/>
-    <hyperlink ref="CC2" r:id="rId6" xr:uid="{80112893-C12E-403E-A8BC-5798F689F083}"/>
+    <hyperlink ref="CF2" r:id="rId6" xr:uid="{80112893-C12E-403E-A8BC-5798F689F083}"/>
     <hyperlink ref="Y2" r:id="rId7" xr:uid="{62DC118F-1CA7-43F0-B74E-A134C0ADFC5E}"/>
+    <hyperlink ref="CN7" r:id="rId8" xr:uid="{138FD361-642A-4ED2-AC8B-F3B54730A49E}"/>
+    <hyperlink ref="CN6" r:id="rId9" xr:uid="{6721425E-A255-4D75-907F-D389AA879CA3}"/>
+    <hyperlink ref="CE6" r:id="rId10" xr:uid="{77FA8301-3CF4-4D8B-ABEB-04C65E5CF446}"/>
+    <hyperlink ref="CE7" r:id="rId11" xr:uid="{3A5B6C6A-A936-4236-9CCF-FF725B33CBF0}"/>
+    <hyperlink ref="CF6" r:id="rId12" xr:uid="{A9EFA7A8-0106-4CAE-A211-01E64635E8C1}"/>
+    <hyperlink ref="CF7" r:id="rId13" xr:uid="{9EF1CB7E-C1EA-4B1A-9C2E-1F2296E13944}"/>
+    <hyperlink ref="C3" r:id="rId14" xr:uid="{6C932D3F-6A8A-4F03-9894-4189DFF27CAF}"/>
+    <hyperlink ref="CG6:CG8" r:id="rId15" display="https://mcloud-na-preprod.drybar.com/" xr:uid="{CC52AACC-9DD3-49A6-B8A6-AE252994F7DE}"/>
+    <hyperlink ref="CG6" r:id="rId16" xr:uid="{BEBCFA7D-4339-4329-9722-F4E67128B662}"/>
+    <hyperlink ref="CG7:CG9" r:id="rId17" display="https://mcloud-na-preprod.drybar.com/" xr:uid="{34D859A8-E2DF-4F71-9026-F2ECE09E21B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -6031,13 +6262,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CW6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CI5" sqref="CI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="69" max="69" width="49.140625" customWidth="1"/>
+    <col min="99" max="99" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7025,7 +7258,7 @@
         <v>391</v>
       </c>
       <c r="AB6" s="17" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -7046,10 +7279,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED12F1E-A6DA-41B0-BA9F-74E8E6545D98}">
-  <dimension ref="A1:BF12"/>
+  <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="X4" workbookViewId="0">
+      <selection sqref="A1:AT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7065,15 +7298,9 @@
     <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="18.140625" customWidth="1"/>
     <col min="23" max="23" width="11.5703125" customWidth="1"/>
-    <col min="47" max="49" width="30.42578125" customWidth="1"/>
-    <col min="51" max="53" width="18.7109375" customWidth="1"/>
-    <col min="54" max="54" width="16.42578125" customWidth="1"/>
-    <col min="55" max="55" width="17.140625" customWidth="1"/>
-    <col min="56" max="56" width="16" customWidth="1"/>
-    <col min="57" max="57" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7096,7 +7323,7 @@
         <v>326</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>415</v>
@@ -7212,52 +7439,16 @@
       <c r="AT1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
     